<commit_message>
docs: Updated till 3rd March 2025
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28619"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28627"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="5659" documentId="11_A036919BCEDCCEE3E979BAFA8980FCDE016F55DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F434F9EB-B0B6-4B2B-AC2F-573712F1BA8F}"/>
+  <xr:revisionPtr revIDLastSave="5665" documentId="11_A036919BCEDCCEE3E979BAFA8980FCDE016F55DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE494D25-A17B-4A68-A534-563B1B9BD649}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="3" r:id="rId1"/>
@@ -1485,12 +1485,12 @@
   </si>
   <si>
     <t>Additional Expense
-    - Cigarette Egg - $325
+    - Cigarette Egg - $0
     - See the psycharitic Doctor ~ $125</t>
   </si>
   <si>
     <t>Additional Expense
-    - Cigarette Egg - $325
+    - Cigarette Egg - $0
     - Add In value for Google Play ~ $150 (don't need to
    include.)
     - See the psycharitic Doctor For Injection ~ $19
@@ -1591,10 +1591,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+    <numFmt numFmtId="178" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="179" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -2316,7 +2316,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2">
+    <xf numFmtId="177" fontId="5" fillId="3" borderId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" applyProtection="0">
@@ -2328,7 +2328,7 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2342,13 +2342,13 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="9" xfId="3" applyFont="1" applyBorder="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="9" xfId="3" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2371,10 +2371,10 @@
     <xf numFmtId="0" fontId="14" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2389,7 +2389,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2406,16 +2406,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2438,7 +2438,7 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2489,7 +2489,7 @@
     <xf numFmtId="40" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="40" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2513,7 +2513,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="20" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="20" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2541,10 +2541,10 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="20" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="20" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2553,10 +2553,10 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="20" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="20" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2568,17 +2568,17 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2596,25 +2596,25 @@
     <xf numFmtId="49" fontId="16" fillId="3" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="4" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2623,21 +2623,30 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="27" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="27" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2663,15 +2672,6 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2687,7 +2687,7 @@
     <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2787,10 +2787,10 @@
     <xf numFmtId="49" fontId="16" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2805,10 +2805,10 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="4" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2823,7 +2823,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2835,10 +2835,10 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="14" fillId="6" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="14" fillId="6" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2937,19 +2937,19 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="20" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="20" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2994,16 +2994,16 @@
     <xf numFmtId="49" fontId="16" fillId="0" borderId="35" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="37" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="36" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="22" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3075,7 +3075,7 @@
     <xf numFmtId="49" fontId="16" fillId="0" borderId="23" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3129,10 +3129,10 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3198,16 +3198,16 @@
     <xf numFmtId="49" fontId="16" fillId="0" borderId="20" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="14" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3217,9 +3217,9 @@
     <cellStyle name="Item Label" xfId="2" xr:uid="{450D122A-8CCB-4DAE-9777-BE5D783E52D6}"/>
     <cellStyle name="Item Text" xfId="6" xr:uid="{30C45D48-83A0-4679-9718-D003D71F93B4}"/>
     <cellStyle name="Legend Sub Header" xfId="1" xr:uid="{D3A4CEDB-A787-40C8-849C-05D075AD4F44}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Revenue Header Font" xfId="5" xr:uid="{7D81E746-ACE1-4A30-98F1-0801F38840B8}"/>
     <cellStyle name="Total Label" xfId="4" xr:uid="{593DEE20-3898-4E84-8526-B94A0DC45249}"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="860">
     <dxf>
@@ -7677,7 +7677,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -7691,7 +7691,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -7702,7 +7702,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -7713,7 +7713,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -7727,7 +7727,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -7738,7 +7738,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -7749,7 +7749,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -7763,7 +7763,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -7774,7 +7774,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -7785,7 +7785,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -7799,7 +7799,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -7810,7 +7810,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -7821,7 +7821,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -8326,7 +8326,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -8340,7 +8340,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -8351,7 +8351,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -8362,7 +8362,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -8376,7 +8376,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -8387,7 +8387,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -8398,7 +8398,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -8409,7 +8409,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -8423,7 +8423,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -8434,7 +8434,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -8445,7 +8445,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -8456,7 +8456,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -8470,7 +8470,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -8481,7 +8481,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -8492,7 +8492,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -8957,7 +8957,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -8971,7 +8971,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -8982,7 +8982,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -8993,7 +8993,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9007,7 +9007,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9018,7 +9018,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9029,7 +9029,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9040,7 +9040,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9054,7 +9054,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9065,7 +9065,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9076,7 +9076,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9087,7 +9087,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9101,7 +9101,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9112,7 +9112,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9123,7 +9123,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9628,7 +9628,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9642,7 +9642,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9653,7 +9653,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9664,7 +9664,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9678,7 +9678,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9689,7 +9689,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9700,7 +9700,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9714,7 +9714,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9725,7 +9725,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9739,7 +9739,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9750,7 +9750,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9761,7 +9761,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9772,7 +9772,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9783,7 +9783,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9794,7 +9794,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9808,7 +9808,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -9819,7 +9819,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10307,7 +10307,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10318,7 +10318,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10332,7 +10332,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10343,7 +10343,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10357,7 +10357,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10368,7 +10368,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10382,7 +10382,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10393,7 +10393,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10407,7 +10407,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10418,7 +10418,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10432,7 +10432,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10443,7 +10443,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10457,7 +10457,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10468,7 +10468,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10482,7 +10482,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10493,7 +10493,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10507,7 +10507,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10518,7 +10518,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10532,7 +10532,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10543,7 +10543,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10557,7 +10557,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10568,7 +10568,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10582,7 +10582,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10593,7 +10593,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10607,7 +10607,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10618,7 +10618,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10632,7 +10632,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10643,7 +10643,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10657,7 +10657,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10668,7 +10668,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10682,7 +10682,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10693,7 +10693,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10704,7 +10704,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10718,7 +10718,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10729,7 +10729,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -10743,7 +10743,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -11228,7 +11228,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -11279,7 +11279,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -11290,7 +11290,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -11321,7 +11321,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -11352,7 +11352,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -11403,7 +11403,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -11928,7 +11928,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
+      <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -12779,12 +12779,12 @@
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="111" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" customHeight="1">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="110" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="11" t="b">
@@ -12840,14 +12840,14 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A10" s="109" t="str">
+      <c r="A10" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,1),"dd mmmm yyyy"),TEXT(B3+(B5-B3)+1,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,2) - 1,"dd mmmm yyyy"),TEXT(B3+(B5-B3)*2+1,"dd mmmm yyyy"))</f>
         <v>20 May 2024 - 19 June 2024</v>
       </c>
       <c r="B10" s="125"/>
     </row>
     <row r="11" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A11" s="109" t="str">
+      <c r="A11" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,2),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*2)+2,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,3) - 1,"dd mmmm yyyy"),TEXT(B3+((B5-B3)*3+2),"dd mmmm yyyy"))</f>
         <v>20 June 2024 - 19 July 2024</v>
       </c>
@@ -12870,14 +12870,14 @@
       <c r="B13" s="120"/>
     </row>
     <row r="14" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A14" s="109" t="str">
+      <c r="A14" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,5),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*5)+5,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,6)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*6)+5),"dd mmmm yyyy"))</f>
         <v>20 September 2024 - 19 October 2024</v>
       </c>
       <c r="B14" s="121"/>
     </row>
     <row r="15" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A15" s="109" t="str">
+      <c r="A15" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,6),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*6)+6,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,7)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*7)+6),"dd mmmm yyyy"))</f>
         <v>20 October 2024 - 19 November 2024</v>
       </c>
@@ -12886,21 +12886,21 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A16" s="109" t="str">
+      <c r="A16" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,7),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*7)+7,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,8)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*8)+7),"dd mmmm yyyy"))</f>
         <v>20 November 2024 - 19 December 2024</v>
       </c>
       <c r="B16" s="120"/>
     </row>
     <row r="17" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A17" s="109" t="str">
+      <c r="A17" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,8),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*8)+8,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,9)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*9)+8),"dd mmmm yyyy"))</f>
         <v>20 December 2024 - 19 January 2025</v>
       </c>
       <c r="B17" s="121"/>
     </row>
     <row r="18" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A18" s="109" t="str">
+      <c r="A18" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,9),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*9)+9,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,10)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*10)+9),"dd mmmm yyyy"))</f>
         <v>20 January 2025 - 19 February 2025</v>
       </c>
@@ -12909,7 +12909,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A19" s="109" t="str">
+      <c r="A19" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,10),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*10)+10,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,11)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*11)+10),"dd mmmm yyyy"))</f>
         <v>20 February 2025 - 19 March 2025</v>
       </c>
@@ -12946,7 +12946,7 @@
       <c r="B23" s="119"/>
     </row>
     <row r="24" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A24" s="109" t="str">
+      <c r="A24" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,15),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*15)+15,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,16)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*16)+15),"dd mmmm yyyy"))</f>
         <v>20 July 2025 - 19 August 2025</v>
       </c>
@@ -12955,21 +12955,21 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A25" s="109" t="str">
+      <c r="A25" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,16),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*16)+16,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,17)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*17)+16),"dd mmmm yyyy"))</f>
         <v>20 August 2025 - 19 September 2025</v>
       </c>
       <c r="B25" s="118"/>
     </row>
     <row r="26" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A26" s="108" t="str">
+      <c r="A26" s="111" t="str">
         <f>IF(B2,TEXT(EDATE(B3,17),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*17)+17,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,18)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*18)+17),"dd mmmm yyyy"))</f>
         <v>20 September 2025 - 19 October 2025</v>
       </c>
       <c r="B26" s="119"/>
     </row>
     <row r="27" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A27" s="109" t="str">
+      <c r="A27" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,18),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*18)+18,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,19)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*19)+18),"dd mmmm yyyy"))</f>
         <v>20 October 2025 - 19 November 2025</v>
       </c>
@@ -12978,21 +12978,21 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A28" s="109" t="str">
+      <c r="A28" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,19),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*19)+19,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,20)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*20)+19),"dd mmmm yyyy"))</f>
         <v>20 November 2025 - 19 December 2025</v>
       </c>
       <c r="B28" s="118"/>
     </row>
     <row r="29" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A29" s="108" t="str">
+      <c r="A29" s="111" t="str">
         <f>IF(B2,TEXT(EDATE(B3,20),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*20)+20,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,21)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*21)+20),"dd mmmm yyyy"))</f>
         <v>20 December 2025 - 19 January 2026</v>
       </c>
       <c r="B29" s="119"/>
     </row>
     <row r="30" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A30" s="109" t="str">
+      <c r="A30" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,21),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*21)+21,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,22)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*22)+21),"dd mmmm yyyy"))</f>
         <v>20 January 2026 - 19 February 2026</v>
       </c>
@@ -13001,21 +13001,21 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A31" s="109" t="str">
+      <c r="A31" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,22),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*22)+22,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,23)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*23)+22),"dd mmmm yyyy"))</f>
         <v>20 February 2026 - 19 March 2026</v>
       </c>
       <c r="B31" s="118"/>
     </row>
     <row r="32" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A32" s="108" t="str">
+      <c r="A32" s="111" t="str">
         <f>IF(B2,TEXT(EDATE(B3,23),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*23)+23,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,24)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*24)+23),"dd mmmm yyyy"))</f>
         <v>20 March 2026 - 19 April 2026</v>
       </c>
       <c r="B32" s="119"/>
     </row>
     <row r="33" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A33" s="109" t="str">
+      <c r="A33" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,24),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*24)+24,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,25)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*25)+24),"dd mmmm yyyy"))</f>
         <v>20 April 2026 - 19 May 2026</v>
       </c>
@@ -13024,21 +13024,21 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A34" s="109" t="str">
+      <c r="A34" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,25),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*25)+25,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,26)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*26)+25),"dd mmmm yyyy"))</f>
         <v>20 May 2026 - 19 June 2026</v>
       </c>
       <c r="B34" s="118"/>
     </row>
     <row r="35" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A35" s="108" t="str">
+      <c r="A35" s="111" t="str">
         <f>IF(B2,TEXT(EDATE(B3,26),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*26)+26,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,27)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*27)+26),"dd mmmm yyyy"))</f>
         <v>20 June 2026 - 19 July 2026</v>
       </c>
       <c r="B35" s="119"/>
     </row>
     <row r="36" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A36" s="109" t="str">
+      <c r="A36" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,27),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*27)+27,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,28)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*28)+27),"dd mmmm yyyy"))</f>
         <v>20 July 2026 - 19 August 2026</v>
       </c>
@@ -13047,21 +13047,21 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A37" s="109" t="str">
+      <c r="A37" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,28),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*28)+28,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,29)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*29)+28),"dd mmmm yyyy"))</f>
         <v>20 August 2026 - 19 September 2026</v>
       </c>
       <c r="B37" s="118"/>
     </row>
     <row r="38" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A38" s="108" t="str">
+      <c r="A38" s="111" t="str">
         <f>IF(B2,TEXT(EDATE(B3,29),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*29)+29,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,30)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*30)+29),"dd mmmm yyyy"))</f>
         <v>20 September 2026 - 19 October 2026</v>
       </c>
       <c r="B38" s="119"/>
     </row>
     <row r="39" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A39" s="109" t="str">
+      <c r="A39" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,30),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*30)+30,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,31)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*31)+30),"dd mmmm yyyy"))</f>
         <v>20 October 2026 - 19 November 2026</v>
       </c>
@@ -13070,21 +13070,21 @@
       </c>
     </row>
     <row r="40" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A40" s="109" t="str">
+      <c r="A40" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,31),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*31)+31,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,32)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*32)+31),"dd mmmm yyyy"))</f>
         <v>20 November 2026 - 19 December 2026</v>
       </c>
       <c r="B40" s="118"/>
     </row>
     <row r="41" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A41" s="108" t="str">
+      <c r="A41" s="111" t="str">
         <f>IF(B2,TEXT(EDATE(B3,32),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*32)+32,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,33)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*33)+32),"dd mmmm yyyy"))</f>
         <v>20 December 2026 - 19 January 2027</v>
       </c>
       <c r="B41" s="119"/>
     </row>
     <row r="42" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A42" s="109" t="str">
+      <c r="A42" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,33),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*33)+33,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,34)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*34)+33),"dd mmmm yyyy"))</f>
         <v>20 January 2027 - 19 February 2027</v>
       </c>
@@ -13093,21 +13093,21 @@
       </c>
     </row>
     <row r="43" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A43" s="109" t="str">
+      <c r="A43" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,34),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*34)+34,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,35)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*35)+34),"dd mmmm yyyy"))</f>
         <v>20 February 2027 - 19 March 2027</v>
       </c>
       <c r="B43" s="118"/>
     </row>
     <row r="44" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A44" s="108" t="str">
+      <c r="A44" s="111" t="str">
         <f>IF(B2,TEXT(EDATE(B3,35),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*35)+35,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,36)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*36)+35),"dd mmmm yyyy"))</f>
         <v>20 March 2027 - 19 April 2027</v>
       </c>
       <c r="B44" s="119"/>
     </row>
     <row r="45" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A45" s="109" t="str">
+      <c r="A45" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,36),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*36)+36,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,37)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*37)+36),"dd mmmm yyyy"))</f>
         <v>20 April 2027 - 19 May 2027</v>
       </c>
@@ -13116,21 +13116,21 @@
       </c>
     </row>
     <row r="46" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A46" s="109" t="str">
+      <c r="A46" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,37),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*37)+37,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,38)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*38)+37),"dd mmmm yyyy"))</f>
         <v>20 May 2027 - 19 June 2027</v>
       </c>
       <c r="B46" s="118"/>
     </row>
     <row r="47" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A47" s="108" t="str">
+      <c r="A47" s="111" t="str">
         <f>IF(B2,TEXT(EDATE(B3,38),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*38)+38,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,39)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*39)+38),"dd mmmm yyyy"))</f>
         <v>20 June 2027 - 19 July 2027</v>
       </c>
       <c r="B47" s="119"/>
     </row>
     <row r="48" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A48" s="109" t="str">
+      <c r="A48" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,39),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*39)+39,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,40)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*40)+39),"dd mmmm yyyy"))</f>
         <v>20 July 2027 - 19 August 2027</v>
       </c>
@@ -13139,21 +13139,21 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A49" s="109" t="str">
+      <c r="A49" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,40),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*40)+40,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,41)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*41)+40),"dd mmmm yyyy"))</f>
         <v>20 August 2027 - 19 September 2027</v>
       </c>
       <c r="B49" s="118"/>
     </row>
     <row r="50" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A50" s="108" t="str">
+      <c r="A50" s="111" t="str">
         <f>IF(B2,TEXT(EDATE(B3,41),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*41)+41,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,42)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*42)+41),"dd mmmm yyyy"))</f>
         <v>20 September 2027 - 19 October 2027</v>
       </c>
       <c r="B50" s="119"/>
     </row>
     <row r="51" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A51" s="109" t="str">
+      <c r="A51" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,42),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*42)+42,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,43)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*43)+42),"dd mmmm yyyy"))</f>
         <v>20 October 2027 - 19 November 2027</v>
       </c>
@@ -13162,21 +13162,21 @@
       </c>
     </row>
     <row r="52" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A52" s="109" t="str">
+      <c r="A52" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,43),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*43)+43,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,44)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*44)+43),"dd mmmm yyyy"))</f>
         <v>20 November 2027 - 19 December 2027</v>
       </c>
       <c r="B52" s="118"/>
     </row>
     <row r="53" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A53" s="108" t="str">
+      <c r="A53" s="111" t="str">
         <f>IF(B2,TEXT(EDATE(B3,44),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*44)+44,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,45)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*45)+44),"dd mmmm yyyy"))</f>
         <v>20 December 2027 - 19 January 2028</v>
       </c>
       <c r="B53" s="119"/>
     </row>
     <row r="54" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A54" s="109" t="str">
+      <c r="A54" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,45),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*45)+45,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,46)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*46)+45),"dd mmmm yyyy"))</f>
         <v>20 January 2028 - 19 February 2028</v>
       </c>
@@ -13185,14 +13185,14 @@
       </c>
     </row>
     <row r="55" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A55" s="109" t="str">
+      <c r="A55" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,46),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*46)+46,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,47)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*47)+46),"dd mmmm yyyy"))</f>
         <v>20 February 2028 - 19 March 2028</v>
       </c>
       <c r="B55" s="118"/>
     </row>
     <row r="56" spans="1:2" ht="20.25" customHeight="1">
-      <c r="A56" s="109" t="str">
+      <c r="A56" s="112" t="str">
         <f>IF(B2,TEXT(EDATE(B3,47),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*47)+47,"dd mmmm yyyy")) &amp; " - " &amp; IF(B2,TEXT(EDATE(B3,48)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*48)+47),"dd mmmm yyyy"))</f>
         <v>20 March 2028 - 19 April 2028</v>
       </c>
@@ -13305,7 +13305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E410128-C7AA-4335-9548-8A1FBFF72764}">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
+    <sheetView topLeftCell="A107" workbookViewId="0">
       <selection activeCell="F130" sqref="F130"/>
     </sheetView>
   </sheetViews>
@@ -13356,7 +13356,7 @@
       </c>
       <c r="C3" s="208">
         <f>E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="D3" s="208"/>
       <c r="E3" s="208"/>
@@ -13372,7 +13372,7 @@
       <c r="B4" s="247"/>
       <c r="C4" s="209">
         <f ca="1">SUM(C2:G3)</f>
-        <v>5125.0999999999995</v>
+        <v>6225.0999999999995</v>
       </c>
       <c r="D4" s="209"/>
       <c r="E4" s="209"/>
@@ -13434,7 +13434,7 @@
       <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="150" t="s">
@@ -13610,7 +13610,7 @@
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A21" s="112" t="s">
+      <c r="A21" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="150" t="s">
@@ -13786,7 +13786,7 @@
       <c r="I32" s="8"/>
     </row>
     <row r="33" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A33" s="112" t="s">
+      <c r="A33" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="150" t="s">
@@ -13968,7 +13968,7 @@
       <c r="B45" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="113" t="s">
+      <c r="C45" s="116" t="s">
         <v>48</v>
       </c>
       <c r="D45" s="42"/>
@@ -15039,7 +15039,7 @@
       <c r="D116" s="204"/>
       <c r="E116" s="55">
         <f>Forecast_8!E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F116" s="42"/>
       <c r="G116" s="42"/>
@@ -15339,7 +15339,7 @@
       <c r="D136" s="190"/>
       <c r="E136" s="29">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F136" s="42"/>
       <c r="G136" s="42"/>
@@ -15431,7 +15431,7 @@
       <c r="D143" s="204"/>
       <c r="E143" s="29">
         <f>E136</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F143" s="42"/>
       <c r="G143" s="42"/>
@@ -15731,7 +15731,7 @@
       <c r="D163" s="190"/>
       <c r="E163" s="38">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F163" s="42"/>
       <c r="G163" s="42"/>
@@ -15823,7 +15823,7 @@
       <c r="D170" s="204"/>
       <c r="E170" s="38">
         <f>E163</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F170" s="42"/>
       <c r="G170" s="42"/>
@@ -16123,7 +16123,7 @@
       <c r="D190" s="190"/>
       <c r="E190" s="38">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F190" s="42"/>
       <c r="G190" s="42"/>
@@ -16634,7 +16634,7 @@
       </c>
       <c r="C3" s="208">
         <f>E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="D3" s="208"/>
       <c r="E3" s="208"/>
@@ -16650,7 +16650,7 @@
       <c r="B4" s="247"/>
       <c r="C4" s="209">
         <f ca="1">SUM(C2:G3)</f>
-        <v>5125.0999999999995</v>
+        <v>6225.0999999999995</v>
       </c>
       <c r="D4" s="209"/>
       <c r="E4" s="209"/>
@@ -16712,7 +16712,7 @@
       <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="150" t="s">
@@ -16888,7 +16888,7 @@
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A21" s="112" t="s">
+      <c r="A21" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="150" t="s">
@@ -17064,7 +17064,7 @@
       <c r="I32" s="8"/>
     </row>
     <row r="33" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A33" s="112" t="s">
+      <c r="A33" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="150" t="s">
@@ -17246,7 +17246,7 @@
       <c r="B45" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="113" t="s">
+      <c r="C45" s="116" t="s">
         <v>48</v>
       </c>
       <c r="D45" s="42"/>
@@ -18317,7 +18317,7 @@
       <c r="D116" s="204"/>
       <c r="E116" s="55">
         <f>Forecast_9!E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F116" s="42"/>
       <c r="G116" s="42"/>
@@ -18617,7 +18617,7 @@
       <c r="D136" s="190"/>
       <c r="E136" s="29">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F136" s="42"/>
       <c r="G136" s="42"/>
@@ -18709,7 +18709,7 @@
       <c r="D143" s="204"/>
       <c r="E143" s="29">
         <f>E136</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F143" s="42"/>
       <c r="G143" s="42"/>
@@ -19009,7 +19009,7 @@
       <c r="D163" s="190"/>
       <c r="E163" s="38">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F163" s="42"/>
       <c r="G163" s="42"/>
@@ -19101,7 +19101,7 @@
       <c r="D170" s="204"/>
       <c r="E170" s="38">
         <f>E163</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F170" s="42"/>
       <c r="G170" s="42"/>
@@ -19401,7 +19401,7 @@
       <c r="D190" s="190"/>
       <c r="E190" s="38">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F190" s="42"/>
       <c r="G190" s="42"/>
@@ -19910,7 +19910,7 @@
       </c>
       <c r="C3" s="208">
         <f>E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="D3" s="208"/>
       <c r="E3" s="208"/>
@@ -19926,7 +19926,7 @@
       <c r="B4" s="247"/>
       <c r="C4" s="209">
         <f ca="1">SUM(C2:G3)</f>
-        <v>5125.0999999999995</v>
+        <v>6225.0999999999995</v>
       </c>
       <c r="D4" s="209"/>
       <c r="E4" s="209"/>
@@ -19988,7 +19988,7 @@
       <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="150" t="s">
@@ -20164,7 +20164,7 @@
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A21" s="112" t="s">
+      <c r="A21" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="150" t="s">
@@ -20340,7 +20340,7 @@
       <c r="I32" s="8"/>
     </row>
     <row r="33" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A33" s="112" t="s">
+      <c r="A33" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="150" t="s">
@@ -20522,7 +20522,7 @@
       <c r="B45" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="113" t="s">
+      <c r="C45" s="116" t="s">
         <v>48</v>
       </c>
       <c r="D45" s="42"/>
@@ -21593,7 +21593,7 @@
       <c r="D116" s="204"/>
       <c r="E116" s="55">
         <f>Forecast_10!E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F116" s="42"/>
       <c r="G116" s="42"/>
@@ -21893,7 +21893,7 @@
       <c r="D136" s="190"/>
       <c r="E136" s="29">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F136" s="42"/>
       <c r="G136" s="42"/>
@@ -21985,7 +21985,7 @@
       <c r="D143" s="204"/>
       <c r="E143" s="29">
         <f>E136</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F143" s="42"/>
       <c r="G143" s="42"/>
@@ -22285,7 +22285,7 @@
       <c r="D163" s="190"/>
       <c r="E163" s="38">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F163" s="42"/>
       <c r="G163" s="42"/>
@@ -22377,7 +22377,7 @@
       <c r="D170" s="204"/>
       <c r="E170" s="38">
         <f>E163</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F170" s="42"/>
       <c r="G170" s="42"/>
@@ -22677,7 +22677,7 @@
       <c r="D190" s="190"/>
       <c r="E190" s="38">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F190" s="42"/>
       <c r="G190" s="42"/>
@@ -23188,7 +23188,7 @@
       </c>
       <c r="C3" s="208">
         <f>E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="D3" s="208"/>
       <c r="E3" s="208"/>
@@ -23204,7 +23204,7 @@
       <c r="B4" s="247"/>
       <c r="C4" s="209">
         <f ca="1">SUM(C2:G3)</f>
-        <v>5125.0999999999995</v>
+        <v>6225.0999999999995</v>
       </c>
       <c r="D4" s="209"/>
       <c r="E4" s="209"/>
@@ -23266,7 +23266,7 @@
       <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="150" t="s">
@@ -23442,7 +23442,7 @@
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A21" s="112" t="s">
+      <c r="A21" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="150" t="s">
@@ -23618,7 +23618,7 @@
       <c r="I32" s="8"/>
     </row>
     <row r="33" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A33" s="112" t="s">
+      <c r="A33" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="150" t="s">
@@ -23800,7 +23800,7 @@
       <c r="B45" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="113" t="s">
+      <c r="C45" s="116" t="s">
         <v>48</v>
       </c>
       <c r="D45" s="42"/>
@@ -24871,7 +24871,7 @@
       <c r="D116" s="204"/>
       <c r="E116" s="55">
         <f>Forecast_11!E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F116" s="42"/>
       <c r="G116" s="42"/>
@@ -25171,7 +25171,7 @@
       <c r="D136" s="190"/>
       <c r="E136" s="29">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F136" s="42"/>
       <c r="G136" s="42"/>
@@ -25263,7 +25263,7 @@
       <c r="D143" s="204"/>
       <c r="E143" s="29">
         <f>E136</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F143" s="42"/>
       <c r="G143" s="42"/>
@@ -25563,7 +25563,7 @@
       <c r="D163" s="190"/>
       <c r="E163" s="38">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F163" s="42"/>
       <c r="G163" s="42"/>
@@ -25655,7 +25655,7 @@
       <c r="D170" s="204"/>
       <c r="E170" s="38">
         <f>E163</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F170" s="42"/>
       <c r="G170" s="42"/>
@@ -25955,7 +25955,7 @@
       <c r="D190" s="190"/>
       <c r="E190" s="38">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F190" s="42"/>
       <c r="G190" s="42"/>
@@ -26464,7 +26464,7 @@
       </c>
       <c r="C3" s="208">
         <f>E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="D3" s="208"/>
       <c r="E3" s="208"/>
@@ -26480,7 +26480,7 @@
       <c r="B4" s="247"/>
       <c r="C4" s="209">
         <f ca="1">SUM(C2:G3)</f>
-        <v>5125.0999999999995</v>
+        <v>6225.0999999999995</v>
       </c>
       <c r="D4" s="209"/>
       <c r="E4" s="209"/>
@@ -26542,7 +26542,7 @@
       <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="150" t="s">
@@ -26718,7 +26718,7 @@
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A21" s="112" t="s">
+      <c r="A21" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="150" t="s">
@@ -26894,7 +26894,7 @@
       <c r="I32" s="8"/>
     </row>
     <row r="33" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A33" s="112" t="s">
+      <c r="A33" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="150" t="s">
@@ -27076,7 +27076,7 @@
       <c r="B45" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="113" t="s">
+      <c r="C45" s="116" t="s">
         <v>48</v>
       </c>
       <c r="D45" s="42"/>
@@ -28147,7 +28147,7 @@
       <c r="D116" s="204"/>
       <c r="E116" s="55">
         <f>Forecast_12!E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F116" s="42"/>
       <c r="G116" s="42"/>
@@ -28447,7 +28447,7 @@
       <c r="D136" s="190"/>
       <c r="E136" s="29">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F136" s="42"/>
       <c r="G136" s="42"/>
@@ -28539,7 +28539,7 @@
       <c r="D143" s="204"/>
       <c r="E143" s="29">
         <f>E136</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F143" s="42"/>
       <c r="G143" s="42"/>
@@ -28839,7 +28839,7 @@
       <c r="D163" s="190"/>
       <c r="E163" s="38">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F163" s="42"/>
       <c r="G163" s="42"/>
@@ -28931,7 +28931,7 @@
       <c r="D170" s="204"/>
       <c r="E170" s="38">
         <f>E163</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F170" s="42"/>
       <c r="G170" s="42"/>
@@ -29231,7 +29231,7 @@
       <c r="D190" s="190"/>
       <c r="E190" s="38">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F190" s="42"/>
       <c r="G190" s="42"/>
@@ -29741,7 +29741,7 @@
       </c>
       <c r="C3" s="208">
         <f>E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="D3" s="208"/>
       <c r="E3" s="208"/>
@@ -29757,7 +29757,7 @@
       <c r="B4" s="247"/>
       <c r="C4" s="209">
         <f ca="1">SUM(C2:G3)</f>
-        <v>5125.0999999999995</v>
+        <v>6225.0999999999995</v>
       </c>
       <c r="D4" s="209"/>
       <c r="E4" s="209"/>
@@ -29819,7 +29819,7 @@
       <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="150" t="s">
@@ -29995,7 +29995,7 @@
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A21" s="112" t="s">
+      <c r="A21" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="150" t="s">
@@ -30171,7 +30171,7 @@
       <c r="I32" s="8"/>
     </row>
     <row r="33" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A33" s="112" t="s">
+      <c r="A33" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="150" t="s">
@@ -30353,7 +30353,7 @@
       <c r="B45" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="113" t="s">
+      <c r="C45" s="116" t="s">
         <v>48</v>
       </c>
       <c r="D45" s="42"/>
@@ -31424,7 +31424,7 @@
       <c r="D116" s="204"/>
       <c r="E116" s="55">
         <f>Forecast_13!E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F116" s="42"/>
       <c r="G116" s="42"/>
@@ -31724,7 +31724,7 @@
       <c r="D136" s="190"/>
       <c r="E136" s="29">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F136" s="42"/>
       <c r="G136" s="42"/>
@@ -31816,7 +31816,7 @@
       <c r="D143" s="204"/>
       <c r="E143" s="29">
         <f>E136</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F143" s="42"/>
       <c r="G143" s="42"/>
@@ -32116,7 +32116,7 @@
       <c r="D163" s="190"/>
       <c r="E163" s="38">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F163" s="42"/>
       <c r="G163" s="42"/>
@@ -32208,7 +32208,7 @@
       <c r="D170" s="204"/>
       <c r="E170" s="38">
         <f>E163</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F170" s="42"/>
       <c r="G170" s="42"/>
@@ -32508,7 +32508,7 @@
       <c r="D190" s="190"/>
       <c r="E190" s="38">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F190" s="42"/>
       <c r="G190" s="42"/>
@@ -33017,7 +33017,7 @@
       </c>
       <c r="C3" s="208">
         <f>E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="D3" s="208"/>
       <c r="E3" s="208"/>
@@ -33033,7 +33033,7 @@
       <c r="B4" s="247"/>
       <c r="C4" s="209">
         <f ca="1">SUM(C2:G3)</f>
-        <v>5125.0999999999995</v>
+        <v>6225.0999999999995</v>
       </c>
       <c r="D4" s="209"/>
       <c r="E4" s="209"/>
@@ -33095,7 +33095,7 @@
       <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="150" t="s">
@@ -33271,7 +33271,7 @@
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A21" s="112" t="s">
+      <c r="A21" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="150" t="s">
@@ -33447,7 +33447,7 @@
       <c r="I32" s="8"/>
     </row>
     <row r="33" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A33" s="112" t="s">
+      <c r="A33" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="150" t="s">
@@ -33629,7 +33629,7 @@
       <c r="B45" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="113" t="s">
+      <c r="C45" s="116" t="s">
         <v>48</v>
       </c>
       <c r="D45" s="42"/>
@@ -34700,7 +34700,7 @@
       <c r="D116" s="204"/>
       <c r="E116" s="55">
         <f>Forecast_14!E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F116" s="42"/>
       <c r="G116" s="42"/>
@@ -35000,7 +35000,7 @@
       <c r="D136" s="190"/>
       <c r="E136" s="29">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F136" s="42"/>
       <c r="G136" s="42"/>
@@ -35092,7 +35092,7 @@
       <c r="D143" s="204"/>
       <c r="E143" s="29">
         <f>E136</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F143" s="42"/>
       <c r="G143" s="42"/>
@@ -35392,7 +35392,7 @@
       <c r="D163" s="190"/>
       <c r="E163" s="38">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F163" s="42"/>
       <c r="G163" s="42"/>
@@ -35484,7 +35484,7 @@
       <c r="D170" s="204"/>
       <c r="E170" s="38">
         <f>E163</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F170" s="42"/>
       <c r="G170" s="42"/>
@@ -35784,7 +35784,7 @@
       <c r="D190" s="190"/>
       <c r="E190" s="38">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F190" s="42"/>
       <c r="G190" s="42"/>
@@ -36295,7 +36295,7 @@
       </c>
       <c r="C3" s="208">
         <f>E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="D3" s="208"/>
       <c r="E3" s="208"/>
@@ -36311,7 +36311,7 @@
       <c r="B4" s="247"/>
       <c r="C4" s="209">
         <f ca="1">SUM(C2:G3)</f>
-        <v>5125.0999999999995</v>
+        <v>6225.0999999999995</v>
       </c>
       <c r="D4" s="209"/>
       <c r="E4" s="209"/>
@@ -36373,7 +36373,7 @@
       <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="150" t="s">
@@ -36549,7 +36549,7 @@
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A21" s="112" t="s">
+      <c r="A21" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="150" t="s">
@@ -36725,7 +36725,7 @@
       <c r="I32" s="8"/>
     </row>
     <row r="33" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A33" s="112" t="s">
+      <c r="A33" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="150" t="s">
@@ -36907,7 +36907,7 @@
       <c r="B45" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="113" t="s">
+      <c r="C45" s="116" t="s">
         <v>48</v>
       </c>
       <c r="D45" s="42"/>
@@ -37978,7 +37978,7 @@
       <c r="D116" s="204"/>
       <c r="E116" s="55">
         <f>Forecast_15!E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F116" s="42"/>
       <c r="G116" s="42"/>
@@ -38278,7 +38278,7 @@
       <c r="D136" s="190"/>
       <c r="E136" s="29">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F136" s="42"/>
       <c r="G136" s="42"/>
@@ -38370,7 +38370,7 @@
       <c r="D143" s="204"/>
       <c r="E143" s="29">
         <f>E136</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F143" s="42"/>
       <c r="G143" s="42"/>
@@ -38670,7 +38670,7 @@
       <c r="D163" s="190"/>
       <c r="E163" s="38">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F163" s="42"/>
       <c r="G163" s="42"/>
@@ -38762,7 +38762,7 @@
       <c r="D170" s="204"/>
       <c r="E170" s="38">
         <f>E163</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F170" s="42"/>
       <c r="G170" s="42"/>
@@ -39062,7 +39062,7 @@
       <c r="D190" s="190"/>
       <c r="E190" s="38">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F190" s="42"/>
       <c r="G190" s="42"/>
@@ -39601,7 +39601,7 @@
       <c r="D4" s="182" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="114" t="s">
+      <c r="E4" s="117" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="7">
@@ -39633,7 +39633,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="183"/>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="117" t="s">
         <v>33</v>
       </c>
       <c r="F5" s="7">
@@ -39665,7 +39665,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="183"/>
-      <c r="E6" s="114" t="s">
+      <c r="E6" s="117" t="s">
         <v>34</v>
       </c>
       <c r="F6" s="7">
@@ -39698,7 +39698,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="183"/>
-      <c r="E7" s="114" t="s">
+      <c r="E7" s="117" t="s">
         <v>35</v>
       </c>
       <c r="F7" s="7">
@@ -39730,7 +39730,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="183"/>
-      <c r="E8" s="114" t="s">
+      <c r="E8" s="117" t="s">
         <v>36</v>
       </c>
       <c r="F8" s="7">
@@ -39762,7 +39762,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="183"/>
-      <c r="E9" s="114" t="s">
+      <c r="E9" s="117" t="s">
         <v>37</v>
       </c>
       <c r="F9" s="7">
@@ -39795,7 +39795,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="183"/>
-      <c r="E10" s="114" t="s">
+      <c r="E10" s="117" t="s">
         <v>38</v>
       </c>
       <c r="F10" s="7">
@@ -39827,7 +39827,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="183"/>
-      <c r="E11" s="114" t="s">
+      <c r="E11" s="117" t="s">
         <v>39</v>
       </c>
       <c r="F11" s="7">
@@ -39859,7 +39859,7 @@
         <v>51.3</v>
       </c>
       <c r="D12" s="183"/>
-      <c r="E12" s="114" t="s">
+      <c r="E12" s="117" t="s">
         <v>40</v>
       </c>
       <c r="F12" s="7">
@@ -40108,7 +40108,7 @@
       </c>
       <c r="J22" s="73">
         <f>'October 2025 - December 2025'!E136</f>
-        <v>2567.5999999999995</v>
+        <v>2892.5999999999995</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="24.75" customHeight="1">
@@ -40128,11 +40128,11 @@
       </c>
       <c r="J23" s="73">
         <f>'October 2025 - December 2025'!E163</f>
-        <v>3862.8999999999996</v>
+        <v>4512.8999999999996</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="24.75" customHeight="1">
-      <c r="A24" s="112" t="s">
+      <c r="A24" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="150" t="s">
@@ -40153,7 +40153,7 @@
       </c>
       <c r="J24" s="73">
         <f>'October 2025 - December 2025'!E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="34.5" customHeight="1">
@@ -40178,7 +40178,7 @@
       </c>
       <c r="J25" s="73">
         <f>Forecast_8!E136</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="30" customHeight="1">
@@ -40197,7 +40197,7 @@
       </c>
       <c r="J26" s="73">
         <f>Forecast_8!E163</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="30" customHeight="1">
@@ -40216,7 +40216,7 @@
       </c>
       <c r="J27" s="73">
         <f>Forecast_8!E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="30" customHeight="1">
@@ -40235,7 +40235,7 @@
       </c>
       <c r="J28" s="73">
         <f>Forecast_9!E136</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="30" customHeight="1">
@@ -40254,7 +40254,7 @@
       </c>
       <c r="J29" s="73">
         <f>Forecast_9!E163</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="30" customHeight="1">
@@ -40273,7 +40273,7 @@
       </c>
       <c r="J30" s="63">
         <f>Forecast_9!E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="30" customHeight="1">
@@ -40295,7 +40295,7 @@
       </c>
       <c r="J31" s="77">
         <f>Forecast_10!E136</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="30" customHeight="1">
@@ -40305,7 +40305,7 @@
       </c>
       <c r="J32" s="73">
         <f>Forecast_10!E163</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="27.75" customHeight="1">
@@ -40315,7 +40315,7 @@
       </c>
       <c r="J33" s="73">
         <f>Forecast_10!E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="30" customHeight="1">
@@ -40325,7 +40325,7 @@
       </c>
       <c r="J34" s="73">
         <f>Forecast_11!E136</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="30" customHeight="1">
@@ -40345,11 +40345,11 @@
       </c>
       <c r="J35" s="73">
         <f>Forecast_11!E163</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="24.75" customHeight="1">
-      <c r="A36" s="112" t="s">
+      <c r="A36" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B36" s="150" t="s">
@@ -40370,7 +40370,7 @@
       </c>
       <c r="J36" s="73">
         <f>Forecast_11!E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="24.75" customHeight="1">
@@ -40395,7 +40395,7 @@
       </c>
       <c r="J37" s="73">
         <f>Forecast_12!E136</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="24.75" customHeight="1">
@@ -40420,7 +40420,7 @@
       </c>
       <c r="J38" s="73">
         <f>Forecast_12!E163</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="20.25" customHeight="1">
@@ -40445,7 +40445,7 @@
       </c>
       <c r="J39" s="73">
         <f>Forecast_12!E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="24.75" customHeight="1">
@@ -40464,7 +40464,7 @@
       </c>
       <c r="J40" s="73">
         <f>Forecast_13!E136</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="24.75" customHeight="1">
@@ -40483,7 +40483,7 @@
       </c>
       <c r="J41" s="73">
         <f>Forecast_13!E163</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="24.75" customHeight="1">
@@ -40502,7 +40502,7 @@
       </c>
       <c r="J42" s="73">
         <f>Forecast_13!E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="24.75" customHeight="1">
@@ -40524,7 +40524,7 @@
       </c>
       <c r="J43" s="73">
         <f>Forecast_14!E136</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="24.75" customHeight="1">
@@ -40534,7 +40534,7 @@
       </c>
       <c r="J44" s="73">
         <f>Forecast_14!E163</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="24.75" customHeight="1">
@@ -40544,7 +40544,7 @@
       </c>
       <c r="J45" s="73">
         <f>Forecast_14!E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="24.75" customHeight="1">
@@ -40554,7 +40554,7 @@
       </c>
       <c r="J46" s="73">
         <f>Forecast_15!E136</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="24.75" customHeight="1">
@@ -40574,11 +40574,11 @@
       </c>
       <c r="J47" s="73">
         <f>Forecast_15!E163</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="24.75" customHeight="1">
-      <c r="A48" s="112" t="s">
+      <c r="A48" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B48" s="150" t="s">
@@ -40599,7 +40599,7 @@
       </c>
       <c r="J48" s="73">
         <f>Forecast_15!E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="24.75" customHeight="1">
@@ -40624,7 +40624,7 @@
       </c>
       <c r="J49" s="73">
         <f>Forecast_16!E136</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="24.75" customHeight="1">
@@ -40649,7 +40649,7 @@
       </c>
       <c r="J50" s="73">
         <f>Forecast_16!E163</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="24.75" customHeight="1">
@@ -40674,7 +40674,7 @@
       </c>
       <c r="J51" s="63">
         <f>Forecast_16!E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="24.75" customHeight="1">
@@ -40842,7 +40842,7 @@
     </row>
     <row r="71" spans="1:3" ht="15.75">
       <c r="A71" s="32"/>
-      <c r="B71" s="115" t="s">
+      <c r="B71" s="107" t="s">
         <v>75</v>
       </c>
       <c r="C71" s="19">
@@ -40930,7 +40930,7 @@
     </row>
     <row r="82" spans="1:3" ht="15.75">
       <c r="A82" s="20"/>
-      <c r="B82" s="116" t="s">
+      <c r="B82" s="108" t="s">
         <v>81</v>
       </c>
       <c r="C82" s="19">
@@ -40957,7 +40957,7 @@
       </c>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="117" t="s">
+      <c r="A85" s="109" t="s">
         <v>85</v>
       </c>
       <c r="B85" s="18" t="s">
@@ -41004,7 +41004,7 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="20"/>
-      <c r="B91" s="116" t="s">
+      <c r="B91" s="108" t="s">
         <v>87</v>
       </c>
       <c r="C91" s="26">
@@ -41079,7 +41079,7 @@
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="21"/>
-      <c r="B101" s="115" t="s">
+      <c r="B101" s="107" t="s">
         <v>90</v>
       </c>
       <c r="C101" s="26">
@@ -41120,7 +41120,7 @@
       <c r="A105" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B105" s="111" t="s">
+      <c r="B105" s="114" t="s">
         <v>97</v>
       </c>
       <c r="C105" s="84">
@@ -41131,7 +41131,7 @@
       <c r="A106" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="B106" s="111" t="s">
+      <c r="B106" s="114" t="s">
         <v>99</v>
       </c>
       <c r="C106" s="84">
@@ -41168,7 +41168,7 @@
     </row>
     <row r="111" spans="1:3" ht="15.75">
       <c r="A111" s="25"/>
-      <c r="B111" s="115" t="s">
+      <c r="B111" s="107" t="s">
         <v>100</v>
       </c>
       <c r="C111" s="19">
@@ -41178,7 +41178,7 @@
     </row>
     <row r="112" spans="1:3" ht="15.75">
       <c r="A112" s="21"/>
-      <c r="B112" s="115" t="s">
+      <c r="B112" s="107" t="s">
         <v>101</v>
       </c>
       <c r="C112" s="19">
@@ -41327,7 +41327,7 @@
     </row>
     <row r="124" spans="1:8" ht="15.75">
       <c r="A124" s="20"/>
-      <c r="B124" s="116" t="s">
+      <c r="B124" s="108" t="s">
         <v>108</v>
       </c>
       <c r="C124" s="19">
@@ -41337,7 +41337,7 @@
     </row>
     <row r="125" spans="1:8" ht="15.75">
       <c r="A125" s="20"/>
-      <c r="B125" s="116" t="s">
+      <c r="B125" s="108" t="s">
         <v>109</v>
       </c>
       <c r="C125" s="19">
@@ -42766,7 +42766,7 @@
       <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="150" t="s">
@@ -42940,7 +42940,7 @@
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A21" s="112" t="s">
+      <c r="A21" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="150" t="s">
@@ -43179,7 +43179,7 @@
       <c r="I35" s="8"/>
     </row>
     <row r="36" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A36" s="112" t="s">
+      <c r="A36" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B36" s="150" t="s">
@@ -43437,7 +43437,7 @@
       <c r="B52" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C52" s="113" t="s">
+      <c r="C52" s="116" t="s">
         <v>48</v>
       </c>
       <c r="D52" s="42"/>
@@ -43574,7 +43574,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="32"/>
-      <c r="B62" s="115" t="s">
+      <c r="B62" s="107" t="s">
         <v>75</v>
       </c>
       <c r="C62" s="26">
@@ -43728,7 +43728,7 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="21"/>
-      <c r="B73" s="115" t="s">
+      <c r="B73" s="107" t="s">
         <v>81</v>
       </c>
       <c r="C73" s="26">
@@ -43856,7 +43856,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="21"/>
-      <c r="B82" s="115" t="s">
+      <c r="B82" s="107" t="s">
         <v>87</v>
       </c>
       <c r="C82" s="26">
@@ -43991,7 +43991,7 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="21"/>
-      <c r="B92" s="115" t="s">
+      <c r="B92" s="107" t="s">
         <v>90</v>
       </c>
       <c r="C92" s="26">
@@ -44056,7 +44056,7 @@
       <c r="A96" s="87" t="s">
         <v>96</v>
       </c>
-      <c r="B96" s="111" t="s">
+      <c r="B96" s="114" t="s">
         <v>168</v>
       </c>
       <c r="C96" s="84">
@@ -44073,7 +44073,7 @@
       <c r="A97" s="87" t="s">
         <v>98</v>
       </c>
-      <c r="B97" s="111" t="s">
+      <c r="B97" s="114" t="s">
         <v>169</v>
       </c>
       <c r="C97" s="84">
@@ -44140,7 +44140,7 @@
     </row>
     <row r="102" spans="1:9">
       <c r="A102" s="25"/>
-      <c r="B102" s="115" t="s">
+      <c r="B102" s="107" t="s">
         <v>100</v>
       </c>
       <c r="C102" s="26">
@@ -44156,7 +44156,7 @@
     </row>
     <row r="103" spans="1:9">
       <c r="A103" s="21"/>
-      <c r="B103" s="115" t="s">
+      <c r="B103" s="107" t="s">
         <v>101</v>
       </c>
       <c r="C103" s="26">
@@ -44335,7 +44335,7 @@
     </row>
     <row r="115" spans="1:9">
       <c r="A115" s="21"/>
-      <c r="B115" s="115" t="s">
+      <c r="B115" s="107" t="s">
         <v>108</v>
       </c>
       <c r="C115" s="26">
@@ -44351,7 +44351,7 @@
     </row>
     <row r="116" spans="1:9">
       <c r="A116" s="21"/>
-      <c r="B116" s="115" t="s">
+      <c r="B116" s="107" t="s">
         <v>109</v>
       </c>
       <c r="C116" s="26">
@@ -46231,7 +46231,7 @@
       <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="277" t="s">
@@ -46427,7 +46427,7 @@
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" ht="30" customHeight="1">
-      <c r="A21" s="112" t="s">
+      <c r="A21" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="277" t="s">
@@ -46718,7 +46718,7 @@
       <c r="I37" s="8"/>
     </row>
     <row r="38" spans="1:9" ht="30" customHeight="1">
-      <c r="A38" s="112" t="s">
+      <c r="A38" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B38" s="277" t="s">
@@ -47028,7 +47028,7 @@
       <c r="B56" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C56" s="113" t="s">
+      <c r="C56" s="116" t="s">
         <v>48</v>
       </c>
       <c r="D56" s="42"/>
@@ -47055,7 +47055,7 @@
       <c r="A58" s="87" t="s">
         <v>195</v>
       </c>
-      <c r="B58" s="110"/>
+      <c r="B58" s="113"/>
       <c r="C58" s="84">
         <v>0</v>
       </c>
@@ -47070,7 +47070,7 @@
       <c r="A59" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="110"/>
+      <c r="B59" s="113"/>
       <c r="C59" s="84">
         <v>0</v>
       </c>
@@ -47085,7 +47085,7 @@
       <c r="A60" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="B60" s="110" t="s">
+      <c r="B60" s="113" t="s">
         <v>245</v>
       </c>
       <c r="C60" s="84">
@@ -47165,7 +47165,7 @@
     </row>
     <row r="66" spans="1:9" ht="30" customHeight="1">
       <c r="A66" s="32"/>
-      <c r="B66" s="115" t="s">
+      <c r="B66" s="107" t="s">
         <v>75</v>
       </c>
       <c r="C66" s="26">
@@ -47319,7 +47319,7 @@
     </row>
     <row r="77" spans="1:9" ht="30" customHeight="1">
       <c r="A77" s="21"/>
-      <c r="B77" s="115" t="s">
+      <c r="B77" s="107" t="s">
         <v>81</v>
       </c>
       <c r="C77" s="26">
@@ -47447,7 +47447,7 @@
     </row>
     <row r="86" spans="1:9" ht="30" customHeight="1">
       <c r="A86" s="21"/>
-      <c r="B86" s="115" t="s">
+      <c r="B86" s="107" t="s">
         <v>246</v>
       </c>
       <c r="C86" s="26">
@@ -47592,7 +47592,7 @@
     </row>
     <row r="96" spans="1:9" ht="30" customHeight="1">
       <c r="A96" s="21"/>
-      <c r="B96" s="115" t="s">
+      <c r="B96" s="107" t="s">
         <v>90</v>
       </c>
       <c r="C96" s="26">
@@ -47657,7 +47657,7 @@
       <c r="A100" s="87" t="s">
         <v>96</v>
       </c>
-      <c r="B100" s="111" t="s">
+      <c r="B100" s="114" t="s">
         <v>252</v>
       </c>
       <c r="C100" s="84">
@@ -47741,7 +47741,7 @@
     </row>
     <row r="106" spans="1:9" ht="30" customHeight="1">
       <c r="A106" s="25"/>
-      <c r="B106" s="115" t="s">
+      <c r="B106" s="107" t="s">
         <v>100</v>
       </c>
       <c r="C106" s="26">
@@ -47757,7 +47757,7 @@
     </row>
     <row r="107" spans="1:9" ht="30" customHeight="1">
       <c r="A107" s="21"/>
-      <c r="B107" s="115" t="s">
+      <c r="B107" s="107" t="s">
         <v>101</v>
       </c>
       <c r="C107" s="26">
@@ -47936,7 +47936,7 @@
     </row>
     <row r="119" spans="1:9" ht="30" customHeight="1">
       <c r="A119" s="21"/>
-      <c r="B119" s="115" t="s">
+      <c r="B119" s="107" t="s">
         <v>108</v>
       </c>
       <c r="C119" s="26">
@@ -47952,7 +47952,7 @@
     </row>
     <row r="120" spans="1:9" ht="30" customHeight="1">
       <c r="A120" s="21"/>
-      <c r="B120" s="115" t="s">
+      <c r="B120" s="107" t="s">
         <v>109</v>
       </c>
       <c r="C120" s="26">
@@ -49864,7 +49864,7 @@
       <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="277" t="s">
@@ -50151,7 +50151,7 @@
       <c r="I25" s="8"/>
     </row>
     <row r="26" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A26" s="112" t="s">
+      <c r="A26" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="277" t="s">
@@ -50343,7 +50343,7 @@
       <c r="I37" s="8"/>
     </row>
     <row r="38" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A38" s="112" t="s">
+      <c r="A38" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B38" s="277" t="s">
@@ -50523,7 +50523,7 @@
       <c r="B50" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C50" s="113" t="s">
+      <c r="C50" s="116" t="s">
         <v>48</v>
       </c>
       <c r="D50" s="42"/>
@@ -50550,7 +50550,7 @@
       <c r="A52" s="87" t="s">
         <v>195</v>
       </c>
-      <c r="B52" s="111"/>
+      <c r="B52" s="114"/>
       <c r="C52" s="84">
         <v>78</v>
       </c>
@@ -50565,7 +50565,7 @@
       <c r="A53" s="87" t="s">
         <v>290</v>
       </c>
-      <c r="B53" s="111" t="s">
+      <c r="B53" s="114" t="s">
         <v>297</v>
       </c>
       <c r="C53" s="84">
@@ -50582,7 +50582,7 @@
       <c r="A54" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="B54" s="111" t="s">
+      <c r="B54" s="114" t="s">
         <v>245</v>
       </c>
       <c r="C54" s="84">
@@ -50662,7 +50662,7 @@
     </row>
     <row r="60" spans="1:9" ht="24.75" customHeight="1">
       <c r="A60" s="32"/>
-      <c r="B60" s="115" t="s">
+      <c r="B60" s="107" t="s">
         <v>75</v>
       </c>
       <c r="C60" s="26">
@@ -50816,7 +50816,7 @@
     </row>
     <row r="71" spans="1:9" ht="24.75" customHeight="1">
       <c r="A71" s="21"/>
-      <c r="B71" s="115" t="s">
+      <c r="B71" s="107" t="s">
         <v>81</v>
       </c>
       <c r="C71" s="26">
@@ -50944,7 +50944,7 @@
     </row>
     <row r="80" spans="1:9" ht="24.75" customHeight="1">
       <c r="A80" s="21"/>
-      <c r="B80" s="115" t="s">
+      <c r="B80" s="107" t="s">
         <v>246</v>
       </c>
       <c r="C80" s="26">
@@ -51079,7 +51079,7 @@
     </row>
     <row r="90" spans="1:9" ht="24.75" customHeight="1">
       <c r="A90" s="21"/>
-      <c r="B90" s="115" t="s">
+      <c r="B90" s="107" t="s">
         <v>90</v>
       </c>
       <c r="C90" s="26">
@@ -51144,7 +51144,7 @@
       <c r="A94" s="87" t="s">
         <v>96</v>
       </c>
-      <c r="B94" s="111" t="s">
+      <c r="B94" s="114" t="s">
         <v>298</v>
       </c>
       <c r="C94" s="84">
@@ -51228,7 +51228,7 @@
     </row>
     <row r="100" spans="1:9" ht="24.75" customHeight="1">
       <c r="A100" s="25"/>
-      <c r="B100" s="115" t="s">
+      <c r="B100" s="107" t="s">
         <v>100</v>
       </c>
       <c r="C100" s="26">
@@ -51244,7 +51244,7 @@
     </row>
     <row r="101" spans="1:9" ht="24.75" customHeight="1">
       <c r="A101" s="21"/>
-      <c r="B101" s="115" t="s">
+      <c r="B101" s="107" t="s">
         <v>101</v>
       </c>
       <c r="C101" s="26">
@@ -51423,7 +51423,7 @@
     </row>
     <row r="113" spans="1:9" ht="24.75" customHeight="1">
       <c r="A113" s="21"/>
-      <c r="B113" s="115" t="s">
+      <c r="B113" s="107" t="s">
         <v>108</v>
       </c>
       <c r="C113" s="26">
@@ -51439,7 +51439,7 @@
     </row>
     <row r="114" spans="1:9" ht="24.75" customHeight="1">
       <c r="A114" s="21"/>
-      <c r="B114" s="115" t="s">
+      <c r="B114" s="107" t="s">
         <v>109</v>
       </c>
       <c r="C114" s="26">
@@ -53112,7 +53112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57149C74-5589-4903-8EFC-FFF56B2CB1C8}">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A76" sqref="A76:C76"/>
     </sheetView>
   </sheetViews>
@@ -53242,7 +53242,7 @@
       <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="277" t="s">
@@ -53420,7 +53420,7 @@
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A21" s="112" t="s">
+      <c r="A21" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="277" t="s">
@@ -53594,7 +53594,7 @@
       <c r="I32" s="8"/>
     </row>
     <row r="33" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A33" s="112" t="s">
+      <c r="A33" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="150" t="s">
@@ -53774,7 +53774,7 @@
       <c r="B45" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="113" t="s">
+      <c r="C45" s="116" t="s">
         <v>48</v>
       </c>
       <c r="D45" s="42"/>
@@ -53801,7 +53801,7 @@
       <c r="A47" s="87" t="s">
         <v>195</v>
       </c>
-      <c r="B47" s="111"/>
+      <c r="B47" s="114"/>
       <c r="C47" s="84">
         <v>78</v>
       </c>
@@ -53816,7 +53816,7 @@
       <c r="A48" s="87" t="s">
         <v>290</v>
       </c>
-      <c r="B48" s="111" t="s">
+      <c r="B48" s="114" t="s">
         <v>297</v>
       </c>
       <c r="C48" s="84">
@@ -53833,7 +53833,7 @@
       <c r="A49" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="B49" s="111" t="s">
+      <c r="B49" s="114" t="s">
         <v>245</v>
       </c>
       <c r="C49" s="84">
@@ -54395,7 +54395,7 @@
       <c r="A89" s="87" t="s">
         <v>96</v>
       </c>
-      <c r="B89" s="111" t="s">
+      <c r="B89" s="114" t="s">
         <v>298</v>
       </c>
       <c r="C89" s="84">
@@ -56320,7 +56320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893696C1-98C3-4F01-A415-90003CF2A311}">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+    <sheetView topLeftCell="A114" workbookViewId="0">
       <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
@@ -56448,7 +56448,7 @@
       <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="277" t="s">
@@ -56622,7 +56622,7 @@
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A21" s="112" t="s">
+      <c r="A21" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="277" t="s">
@@ -56794,7 +56794,7 @@
       <c r="I32" s="8"/>
     </row>
     <row r="33" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A33" s="112" t="s">
+      <c r="A33" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="277" t="s">
@@ -56970,7 +56970,7 @@
       <c r="B45" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="113" t="s">
+      <c r="C45" s="116" t="s">
         <v>48</v>
       </c>
       <c r="D45" s="42"/>
@@ -56997,7 +56997,7 @@
       <c r="A47" s="87" t="s">
         <v>195</v>
       </c>
-      <c r="B47" s="111"/>
+      <c r="B47" s="114"/>
       <c r="C47" s="84">
         <v>78</v>
       </c>
@@ -57012,7 +57012,7 @@
       <c r="A48" s="87" t="s">
         <v>290</v>
       </c>
-      <c r="B48" s="111" t="s">
+      <c r="B48" s="114" t="s">
         <v>297</v>
       </c>
       <c r="C48" s="84">
@@ -57029,7 +57029,7 @@
       <c r="A49" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="B49" s="111" t="s">
+      <c r="B49" s="114" t="s">
         <v>245</v>
       </c>
       <c r="C49" s="84">
@@ -57109,7 +57109,7 @@
     </row>
     <row r="55" spans="1:9" ht="24.75" customHeight="1">
       <c r="A55" s="32"/>
-      <c r="B55" s="115" t="s">
+      <c r="B55" s="107" t="s">
         <v>75</v>
       </c>
       <c r="C55" s="26">
@@ -57265,7 +57265,7 @@
     </row>
     <row r="66" spans="1:9" ht="24.75" customHeight="1">
       <c r="A66" s="21"/>
-      <c r="B66" s="115" t="s">
+      <c r="B66" s="107" t="s">
         <v>81</v>
       </c>
       <c r="C66" s="26">
@@ -57393,7 +57393,7 @@
     </row>
     <row r="75" spans="1:9" ht="24.75" customHeight="1">
       <c r="A75" s="21"/>
-      <c r="B75" s="115" t="s">
+      <c r="B75" s="107" t="s">
         <v>246</v>
       </c>
       <c r="C75" s="26">
@@ -57528,7 +57528,7 @@
     </row>
     <row r="85" spans="1:9" ht="24.75" customHeight="1">
       <c r="A85" s="21"/>
-      <c r="B85" s="115" t="s">
+      <c r="B85" s="107" t="s">
         <v>328</v>
       </c>
       <c r="C85" s="26">
@@ -57593,7 +57593,7 @@
       <c r="A89" s="87" t="s">
         <v>96</v>
       </c>
-      <c r="B89" s="111" t="s">
+      <c r="B89" s="114" t="s">
         <v>298</v>
       </c>
       <c r="C89" s="84">
@@ -57677,7 +57677,7 @@
     </row>
     <row r="95" spans="1:9" ht="24.75" customHeight="1">
       <c r="A95" s="25"/>
-      <c r="B95" s="115" t="s">
+      <c r="B95" s="107" t="s">
         <v>100</v>
       </c>
       <c r="C95" s="26">
@@ -57693,7 +57693,7 @@
     </row>
     <row r="96" spans="1:9" ht="24.75" customHeight="1">
       <c r="A96" s="21"/>
-      <c r="B96" s="115" t="s">
+      <c r="B96" s="107" t="s">
         <v>101</v>
       </c>
       <c r="C96" s="26">
@@ -57872,7 +57872,7 @@
     </row>
     <row r="108" spans="1:9" ht="24.75" customHeight="1">
       <c r="A108" s="21"/>
-      <c r="B108" s="115" t="s">
+      <c r="B108" s="107" t="s">
         <v>108</v>
       </c>
       <c r="C108" s="26">
@@ -57888,7 +57888,7 @@
     </row>
     <row r="109" spans="1:9" ht="24.75" customHeight="1">
       <c r="A109" s="21"/>
-      <c r="B109" s="115" t="s">
+      <c r="B109" s="107" t="s">
         <v>109</v>
       </c>
       <c r="C109" s="26">
@@ -59520,8 +59520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDDCB6F-10E3-4F34-B456-81FA80F60BFA}">
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26:G26"/>
+    <sheetView topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="G187" sqref="G187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -59570,7 +59570,7 @@
       </c>
       <c r="C3" s="208">
         <f>E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="D3" s="208"/>
       <c r="E3" s="208"/>
@@ -59586,7 +59586,7 @@
       <c r="B4" s="247"/>
       <c r="C4" s="209">
         <f ca="1">SUM(C2:G3)</f>
-        <v>5125.0999999999995</v>
+        <v>6225.0999999999995</v>
       </c>
       <c r="D4" s="209"/>
       <c r="E4" s="209"/>
@@ -59648,7 +59648,7 @@
       <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="277" t="s">
@@ -59822,7 +59822,7 @@
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A21" s="112" t="s">
+      <c r="A21" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="277" t="s">
@@ -60172,7 +60172,7 @@
       <c r="B45" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="113" t="s">
+      <c r="C45" s="116" t="s">
         <v>48</v>
       </c>
       <c r="D45" s="42"/>
@@ -60199,7 +60199,7 @@
       <c r="A47" s="87" t="s">
         <v>195</v>
       </c>
-      <c r="B47" s="111"/>
+      <c r="B47" s="114"/>
       <c r="C47" s="84">
         <v>78</v>
       </c>
@@ -60214,7 +60214,7 @@
       <c r="A48" s="87" t="s">
         <v>290</v>
       </c>
-      <c r="B48" s="111" t="s">
+      <c r="B48" s="114" t="s">
         <v>297</v>
       </c>
       <c r="C48" s="84">
@@ -60231,7 +60231,7 @@
       <c r="A49" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="B49" s="111" t="s">
+      <c r="B49" s="114" t="s">
         <v>245</v>
       </c>
       <c r="C49" s="84">
@@ -60311,7 +60311,7 @@
     </row>
     <row r="55" spans="1:9" ht="24.75" customHeight="1">
       <c r="A55" s="32"/>
-      <c r="B55" s="115" t="s">
+      <c r="B55" s="107" t="s">
         <v>75</v>
       </c>
       <c r="C55" s="26">
@@ -60465,7 +60465,7 @@
     </row>
     <row r="66" spans="1:9" ht="24.75" customHeight="1">
       <c r="A66" s="21"/>
-      <c r="B66" s="115" t="s">
+      <c r="B66" s="107" t="s">
         <v>81</v>
       </c>
       <c r="C66" s="26">
@@ -60593,7 +60593,7 @@
     </row>
     <row r="75" spans="1:9" ht="24.75" customHeight="1">
       <c r="A75" s="21"/>
-      <c r="B75" s="115" t="s">
+      <c r="B75" s="107" t="s">
         <v>246</v>
       </c>
       <c r="C75" s="26">
@@ -60728,7 +60728,7 @@
     </row>
     <row r="85" spans="1:9" ht="24.75" customHeight="1">
       <c r="A85" s="21"/>
-      <c r="B85" s="115" t="s">
+      <c r="B85" s="107" t="s">
         <v>90</v>
       </c>
       <c r="C85" s="26">
@@ -60793,7 +60793,7 @@
       <c r="A89" s="87" t="s">
         <v>96</v>
       </c>
-      <c r="B89" s="111" t="s">
+      <c r="B89" s="114" t="s">
         <v>298</v>
       </c>
       <c r="C89" s="84">
@@ -60877,7 +60877,7 @@
     </row>
     <row r="95" spans="1:9" ht="24.75" customHeight="1">
       <c r="A95" s="25"/>
-      <c r="B95" s="115" t="s">
+      <c r="B95" s="107" t="s">
         <v>100</v>
       </c>
       <c r="C95" s="26">
@@ -60893,7 +60893,7 @@
     </row>
     <row r="96" spans="1:9" ht="24.75" customHeight="1">
       <c r="A96" s="21"/>
-      <c r="B96" s="115" t="s">
+      <c r="B96" s="107" t="s">
         <v>101</v>
       </c>
       <c r="C96" s="26">
@@ -61072,7 +61072,7 @@
     </row>
     <row r="108" spans="1:9" ht="24.75" customHeight="1">
       <c r="A108" s="21"/>
-      <c r="B108" s="115" t="s">
+      <c r="B108" s="107" t="s">
         <v>108</v>
       </c>
       <c r="C108" s="26">
@@ -61088,7 +61088,7 @@
     </row>
     <row r="109" spans="1:9" ht="24.75" customHeight="1">
       <c r="A109" s="21"/>
-      <c r="B109" s="115" t="s">
+      <c r="B109" s="107" t="s">
         <v>109</v>
       </c>
       <c r="C109" s="26">
@@ -61360,7 +61360,7 @@
       </c>
       <c r="D129" s="193"/>
       <c r="E129" s="84">
-        <v>450</v>
+        <v>125</v>
       </c>
       <c r="F129" s="42"/>
       <c r="G129" s="42"/>
@@ -61459,7 +61459,7 @@
       <c r="D136" s="190"/>
       <c r="E136" s="29">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>2567.5999999999995</v>
+        <v>2892.5999999999995</v>
       </c>
       <c r="F136" s="42"/>
       <c r="G136" s="42"/>
@@ -61551,7 +61551,7 @@
       <c r="D143" s="204"/>
       <c r="E143" s="29">
         <f>E136</f>
-        <v>2567.5999999999995</v>
+        <v>2892.5999999999995</v>
       </c>
       <c r="F143" s="42"/>
       <c r="G143" s="42"/>
@@ -61724,7 +61724,7 @@
       </c>
       <c r="D156" s="193"/>
       <c r="E156" s="98">
-        <v>394</v>
+        <v>69</v>
       </c>
       <c r="F156" s="42"/>
       <c r="G156" s="42"/>
@@ -61823,7 +61823,7 @@
       <c r="D163" s="190"/>
       <c r="E163" s="38">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>3862.8999999999996</v>
+        <v>4512.8999999999996</v>
       </c>
       <c r="F163" s="42"/>
       <c r="G163" s="42"/>
@@ -61915,7 +61915,7 @@
       <c r="D170" s="204"/>
       <c r="E170" s="38">
         <f>E163</f>
-        <v>3862.8999999999996</v>
+        <v>4512.8999999999996</v>
       </c>
       <c r="F170" s="42"/>
       <c r="G170" s="42"/>
@@ -62088,7 +62088,7 @@
       </c>
       <c r="D183" s="193"/>
       <c r="E183" s="84">
-        <v>450</v>
+        <v>0</v>
       </c>
       <c r="F183" s="42"/>
       <c r="G183" s="42"/>
@@ -62187,7 +62187,7 @@
       <c r="D190" s="190"/>
       <c r="E190" s="38">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F190" s="42"/>
       <c r="G190" s="42"/>
@@ -62753,7 +62753,7 @@
       </c>
       <c r="C3" s="208">
         <f>E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="D3" s="208"/>
       <c r="E3" s="208"/>
@@ -62769,7 +62769,7 @@
       <c r="B4" s="247"/>
       <c r="C4" s="209">
         <f ca="1">SUM(C2:G3)</f>
-        <v>5125.0999999999995</v>
+        <v>6225.0999999999995</v>
       </c>
       <c r="D4" s="209"/>
       <c r="E4" s="209"/>
@@ -62831,7 +62831,7 @@
       <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A9" s="112" t="s">
+      <c r="A9" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="150" t="s">
@@ -63007,7 +63007,7 @@
       <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A21" s="112" t="s">
+      <c r="A21" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="150" t="s">
@@ -63183,7 +63183,7 @@
       <c r="I32" s="8"/>
     </row>
     <row r="33" spans="1:9" ht="24.75" customHeight="1">
-      <c r="A33" s="112" t="s">
+      <c r="A33" s="115" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="150" t="s">
@@ -63365,7 +63365,7 @@
       <c r="B45" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="113" t="s">
+      <c r="C45" s="116" t="s">
         <v>48</v>
       </c>
       <c r="D45" s="42"/>
@@ -64436,7 +64436,7 @@
       <c r="D116" s="204"/>
       <c r="E116" s="55">
         <f>'October 2025 - December 2025'!E190</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F116" s="42"/>
       <c r="G116" s="42"/>
@@ -64736,7 +64736,7 @@
       <c r="D136" s="190"/>
       <c r="E136" s="29">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F136" s="42"/>
       <c r="G136" s="42"/>
@@ -64828,7 +64828,7 @@
       <c r="D143" s="204"/>
       <c r="E143" s="29">
         <f>E136</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F143" s="42"/>
       <c r="G143" s="42"/>
@@ -65128,7 +65128,7 @@
       <c r="D163" s="190"/>
       <c r="E163" s="38">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F163" s="42"/>
       <c r="G163" s="42"/>
@@ -65220,7 +65220,7 @@
       <c r="D170" s="204"/>
       <c r="E170" s="38">
         <f>E163</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F170" s="42"/>
       <c r="G170" s="42"/>
@@ -65520,7 +65520,7 @@
       <c r="D190" s="190"/>
       <c r="E190" s="38">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>5102.2</v>
+        <v>6202.2</v>
       </c>
       <c r="F190" s="42"/>
       <c r="G190" s="42"/>

</xml_diff>

<commit_message>
docs: Added indicator for all debts settlement.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560" activeTab="1"/>
+    <workbookView windowHeight="21560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -1618,7 +1618,7 @@
     <numFmt numFmtId="179" formatCode="mmm\-yy"/>
     <numFmt numFmtId="180" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="49">
+  <fonts count="50">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1755,6 +1755,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
@@ -2809,31 +2815,28 @@
   </borders>
   <cellStyleXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="41" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="41" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2842,140 +2845,143 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="43" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="43" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="12" borderId="44" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="12" borderId="44" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="13" borderId="44" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="13" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="14" borderId="46" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="13" borderId="44" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="14" borderId="46" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="44" fillId="3" borderId="49">
+    <xf numFmtId="0" fontId="43" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="45" fillId="3" borderId="49">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="45" fillId="0" borderId="0" applyProtection="0">
+    <xf numFmtId="49" fontId="46" fillId="0" borderId="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="46" fillId="9" borderId="0" applyProtection="0">
+    <xf numFmtId="49" fontId="47" fillId="9" borderId="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="47" fillId="5" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="49" fontId="48" fillId="5" borderId="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="293">
+  <cellXfs count="295">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3713,6 +3719,12 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="20" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3770,19 +3782,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="180" fontId="9" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3800,7 +3812,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3827,10 +3839,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -4274,1744 +4286,1744 @@
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="17.6"/>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="A1" s="291" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="291"/>
-      <c r="C1" s="291"/>
-      <c r="D1" s="291"/>
-      <c r="E1" s="291"/>
-      <c r="F1" s="291"/>
-      <c r="G1" s="291"/>
-      <c r="H1" s="291"/>
-      <c r="I1" s="291"/>
-      <c r="J1" s="291"/>
-      <c r="K1" s="291"/>
-      <c r="L1" s="291"/>
-      <c r="M1" s="291"/>
-      <c r="N1" s="291"/>
-      <c r="O1" s="291"/>
-      <c r="P1" s="291"/>
-      <c r="Q1" s="291"/>
-      <c r="R1" s="291"/>
-      <c r="S1" s="291"/>
-      <c r="T1" s="291"/>
-      <c r="U1" s="291"/>
-      <c r="V1" s="291"/>
-      <c r="W1" s="291"/>
-      <c r="X1" s="291"/>
-      <c r="Y1" s="291"/>
-      <c r="Z1" s="291"/>
+      <c r="A1" s="293" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="293"/>
+      <c r="C1" s="293"/>
+      <c r="D1" s="293"/>
+      <c r="E1" s="293"/>
+      <c r="F1" s="293"/>
+      <c r="G1" s="293"/>
+      <c r="H1" s="293"/>
+      <c r="I1" s="293"/>
+      <c r="J1" s="293"/>
+      <c r="K1" s="293"/>
+      <c r="L1" s="293"/>
+      <c r="M1" s="293"/>
+      <c r="N1" s="293"/>
+      <c r="O1" s="293"/>
+      <c r="P1" s="293"/>
+      <c r="Q1" s="293"/>
+      <c r="R1" s="293"/>
+      <c r="S1" s="293"/>
+      <c r="T1" s="293"/>
+      <c r="U1" s="293"/>
+      <c r="V1" s="293"/>
+      <c r="W1" s="293"/>
+      <c r="X1" s="293"/>
+      <c r="Y1" s="293"/>
+      <c r="Z1" s="293"/>
     </row>
     <row r="2" spans="1:26">
-      <c r="A2" s="291"/>
-      <c r="B2" s="291"/>
-      <c r="C2" s="291"/>
-      <c r="D2" s="291"/>
-      <c r="E2" s="291"/>
-      <c r="F2" s="291"/>
-      <c r="G2" s="291"/>
-      <c r="H2" s="291"/>
-      <c r="I2" s="291"/>
-      <c r="J2" s="291"/>
-      <c r="K2" s="291"/>
-      <c r="L2" s="291"/>
-      <c r="M2" s="291"/>
-      <c r="N2" s="291"/>
-      <c r="O2" s="291"/>
-      <c r="P2" s="291"/>
-      <c r="Q2" s="291"/>
-      <c r="R2" s="291"/>
-      <c r="S2" s="291"/>
-      <c r="T2" s="291"/>
-      <c r="U2" s="291"/>
-      <c r="V2" s="291"/>
-      <c r="W2" s="291"/>
-      <c r="X2" s="291"/>
-      <c r="Y2" s="291"/>
-      <c r="Z2" s="291"/>
+      <c r="A2" s="293"/>
+      <c r="B2" s="293"/>
+      <c r="C2" s="293"/>
+      <c r="D2" s="293"/>
+      <c r="E2" s="293"/>
+      <c r="F2" s="293"/>
+      <c r="G2" s="293"/>
+      <c r="H2" s="293"/>
+      <c r="I2" s="293"/>
+      <c r="J2" s="293"/>
+      <c r="K2" s="293"/>
+      <c r="L2" s="293"/>
+      <c r="M2" s="293"/>
+      <c r="N2" s="293"/>
+      <c r="O2" s="293"/>
+      <c r="P2" s="293"/>
+      <c r="Q2" s="293"/>
+      <c r="R2" s="293"/>
+      <c r="S2" s="293"/>
+      <c r="T2" s="293"/>
+      <c r="U2" s="293"/>
+      <c r="V2" s="293"/>
+      <c r="W2" s="293"/>
+      <c r="X2" s="293"/>
+      <c r="Y2" s="293"/>
+      <c r="Z2" s="293"/>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="291"/>
-      <c r="B3" s="291"/>
-      <c r="C3" s="291"/>
-      <c r="D3" s="291"/>
-      <c r="E3" s="291"/>
-      <c r="F3" s="291"/>
-      <c r="G3" s="291"/>
-      <c r="H3" s="291"/>
-      <c r="I3" s="291"/>
-      <c r="J3" s="291"/>
-      <c r="K3" s="291"/>
-      <c r="L3" s="291"/>
-      <c r="M3" s="291"/>
-      <c r="N3" s="291"/>
-      <c r="O3" s="291"/>
-      <c r="P3" s="291"/>
-      <c r="Q3" s="291"/>
-      <c r="R3" s="291"/>
-      <c r="S3" s="291"/>
-      <c r="T3" s="291"/>
-      <c r="U3" s="291"/>
-      <c r="V3" s="291"/>
-      <c r="W3" s="291"/>
-      <c r="X3" s="291"/>
-      <c r="Y3" s="291"/>
-      <c r="Z3" s="291"/>
+      <c r="A3" s="293"/>
+      <c r="B3" s="293"/>
+      <c r="C3" s="293"/>
+      <c r="D3" s="293"/>
+      <c r="E3" s="293"/>
+      <c r="F3" s="293"/>
+      <c r="G3" s="293"/>
+      <c r="H3" s="293"/>
+      <c r="I3" s="293"/>
+      <c r="J3" s="293"/>
+      <c r="K3" s="293"/>
+      <c r="L3" s="293"/>
+      <c r="M3" s="293"/>
+      <c r="N3" s="293"/>
+      <c r="O3" s="293"/>
+      <c r="P3" s="293"/>
+      <c r="Q3" s="293"/>
+      <c r="R3" s="293"/>
+      <c r="S3" s="293"/>
+      <c r="T3" s="293"/>
+      <c r="U3" s="293"/>
+      <c r="V3" s="293"/>
+      <c r="W3" s="293"/>
+      <c r="X3" s="293"/>
+      <c r="Y3" s="293"/>
+      <c r="Z3" s="293"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="291"/>
-      <c r="B4" s="291"/>
-      <c r="C4" s="291"/>
-      <c r="D4" s="291"/>
-      <c r="E4" s="291"/>
-      <c r="F4" s="291"/>
-      <c r="G4" s="291"/>
-      <c r="H4" s="291"/>
-      <c r="I4" s="291"/>
-      <c r="J4" s="291"/>
-      <c r="K4" s="291"/>
-      <c r="L4" s="291"/>
-      <c r="M4" s="291"/>
-      <c r="N4" s="291"/>
-      <c r="O4" s="291"/>
-      <c r="P4" s="291"/>
-      <c r="Q4" s="291"/>
-      <c r="R4" s="291"/>
-      <c r="S4" s="291"/>
-      <c r="T4" s="291"/>
-      <c r="U4" s="291"/>
-      <c r="V4" s="291"/>
-      <c r="W4" s="291"/>
-      <c r="X4" s="291"/>
-      <c r="Y4" s="291"/>
-      <c r="Z4" s="291"/>
+      <c r="A4" s="293"/>
+      <c r="B4" s="293"/>
+      <c r="C4" s="293"/>
+      <c r="D4" s="293"/>
+      <c r="E4" s="293"/>
+      <c r="F4" s="293"/>
+      <c r="G4" s="293"/>
+      <c r="H4" s="293"/>
+      <c r="I4" s="293"/>
+      <c r="J4" s="293"/>
+      <c r="K4" s="293"/>
+      <c r="L4" s="293"/>
+      <c r="M4" s="293"/>
+      <c r="N4" s="293"/>
+      <c r="O4" s="293"/>
+      <c r="P4" s="293"/>
+      <c r="Q4" s="293"/>
+      <c r="R4" s="293"/>
+      <c r="S4" s="293"/>
+      <c r="T4" s="293"/>
+      <c r="U4" s="293"/>
+      <c r="V4" s="293"/>
+      <c r="W4" s="293"/>
+      <c r="X4" s="293"/>
+      <c r="Y4" s="293"/>
+      <c r="Z4" s="293"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="291"/>
-      <c r="B5" s="291"/>
-      <c r="C5" s="291"/>
-      <c r="D5" s="291"/>
-      <c r="E5" s="291"/>
-      <c r="F5" s="291"/>
-      <c r="G5" s="291"/>
-      <c r="H5" s="291"/>
-      <c r="I5" s="291"/>
-      <c r="J5" s="291"/>
-      <c r="K5" s="291"/>
-      <c r="L5" s="291"/>
-      <c r="M5" s="291"/>
-      <c r="N5" s="291"/>
-      <c r="O5" s="291"/>
-      <c r="P5" s="291"/>
-      <c r="Q5" s="291"/>
-      <c r="R5" s="291"/>
-      <c r="S5" s="291"/>
-      <c r="T5" s="291"/>
-      <c r="U5" s="291"/>
-      <c r="V5" s="291"/>
-      <c r="W5" s="291"/>
-      <c r="X5" s="291"/>
-      <c r="Y5" s="291"/>
-      <c r="Z5" s="291"/>
+      <c r="A5" s="293"/>
+      <c r="B5" s="293"/>
+      <c r="C5" s="293"/>
+      <c r="D5" s="293"/>
+      <c r="E5" s="293"/>
+      <c r="F5" s="293"/>
+      <c r="G5" s="293"/>
+      <c r="H5" s="293"/>
+      <c r="I5" s="293"/>
+      <c r="J5" s="293"/>
+      <c r="K5" s="293"/>
+      <c r="L5" s="293"/>
+      <c r="M5" s="293"/>
+      <c r="N5" s="293"/>
+      <c r="O5" s="293"/>
+      <c r="P5" s="293"/>
+      <c r="Q5" s="293"/>
+      <c r="R5" s="293"/>
+      <c r="S5" s="293"/>
+      <c r="T5" s="293"/>
+      <c r="U5" s="293"/>
+      <c r="V5" s="293"/>
+      <c r="W5" s="293"/>
+      <c r="X5" s="293"/>
+      <c r="Y5" s="293"/>
+      <c r="Z5" s="293"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="291"/>
-      <c r="B6" s="291"/>
-      <c r="C6" s="291"/>
-      <c r="D6" s="291"/>
-      <c r="E6" s="291"/>
-      <c r="F6" s="291"/>
-      <c r="G6" s="291"/>
-      <c r="H6" s="291"/>
-      <c r="I6" s="291"/>
-      <c r="J6" s="291"/>
-      <c r="K6" s="291"/>
-      <c r="L6" s="291"/>
-      <c r="M6" s="291"/>
-      <c r="N6" s="291"/>
-      <c r="O6" s="291"/>
-      <c r="P6" s="291"/>
-      <c r="Q6" s="291"/>
-      <c r="R6" s="291"/>
-      <c r="S6" s="291"/>
-      <c r="T6" s="291"/>
-      <c r="U6" s="291"/>
-      <c r="V6" s="291"/>
-      <c r="W6" s="291"/>
-      <c r="X6" s="291"/>
-      <c r="Y6" s="291"/>
-      <c r="Z6" s="291"/>
+      <c r="A6" s="293"/>
+      <c r="B6" s="293"/>
+      <c r="C6" s="293"/>
+      <c r="D6" s="293"/>
+      <c r="E6" s="293"/>
+      <c r="F6" s="293"/>
+      <c r="G6" s="293"/>
+      <c r="H6" s="293"/>
+      <c r="I6" s="293"/>
+      <c r="J6" s="293"/>
+      <c r="K6" s="293"/>
+      <c r="L6" s="293"/>
+      <c r="M6" s="293"/>
+      <c r="N6" s="293"/>
+      <c r="O6" s="293"/>
+      <c r="P6" s="293"/>
+      <c r="Q6" s="293"/>
+      <c r="R6" s="293"/>
+      <c r="S6" s="293"/>
+      <c r="T6" s="293"/>
+      <c r="U6" s="293"/>
+      <c r="V6" s="293"/>
+      <c r="W6" s="293"/>
+      <c r="X6" s="293"/>
+      <c r="Y6" s="293"/>
+      <c r="Z6" s="293"/>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" s="291"/>
-      <c r="B7" s="291"/>
-      <c r="C7" s="291"/>
-      <c r="D7" s="291"/>
-      <c r="E7" s="291"/>
-      <c r="F7" s="291"/>
-      <c r="G7" s="291"/>
-      <c r="H7" s="291"/>
-      <c r="I7" s="291"/>
-      <c r="J7" s="291"/>
-      <c r="K7" s="291"/>
-      <c r="L7" s="291"/>
-      <c r="M7" s="291"/>
-      <c r="N7" s="291"/>
-      <c r="O7" s="291"/>
-      <c r="P7" s="291"/>
-      <c r="Q7" s="291"/>
-      <c r="R7" s="291"/>
-      <c r="S7" s="291"/>
-      <c r="T7" s="291"/>
-      <c r="U7" s="291"/>
-      <c r="V7" s="291"/>
-      <c r="W7" s="291"/>
-      <c r="X7" s="291"/>
-      <c r="Y7" s="291"/>
-      <c r="Z7" s="291"/>
+      <c r="A7" s="293"/>
+      <c r="B7" s="293"/>
+      <c r="C7" s="293"/>
+      <c r="D7" s="293"/>
+      <c r="E7" s="293"/>
+      <c r="F7" s="293"/>
+      <c r="G7" s="293"/>
+      <c r="H7" s="293"/>
+      <c r="I7" s="293"/>
+      <c r="J7" s="293"/>
+      <c r="K7" s="293"/>
+      <c r="L7" s="293"/>
+      <c r="M7" s="293"/>
+      <c r="N7" s="293"/>
+      <c r="O7" s="293"/>
+      <c r="P7" s="293"/>
+      <c r="Q7" s="293"/>
+      <c r="R7" s="293"/>
+      <c r="S7" s="293"/>
+      <c r="T7" s="293"/>
+      <c r="U7" s="293"/>
+      <c r="V7" s="293"/>
+      <c r="W7" s="293"/>
+      <c r="X7" s="293"/>
+      <c r="Y7" s="293"/>
+      <c r="Z7" s="293"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" s="291"/>
-      <c r="B8" s="291"/>
-      <c r="C8" s="291"/>
-      <c r="D8" s="291"/>
-      <c r="E8" s="291"/>
-      <c r="F8" s="291"/>
-      <c r="G8" s="291"/>
-      <c r="H8" s="291"/>
-      <c r="I8" s="291"/>
-      <c r="J8" s="291"/>
-      <c r="K8" s="291"/>
-      <c r="L8" s="291"/>
-      <c r="M8" s="291"/>
-      <c r="N8" s="291"/>
-      <c r="O8" s="291"/>
-      <c r="P8" s="291"/>
-      <c r="Q8" s="291"/>
-      <c r="R8" s="291"/>
-      <c r="S8" s="291"/>
-      <c r="T8" s="291"/>
-      <c r="U8" s="291"/>
-      <c r="V8" s="291"/>
-      <c r="W8" s="291"/>
-      <c r="X8" s="291"/>
-      <c r="Y8" s="291"/>
-      <c r="Z8" s="291"/>
+      <c r="A8" s="293"/>
+      <c r="B8" s="293"/>
+      <c r="C8" s="293"/>
+      <c r="D8" s="293"/>
+      <c r="E8" s="293"/>
+      <c r="F8" s="293"/>
+      <c r="G8" s="293"/>
+      <c r="H8" s="293"/>
+      <c r="I8" s="293"/>
+      <c r="J8" s="293"/>
+      <c r="K8" s="293"/>
+      <c r="L8" s="293"/>
+      <c r="M8" s="293"/>
+      <c r="N8" s="293"/>
+      <c r="O8" s="293"/>
+      <c r="P8" s="293"/>
+      <c r="Q8" s="293"/>
+      <c r="R8" s="293"/>
+      <c r="S8" s="293"/>
+      <c r="T8" s="293"/>
+      <c r="U8" s="293"/>
+      <c r="V8" s="293"/>
+      <c r="W8" s="293"/>
+      <c r="X8" s="293"/>
+      <c r="Y8" s="293"/>
+      <c r="Z8" s="293"/>
     </row>
     <row r="9" spans="1:26">
-      <c r="A9" s="291"/>
-      <c r="B9" s="291"/>
-      <c r="C9" s="291"/>
-      <c r="D9" s="291"/>
-      <c r="E9" s="291"/>
-      <c r="F9" s="291"/>
-      <c r="G9" s="291"/>
-      <c r="H9" s="291"/>
-      <c r="I9" s="291"/>
-      <c r="J9" s="291"/>
-      <c r="K9" s="291"/>
-      <c r="L9" s="291"/>
-      <c r="M9" s="291"/>
-      <c r="N9" s="291"/>
-      <c r="O9" s="291"/>
-      <c r="P9" s="291"/>
-      <c r="Q9" s="291"/>
-      <c r="R9" s="291"/>
-      <c r="S9" s="291"/>
-      <c r="T9" s="291"/>
-      <c r="U9" s="291"/>
-      <c r="V9" s="291"/>
-      <c r="W9" s="291"/>
-      <c r="X9" s="291"/>
-      <c r="Y9" s="291"/>
-      <c r="Z9" s="291"/>
+      <c r="A9" s="293"/>
+      <c r="B9" s="293"/>
+      <c r="C9" s="293"/>
+      <c r="D9" s="293"/>
+      <c r="E9" s="293"/>
+      <c r="F9" s="293"/>
+      <c r="G9" s="293"/>
+      <c r="H9" s="293"/>
+      <c r="I9" s="293"/>
+      <c r="J9" s="293"/>
+      <c r="K9" s="293"/>
+      <c r="L9" s="293"/>
+      <c r="M9" s="293"/>
+      <c r="N9" s="293"/>
+      <c r="O9" s="293"/>
+      <c r="P9" s="293"/>
+      <c r="Q9" s="293"/>
+      <c r="R9" s="293"/>
+      <c r="S9" s="293"/>
+      <c r="T9" s="293"/>
+      <c r="U9" s="293"/>
+      <c r="V9" s="293"/>
+      <c r="W9" s="293"/>
+      <c r="X9" s="293"/>
+      <c r="Y9" s="293"/>
+      <c r="Z9" s="293"/>
     </row>
     <row r="10" spans="1:26">
-      <c r="A10" s="291"/>
-      <c r="B10" s="291"/>
-      <c r="C10" s="291"/>
-      <c r="D10" s="291"/>
-      <c r="E10" s="291"/>
-      <c r="F10" s="291"/>
-      <c r="G10" s="291"/>
-      <c r="H10" s="291"/>
-      <c r="I10" s="291"/>
-      <c r="J10" s="291"/>
-      <c r="K10" s="291"/>
-      <c r="L10" s="291"/>
-      <c r="M10" s="291"/>
-      <c r="N10" s="291"/>
-      <c r="O10" s="291"/>
-      <c r="P10" s="291"/>
-      <c r="Q10" s="291"/>
-      <c r="R10" s="291"/>
-      <c r="S10" s="291"/>
-      <c r="T10" s="291"/>
-      <c r="U10" s="291"/>
-      <c r="V10" s="291"/>
-      <c r="W10" s="291"/>
-      <c r="X10" s="291"/>
-      <c r="Y10" s="291"/>
-      <c r="Z10" s="291"/>
+      <c r="A10" s="293"/>
+      <c r="B10" s="293"/>
+      <c r="C10" s="293"/>
+      <c r="D10" s="293"/>
+      <c r="E10" s="293"/>
+      <c r="F10" s="293"/>
+      <c r="G10" s="293"/>
+      <c r="H10" s="293"/>
+      <c r="I10" s="293"/>
+      <c r="J10" s="293"/>
+      <c r="K10" s="293"/>
+      <c r="L10" s="293"/>
+      <c r="M10" s="293"/>
+      <c r="N10" s="293"/>
+      <c r="O10" s="293"/>
+      <c r="P10" s="293"/>
+      <c r="Q10" s="293"/>
+      <c r="R10" s="293"/>
+      <c r="S10" s="293"/>
+      <c r="T10" s="293"/>
+      <c r="U10" s="293"/>
+      <c r="V10" s="293"/>
+      <c r="W10" s="293"/>
+      <c r="X10" s="293"/>
+      <c r="Y10" s="293"/>
+      <c r="Z10" s="293"/>
     </row>
     <row r="11" spans="1:26">
-      <c r="A11" s="291"/>
-      <c r="B11" s="291"/>
-      <c r="C11" s="291"/>
-      <c r="D11" s="291"/>
-      <c r="E11" s="291"/>
-      <c r="F11" s="291"/>
-      <c r="G11" s="291"/>
-      <c r="H11" s="291"/>
-      <c r="I11" s="291"/>
-      <c r="J11" s="291"/>
-      <c r="K11" s="291"/>
-      <c r="L11" s="291"/>
-      <c r="M11" s="291"/>
-      <c r="N11" s="291"/>
-      <c r="O11" s="291"/>
-      <c r="P11" s="291"/>
-      <c r="Q11" s="291"/>
-      <c r="R11" s="291"/>
-      <c r="S11" s="291"/>
-      <c r="T11" s="291"/>
-      <c r="U11" s="291"/>
-      <c r="V11" s="291"/>
-      <c r="W11" s="291"/>
-      <c r="X11" s="291"/>
-      <c r="Y11" s="291"/>
-      <c r="Z11" s="291"/>
+      <c r="A11" s="293"/>
+      <c r="B11" s="293"/>
+      <c r="C11" s="293"/>
+      <c r="D11" s="293"/>
+      <c r="E11" s="293"/>
+      <c r="F11" s="293"/>
+      <c r="G11" s="293"/>
+      <c r="H11" s="293"/>
+      <c r="I11" s="293"/>
+      <c r="J11" s="293"/>
+      <c r="K11" s="293"/>
+      <c r="L11" s="293"/>
+      <c r="M11" s="293"/>
+      <c r="N11" s="293"/>
+      <c r="O11" s="293"/>
+      <c r="P11" s="293"/>
+      <c r="Q11" s="293"/>
+      <c r="R11" s="293"/>
+      <c r="S11" s="293"/>
+      <c r="T11" s="293"/>
+      <c r="U11" s="293"/>
+      <c r="V11" s="293"/>
+      <c r="W11" s="293"/>
+      <c r="X11" s="293"/>
+      <c r="Y11" s="293"/>
+      <c r="Z11" s="293"/>
     </row>
     <row r="12" spans="1:26">
-      <c r="A12" s="291"/>
-      <c r="B12" s="291"/>
-      <c r="C12" s="291"/>
-      <c r="D12" s="291"/>
-      <c r="E12" s="291"/>
-      <c r="F12" s="291"/>
-      <c r="G12" s="291"/>
-      <c r="H12" s="291"/>
-      <c r="I12" s="291"/>
-      <c r="J12" s="291"/>
-      <c r="K12" s="291"/>
-      <c r="L12" s="291"/>
-      <c r="M12" s="291"/>
-      <c r="N12" s="291"/>
-      <c r="O12" s="291"/>
-      <c r="P12" s="291"/>
-      <c r="Q12" s="291"/>
-      <c r="R12" s="291"/>
-      <c r="S12" s="291"/>
-      <c r="T12" s="291"/>
-      <c r="U12" s="291"/>
-      <c r="V12" s="291"/>
-      <c r="W12" s="291"/>
-      <c r="X12" s="291"/>
-      <c r="Y12" s="291"/>
-      <c r="Z12" s="291"/>
+      <c r="A12" s="293"/>
+      <c r="B12" s="293"/>
+      <c r="C12" s="293"/>
+      <c r="D12" s="293"/>
+      <c r="E12" s="293"/>
+      <c r="F12" s="293"/>
+      <c r="G12" s="293"/>
+      <c r="H12" s="293"/>
+      <c r="I12" s="293"/>
+      <c r="J12" s="293"/>
+      <c r="K12" s="293"/>
+      <c r="L12" s="293"/>
+      <c r="M12" s="293"/>
+      <c r="N12" s="293"/>
+      <c r="O12" s="293"/>
+      <c r="P12" s="293"/>
+      <c r="Q12" s="293"/>
+      <c r="R12" s="293"/>
+      <c r="S12" s="293"/>
+      <c r="T12" s="293"/>
+      <c r="U12" s="293"/>
+      <c r="V12" s="293"/>
+      <c r="W12" s="293"/>
+      <c r="X12" s="293"/>
+      <c r="Y12" s="293"/>
+      <c r="Z12" s="293"/>
     </row>
     <row r="13" spans="1:26">
-      <c r="A13" s="291"/>
-      <c r="B13" s="291"/>
-      <c r="C13" s="291"/>
-      <c r="D13" s="291"/>
-      <c r="E13" s="291"/>
-      <c r="F13" s="291"/>
-      <c r="G13" s="291"/>
-      <c r="H13" s="291"/>
-      <c r="I13" s="291"/>
-      <c r="J13" s="291"/>
-      <c r="K13" s="291"/>
-      <c r="L13" s="291"/>
-      <c r="M13" s="291"/>
-      <c r="N13" s="291"/>
-      <c r="O13" s="291"/>
-      <c r="P13" s="291"/>
-      <c r="Q13" s="291"/>
-      <c r="R13" s="291"/>
-      <c r="S13" s="291"/>
-      <c r="T13" s="291"/>
-      <c r="U13" s="291"/>
-      <c r="V13" s="291"/>
-      <c r="W13" s="291"/>
-      <c r="X13" s="291"/>
-      <c r="Y13" s="291"/>
-      <c r="Z13" s="291"/>
+      <c r="A13" s="293"/>
+      <c r="B13" s="293"/>
+      <c r="C13" s="293"/>
+      <c r="D13" s="293"/>
+      <c r="E13" s="293"/>
+      <c r="F13" s="293"/>
+      <c r="G13" s="293"/>
+      <c r="H13" s="293"/>
+      <c r="I13" s="293"/>
+      <c r="J13" s="293"/>
+      <c r="K13" s="293"/>
+      <c r="L13" s="293"/>
+      <c r="M13" s="293"/>
+      <c r="N13" s="293"/>
+      <c r="O13" s="293"/>
+      <c r="P13" s="293"/>
+      <c r="Q13" s="293"/>
+      <c r="R13" s="293"/>
+      <c r="S13" s="293"/>
+      <c r="T13" s="293"/>
+      <c r="U13" s="293"/>
+      <c r="V13" s="293"/>
+      <c r="W13" s="293"/>
+      <c r="X13" s="293"/>
+      <c r="Y13" s="293"/>
+      <c r="Z13" s="293"/>
     </row>
     <row r="14" spans="1:26">
-      <c r="A14" s="291"/>
-      <c r="B14" s="291"/>
-      <c r="C14" s="291"/>
-      <c r="D14" s="291"/>
-      <c r="E14" s="291"/>
-      <c r="F14" s="291"/>
-      <c r="G14" s="291"/>
-      <c r="H14" s="291"/>
-      <c r="I14" s="291"/>
-      <c r="J14" s="291"/>
-      <c r="K14" s="291"/>
-      <c r="L14" s="291"/>
-      <c r="M14" s="291"/>
-      <c r="N14" s="291"/>
-      <c r="O14" s="291"/>
-      <c r="P14" s="291"/>
-      <c r="Q14" s="291"/>
-      <c r="R14" s="291"/>
-      <c r="S14" s="291"/>
-      <c r="T14" s="291"/>
-      <c r="U14" s="291"/>
-      <c r="V14" s="291"/>
-      <c r="W14" s="291"/>
-      <c r="X14" s="291"/>
-      <c r="Y14" s="291"/>
-      <c r="Z14" s="291"/>
+      <c r="A14" s="293"/>
+      <c r="B14" s="293"/>
+      <c r="C14" s="293"/>
+      <c r="D14" s="293"/>
+      <c r="E14" s="293"/>
+      <c r="F14" s="293"/>
+      <c r="G14" s="293"/>
+      <c r="H14" s="293"/>
+      <c r="I14" s="293"/>
+      <c r="J14" s="293"/>
+      <c r="K14" s="293"/>
+      <c r="L14" s="293"/>
+      <c r="M14" s="293"/>
+      <c r="N14" s="293"/>
+      <c r="O14" s="293"/>
+      <c r="P14" s="293"/>
+      <c r="Q14" s="293"/>
+      <c r="R14" s="293"/>
+      <c r="S14" s="293"/>
+      <c r="T14" s="293"/>
+      <c r="U14" s="293"/>
+      <c r="V14" s="293"/>
+      <c r="W14" s="293"/>
+      <c r="X14" s="293"/>
+      <c r="Y14" s="293"/>
+      <c r="Z14" s="293"/>
     </row>
     <row r="15" spans="1:26">
-      <c r="A15" s="291"/>
-      <c r="B15" s="291"/>
-      <c r="C15" s="291"/>
-      <c r="D15" s="291"/>
-      <c r="E15" s="291"/>
-      <c r="F15" s="291"/>
-      <c r="G15" s="291"/>
-      <c r="H15" s="291"/>
-      <c r="I15" s="291"/>
-      <c r="J15" s="291"/>
-      <c r="K15" s="291"/>
-      <c r="L15" s="291"/>
-      <c r="M15" s="291"/>
-      <c r="N15" s="291"/>
-      <c r="O15" s="291"/>
-      <c r="P15" s="291"/>
-      <c r="Q15" s="291"/>
-      <c r="R15" s="291"/>
-      <c r="S15" s="291"/>
-      <c r="T15" s="291"/>
-      <c r="U15" s="291"/>
-      <c r="V15" s="291"/>
-      <c r="W15" s="291"/>
-      <c r="X15" s="291"/>
-      <c r="Y15" s="291"/>
-      <c r="Z15" s="291"/>
+      <c r="A15" s="293"/>
+      <c r="B15" s="293"/>
+      <c r="C15" s="293"/>
+      <c r="D15" s="293"/>
+      <c r="E15" s="293"/>
+      <c r="F15" s="293"/>
+      <c r="G15" s="293"/>
+      <c r="H15" s="293"/>
+      <c r="I15" s="293"/>
+      <c r="J15" s="293"/>
+      <c r="K15" s="293"/>
+      <c r="L15" s="293"/>
+      <c r="M15" s="293"/>
+      <c r="N15" s="293"/>
+      <c r="O15" s="293"/>
+      <c r="P15" s="293"/>
+      <c r="Q15" s="293"/>
+      <c r="R15" s="293"/>
+      <c r="S15" s="293"/>
+      <c r="T15" s="293"/>
+      <c r="U15" s="293"/>
+      <c r="V15" s="293"/>
+      <c r="W15" s="293"/>
+      <c r="X15" s="293"/>
+      <c r="Y15" s="293"/>
+      <c r="Z15" s="293"/>
     </row>
     <row r="16" spans="1:26">
-      <c r="A16" s="291"/>
-      <c r="B16" s="291"/>
-      <c r="C16" s="291"/>
-      <c r="D16" s="291"/>
-      <c r="E16" s="291"/>
-      <c r="F16" s="291"/>
-      <c r="G16" s="291"/>
-      <c r="H16" s="291"/>
-      <c r="I16" s="291"/>
-      <c r="J16" s="291"/>
-      <c r="K16" s="291"/>
-      <c r="L16" s="291"/>
-      <c r="M16" s="291"/>
-      <c r="N16" s="291"/>
-      <c r="O16" s="291"/>
-      <c r="P16" s="291"/>
-      <c r="Q16" s="291"/>
-      <c r="R16" s="291"/>
-      <c r="S16" s="291"/>
-      <c r="T16" s="291"/>
-      <c r="U16" s="291"/>
-      <c r="V16" s="291"/>
-      <c r="W16" s="291"/>
-      <c r="X16" s="291"/>
-      <c r="Y16" s="291"/>
-      <c r="Z16" s="291"/>
+      <c r="A16" s="293"/>
+      <c r="B16" s="293"/>
+      <c r="C16" s="293"/>
+      <c r="D16" s="293"/>
+      <c r="E16" s="293"/>
+      <c r="F16" s="293"/>
+      <c r="G16" s="293"/>
+      <c r="H16" s="293"/>
+      <c r="I16" s="293"/>
+      <c r="J16" s="293"/>
+      <c r="K16" s="293"/>
+      <c r="L16" s="293"/>
+      <c r="M16" s="293"/>
+      <c r="N16" s="293"/>
+      <c r="O16" s="293"/>
+      <c r="P16" s="293"/>
+      <c r="Q16" s="293"/>
+      <c r="R16" s="293"/>
+      <c r="S16" s="293"/>
+      <c r="T16" s="293"/>
+      <c r="U16" s="293"/>
+      <c r="V16" s="293"/>
+      <c r="W16" s="293"/>
+      <c r="X16" s="293"/>
+      <c r="Y16" s="293"/>
+      <c r="Z16" s="293"/>
     </row>
     <row r="17" spans="1:26">
-      <c r="A17" s="291"/>
-      <c r="B17" s="291"/>
-      <c r="C17" s="291"/>
-      <c r="D17" s="291"/>
-      <c r="E17" s="291"/>
-      <c r="F17" s="291"/>
-      <c r="G17" s="291"/>
-      <c r="H17" s="291"/>
-      <c r="I17" s="291"/>
-      <c r="J17" s="291"/>
-      <c r="K17" s="291"/>
-      <c r="L17" s="291"/>
-      <c r="M17" s="291"/>
-      <c r="N17" s="291"/>
-      <c r="O17" s="291"/>
-      <c r="P17" s="291"/>
-      <c r="Q17" s="291"/>
-      <c r="R17" s="291"/>
-      <c r="S17" s="291"/>
-      <c r="T17" s="291"/>
-      <c r="U17" s="291"/>
-      <c r="V17" s="291"/>
-      <c r="W17" s="291"/>
-      <c r="X17" s="291"/>
-      <c r="Y17" s="291"/>
-      <c r="Z17" s="291"/>
+      <c r="A17" s="293"/>
+      <c r="B17" s="293"/>
+      <c r="C17" s="293"/>
+      <c r="D17" s="293"/>
+      <c r="E17" s="293"/>
+      <c r="F17" s="293"/>
+      <c r="G17" s="293"/>
+      <c r="H17" s="293"/>
+      <c r="I17" s="293"/>
+      <c r="J17" s="293"/>
+      <c r="K17" s="293"/>
+      <c r="L17" s="293"/>
+      <c r="M17" s="293"/>
+      <c r="N17" s="293"/>
+      <c r="O17" s="293"/>
+      <c r="P17" s="293"/>
+      <c r="Q17" s="293"/>
+      <c r="R17" s="293"/>
+      <c r="S17" s="293"/>
+      <c r="T17" s="293"/>
+      <c r="U17" s="293"/>
+      <c r="V17" s="293"/>
+      <c r="W17" s="293"/>
+      <c r="X17" s="293"/>
+      <c r="Y17" s="293"/>
+      <c r="Z17" s="293"/>
     </row>
     <row r="18" spans="1:26">
-      <c r="A18" s="291"/>
-      <c r="B18" s="291"/>
-      <c r="C18" s="291"/>
-      <c r="D18" s="291"/>
-      <c r="E18" s="291"/>
-      <c r="F18" s="291"/>
-      <c r="G18" s="291"/>
-      <c r="H18" s="291"/>
-      <c r="I18" s="291"/>
-      <c r="J18" s="291"/>
-      <c r="K18" s="291"/>
-      <c r="L18" s="291"/>
-      <c r="M18" s="291"/>
-      <c r="N18" s="291"/>
-      <c r="O18" s="291"/>
-      <c r="P18" s="291"/>
-      <c r="Q18" s="291"/>
-      <c r="R18" s="291"/>
-      <c r="S18" s="291"/>
-      <c r="T18" s="291"/>
-      <c r="U18" s="291"/>
-      <c r="V18" s="291"/>
-      <c r="W18" s="291"/>
-      <c r="X18" s="291"/>
-      <c r="Y18" s="291"/>
-      <c r="Z18" s="291"/>
+      <c r="A18" s="293"/>
+      <c r="B18" s="293"/>
+      <c r="C18" s="293"/>
+      <c r="D18" s="293"/>
+      <c r="E18" s="293"/>
+      <c r="F18" s="293"/>
+      <c r="G18" s="293"/>
+      <c r="H18" s="293"/>
+      <c r="I18" s="293"/>
+      <c r="J18" s="293"/>
+      <c r="K18" s="293"/>
+      <c r="L18" s="293"/>
+      <c r="M18" s="293"/>
+      <c r="N18" s="293"/>
+      <c r="O18" s="293"/>
+      <c r="P18" s="293"/>
+      <c r="Q18" s="293"/>
+      <c r="R18" s="293"/>
+      <c r="S18" s="293"/>
+      <c r="T18" s="293"/>
+      <c r="U18" s="293"/>
+      <c r="V18" s="293"/>
+      <c r="W18" s="293"/>
+      <c r="X18" s="293"/>
+      <c r="Y18" s="293"/>
+      <c r="Z18" s="293"/>
     </row>
     <row r="19" spans="1:26">
-      <c r="A19" s="291"/>
-      <c r="B19" s="291"/>
-      <c r="C19" s="291"/>
-      <c r="D19" s="291"/>
-      <c r="E19" s="291"/>
-      <c r="F19" s="291"/>
-      <c r="G19" s="291"/>
-      <c r="H19" s="291"/>
-      <c r="I19" s="291"/>
-      <c r="J19" s="291"/>
-      <c r="K19" s="291"/>
-      <c r="L19" s="291"/>
-      <c r="M19" s="291"/>
-      <c r="N19" s="291"/>
-      <c r="O19" s="291"/>
-      <c r="P19" s="291"/>
-      <c r="Q19" s="291"/>
-      <c r="R19" s="291"/>
-      <c r="S19" s="291"/>
-      <c r="T19" s="291"/>
-      <c r="U19" s="291"/>
-      <c r="V19" s="291"/>
-      <c r="W19" s="291"/>
-      <c r="X19" s="291"/>
-      <c r="Y19" s="291"/>
-      <c r="Z19" s="291"/>
+      <c r="A19" s="293"/>
+      <c r="B19" s="293"/>
+      <c r="C19" s="293"/>
+      <c r="D19" s="293"/>
+      <c r="E19" s="293"/>
+      <c r="F19" s="293"/>
+      <c r="G19" s="293"/>
+      <c r="H19" s="293"/>
+      <c r="I19" s="293"/>
+      <c r="J19" s="293"/>
+      <c r="K19" s="293"/>
+      <c r="L19" s="293"/>
+      <c r="M19" s="293"/>
+      <c r="N19" s="293"/>
+      <c r="O19" s="293"/>
+      <c r="P19" s="293"/>
+      <c r="Q19" s="293"/>
+      <c r="R19" s="293"/>
+      <c r="S19" s="293"/>
+      <c r="T19" s="293"/>
+      <c r="U19" s="293"/>
+      <c r="V19" s="293"/>
+      <c r="W19" s="293"/>
+      <c r="X19" s="293"/>
+      <c r="Y19" s="293"/>
+      <c r="Z19" s="293"/>
     </row>
     <row r="20" spans="1:26">
-      <c r="A20" s="291"/>
-      <c r="B20" s="291"/>
-      <c r="C20" s="291"/>
-      <c r="D20" s="291"/>
-      <c r="E20" s="291"/>
-      <c r="F20" s="291"/>
-      <c r="G20" s="291"/>
-      <c r="H20" s="291"/>
-      <c r="I20" s="291"/>
-      <c r="J20" s="291"/>
-      <c r="K20" s="291"/>
-      <c r="L20" s="291"/>
-      <c r="M20" s="291"/>
-      <c r="N20" s="291"/>
-      <c r="O20" s="291"/>
-      <c r="P20" s="291"/>
-      <c r="Q20" s="291"/>
-      <c r="R20" s="291"/>
-      <c r="S20" s="291"/>
-      <c r="T20" s="291"/>
-      <c r="U20" s="291"/>
-      <c r="V20" s="291"/>
-      <c r="W20" s="291"/>
-      <c r="X20" s="291"/>
-      <c r="Y20" s="291"/>
-      <c r="Z20" s="291"/>
+      <c r="A20" s="293"/>
+      <c r="B20" s="293"/>
+      <c r="C20" s="293"/>
+      <c r="D20" s="293"/>
+      <c r="E20" s="293"/>
+      <c r="F20" s="293"/>
+      <c r="G20" s="293"/>
+      <c r="H20" s="293"/>
+      <c r="I20" s="293"/>
+      <c r="J20" s="293"/>
+      <c r="K20" s="293"/>
+      <c r="L20" s="293"/>
+      <c r="M20" s="293"/>
+      <c r="N20" s="293"/>
+      <c r="O20" s="293"/>
+      <c r="P20" s="293"/>
+      <c r="Q20" s="293"/>
+      <c r="R20" s="293"/>
+      <c r="S20" s="293"/>
+      <c r="T20" s="293"/>
+      <c r="U20" s="293"/>
+      <c r="V20" s="293"/>
+      <c r="W20" s="293"/>
+      <c r="X20" s="293"/>
+      <c r="Y20" s="293"/>
+      <c r="Z20" s="293"/>
     </row>
     <row r="21" spans="1:26">
-      <c r="A21" s="291"/>
-      <c r="B21" s="291"/>
-      <c r="C21" s="291"/>
-      <c r="D21" s="291"/>
-      <c r="E21" s="291"/>
-      <c r="F21" s="291"/>
-      <c r="G21" s="291"/>
-      <c r="H21" s="291"/>
-      <c r="I21" s="291"/>
-      <c r="J21" s="291"/>
-      <c r="K21" s="291"/>
-      <c r="L21" s="291"/>
-      <c r="M21" s="291"/>
-      <c r="N21" s="291"/>
-      <c r="O21" s="291"/>
-      <c r="P21" s="291"/>
-      <c r="Q21" s="291"/>
-      <c r="R21" s="291"/>
-      <c r="S21" s="291"/>
-      <c r="T21" s="291"/>
-      <c r="U21" s="291"/>
-      <c r="V21" s="291"/>
-      <c r="W21" s="291"/>
-      <c r="X21" s="291"/>
-      <c r="Y21" s="291"/>
-      <c r="Z21" s="291"/>
+      <c r="A21" s="293"/>
+      <c r="B21" s="293"/>
+      <c r="C21" s="293"/>
+      <c r="D21" s="293"/>
+      <c r="E21" s="293"/>
+      <c r="F21" s="293"/>
+      <c r="G21" s="293"/>
+      <c r="H21" s="293"/>
+      <c r="I21" s="293"/>
+      <c r="J21" s="293"/>
+      <c r="K21" s="293"/>
+      <c r="L21" s="293"/>
+      <c r="M21" s="293"/>
+      <c r="N21" s="293"/>
+      <c r="O21" s="293"/>
+      <c r="P21" s="293"/>
+      <c r="Q21" s="293"/>
+      <c r="R21" s="293"/>
+      <c r="S21" s="293"/>
+      <c r="T21" s="293"/>
+      <c r="U21" s="293"/>
+      <c r="V21" s="293"/>
+      <c r="W21" s="293"/>
+      <c r="X21" s="293"/>
+      <c r="Y21" s="293"/>
+      <c r="Z21" s="293"/>
     </row>
     <row r="22" spans="1:26">
-      <c r="A22" s="291"/>
-      <c r="B22" s="291"/>
-      <c r="C22" s="291"/>
-      <c r="D22" s="291"/>
-      <c r="E22" s="291"/>
-      <c r="F22" s="291"/>
-      <c r="G22" s="291"/>
-      <c r="H22" s="291"/>
-      <c r="I22" s="291"/>
-      <c r="J22" s="291"/>
-      <c r="K22" s="291"/>
-      <c r="L22" s="291"/>
-      <c r="M22" s="291"/>
-      <c r="N22" s="291"/>
-      <c r="O22" s="291"/>
-      <c r="P22" s="291"/>
-      <c r="Q22" s="291"/>
-      <c r="R22" s="291"/>
-      <c r="S22" s="291"/>
-      <c r="T22" s="291"/>
-      <c r="U22" s="291"/>
-      <c r="V22" s="291"/>
-      <c r="W22" s="291"/>
-      <c r="X22" s="291"/>
-      <c r="Y22" s="291"/>
-      <c r="Z22" s="291"/>
+      <c r="A22" s="293"/>
+      <c r="B22" s="293"/>
+      <c r="C22" s="293"/>
+      <c r="D22" s="293"/>
+      <c r="E22" s="293"/>
+      <c r="F22" s="293"/>
+      <c r="G22" s="293"/>
+      <c r="H22" s="293"/>
+      <c r="I22" s="293"/>
+      <c r="J22" s="293"/>
+      <c r="K22" s="293"/>
+      <c r="L22" s="293"/>
+      <c r="M22" s="293"/>
+      <c r="N22" s="293"/>
+      <c r="O22" s="293"/>
+      <c r="P22" s="293"/>
+      <c r="Q22" s="293"/>
+      <c r="R22" s="293"/>
+      <c r="S22" s="293"/>
+      <c r="T22" s="293"/>
+      <c r="U22" s="293"/>
+      <c r="V22" s="293"/>
+      <c r="W22" s="293"/>
+      <c r="X22" s="293"/>
+      <c r="Y22" s="293"/>
+      <c r="Z22" s="293"/>
     </row>
     <row r="23" spans="1:26">
-      <c r="A23" s="291"/>
-      <c r="B23" s="291"/>
-      <c r="C23" s="291"/>
-      <c r="D23" s="291"/>
-      <c r="E23" s="291"/>
-      <c r="F23" s="291"/>
-      <c r="G23" s="291"/>
-      <c r="H23" s="291"/>
-      <c r="I23" s="291"/>
-      <c r="J23" s="291"/>
-      <c r="K23" s="291"/>
-      <c r="L23" s="291"/>
-      <c r="M23" s="291"/>
-      <c r="N23" s="291"/>
-      <c r="O23" s="291"/>
-      <c r="P23" s="291"/>
-      <c r="Q23" s="291"/>
-      <c r="R23" s="291"/>
-      <c r="S23" s="291"/>
-      <c r="T23" s="291"/>
-      <c r="U23" s="291"/>
-      <c r="V23" s="291"/>
-      <c r="W23" s="291"/>
-      <c r="X23" s="291"/>
-      <c r="Y23" s="291"/>
-      <c r="Z23" s="291"/>
+      <c r="A23" s="293"/>
+      <c r="B23" s="293"/>
+      <c r="C23" s="293"/>
+      <c r="D23" s="293"/>
+      <c r="E23" s="293"/>
+      <c r="F23" s="293"/>
+      <c r="G23" s="293"/>
+      <c r="H23" s="293"/>
+      <c r="I23" s="293"/>
+      <c r="J23" s="293"/>
+      <c r="K23" s="293"/>
+      <c r="L23" s="293"/>
+      <c r="M23" s="293"/>
+      <c r="N23" s="293"/>
+      <c r="O23" s="293"/>
+      <c r="P23" s="293"/>
+      <c r="Q23" s="293"/>
+      <c r="R23" s="293"/>
+      <c r="S23" s="293"/>
+      <c r="T23" s="293"/>
+      <c r="U23" s="293"/>
+      <c r="V23" s="293"/>
+      <c r="W23" s="293"/>
+      <c r="X23" s="293"/>
+      <c r="Y23" s="293"/>
+      <c r="Z23" s="293"/>
     </row>
     <row r="24" spans="1:26">
-      <c r="A24" s="291"/>
-      <c r="B24" s="291"/>
-      <c r="C24" s="291"/>
-      <c r="D24" s="291"/>
-      <c r="E24" s="291"/>
-      <c r="F24" s="291"/>
-      <c r="G24" s="291"/>
-      <c r="H24" s="291"/>
-      <c r="I24" s="291"/>
-      <c r="J24" s="291"/>
-      <c r="K24" s="291"/>
-      <c r="L24" s="291"/>
-      <c r="M24" s="291"/>
-      <c r="N24" s="291"/>
-      <c r="O24" s="291"/>
-      <c r="P24" s="291"/>
-      <c r="Q24" s="291"/>
-      <c r="R24" s="291"/>
-      <c r="S24" s="291"/>
-      <c r="T24" s="291"/>
-      <c r="U24" s="291"/>
-      <c r="V24" s="291"/>
-      <c r="W24" s="291"/>
-      <c r="X24" s="291"/>
-      <c r="Y24" s="291"/>
-      <c r="Z24" s="291"/>
+      <c r="A24" s="293"/>
+      <c r="B24" s="293"/>
+      <c r="C24" s="293"/>
+      <c r="D24" s="293"/>
+      <c r="E24" s="293"/>
+      <c r="F24" s="293"/>
+      <c r="G24" s="293"/>
+      <c r="H24" s="293"/>
+      <c r="I24" s="293"/>
+      <c r="J24" s="293"/>
+      <c r="K24" s="293"/>
+      <c r="L24" s="293"/>
+      <c r="M24" s="293"/>
+      <c r="N24" s="293"/>
+      <c r="O24" s="293"/>
+      <c r="P24" s="293"/>
+      <c r="Q24" s="293"/>
+      <c r="R24" s="293"/>
+      <c r="S24" s="293"/>
+      <c r="T24" s="293"/>
+      <c r="U24" s="293"/>
+      <c r="V24" s="293"/>
+      <c r="W24" s="293"/>
+      <c r="X24" s="293"/>
+      <c r="Y24" s="293"/>
+      <c r="Z24" s="293"/>
     </row>
     <row r="25" spans="1:26">
-      <c r="A25" s="291"/>
-      <c r="B25" s="291"/>
-      <c r="C25" s="291"/>
-      <c r="D25" s="291"/>
-      <c r="E25" s="291"/>
-      <c r="F25" s="291"/>
-      <c r="G25" s="291"/>
-      <c r="H25" s="291"/>
-      <c r="I25" s="291"/>
-      <c r="J25" s="291"/>
-      <c r="K25" s="291"/>
-      <c r="L25" s="291"/>
-      <c r="M25" s="291"/>
-      <c r="N25" s="291"/>
-      <c r="O25" s="291"/>
-      <c r="P25" s="291"/>
-      <c r="Q25" s="291"/>
-      <c r="R25" s="291"/>
-      <c r="S25" s="291"/>
-      <c r="T25" s="291"/>
-      <c r="U25" s="291"/>
-      <c r="V25" s="291"/>
-      <c r="W25" s="291"/>
-      <c r="X25" s="291"/>
-      <c r="Y25" s="291"/>
-      <c r="Z25" s="291"/>
+      <c r="A25" s="293"/>
+      <c r="B25" s="293"/>
+      <c r="C25" s="293"/>
+      <c r="D25" s="293"/>
+      <c r="E25" s="293"/>
+      <c r="F25" s="293"/>
+      <c r="G25" s="293"/>
+      <c r="H25" s="293"/>
+      <c r="I25" s="293"/>
+      <c r="J25" s="293"/>
+      <c r="K25" s="293"/>
+      <c r="L25" s="293"/>
+      <c r="M25" s="293"/>
+      <c r="N25" s="293"/>
+      <c r="O25" s="293"/>
+      <c r="P25" s="293"/>
+      <c r="Q25" s="293"/>
+      <c r="R25" s="293"/>
+      <c r="S25" s="293"/>
+      <c r="T25" s="293"/>
+      <c r="U25" s="293"/>
+      <c r="V25" s="293"/>
+      <c r="W25" s="293"/>
+      <c r="X25" s="293"/>
+      <c r="Y25" s="293"/>
+      <c r="Z25" s="293"/>
     </row>
     <row r="26" spans="1:26">
-      <c r="A26" s="291"/>
-      <c r="B26" s="291"/>
-      <c r="C26" s="291"/>
-      <c r="D26" s="291"/>
-      <c r="E26" s="291"/>
-      <c r="F26" s="291"/>
-      <c r="G26" s="291"/>
-      <c r="H26" s="291"/>
-      <c r="I26" s="291"/>
-      <c r="J26" s="291"/>
-      <c r="K26" s="291"/>
-      <c r="L26" s="291"/>
-      <c r="M26" s="291"/>
-      <c r="N26" s="291"/>
-      <c r="O26" s="291"/>
-      <c r="P26" s="291"/>
-      <c r="Q26" s="291"/>
-      <c r="R26" s="291"/>
-      <c r="S26" s="291"/>
-      <c r="T26" s="291"/>
-      <c r="U26" s="291"/>
-      <c r="V26" s="291"/>
-      <c r="W26" s="291"/>
-      <c r="X26" s="291"/>
-      <c r="Y26" s="291"/>
-      <c r="Z26" s="291"/>
+      <c r="A26" s="293"/>
+      <c r="B26" s="293"/>
+      <c r="C26" s="293"/>
+      <c r="D26" s="293"/>
+      <c r="E26" s="293"/>
+      <c r="F26" s="293"/>
+      <c r="G26" s="293"/>
+      <c r="H26" s="293"/>
+      <c r="I26" s="293"/>
+      <c r="J26" s="293"/>
+      <c r="K26" s="293"/>
+      <c r="L26" s="293"/>
+      <c r="M26" s="293"/>
+      <c r="N26" s="293"/>
+      <c r="O26" s="293"/>
+      <c r="P26" s="293"/>
+      <c r="Q26" s="293"/>
+      <c r="R26" s="293"/>
+      <c r="S26" s="293"/>
+      <c r="T26" s="293"/>
+      <c r="U26" s="293"/>
+      <c r="V26" s="293"/>
+      <c r="W26" s="293"/>
+      <c r="X26" s="293"/>
+      <c r="Y26" s="293"/>
+      <c r="Z26" s="293"/>
     </row>
     <row r="27" spans="1:26">
-      <c r="A27" s="291"/>
-      <c r="B27" s="291"/>
-      <c r="C27" s="291"/>
-      <c r="D27" s="291"/>
-      <c r="E27" s="291"/>
-      <c r="F27" s="291"/>
-      <c r="G27" s="291"/>
-      <c r="H27" s="291"/>
-      <c r="I27" s="291"/>
-      <c r="J27" s="291"/>
-      <c r="K27" s="291"/>
-      <c r="L27" s="291"/>
-      <c r="M27" s="291"/>
-      <c r="N27" s="291"/>
-      <c r="O27" s="291"/>
-      <c r="P27" s="291"/>
-      <c r="Q27" s="291"/>
-      <c r="R27" s="291"/>
-      <c r="S27" s="291"/>
-      <c r="T27" s="291"/>
-      <c r="U27" s="291"/>
-      <c r="V27" s="291"/>
-      <c r="W27" s="291"/>
-      <c r="X27" s="291"/>
-      <c r="Y27" s="291"/>
-      <c r="Z27" s="291"/>
+      <c r="A27" s="293"/>
+      <c r="B27" s="293"/>
+      <c r="C27" s="293"/>
+      <c r="D27" s="293"/>
+      <c r="E27" s="293"/>
+      <c r="F27" s="293"/>
+      <c r="G27" s="293"/>
+      <c r="H27" s="293"/>
+      <c r="I27" s="293"/>
+      <c r="J27" s="293"/>
+      <c r="K27" s="293"/>
+      <c r="L27" s="293"/>
+      <c r="M27" s="293"/>
+      <c r="N27" s="293"/>
+      <c r="O27" s="293"/>
+      <c r="P27" s="293"/>
+      <c r="Q27" s="293"/>
+      <c r="R27" s="293"/>
+      <c r="S27" s="293"/>
+      <c r="T27" s="293"/>
+      <c r="U27" s="293"/>
+      <c r="V27" s="293"/>
+      <c r="W27" s="293"/>
+      <c r="X27" s="293"/>
+      <c r="Y27" s="293"/>
+      <c r="Z27" s="293"/>
     </row>
     <row r="28" spans="1:26">
-      <c r="A28" s="291"/>
-      <c r="B28" s="291"/>
-      <c r="C28" s="291"/>
-      <c r="D28" s="291"/>
-      <c r="E28" s="291"/>
-      <c r="F28" s="291"/>
-      <c r="G28" s="291"/>
-      <c r="H28" s="291"/>
-      <c r="I28" s="291"/>
-      <c r="J28" s="291"/>
-      <c r="K28" s="291"/>
-      <c r="L28" s="291"/>
-      <c r="M28" s="291"/>
-      <c r="N28" s="291"/>
-      <c r="O28" s="291"/>
-      <c r="P28" s="291"/>
-      <c r="Q28" s="291"/>
-      <c r="R28" s="291"/>
-      <c r="S28" s="291"/>
-      <c r="T28" s="291"/>
-      <c r="U28" s="291"/>
-      <c r="V28" s="291"/>
-      <c r="W28" s="291"/>
-      <c r="X28" s="291"/>
-      <c r="Y28" s="291"/>
-      <c r="Z28" s="291"/>
+      <c r="A28" s="293"/>
+      <c r="B28" s="293"/>
+      <c r="C28" s="293"/>
+      <c r="D28" s="293"/>
+      <c r="E28" s="293"/>
+      <c r="F28" s="293"/>
+      <c r="G28" s="293"/>
+      <c r="H28" s="293"/>
+      <c r="I28" s="293"/>
+      <c r="J28" s="293"/>
+      <c r="K28" s="293"/>
+      <c r="L28" s="293"/>
+      <c r="M28" s="293"/>
+      <c r="N28" s="293"/>
+      <c r="O28" s="293"/>
+      <c r="P28" s="293"/>
+      <c r="Q28" s="293"/>
+      <c r="R28" s="293"/>
+      <c r="S28" s="293"/>
+      <c r="T28" s="293"/>
+      <c r="U28" s="293"/>
+      <c r="V28" s="293"/>
+      <c r="W28" s="293"/>
+      <c r="X28" s="293"/>
+      <c r="Y28" s="293"/>
+      <c r="Z28" s="293"/>
     </row>
     <row r="29" spans="1:26">
-      <c r="A29" s="291"/>
-      <c r="B29" s="291"/>
-      <c r="C29" s="291"/>
-      <c r="D29" s="291"/>
-      <c r="E29" s="291"/>
-      <c r="F29" s="291"/>
-      <c r="G29" s="291"/>
-      <c r="H29" s="291"/>
-      <c r="I29" s="291"/>
-      <c r="J29" s="291"/>
-      <c r="K29" s="291"/>
-      <c r="L29" s="291"/>
-      <c r="M29" s="291"/>
-      <c r="N29" s="291"/>
-      <c r="O29" s="291"/>
-      <c r="P29" s="291"/>
-      <c r="Q29" s="291"/>
-      <c r="R29" s="291"/>
-      <c r="S29" s="291"/>
-      <c r="T29" s="291"/>
-      <c r="U29" s="291"/>
-      <c r="V29" s="291"/>
-      <c r="W29" s="291"/>
-      <c r="X29" s="291"/>
-      <c r="Y29" s="291"/>
-      <c r="Z29" s="291"/>
+      <c r="A29" s="293"/>
+      <c r="B29" s="293"/>
+      <c r="C29" s="293"/>
+      <c r="D29" s="293"/>
+      <c r="E29" s="293"/>
+      <c r="F29" s="293"/>
+      <c r="G29" s="293"/>
+      <c r="H29" s="293"/>
+      <c r="I29" s="293"/>
+      <c r="J29" s="293"/>
+      <c r="K29" s="293"/>
+      <c r="L29" s="293"/>
+      <c r="M29" s="293"/>
+      <c r="N29" s="293"/>
+      <c r="O29" s="293"/>
+      <c r="P29" s="293"/>
+      <c r="Q29" s="293"/>
+      <c r="R29" s="293"/>
+      <c r="S29" s="293"/>
+      <c r="T29" s="293"/>
+      <c r="U29" s="293"/>
+      <c r="V29" s="293"/>
+      <c r="W29" s="293"/>
+      <c r="X29" s="293"/>
+      <c r="Y29" s="293"/>
+      <c r="Z29" s="293"/>
     </row>
     <row r="30" spans="1:26">
-      <c r="A30" s="291"/>
-      <c r="B30" s="291"/>
-      <c r="C30" s="291"/>
-      <c r="D30" s="291"/>
-      <c r="E30" s="291"/>
-      <c r="F30" s="291"/>
-      <c r="G30" s="291"/>
-      <c r="H30" s="291"/>
-      <c r="I30" s="291"/>
-      <c r="J30" s="291"/>
-      <c r="K30" s="291"/>
-      <c r="L30" s="291"/>
-      <c r="M30" s="291"/>
-      <c r="N30" s="291"/>
-      <c r="O30" s="291"/>
-      <c r="P30" s="291"/>
-      <c r="Q30" s="291"/>
-      <c r="R30" s="291"/>
-      <c r="S30" s="291"/>
-      <c r="T30" s="291"/>
-      <c r="U30" s="291"/>
-      <c r="V30" s="291"/>
-      <c r="W30" s="291"/>
-      <c r="X30" s="291"/>
-      <c r="Y30" s="291"/>
-      <c r="Z30" s="291"/>
+      <c r="A30" s="293"/>
+      <c r="B30" s="293"/>
+      <c r="C30" s="293"/>
+      <c r="D30" s="293"/>
+      <c r="E30" s="293"/>
+      <c r="F30" s="293"/>
+      <c r="G30" s="293"/>
+      <c r="H30" s="293"/>
+      <c r="I30" s="293"/>
+      <c r="J30" s="293"/>
+      <c r="K30" s="293"/>
+      <c r="L30" s="293"/>
+      <c r="M30" s="293"/>
+      <c r="N30" s="293"/>
+      <c r="O30" s="293"/>
+      <c r="P30" s="293"/>
+      <c r="Q30" s="293"/>
+      <c r="R30" s="293"/>
+      <c r="S30" s="293"/>
+      <c r="T30" s="293"/>
+      <c r="U30" s="293"/>
+      <c r="V30" s="293"/>
+      <c r="W30" s="293"/>
+      <c r="X30" s="293"/>
+      <c r="Y30" s="293"/>
+      <c r="Z30" s="293"/>
     </row>
     <row r="31" spans="1:26">
-      <c r="A31" s="291"/>
-      <c r="B31" s="291"/>
-      <c r="C31" s="291"/>
-      <c r="D31" s="291"/>
-      <c r="E31" s="291"/>
-      <c r="F31" s="291"/>
-      <c r="G31" s="291"/>
-      <c r="H31" s="291"/>
-      <c r="I31" s="291"/>
-      <c r="J31" s="291"/>
-      <c r="K31" s="291"/>
-      <c r="L31" s="291"/>
-      <c r="M31" s="291"/>
-      <c r="N31" s="291"/>
-      <c r="O31" s="291"/>
-      <c r="P31" s="291"/>
-      <c r="Q31" s="291"/>
-      <c r="R31" s="291"/>
-      <c r="S31" s="291"/>
-      <c r="T31" s="291"/>
-      <c r="U31" s="291"/>
-      <c r="V31" s="291"/>
-      <c r="W31" s="291"/>
-      <c r="X31" s="291"/>
-      <c r="Y31" s="291"/>
-      <c r="Z31" s="291"/>
+      <c r="A31" s="293"/>
+      <c r="B31" s="293"/>
+      <c r="C31" s="293"/>
+      <c r="D31" s="293"/>
+      <c r="E31" s="293"/>
+      <c r="F31" s="293"/>
+      <c r="G31" s="293"/>
+      <c r="H31" s="293"/>
+      <c r="I31" s="293"/>
+      <c r="J31" s="293"/>
+      <c r="K31" s="293"/>
+      <c r="L31" s="293"/>
+      <c r="M31" s="293"/>
+      <c r="N31" s="293"/>
+      <c r="O31" s="293"/>
+      <c r="P31" s="293"/>
+      <c r="Q31" s="293"/>
+      <c r="R31" s="293"/>
+      <c r="S31" s="293"/>
+      <c r="T31" s="293"/>
+      <c r="U31" s="293"/>
+      <c r="V31" s="293"/>
+      <c r="W31" s="293"/>
+      <c r="X31" s="293"/>
+      <c r="Y31" s="293"/>
+      <c r="Z31" s="293"/>
     </row>
     <row r="32" spans="1:26">
-      <c r="A32" s="292" t="s">
+      <c r="A32" s="294" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="292"/>
-      <c r="C32" s="292"/>
-      <c r="D32" s="292"/>
-      <c r="E32" s="292"/>
-      <c r="F32" s="292"/>
-      <c r="G32" s="292"/>
-      <c r="H32" s="292"/>
-      <c r="I32" s="292"/>
-      <c r="J32" s="292"/>
-      <c r="K32" s="292"/>
-      <c r="L32" s="292"/>
-      <c r="M32" s="292"/>
-      <c r="N32" s="292"/>
-      <c r="O32" s="292"/>
-      <c r="P32" s="292"/>
-      <c r="Q32" s="292"/>
-      <c r="R32" s="292"/>
-      <c r="S32" s="292"/>
-      <c r="T32" s="292"/>
-      <c r="U32" s="292"/>
-      <c r="V32" s="292"/>
-      <c r="W32" s="292"/>
-      <c r="X32" s="292"/>
-      <c r="Y32" s="292"/>
-      <c r="Z32" s="292"/>
+      <c r="B32" s="294"/>
+      <c r="C32" s="294"/>
+      <c r="D32" s="294"/>
+      <c r="E32" s="294"/>
+      <c r="F32" s="294"/>
+      <c r="G32" s="294"/>
+      <c r="H32" s="294"/>
+      <c r="I32" s="294"/>
+      <c r="J32" s="294"/>
+      <c r="K32" s="294"/>
+      <c r="L32" s="294"/>
+      <c r="M32" s="294"/>
+      <c r="N32" s="294"/>
+      <c r="O32" s="294"/>
+      <c r="P32" s="294"/>
+      <c r="Q32" s="294"/>
+      <c r="R32" s="294"/>
+      <c r="S32" s="294"/>
+      <c r="T32" s="294"/>
+      <c r="U32" s="294"/>
+      <c r="V32" s="294"/>
+      <c r="W32" s="294"/>
+      <c r="X32" s="294"/>
+      <c r="Y32" s="294"/>
+      <c r="Z32" s="294"/>
     </row>
     <row r="33" spans="1:26">
-      <c r="A33" s="292"/>
-      <c r="B33" s="292"/>
-      <c r="C33" s="292"/>
-      <c r="D33" s="292"/>
-      <c r="E33" s="292"/>
-      <c r="F33" s="292"/>
-      <c r="G33" s="292"/>
-      <c r="H33" s="292"/>
-      <c r="I33" s="292"/>
-      <c r="J33" s="292"/>
-      <c r="K33" s="292"/>
-      <c r="L33" s="292"/>
-      <c r="M33" s="292"/>
-      <c r="N33" s="292"/>
-      <c r="O33" s="292"/>
-      <c r="P33" s="292"/>
-      <c r="Q33" s="292"/>
-      <c r="R33" s="292"/>
-      <c r="S33" s="292"/>
-      <c r="T33" s="292"/>
-      <c r="U33" s="292"/>
-      <c r="V33" s="292"/>
-      <c r="W33" s="292"/>
-      <c r="X33" s="292"/>
-      <c r="Y33" s="292"/>
-      <c r="Z33" s="292"/>
+      <c r="A33" s="294"/>
+      <c r="B33" s="294"/>
+      <c r="C33" s="294"/>
+      <c r="D33" s="294"/>
+      <c r="E33" s="294"/>
+      <c r="F33" s="294"/>
+      <c r="G33" s="294"/>
+      <c r="H33" s="294"/>
+      <c r="I33" s="294"/>
+      <c r="J33" s="294"/>
+      <c r="K33" s="294"/>
+      <c r="L33" s="294"/>
+      <c r="M33" s="294"/>
+      <c r="N33" s="294"/>
+      <c r="O33" s="294"/>
+      <c r="P33" s="294"/>
+      <c r="Q33" s="294"/>
+      <c r="R33" s="294"/>
+      <c r="S33" s="294"/>
+      <c r="T33" s="294"/>
+      <c r="U33" s="294"/>
+      <c r="V33" s="294"/>
+      <c r="W33" s="294"/>
+      <c r="X33" s="294"/>
+      <c r="Y33" s="294"/>
+      <c r="Z33" s="294"/>
     </row>
     <row r="34" spans="1:26">
-      <c r="A34" s="292"/>
-      <c r="B34" s="292"/>
-      <c r="C34" s="292"/>
-      <c r="D34" s="292"/>
-      <c r="E34" s="292"/>
-      <c r="F34" s="292"/>
-      <c r="G34" s="292"/>
-      <c r="H34" s="292"/>
-      <c r="I34" s="292"/>
-      <c r="J34" s="292"/>
-      <c r="K34" s="292"/>
-      <c r="L34" s="292"/>
-      <c r="M34" s="292"/>
-      <c r="N34" s="292"/>
-      <c r="O34" s="292"/>
-      <c r="P34" s="292"/>
-      <c r="Q34" s="292"/>
-      <c r="R34" s="292"/>
-      <c r="S34" s="292"/>
-      <c r="T34" s="292"/>
-      <c r="U34" s="292"/>
-      <c r="V34" s="292"/>
-      <c r="W34" s="292"/>
-      <c r="X34" s="292"/>
-      <c r="Y34" s="292"/>
-      <c r="Z34" s="292"/>
+      <c r="A34" s="294"/>
+      <c r="B34" s="294"/>
+      <c r="C34" s="294"/>
+      <c r="D34" s="294"/>
+      <c r="E34" s="294"/>
+      <c r="F34" s="294"/>
+      <c r="G34" s="294"/>
+      <c r="H34" s="294"/>
+      <c r="I34" s="294"/>
+      <c r="J34" s="294"/>
+      <c r="K34" s="294"/>
+      <c r="L34" s="294"/>
+      <c r="M34" s="294"/>
+      <c r="N34" s="294"/>
+      <c r="O34" s="294"/>
+      <c r="P34" s="294"/>
+      <c r="Q34" s="294"/>
+      <c r="R34" s="294"/>
+      <c r="S34" s="294"/>
+      <c r="T34" s="294"/>
+      <c r="U34" s="294"/>
+      <c r="V34" s="294"/>
+      <c r="W34" s="294"/>
+      <c r="X34" s="294"/>
+      <c r="Y34" s="294"/>
+      <c r="Z34" s="294"/>
     </row>
     <row r="35" spans="1:26">
-      <c r="A35" s="292"/>
-      <c r="B35" s="292"/>
-      <c r="C35" s="292"/>
-      <c r="D35" s="292"/>
-      <c r="E35" s="292"/>
-      <c r="F35" s="292"/>
-      <c r="G35" s="292"/>
-      <c r="H35" s="292"/>
-      <c r="I35" s="292"/>
-      <c r="J35" s="292"/>
-      <c r="K35" s="292"/>
-      <c r="L35" s="292"/>
-      <c r="M35" s="292"/>
-      <c r="N35" s="292"/>
-      <c r="O35" s="292"/>
-      <c r="P35" s="292"/>
-      <c r="Q35" s="292"/>
-      <c r="R35" s="292"/>
-      <c r="S35" s="292"/>
-      <c r="T35" s="292"/>
-      <c r="U35" s="292"/>
-      <c r="V35" s="292"/>
-      <c r="W35" s="292"/>
-      <c r="X35" s="292"/>
-      <c r="Y35" s="292"/>
-      <c r="Z35" s="292"/>
+      <c r="A35" s="294"/>
+      <c r="B35" s="294"/>
+      <c r="C35" s="294"/>
+      <c r="D35" s="294"/>
+      <c r="E35" s="294"/>
+      <c r="F35" s="294"/>
+      <c r="G35" s="294"/>
+      <c r="H35" s="294"/>
+      <c r="I35" s="294"/>
+      <c r="J35" s="294"/>
+      <c r="K35" s="294"/>
+      <c r="L35" s="294"/>
+      <c r="M35" s="294"/>
+      <c r="N35" s="294"/>
+      <c r="O35" s="294"/>
+      <c r="P35" s="294"/>
+      <c r="Q35" s="294"/>
+      <c r="R35" s="294"/>
+      <c r="S35" s="294"/>
+      <c r="T35" s="294"/>
+      <c r="U35" s="294"/>
+      <c r="V35" s="294"/>
+      <c r="W35" s="294"/>
+      <c r="X35" s="294"/>
+      <c r="Y35" s="294"/>
+      <c r="Z35" s="294"/>
     </row>
     <row r="36" spans="1:26">
-      <c r="A36" s="292"/>
-      <c r="B36" s="292"/>
-      <c r="C36" s="292"/>
-      <c r="D36" s="292"/>
-      <c r="E36" s="292"/>
-      <c r="F36" s="292"/>
-      <c r="G36" s="292"/>
-      <c r="H36" s="292"/>
-      <c r="I36" s="292"/>
-      <c r="J36" s="292"/>
-      <c r="K36" s="292"/>
-      <c r="L36" s="292"/>
-      <c r="M36" s="292"/>
-      <c r="N36" s="292"/>
-      <c r="O36" s="292"/>
-      <c r="P36" s="292"/>
-      <c r="Q36" s="292"/>
-      <c r="R36" s="292"/>
-      <c r="S36" s="292"/>
-      <c r="T36" s="292"/>
-      <c r="U36" s="292"/>
-      <c r="V36" s="292"/>
-      <c r="W36" s="292"/>
-      <c r="X36" s="292"/>
-      <c r="Y36" s="292"/>
-      <c r="Z36" s="292"/>
+      <c r="A36" s="294"/>
+      <c r="B36" s="294"/>
+      <c r="C36" s="294"/>
+      <c r="D36" s="294"/>
+      <c r="E36" s="294"/>
+      <c r="F36" s="294"/>
+      <c r="G36" s="294"/>
+      <c r="H36" s="294"/>
+      <c r="I36" s="294"/>
+      <c r="J36" s="294"/>
+      <c r="K36" s="294"/>
+      <c r="L36" s="294"/>
+      <c r="M36" s="294"/>
+      <c r="N36" s="294"/>
+      <c r="O36" s="294"/>
+      <c r="P36" s="294"/>
+      <c r="Q36" s="294"/>
+      <c r="R36" s="294"/>
+      <c r="S36" s="294"/>
+      <c r="T36" s="294"/>
+      <c r="U36" s="294"/>
+      <c r="V36" s="294"/>
+      <c r="W36" s="294"/>
+      <c r="X36" s="294"/>
+      <c r="Y36" s="294"/>
+      <c r="Z36" s="294"/>
     </row>
     <row r="37" spans="1:26">
-      <c r="A37" s="292"/>
-      <c r="B37" s="292"/>
-      <c r="C37" s="292"/>
-      <c r="D37" s="292"/>
-      <c r="E37" s="292"/>
-      <c r="F37" s="292"/>
-      <c r="G37" s="292"/>
-      <c r="H37" s="292"/>
-      <c r="I37" s="292"/>
-      <c r="J37" s="292"/>
-      <c r="K37" s="292"/>
-      <c r="L37" s="292"/>
-      <c r="M37" s="292"/>
-      <c r="N37" s="292"/>
-      <c r="O37" s="292"/>
-      <c r="P37" s="292"/>
-      <c r="Q37" s="292"/>
-      <c r="R37" s="292"/>
-      <c r="S37" s="292"/>
-      <c r="T37" s="292"/>
-      <c r="U37" s="292"/>
-      <c r="V37" s="292"/>
-      <c r="W37" s="292"/>
-      <c r="X37" s="292"/>
-      <c r="Y37" s="292"/>
-      <c r="Z37" s="292"/>
+      <c r="A37" s="294"/>
+      <c r="B37" s="294"/>
+      <c r="C37" s="294"/>
+      <c r="D37" s="294"/>
+      <c r="E37" s="294"/>
+      <c r="F37" s="294"/>
+      <c r="G37" s="294"/>
+      <c r="H37" s="294"/>
+      <c r="I37" s="294"/>
+      <c r="J37" s="294"/>
+      <c r="K37" s="294"/>
+      <c r="L37" s="294"/>
+      <c r="M37" s="294"/>
+      <c r="N37" s="294"/>
+      <c r="O37" s="294"/>
+      <c r="P37" s="294"/>
+      <c r="Q37" s="294"/>
+      <c r="R37" s="294"/>
+      <c r="S37" s="294"/>
+      <c r="T37" s="294"/>
+      <c r="U37" s="294"/>
+      <c r="V37" s="294"/>
+      <c r="W37" s="294"/>
+      <c r="X37" s="294"/>
+      <c r="Y37" s="294"/>
+      <c r="Z37" s="294"/>
     </row>
     <row r="38" spans="1:26">
-      <c r="A38" s="292"/>
-      <c r="B38" s="292"/>
-      <c r="C38" s="292"/>
-      <c r="D38" s="292"/>
-      <c r="E38" s="292"/>
-      <c r="F38" s="292"/>
-      <c r="G38" s="292"/>
-      <c r="H38" s="292"/>
-      <c r="I38" s="292"/>
-      <c r="J38" s="292"/>
-      <c r="K38" s="292"/>
-      <c r="L38" s="292"/>
-      <c r="M38" s="292"/>
-      <c r="N38" s="292"/>
-      <c r="O38" s="292"/>
-      <c r="P38" s="292"/>
-      <c r="Q38" s="292"/>
-      <c r="R38" s="292"/>
-      <c r="S38" s="292"/>
-      <c r="T38" s="292"/>
-      <c r="U38" s="292"/>
-      <c r="V38" s="292"/>
-      <c r="W38" s="292"/>
-      <c r="X38" s="292"/>
-      <c r="Y38" s="292"/>
-      <c r="Z38" s="292"/>
+      <c r="A38" s="294"/>
+      <c r="B38" s="294"/>
+      <c r="C38" s="294"/>
+      <c r="D38" s="294"/>
+      <c r="E38" s="294"/>
+      <c r="F38" s="294"/>
+      <c r="G38" s="294"/>
+      <c r="H38" s="294"/>
+      <c r="I38" s="294"/>
+      <c r="J38" s="294"/>
+      <c r="K38" s="294"/>
+      <c r="L38" s="294"/>
+      <c r="M38" s="294"/>
+      <c r="N38" s="294"/>
+      <c r="O38" s="294"/>
+      <c r="P38" s="294"/>
+      <c r="Q38" s="294"/>
+      <c r="R38" s="294"/>
+      <c r="S38" s="294"/>
+      <c r="T38" s="294"/>
+      <c r="U38" s="294"/>
+      <c r="V38" s="294"/>
+      <c r="W38" s="294"/>
+      <c r="X38" s="294"/>
+      <c r="Y38" s="294"/>
+      <c r="Z38" s="294"/>
     </row>
     <row r="39" spans="1:26">
-      <c r="A39" s="292"/>
-      <c r="B39" s="292"/>
-      <c r="C39" s="292"/>
-      <c r="D39" s="292"/>
-      <c r="E39" s="292"/>
-      <c r="F39" s="292"/>
-      <c r="G39" s="292"/>
-      <c r="H39" s="292"/>
-      <c r="I39" s="292"/>
-      <c r="J39" s="292"/>
-      <c r="K39" s="292"/>
-      <c r="L39" s="292"/>
-      <c r="M39" s="292"/>
-      <c r="N39" s="292"/>
-      <c r="O39" s="292"/>
-      <c r="P39" s="292"/>
-      <c r="Q39" s="292"/>
-      <c r="R39" s="292"/>
-      <c r="S39" s="292"/>
-      <c r="T39" s="292"/>
-      <c r="U39" s="292"/>
-      <c r="V39" s="292"/>
-      <c r="W39" s="292"/>
-      <c r="X39" s="292"/>
-      <c r="Y39" s="292"/>
-      <c r="Z39" s="292"/>
+      <c r="A39" s="294"/>
+      <c r="B39" s="294"/>
+      <c r="C39" s="294"/>
+      <c r="D39" s="294"/>
+      <c r="E39" s="294"/>
+      <c r="F39" s="294"/>
+      <c r="G39" s="294"/>
+      <c r="H39" s="294"/>
+      <c r="I39" s="294"/>
+      <c r="J39" s="294"/>
+      <c r="K39" s="294"/>
+      <c r="L39" s="294"/>
+      <c r="M39" s="294"/>
+      <c r="N39" s="294"/>
+      <c r="O39" s="294"/>
+      <c r="P39" s="294"/>
+      <c r="Q39" s="294"/>
+      <c r="R39" s="294"/>
+      <c r="S39" s="294"/>
+      <c r="T39" s="294"/>
+      <c r="U39" s="294"/>
+      <c r="V39" s="294"/>
+      <c r="W39" s="294"/>
+      <c r="X39" s="294"/>
+      <c r="Y39" s="294"/>
+      <c r="Z39" s="294"/>
     </row>
     <row r="40" spans="1:26">
-      <c r="A40" s="292"/>
-      <c r="B40" s="292"/>
-      <c r="C40" s="292"/>
-      <c r="D40" s="292"/>
-      <c r="E40" s="292"/>
-      <c r="F40" s="292"/>
-      <c r="G40" s="292"/>
-      <c r="H40" s="292"/>
-      <c r="I40" s="292"/>
-      <c r="J40" s="292"/>
-      <c r="K40" s="292"/>
-      <c r="L40" s="292"/>
-      <c r="M40" s="292"/>
-      <c r="N40" s="292"/>
-      <c r="O40" s="292"/>
-      <c r="P40" s="292"/>
-      <c r="Q40" s="292"/>
-      <c r="R40" s="292"/>
-      <c r="S40" s="292"/>
-      <c r="T40" s="292"/>
-      <c r="U40" s="292"/>
-      <c r="V40" s="292"/>
-      <c r="W40" s="292"/>
-      <c r="X40" s="292"/>
-      <c r="Y40" s="292"/>
-      <c r="Z40" s="292"/>
+      <c r="A40" s="294"/>
+      <c r="B40" s="294"/>
+      <c r="C40" s="294"/>
+      <c r="D40" s="294"/>
+      <c r="E40" s="294"/>
+      <c r="F40" s="294"/>
+      <c r="G40" s="294"/>
+      <c r="H40" s="294"/>
+      <c r="I40" s="294"/>
+      <c r="J40" s="294"/>
+      <c r="K40" s="294"/>
+      <c r="L40" s="294"/>
+      <c r="M40" s="294"/>
+      <c r="N40" s="294"/>
+      <c r="O40" s="294"/>
+      <c r="P40" s="294"/>
+      <c r="Q40" s="294"/>
+      <c r="R40" s="294"/>
+      <c r="S40" s="294"/>
+      <c r="T40" s="294"/>
+      <c r="U40" s="294"/>
+      <c r="V40" s="294"/>
+      <c r="W40" s="294"/>
+      <c r="X40" s="294"/>
+      <c r="Y40" s="294"/>
+      <c r="Z40" s="294"/>
     </row>
     <row r="41" spans="1:26">
-      <c r="A41" s="292"/>
-      <c r="B41" s="292"/>
-      <c r="C41" s="292"/>
-      <c r="D41" s="292"/>
-      <c r="E41" s="292"/>
-      <c r="F41" s="292"/>
-      <c r="G41" s="292"/>
-      <c r="H41" s="292"/>
-      <c r="I41" s="292"/>
-      <c r="J41" s="292"/>
-      <c r="K41" s="292"/>
-      <c r="L41" s="292"/>
-      <c r="M41" s="292"/>
-      <c r="N41" s="292"/>
-      <c r="O41" s="292"/>
-      <c r="P41" s="292"/>
-      <c r="Q41" s="292"/>
-      <c r="R41" s="292"/>
-      <c r="S41" s="292"/>
-      <c r="T41" s="292"/>
-      <c r="U41" s="292"/>
-      <c r="V41" s="292"/>
-      <c r="W41" s="292"/>
-      <c r="X41" s="292"/>
-      <c r="Y41" s="292"/>
-      <c r="Z41" s="292"/>
+      <c r="A41" s="294"/>
+      <c r="B41" s="294"/>
+      <c r="C41" s="294"/>
+      <c r="D41" s="294"/>
+      <c r="E41" s="294"/>
+      <c r="F41" s="294"/>
+      <c r="G41" s="294"/>
+      <c r="H41" s="294"/>
+      <c r="I41" s="294"/>
+      <c r="J41" s="294"/>
+      <c r="K41" s="294"/>
+      <c r="L41" s="294"/>
+      <c r="M41" s="294"/>
+      <c r="N41" s="294"/>
+      <c r="O41" s="294"/>
+      <c r="P41" s="294"/>
+      <c r="Q41" s="294"/>
+      <c r="R41" s="294"/>
+      <c r="S41" s="294"/>
+      <c r="T41" s="294"/>
+      <c r="U41" s="294"/>
+      <c r="V41" s="294"/>
+      <c r="W41" s="294"/>
+      <c r="X41" s="294"/>
+      <c r="Y41" s="294"/>
+      <c r="Z41" s="294"/>
     </row>
     <row r="42" spans="1:26">
-      <c r="A42" s="292"/>
-      <c r="B42" s="292"/>
-      <c r="C42" s="292"/>
-      <c r="D42" s="292"/>
-      <c r="E42" s="292"/>
-      <c r="F42" s="292"/>
-      <c r="G42" s="292"/>
-      <c r="H42" s="292"/>
-      <c r="I42" s="292"/>
-      <c r="J42" s="292"/>
-      <c r="K42" s="292"/>
-      <c r="L42" s="292"/>
-      <c r="M42" s="292"/>
-      <c r="N42" s="292"/>
-      <c r="O42" s="292"/>
-      <c r="P42" s="292"/>
-      <c r="Q42" s="292"/>
-      <c r="R42" s="292"/>
-      <c r="S42" s="292"/>
-      <c r="T42" s="292"/>
-      <c r="U42" s="292"/>
-      <c r="V42" s="292"/>
-      <c r="W42" s="292"/>
-      <c r="X42" s="292"/>
-      <c r="Y42" s="292"/>
-      <c r="Z42" s="292"/>
+      <c r="A42" s="294"/>
+      <c r="B42" s="294"/>
+      <c r="C42" s="294"/>
+      <c r="D42" s="294"/>
+      <c r="E42" s="294"/>
+      <c r="F42" s="294"/>
+      <c r="G42" s="294"/>
+      <c r="H42" s="294"/>
+      <c r="I42" s="294"/>
+      <c r="J42" s="294"/>
+      <c r="K42" s="294"/>
+      <c r="L42" s="294"/>
+      <c r="M42" s="294"/>
+      <c r="N42" s="294"/>
+      <c r="O42" s="294"/>
+      <c r="P42" s="294"/>
+      <c r="Q42" s="294"/>
+      <c r="R42" s="294"/>
+      <c r="S42" s="294"/>
+      <c r="T42" s="294"/>
+      <c r="U42" s="294"/>
+      <c r="V42" s="294"/>
+      <c r="W42" s="294"/>
+      <c r="X42" s="294"/>
+      <c r="Y42" s="294"/>
+      <c r="Z42" s="294"/>
     </row>
     <row r="43" spans="1:26">
-      <c r="A43" s="292"/>
-      <c r="B43" s="292"/>
-      <c r="C43" s="292"/>
-      <c r="D43" s="292"/>
-      <c r="E43" s="292"/>
-      <c r="F43" s="292"/>
-      <c r="G43" s="292"/>
-      <c r="H43" s="292"/>
-      <c r="I43" s="292"/>
-      <c r="J43" s="292"/>
-      <c r="K43" s="292"/>
-      <c r="L43" s="292"/>
-      <c r="M43" s="292"/>
-      <c r="N43" s="292"/>
-      <c r="O43" s="292"/>
-      <c r="P43" s="292"/>
-      <c r="Q43" s="292"/>
-      <c r="R43" s="292"/>
-      <c r="S43" s="292"/>
-      <c r="T43" s="292"/>
-      <c r="U43" s="292"/>
-      <c r="V43" s="292"/>
-      <c r="W43" s="292"/>
-      <c r="X43" s="292"/>
-      <c r="Y43" s="292"/>
-      <c r="Z43" s="292"/>
+      <c r="A43" s="294"/>
+      <c r="B43" s="294"/>
+      <c r="C43" s="294"/>
+      <c r="D43" s="294"/>
+      <c r="E43" s="294"/>
+      <c r="F43" s="294"/>
+      <c r="G43" s="294"/>
+      <c r="H43" s="294"/>
+      <c r="I43" s="294"/>
+      <c r="J43" s="294"/>
+      <c r="K43" s="294"/>
+      <c r="L43" s="294"/>
+      <c r="M43" s="294"/>
+      <c r="N43" s="294"/>
+      <c r="O43" s="294"/>
+      <c r="P43" s="294"/>
+      <c r="Q43" s="294"/>
+      <c r="R43" s="294"/>
+      <c r="S43" s="294"/>
+      <c r="T43" s="294"/>
+      <c r="U43" s="294"/>
+      <c r="V43" s="294"/>
+      <c r="W43" s="294"/>
+      <c r="X43" s="294"/>
+      <c r="Y43" s="294"/>
+      <c r="Z43" s="294"/>
     </row>
     <row r="44" spans="1:26">
-      <c r="A44" s="292"/>
-      <c r="B44" s="292"/>
-      <c r="C44" s="292"/>
-      <c r="D44" s="292"/>
-      <c r="E44" s="292"/>
-      <c r="F44" s="292"/>
-      <c r="G44" s="292"/>
-      <c r="H44" s="292"/>
-      <c r="I44" s="292"/>
-      <c r="J44" s="292"/>
-      <c r="K44" s="292"/>
-      <c r="L44" s="292"/>
-      <c r="M44" s="292"/>
-      <c r="N44" s="292"/>
-      <c r="O44" s="292"/>
-      <c r="P44" s="292"/>
-      <c r="Q44" s="292"/>
-      <c r="R44" s="292"/>
-      <c r="S44" s="292"/>
-      <c r="T44" s="292"/>
-      <c r="U44" s="292"/>
-      <c r="V44" s="292"/>
-      <c r="W44" s="292"/>
-      <c r="X44" s="292"/>
-      <c r="Y44" s="292"/>
-      <c r="Z44" s="292"/>
+      <c r="A44" s="294"/>
+      <c r="B44" s="294"/>
+      <c r="C44" s="294"/>
+      <c r="D44" s="294"/>
+      <c r="E44" s="294"/>
+      <c r="F44" s="294"/>
+      <c r="G44" s="294"/>
+      <c r="H44" s="294"/>
+      <c r="I44" s="294"/>
+      <c r="J44" s="294"/>
+      <c r="K44" s="294"/>
+      <c r="L44" s="294"/>
+      <c r="M44" s="294"/>
+      <c r="N44" s="294"/>
+      <c r="O44" s="294"/>
+      <c r="P44" s="294"/>
+      <c r="Q44" s="294"/>
+      <c r="R44" s="294"/>
+      <c r="S44" s="294"/>
+      <c r="T44" s="294"/>
+      <c r="U44" s="294"/>
+      <c r="V44" s="294"/>
+      <c r="W44" s="294"/>
+      <c r="X44" s="294"/>
+      <c r="Y44" s="294"/>
+      <c r="Z44" s="294"/>
     </row>
     <row r="45" spans="1:26">
-      <c r="A45" s="292"/>
-      <c r="B45" s="292"/>
-      <c r="C45" s="292"/>
-      <c r="D45" s="292"/>
-      <c r="E45" s="292"/>
-      <c r="F45" s="292"/>
-      <c r="G45" s="292"/>
-      <c r="H45" s="292"/>
-      <c r="I45" s="292"/>
-      <c r="J45" s="292"/>
-      <c r="K45" s="292"/>
-      <c r="L45" s="292"/>
-      <c r="M45" s="292"/>
-      <c r="N45" s="292"/>
-      <c r="O45" s="292"/>
-      <c r="P45" s="292"/>
-      <c r="Q45" s="292"/>
-      <c r="R45" s="292"/>
-      <c r="S45" s="292"/>
-      <c r="T45" s="292"/>
-      <c r="U45" s="292"/>
-      <c r="V45" s="292"/>
-      <c r="W45" s="292"/>
-      <c r="X45" s="292"/>
-      <c r="Y45" s="292"/>
-      <c r="Z45" s="292"/>
+      <c r="A45" s="294"/>
+      <c r="B45" s="294"/>
+      <c r="C45" s="294"/>
+      <c r="D45" s="294"/>
+      <c r="E45" s="294"/>
+      <c r="F45" s="294"/>
+      <c r="G45" s="294"/>
+      <c r="H45" s="294"/>
+      <c r="I45" s="294"/>
+      <c r="J45" s="294"/>
+      <c r="K45" s="294"/>
+      <c r="L45" s="294"/>
+      <c r="M45" s="294"/>
+      <c r="N45" s="294"/>
+      <c r="O45" s="294"/>
+      <c r="P45" s="294"/>
+      <c r="Q45" s="294"/>
+      <c r="R45" s="294"/>
+      <c r="S45" s="294"/>
+      <c r="T45" s="294"/>
+      <c r="U45" s="294"/>
+      <c r="V45" s="294"/>
+      <c r="W45" s="294"/>
+      <c r="X45" s="294"/>
+      <c r="Y45" s="294"/>
+      <c r="Z45" s="294"/>
     </row>
     <row r="46" spans="1:26">
-      <c r="A46" s="292"/>
-      <c r="B46" s="292"/>
-      <c r="C46" s="292"/>
-      <c r="D46" s="292"/>
-      <c r="E46" s="292"/>
-      <c r="F46" s="292"/>
-      <c r="G46" s="292"/>
-      <c r="H46" s="292"/>
-      <c r="I46" s="292"/>
-      <c r="J46" s="292"/>
-      <c r="K46" s="292"/>
-      <c r="L46" s="292"/>
-      <c r="M46" s="292"/>
-      <c r="N46" s="292"/>
-      <c r="O46" s="292"/>
-      <c r="P46" s="292"/>
-      <c r="Q46" s="292"/>
-      <c r="R46" s="292"/>
-      <c r="S46" s="292"/>
-      <c r="T46" s="292"/>
-      <c r="U46" s="292"/>
-      <c r="V46" s="292"/>
-      <c r="W46" s="292"/>
-      <c r="X46" s="292"/>
-      <c r="Y46" s="292"/>
-      <c r="Z46" s="292"/>
+      <c r="A46" s="294"/>
+      <c r="B46" s="294"/>
+      <c r="C46" s="294"/>
+      <c r="D46" s="294"/>
+      <c r="E46" s="294"/>
+      <c r="F46" s="294"/>
+      <c r="G46" s="294"/>
+      <c r="H46" s="294"/>
+      <c r="I46" s="294"/>
+      <c r="J46" s="294"/>
+      <c r="K46" s="294"/>
+      <c r="L46" s="294"/>
+      <c r="M46" s="294"/>
+      <c r="N46" s="294"/>
+      <c r="O46" s="294"/>
+      <c r="P46" s="294"/>
+      <c r="Q46" s="294"/>
+      <c r="R46" s="294"/>
+      <c r="S46" s="294"/>
+      <c r="T46" s="294"/>
+      <c r="U46" s="294"/>
+      <c r="V46" s="294"/>
+      <c r="W46" s="294"/>
+      <c r="X46" s="294"/>
+      <c r="Y46" s="294"/>
+      <c r="Z46" s="294"/>
     </row>
     <row r="47" spans="1:26">
-      <c r="A47" s="292"/>
-      <c r="B47" s="292"/>
-      <c r="C47" s="292"/>
-      <c r="D47" s="292"/>
-      <c r="E47" s="292"/>
-      <c r="F47" s="292"/>
-      <c r="G47" s="292"/>
-      <c r="H47" s="292"/>
-      <c r="I47" s="292"/>
-      <c r="J47" s="292"/>
-      <c r="K47" s="292"/>
-      <c r="L47" s="292"/>
-      <c r="M47" s="292"/>
-      <c r="N47" s="292"/>
-      <c r="O47" s="292"/>
-      <c r="P47" s="292"/>
-      <c r="Q47" s="292"/>
-      <c r="R47" s="292"/>
-      <c r="S47" s="292"/>
-      <c r="T47" s="292"/>
-      <c r="U47" s="292"/>
-      <c r="V47" s="292"/>
-      <c r="W47" s="292"/>
-      <c r="X47" s="292"/>
-      <c r="Y47" s="292"/>
-      <c r="Z47" s="292"/>
+      <c r="A47" s="294"/>
+      <c r="B47" s="294"/>
+      <c r="C47" s="294"/>
+      <c r="D47" s="294"/>
+      <c r="E47" s="294"/>
+      <c r="F47" s="294"/>
+      <c r="G47" s="294"/>
+      <c r="H47" s="294"/>
+      <c r="I47" s="294"/>
+      <c r="J47" s="294"/>
+      <c r="K47" s="294"/>
+      <c r="L47" s="294"/>
+      <c r="M47" s="294"/>
+      <c r="N47" s="294"/>
+      <c r="O47" s="294"/>
+      <c r="P47" s="294"/>
+      <c r="Q47" s="294"/>
+      <c r="R47" s="294"/>
+      <c r="S47" s="294"/>
+      <c r="T47" s="294"/>
+      <c r="U47" s="294"/>
+      <c r="V47" s="294"/>
+      <c r="W47" s="294"/>
+      <c r="X47" s="294"/>
+      <c r="Y47" s="294"/>
+      <c r="Z47" s="294"/>
     </row>
     <row r="48" spans="1:26">
-      <c r="A48" s="292"/>
-      <c r="B48" s="292"/>
-      <c r="C48" s="292"/>
-      <c r="D48" s="292"/>
-      <c r="E48" s="292"/>
-      <c r="F48" s="292"/>
-      <c r="G48" s="292"/>
-      <c r="H48" s="292"/>
-      <c r="I48" s="292"/>
-      <c r="J48" s="292"/>
-      <c r="K48" s="292"/>
-      <c r="L48" s="292"/>
-      <c r="M48" s="292"/>
-      <c r="N48" s="292"/>
-      <c r="O48" s="292"/>
-      <c r="P48" s="292"/>
-      <c r="Q48" s="292"/>
-      <c r="R48" s="292"/>
-      <c r="S48" s="292"/>
-      <c r="T48" s="292"/>
-      <c r="U48" s="292"/>
-      <c r="V48" s="292"/>
-      <c r="W48" s="292"/>
-      <c r="X48" s="292"/>
-      <c r="Y48" s="292"/>
-      <c r="Z48" s="292"/>
+      <c r="A48" s="294"/>
+      <c r="B48" s="294"/>
+      <c r="C48" s="294"/>
+      <c r="D48" s="294"/>
+      <c r="E48" s="294"/>
+      <c r="F48" s="294"/>
+      <c r="G48" s="294"/>
+      <c r="H48" s="294"/>
+      <c r="I48" s="294"/>
+      <c r="J48" s="294"/>
+      <c r="K48" s="294"/>
+      <c r="L48" s="294"/>
+      <c r="M48" s="294"/>
+      <c r="N48" s="294"/>
+      <c r="O48" s="294"/>
+      <c r="P48" s="294"/>
+      <c r="Q48" s="294"/>
+      <c r="R48" s="294"/>
+      <c r="S48" s="294"/>
+      <c r="T48" s="294"/>
+      <c r="U48" s="294"/>
+      <c r="V48" s="294"/>
+      <c r="W48" s="294"/>
+      <c r="X48" s="294"/>
+      <c r="Y48" s="294"/>
+      <c r="Z48" s="294"/>
     </row>
     <row r="49" spans="1:26">
-      <c r="A49" s="292"/>
-      <c r="B49" s="292"/>
-      <c r="C49" s="292"/>
-      <c r="D49" s="292"/>
-      <c r="E49" s="292"/>
-      <c r="F49" s="292"/>
-      <c r="G49" s="292"/>
-      <c r="H49" s="292"/>
-      <c r="I49" s="292"/>
-      <c r="J49" s="292"/>
-      <c r="K49" s="292"/>
-      <c r="L49" s="292"/>
-      <c r="M49" s="292"/>
-      <c r="N49" s="292"/>
-      <c r="O49" s="292"/>
-      <c r="P49" s="292"/>
-      <c r="Q49" s="292"/>
-      <c r="R49" s="292"/>
-      <c r="S49" s="292"/>
-      <c r="T49" s="292"/>
-      <c r="U49" s="292"/>
-      <c r="V49" s="292"/>
-      <c r="W49" s="292"/>
-      <c r="X49" s="292"/>
-      <c r="Y49" s="292"/>
-      <c r="Z49" s="292"/>
+      <c r="A49" s="294"/>
+      <c r="B49" s="294"/>
+      <c r="C49" s="294"/>
+      <c r="D49" s="294"/>
+      <c r="E49" s="294"/>
+      <c r="F49" s="294"/>
+      <c r="G49" s="294"/>
+      <c r="H49" s="294"/>
+      <c r="I49" s="294"/>
+      <c r="J49" s="294"/>
+      <c r="K49" s="294"/>
+      <c r="L49" s="294"/>
+      <c r="M49" s="294"/>
+      <c r="N49" s="294"/>
+      <c r="O49" s="294"/>
+      <c r="P49" s="294"/>
+      <c r="Q49" s="294"/>
+      <c r="R49" s="294"/>
+      <c r="S49" s="294"/>
+      <c r="T49" s="294"/>
+      <c r="U49" s="294"/>
+      <c r="V49" s="294"/>
+      <c r="W49" s="294"/>
+      <c r="X49" s="294"/>
+      <c r="Y49" s="294"/>
+      <c r="Z49" s="294"/>
     </row>
     <row r="50" spans="1:26">
-      <c r="A50" s="292"/>
-      <c r="B50" s="292"/>
-      <c r="C50" s="292"/>
-      <c r="D50" s="292"/>
-      <c r="E50" s="292"/>
-      <c r="F50" s="292"/>
-      <c r="G50" s="292"/>
-      <c r="H50" s="292"/>
-      <c r="I50" s="292"/>
-      <c r="J50" s="292"/>
-      <c r="K50" s="292"/>
-      <c r="L50" s="292"/>
-      <c r="M50" s="292"/>
-      <c r="N50" s="292"/>
-      <c r="O50" s="292"/>
-      <c r="P50" s="292"/>
-      <c r="Q50" s="292"/>
-      <c r="R50" s="292"/>
-      <c r="S50" s="292"/>
-      <c r="T50" s="292"/>
-      <c r="U50" s="292"/>
-      <c r="V50" s="292"/>
-      <c r="W50" s="292"/>
-      <c r="X50" s="292"/>
-      <c r="Y50" s="292"/>
-      <c r="Z50" s="292"/>
+      <c r="A50" s="294"/>
+      <c r="B50" s="294"/>
+      <c r="C50" s="294"/>
+      <c r="D50" s="294"/>
+      <c r="E50" s="294"/>
+      <c r="F50" s="294"/>
+      <c r="G50" s="294"/>
+      <c r="H50" s="294"/>
+      <c r="I50" s="294"/>
+      <c r="J50" s="294"/>
+      <c r="K50" s="294"/>
+      <c r="L50" s="294"/>
+      <c r="M50" s="294"/>
+      <c r="N50" s="294"/>
+      <c r="O50" s="294"/>
+      <c r="P50" s="294"/>
+      <c r="Q50" s="294"/>
+      <c r="R50" s="294"/>
+      <c r="S50" s="294"/>
+      <c r="T50" s="294"/>
+      <c r="U50" s="294"/>
+      <c r="V50" s="294"/>
+      <c r="W50" s="294"/>
+      <c r="X50" s="294"/>
+      <c r="Y50" s="294"/>
+      <c r="Z50" s="294"/>
     </row>
     <row r="51" spans="1:26">
-      <c r="A51" s="292"/>
-      <c r="B51" s="292"/>
-      <c r="C51" s="292"/>
-      <c r="D51" s="292"/>
-      <c r="E51" s="292"/>
-      <c r="F51" s="292"/>
-      <c r="G51" s="292"/>
-      <c r="H51" s="292"/>
-      <c r="I51" s="292"/>
-      <c r="J51" s="292"/>
-      <c r="K51" s="292"/>
-      <c r="L51" s="292"/>
-      <c r="M51" s="292"/>
-      <c r="N51" s="292"/>
-      <c r="O51" s="292"/>
-      <c r="P51" s="292"/>
-      <c r="Q51" s="292"/>
-      <c r="R51" s="292"/>
-      <c r="S51" s="292"/>
-      <c r="T51" s="292"/>
-      <c r="U51" s="292"/>
-      <c r="V51" s="292"/>
-      <c r="W51" s="292"/>
-      <c r="X51" s="292"/>
-      <c r="Y51" s="292"/>
-      <c r="Z51" s="292"/>
+      <c r="A51" s="294"/>
+      <c r="B51" s="294"/>
+      <c r="C51" s="294"/>
+      <c r="D51" s="294"/>
+      <c r="E51" s="294"/>
+      <c r="F51" s="294"/>
+      <c r="G51" s="294"/>
+      <c r="H51" s="294"/>
+      <c r="I51" s="294"/>
+      <c r="J51" s="294"/>
+      <c r="K51" s="294"/>
+      <c r="L51" s="294"/>
+      <c r="M51" s="294"/>
+      <c r="N51" s="294"/>
+      <c r="O51" s="294"/>
+      <c r="P51" s="294"/>
+      <c r="Q51" s="294"/>
+      <c r="R51" s="294"/>
+      <c r="S51" s="294"/>
+      <c r="T51" s="294"/>
+      <c r="U51" s="294"/>
+      <c r="V51" s="294"/>
+      <c r="W51" s="294"/>
+      <c r="X51" s="294"/>
+      <c r="Y51" s="294"/>
+      <c r="Z51" s="294"/>
     </row>
     <row r="52" spans="1:26">
-      <c r="A52" s="292"/>
-      <c r="B52" s="292"/>
-      <c r="C52" s="292"/>
-      <c r="D52" s="292"/>
-      <c r="E52" s="292"/>
-      <c r="F52" s="292"/>
-      <c r="G52" s="292"/>
-      <c r="H52" s="292"/>
-      <c r="I52" s="292"/>
-      <c r="J52" s="292"/>
-      <c r="K52" s="292"/>
-      <c r="L52" s="292"/>
-      <c r="M52" s="292"/>
-      <c r="N52" s="292"/>
-      <c r="O52" s="292"/>
-      <c r="P52" s="292"/>
-      <c r="Q52" s="292"/>
-      <c r="R52" s="292"/>
-      <c r="S52" s="292"/>
-      <c r="T52" s="292"/>
-      <c r="U52" s="292"/>
-      <c r="V52" s="292"/>
-      <c r="W52" s="292"/>
-      <c r="X52" s="292"/>
-      <c r="Y52" s="292"/>
-      <c r="Z52" s="292"/>
+      <c r="A52" s="294"/>
+      <c r="B52" s="294"/>
+      <c r="C52" s="294"/>
+      <c r="D52" s="294"/>
+      <c r="E52" s="294"/>
+      <c r="F52" s="294"/>
+      <c r="G52" s="294"/>
+      <c r="H52" s="294"/>
+      <c r="I52" s="294"/>
+      <c r="J52" s="294"/>
+      <c r="K52" s="294"/>
+      <c r="L52" s="294"/>
+      <c r="M52" s="294"/>
+      <c r="N52" s="294"/>
+      <c r="O52" s="294"/>
+      <c r="P52" s="294"/>
+      <c r="Q52" s="294"/>
+      <c r="R52" s="294"/>
+      <c r="S52" s="294"/>
+      <c r="T52" s="294"/>
+      <c r="U52" s="294"/>
+      <c r="V52" s="294"/>
+      <c r="W52" s="294"/>
+      <c r="X52" s="294"/>
+      <c r="Y52" s="294"/>
+      <c r="Z52" s="294"/>
     </row>
     <row r="53" spans="1:26">
-      <c r="A53" s="292"/>
-      <c r="B53" s="292"/>
-      <c r="C53" s="292"/>
-      <c r="D53" s="292"/>
-      <c r="E53" s="292"/>
-      <c r="F53" s="292"/>
-      <c r="G53" s="292"/>
-      <c r="H53" s="292"/>
-      <c r="I53" s="292"/>
-      <c r="J53" s="292"/>
-      <c r="K53" s="292"/>
-      <c r="L53" s="292"/>
-      <c r="M53" s="292"/>
-      <c r="N53" s="292"/>
-      <c r="O53" s="292"/>
-      <c r="P53" s="292"/>
-      <c r="Q53" s="292"/>
-      <c r="R53" s="292"/>
-      <c r="S53" s="292"/>
-      <c r="T53" s="292"/>
-      <c r="U53" s="292"/>
-      <c r="V53" s="292"/>
-      <c r="W53" s="292"/>
-      <c r="X53" s="292"/>
-      <c r="Y53" s="292"/>
-      <c r="Z53" s="292"/>
+      <c r="A53" s="294"/>
+      <c r="B53" s="294"/>
+      <c r="C53" s="294"/>
+      <c r="D53" s="294"/>
+      <c r="E53" s="294"/>
+      <c r="F53" s="294"/>
+      <c r="G53" s="294"/>
+      <c r="H53" s="294"/>
+      <c r="I53" s="294"/>
+      <c r="J53" s="294"/>
+      <c r="K53" s="294"/>
+      <c r="L53" s="294"/>
+      <c r="M53" s="294"/>
+      <c r="N53" s="294"/>
+      <c r="O53" s="294"/>
+      <c r="P53" s="294"/>
+      <c r="Q53" s="294"/>
+      <c r="R53" s="294"/>
+      <c r="S53" s="294"/>
+      <c r="T53" s="294"/>
+      <c r="U53" s="294"/>
+      <c r="V53" s="294"/>
+      <c r="W53" s="294"/>
+      <c r="X53" s="294"/>
+      <c r="Y53" s="294"/>
+      <c r="Z53" s="294"/>
     </row>
     <row r="54" spans="1:26">
-      <c r="A54" s="292"/>
-      <c r="B54" s="292"/>
-      <c r="C54" s="292"/>
-      <c r="D54" s="292"/>
-      <c r="E54" s="292"/>
-      <c r="F54" s="292"/>
-      <c r="G54" s="292"/>
-      <c r="H54" s="292"/>
-      <c r="I54" s="292"/>
-      <c r="J54" s="292"/>
-      <c r="K54" s="292"/>
-      <c r="L54" s="292"/>
-      <c r="M54" s="292"/>
-      <c r="N54" s="292"/>
-      <c r="O54" s="292"/>
-      <c r="P54" s="292"/>
-      <c r="Q54" s="292"/>
-      <c r="R54" s="292"/>
-      <c r="S54" s="292"/>
-      <c r="T54" s="292"/>
-      <c r="U54" s="292"/>
-      <c r="V54" s="292"/>
-      <c r="W54" s="292"/>
-      <c r="X54" s="292"/>
-      <c r="Y54" s="292"/>
-      <c r="Z54" s="292"/>
+      <c r="A54" s="294"/>
+      <c r="B54" s="294"/>
+      <c r="C54" s="294"/>
+      <c r="D54" s="294"/>
+      <c r="E54" s="294"/>
+      <c r="F54" s="294"/>
+      <c r="G54" s="294"/>
+      <c r="H54" s="294"/>
+      <c r="I54" s="294"/>
+      <c r="J54" s="294"/>
+      <c r="K54" s="294"/>
+      <c r="L54" s="294"/>
+      <c r="M54" s="294"/>
+      <c r="N54" s="294"/>
+      <c r="O54" s="294"/>
+      <c r="P54" s="294"/>
+      <c r="Q54" s="294"/>
+      <c r="R54" s="294"/>
+      <c r="S54" s="294"/>
+      <c r="T54" s="294"/>
+      <c r="U54" s="294"/>
+      <c r="V54" s="294"/>
+      <c r="W54" s="294"/>
+      <c r="X54" s="294"/>
+      <c r="Y54" s="294"/>
+      <c r="Z54" s="294"/>
     </row>
     <row r="55" spans="1:26">
-      <c r="A55" s="292"/>
-      <c r="B55" s="292"/>
-      <c r="C55" s="292"/>
-      <c r="D55" s="292"/>
-      <c r="E55" s="292"/>
-      <c r="F55" s="292"/>
-      <c r="G55" s="292"/>
-      <c r="H55" s="292"/>
-      <c r="I55" s="292"/>
-      <c r="J55" s="292"/>
-      <c r="K55" s="292"/>
-      <c r="L55" s="292"/>
-      <c r="M55" s="292"/>
-      <c r="N55" s="292"/>
-      <c r="O55" s="292"/>
-      <c r="P55" s="292"/>
-      <c r="Q55" s="292"/>
-      <c r="R55" s="292"/>
-      <c r="S55" s="292"/>
-      <c r="T55" s="292"/>
-      <c r="U55" s="292"/>
-      <c r="V55" s="292"/>
-      <c r="W55" s="292"/>
-      <c r="X55" s="292"/>
-      <c r="Y55" s="292"/>
-      <c r="Z55" s="292"/>
+      <c r="A55" s="294"/>
+      <c r="B55" s="294"/>
+      <c r="C55" s="294"/>
+      <c r="D55" s="294"/>
+      <c r="E55" s="294"/>
+      <c r="F55" s="294"/>
+      <c r="G55" s="294"/>
+      <c r="H55" s="294"/>
+      <c r="I55" s="294"/>
+      <c r="J55" s="294"/>
+      <c r="K55" s="294"/>
+      <c r="L55" s="294"/>
+      <c r="M55" s="294"/>
+      <c r="N55" s="294"/>
+      <c r="O55" s="294"/>
+      <c r="P55" s="294"/>
+      <c r="Q55" s="294"/>
+      <c r="R55" s="294"/>
+      <c r="S55" s="294"/>
+      <c r="T55" s="294"/>
+      <c r="U55" s="294"/>
+      <c r="V55" s="294"/>
+      <c r="W55" s="294"/>
+      <c r="X55" s="294"/>
+      <c r="Y55" s="294"/>
+      <c r="Z55" s="294"/>
     </row>
     <row r="56" spans="1:26">
-      <c r="A56" s="292"/>
-      <c r="B56" s="292"/>
-      <c r="C56" s="292"/>
-      <c r="D56" s="292"/>
-      <c r="E56" s="292"/>
-      <c r="F56" s="292"/>
-      <c r="G56" s="292"/>
-      <c r="H56" s="292"/>
-      <c r="I56" s="292"/>
-      <c r="J56" s="292"/>
-      <c r="K56" s="292"/>
-      <c r="L56" s="292"/>
-      <c r="M56" s="292"/>
-      <c r="N56" s="292"/>
-      <c r="O56" s="292"/>
-      <c r="P56" s="292"/>
-      <c r="Q56" s="292"/>
-      <c r="R56" s="292"/>
-      <c r="S56" s="292"/>
-      <c r="T56" s="292"/>
-      <c r="U56" s="292"/>
-      <c r="V56" s="292"/>
-      <c r="W56" s="292"/>
-      <c r="X56" s="292"/>
-      <c r="Y56" s="292"/>
-      <c r="Z56" s="292"/>
+      <c r="A56" s="294"/>
+      <c r="B56" s="294"/>
+      <c r="C56" s="294"/>
+      <c r="D56" s="294"/>
+      <c r="E56" s="294"/>
+      <c r="F56" s="294"/>
+      <c r="G56" s="294"/>
+      <c r="H56" s="294"/>
+      <c r="I56" s="294"/>
+      <c r="J56" s="294"/>
+      <c r="K56" s="294"/>
+      <c r="L56" s="294"/>
+      <c r="M56" s="294"/>
+      <c r="N56" s="294"/>
+      <c r="O56" s="294"/>
+      <c r="P56" s="294"/>
+      <c r="Q56" s="294"/>
+      <c r="R56" s="294"/>
+      <c r="S56" s="294"/>
+      <c r="T56" s="294"/>
+      <c r="U56" s="294"/>
+      <c r="V56" s="294"/>
+      <c r="W56" s="294"/>
+      <c r="X56" s="294"/>
+      <c r="Y56" s="294"/>
+      <c r="Z56" s="294"/>
     </row>
     <row r="57" spans="1:26">
-      <c r="A57" s="292"/>
-      <c r="B57" s="292"/>
-      <c r="C57" s="292"/>
-      <c r="D57" s="292"/>
-      <c r="E57" s="292"/>
-      <c r="F57" s="292"/>
-      <c r="G57" s="292"/>
-      <c r="H57" s="292"/>
-      <c r="I57" s="292"/>
-      <c r="J57" s="292"/>
-      <c r="K57" s="292"/>
-      <c r="L57" s="292"/>
-      <c r="M57" s="292"/>
-      <c r="N57" s="292"/>
-      <c r="O57" s="292"/>
-      <c r="P57" s="292"/>
-      <c r="Q57" s="292"/>
-      <c r="R57" s="292"/>
-      <c r="S57" s="292"/>
-      <c r="T57" s="292"/>
-      <c r="U57" s="292"/>
-      <c r="V57" s="292"/>
-      <c r="W57" s="292"/>
-      <c r="X57" s="292"/>
-      <c r="Y57" s="292"/>
-      <c r="Z57" s="292"/>
+      <c r="A57" s="294"/>
+      <c r="B57" s="294"/>
+      <c r="C57" s="294"/>
+      <c r="D57" s="294"/>
+      <c r="E57" s="294"/>
+      <c r="F57" s="294"/>
+      <c r="G57" s="294"/>
+      <c r="H57" s="294"/>
+      <c r="I57" s="294"/>
+      <c r="J57" s="294"/>
+      <c r="K57" s="294"/>
+      <c r="L57" s="294"/>
+      <c r="M57" s="294"/>
+      <c r="N57" s="294"/>
+      <c r="O57" s="294"/>
+      <c r="P57" s="294"/>
+      <c r="Q57" s="294"/>
+      <c r="R57" s="294"/>
+      <c r="S57" s="294"/>
+      <c r="T57" s="294"/>
+      <c r="U57" s="294"/>
+      <c r="V57" s="294"/>
+      <c r="W57" s="294"/>
+      <c r="X57" s="294"/>
+      <c r="Y57" s="294"/>
+      <c r="Z57" s="294"/>
     </row>
     <row r="58" spans="1:26">
-      <c r="A58" s="292"/>
-      <c r="B58" s="292"/>
-      <c r="C58" s="292"/>
-      <c r="D58" s="292"/>
-      <c r="E58" s="292"/>
-      <c r="F58" s="292"/>
-      <c r="G58" s="292"/>
-      <c r="H58" s="292"/>
-      <c r="I58" s="292"/>
-      <c r="J58" s="292"/>
-      <c r="K58" s="292"/>
-      <c r="L58" s="292"/>
-      <c r="M58" s="292"/>
-      <c r="N58" s="292"/>
-      <c r="O58" s="292"/>
-      <c r="P58" s="292"/>
-      <c r="Q58" s="292"/>
-      <c r="R58" s="292"/>
-      <c r="S58" s="292"/>
-      <c r="T58" s="292"/>
-      <c r="U58" s="292"/>
-      <c r="V58" s="292"/>
-      <c r="W58" s="292"/>
-      <c r="X58" s="292"/>
-      <c r="Y58" s="292"/>
-      <c r="Z58" s="292"/>
+      <c r="A58" s="294"/>
+      <c r="B58" s="294"/>
+      <c r="C58" s="294"/>
+      <c r="D58" s="294"/>
+      <c r="E58" s="294"/>
+      <c r="F58" s="294"/>
+      <c r="G58" s="294"/>
+      <c r="H58" s="294"/>
+      <c r="I58" s="294"/>
+      <c r="J58" s="294"/>
+      <c r="K58" s="294"/>
+      <c r="L58" s="294"/>
+      <c r="M58" s="294"/>
+      <c r="N58" s="294"/>
+      <c r="O58" s="294"/>
+      <c r="P58" s="294"/>
+      <c r="Q58" s="294"/>
+      <c r="R58" s="294"/>
+      <c r="S58" s="294"/>
+      <c r="T58" s="294"/>
+      <c r="U58" s="294"/>
+      <c r="V58" s="294"/>
+      <c r="W58" s="294"/>
+      <c r="X58" s="294"/>
+      <c r="Y58" s="294"/>
+      <c r="Z58" s="294"/>
     </row>
     <row r="59" spans="1:26">
-      <c r="A59" s="292"/>
-      <c r="B59" s="292"/>
-      <c r="C59" s="292"/>
-      <c r="D59" s="292"/>
-      <c r="E59" s="292"/>
-      <c r="F59" s="292"/>
-      <c r="G59" s="292"/>
-      <c r="H59" s="292"/>
-      <c r="I59" s="292"/>
-      <c r="J59" s="292"/>
-      <c r="K59" s="292"/>
-      <c r="L59" s="292"/>
-      <c r="M59" s="292"/>
-      <c r="N59" s="292"/>
-      <c r="O59" s="292"/>
-      <c r="P59" s="292"/>
-      <c r="Q59" s="292"/>
-      <c r="R59" s="292"/>
-      <c r="S59" s="292"/>
-      <c r="T59" s="292"/>
-      <c r="U59" s="292"/>
-      <c r="V59" s="292"/>
-      <c r="W59" s="292"/>
-      <c r="X59" s="292"/>
-      <c r="Y59" s="292"/>
-      <c r="Z59" s="292"/>
+      <c r="A59" s="294"/>
+      <c r="B59" s="294"/>
+      <c r="C59" s="294"/>
+      <c r="D59" s="294"/>
+      <c r="E59" s="294"/>
+      <c r="F59" s="294"/>
+      <c r="G59" s="294"/>
+      <c r="H59" s="294"/>
+      <c r="I59" s="294"/>
+      <c r="J59" s="294"/>
+      <c r="K59" s="294"/>
+      <c r="L59" s="294"/>
+      <c r="M59" s="294"/>
+      <c r="N59" s="294"/>
+      <c r="O59" s="294"/>
+      <c r="P59" s="294"/>
+      <c r="Q59" s="294"/>
+      <c r="R59" s="294"/>
+      <c r="S59" s="294"/>
+      <c r="T59" s="294"/>
+      <c r="U59" s="294"/>
+      <c r="V59" s="294"/>
+      <c r="W59" s="294"/>
+      <c r="X59" s="294"/>
+      <c r="Y59" s="294"/>
+      <c r="Z59" s="294"/>
     </row>
     <row r="60" spans="1:26">
-      <c r="A60" s="292"/>
-      <c r="B60" s="292"/>
-      <c r="C60" s="292"/>
-      <c r="D60" s="292"/>
-      <c r="E60" s="292"/>
-      <c r="F60" s="292"/>
-      <c r="G60" s="292"/>
-      <c r="H60" s="292"/>
-      <c r="I60" s="292"/>
-      <c r="J60" s="292"/>
-      <c r="K60" s="292"/>
-      <c r="L60" s="292"/>
-      <c r="M60" s="292"/>
-      <c r="N60" s="292"/>
-      <c r="O60" s="292"/>
-      <c r="P60" s="292"/>
-      <c r="Q60" s="292"/>
-      <c r="R60" s="292"/>
-      <c r="S60" s="292"/>
-      <c r="T60" s="292"/>
-      <c r="U60" s="292"/>
-      <c r="V60" s="292"/>
-      <c r="W60" s="292"/>
-      <c r="X60" s="292"/>
-      <c r="Y60" s="292"/>
-      <c r="Z60" s="292"/>
+      <c r="A60" s="294"/>
+      <c r="B60" s="294"/>
+      <c r="C60" s="294"/>
+      <c r="D60" s="294"/>
+      <c r="E60" s="294"/>
+      <c r="F60" s="294"/>
+      <c r="G60" s="294"/>
+      <c r="H60" s="294"/>
+      <c r="I60" s="294"/>
+      <c r="J60" s="294"/>
+      <c r="K60" s="294"/>
+      <c r="L60" s="294"/>
+      <c r="M60" s="294"/>
+      <c r="N60" s="294"/>
+      <c r="O60" s="294"/>
+      <c r="P60" s="294"/>
+      <c r="Q60" s="294"/>
+      <c r="R60" s="294"/>
+      <c r="S60" s="294"/>
+      <c r="T60" s="294"/>
+      <c r="U60" s="294"/>
+      <c r="V60" s="294"/>
+      <c r="W60" s="294"/>
+      <c r="X60" s="294"/>
+      <c r="Y60" s="294"/>
+      <c r="Z60" s="294"/>
     </row>
     <row r="61" spans="1:26">
-      <c r="A61" s="292"/>
-      <c r="B61" s="292"/>
-      <c r="C61" s="292"/>
-      <c r="D61" s="292"/>
-      <c r="E61" s="292"/>
-      <c r="F61" s="292"/>
-      <c r="G61" s="292"/>
-      <c r="H61" s="292"/>
-      <c r="I61" s="292"/>
-      <c r="J61" s="292"/>
-      <c r="K61" s="292"/>
-      <c r="L61" s="292"/>
-      <c r="M61" s="292"/>
-      <c r="N61" s="292"/>
-      <c r="O61" s="292"/>
-      <c r="P61" s="292"/>
-      <c r="Q61" s="292"/>
-      <c r="R61" s="292"/>
-      <c r="S61" s="292"/>
-      <c r="T61" s="292"/>
-      <c r="U61" s="292"/>
-      <c r="V61" s="292"/>
-      <c r="W61" s="292"/>
-      <c r="X61" s="292"/>
-      <c r="Y61" s="292"/>
-      <c r="Z61" s="292"/>
+      <c r="A61" s="294"/>
+      <c r="B61" s="294"/>
+      <c r="C61" s="294"/>
+      <c r="D61" s="294"/>
+      <c r="E61" s="294"/>
+      <c r="F61" s="294"/>
+      <c r="G61" s="294"/>
+      <c r="H61" s="294"/>
+      <c r="I61" s="294"/>
+      <c r="J61" s="294"/>
+      <c r="K61" s="294"/>
+      <c r="L61" s="294"/>
+      <c r="M61" s="294"/>
+      <c r="N61" s="294"/>
+      <c r="O61" s="294"/>
+      <c r="P61" s="294"/>
+      <c r="Q61" s="294"/>
+      <c r="R61" s="294"/>
+      <c r="S61" s="294"/>
+      <c r="T61" s="294"/>
+      <c r="U61" s="294"/>
+      <c r="V61" s="294"/>
+      <c r="W61" s="294"/>
+      <c r="X61" s="294"/>
+      <c r="Y61" s="294"/>
+      <c r="Z61" s="294"/>
     </row>
     <row r="62" spans="1:26">
-      <c r="A62" s="292"/>
-      <c r="B62" s="292"/>
-      <c r="C62" s="292"/>
-      <c r="D62" s="292"/>
-      <c r="E62" s="292"/>
-      <c r="F62" s="292"/>
-      <c r="G62" s="292"/>
-      <c r="H62" s="292"/>
-      <c r="I62" s="292"/>
-      <c r="J62" s="292"/>
-      <c r="K62" s="292"/>
-      <c r="L62" s="292"/>
-      <c r="M62" s="292"/>
-      <c r="N62" s="292"/>
-      <c r="O62" s="292"/>
-      <c r="P62" s="292"/>
-      <c r="Q62" s="292"/>
-      <c r="R62" s="292"/>
-      <c r="S62" s="292"/>
-      <c r="T62" s="292"/>
-      <c r="U62" s="292"/>
-      <c r="V62" s="292"/>
-      <c r="W62" s="292"/>
-      <c r="X62" s="292"/>
-      <c r="Y62" s="292"/>
-      <c r="Z62" s="292"/>
+      <c r="A62" s="294"/>
+      <c r="B62" s="294"/>
+      <c r="C62" s="294"/>
+      <c r="D62" s="294"/>
+      <c r="E62" s="294"/>
+      <c r="F62" s="294"/>
+      <c r="G62" s="294"/>
+      <c r="H62" s="294"/>
+      <c r="I62" s="294"/>
+      <c r="J62" s="294"/>
+      <c r="K62" s="294"/>
+      <c r="L62" s="294"/>
+      <c r="M62" s="294"/>
+      <c r="N62" s="294"/>
+      <c r="O62" s="294"/>
+      <c r="P62" s="294"/>
+      <c r="Q62" s="294"/>
+      <c r="R62" s="294"/>
+      <c r="S62" s="294"/>
+      <c r="T62" s="294"/>
+      <c r="U62" s="294"/>
+      <c r="V62" s="294"/>
+      <c r="W62" s="294"/>
+      <c r="X62" s="294"/>
+      <c r="Y62" s="294"/>
+      <c r="Z62" s="294"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1"/>
@@ -32956,439 +32968,439 @@
   <sheetPr/>
   <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="43.25" style="271" customWidth="1"/>
-    <col min="2" max="2" width="34.125" style="271" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="271"/>
+    <col min="1" max="1" width="43.25" style="273" customWidth="1"/>
+    <col min="2" max="2" width="34.125" style="273" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="273"/>
   </cols>
   <sheetData>
     <row r="1" ht="45" customHeight="1" spans="1:2">
-      <c r="A1" s="272" t="s">
+      <c r="A1" s="274" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="273" t="s">
+      <c r="B1" s="275" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" ht="45" customHeight="1" spans="1:2">
-      <c r="A2" s="274" t="s">
+      <c r="A2" s="276" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="275" t="b">
+      <c r="B2" s="277" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="36" customHeight="1" spans="1:2">
-      <c r="A3" s="276" t="s">
+      <c r="A3" s="278" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="277">
+      <c r="B3" s="279">
         <v>45402</v>
       </c>
     </row>
     <row r="4" ht="45" customHeight="1" spans="1:2">
-      <c r="A4" s="272" t="s">
+      <c r="A4" s="274" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="278" t="str">
+      <c r="B4" s="280" t="str">
         <f>IF(B2,TEXT(EDATE(B3,1)-1,"dd-mmm-yyyy"),B4)</f>
         <v>19-May-2024</v>
       </c>
     </row>
     <row r="5" ht="45" customHeight="1" spans="1:2">
-      <c r="A5" s="274" t="s">
+      <c r="A5" s="276" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="279">
+      <c r="B5" s="281">
         <v>45761</v>
       </c>
     </row>
     <row r="6" ht="45" customHeight="1" spans="1:2">
-      <c r="A6" s="274"/>
-      <c r="B6" s="279"/>
+      <c r="A6" s="276"/>
+      <c r="B6" s="281"/>
     </row>
     <row r="7" ht="24.75" customHeight="1" spans="1:2">
-      <c r="A7" s="280"/>
-      <c r="B7" s="281"/>
+      <c r="A7" s="282"/>
+      <c r="B7" s="283"/>
     </row>
     <row r="8" ht="30" customHeight="1" spans="1:2">
-      <c r="A8" s="282" t="s">
+      <c r="A8" s="284" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="282"/>
+      <c r="B8" s="284"/>
     </row>
     <row r="9" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A9" s="283" t="str">
+      <c r="A9" s="285" t="str">
         <f>TEXT(B3,"dd mmmm yyyy")&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,1)-1,"dd mmmm yyyy"),TEXT(B3+B5-B3,"dd mmmm yyyy"))</f>
         <v>20 April 2024 - 19 May 2024</v>
       </c>
-      <c r="B9" s="284" t="s">
+      <c r="B9" s="286" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A10" s="275" t="str">
+      <c r="A10" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,1),"dd mmmm yyyy"),TEXT(B3+(B5-B3)+1,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,2)-1,"dd mmmm yyyy"),TEXT(B3+(B5-B3)*2+1,"dd mmmm yyyy"))</f>
         <v>20 May 2024 - 19 June 2024</v>
       </c>
-      <c r="B10" s="284"/>
+      <c r="B10" s="286"/>
     </row>
     <row r="11" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A11" s="275" t="str">
+      <c r="A11" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,2),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*2)+2,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,3)-1,"dd mmmm yyyy"),TEXT(B3+((B5-B3)*3+2),"dd mmmm yyyy"))</f>
         <v>20 June 2024 - 19 July 2024</v>
       </c>
-      <c r="B11" s="285"/>
+      <c r="B11" s="287"/>
     </row>
     <row r="12" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A12" s="286" t="str">
+      <c r="A12" s="288" t="str">
         <f>IF(B2,TEXT(EDATE(B3,3),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*3)+3,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,4)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*4)+3),"dd mmmm yyyy"))</f>
         <v>20 July 2024 - 19 August 2024</v>
       </c>
-      <c r="B12" s="273" t="s">
+      <c r="B12" s="275" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A13" s="286" t="str">
+      <c r="A13" s="288" t="str">
         <f>IF(B2,TEXT(EDATE(B3,4),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*4)+4,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,5)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*5)+4),"dd mmmm yyyy"))</f>
         <v>20 August 2024 - 19 September 2024</v>
       </c>
-      <c r="B13" s="287"/>
+      <c r="B13" s="289"/>
     </row>
     <row r="14" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A14" s="275" t="str">
+      <c r="A14" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,5),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*5)+5,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,6)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*6)+5),"dd mmmm yyyy"))</f>
         <v>20 September 2024 - 19 October 2024</v>
       </c>
-      <c r="B14" s="288"/>
+      <c r="B14" s="290"/>
     </row>
     <row r="15" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A15" s="275" t="str">
+      <c r="A15" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,6),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*6)+6,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,7)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*7)+6),"dd mmmm yyyy"))</f>
         <v>20 October 2024 - 19 November 2024</v>
       </c>
-      <c r="B15" s="273" t="s">
+      <c r="B15" s="275" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A16" s="275" t="str">
+      <c r="A16" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,7),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*7)+7,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,8)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*8)+7),"dd mmmm yyyy"))</f>
         <v>20 November 2024 - 19 December 2024</v>
       </c>
-      <c r="B16" s="287"/>
+      <c r="B16" s="289"/>
     </row>
     <row r="17" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A17" s="275" t="str">
+      <c r="A17" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,8),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*8)+8,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,9)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*9)+8),"dd mmmm yyyy"))</f>
         <v>20 December 2024 - 19 January 2025</v>
       </c>
-      <c r="B17" s="288"/>
+      <c r="B17" s="290"/>
     </row>
     <row r="18" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A18" s="275" t="str">
+      <c r="A18" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,9),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*9)+9,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,10)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*10)+9),"dd mmmm yyyy"))</f>
         <v>20 January 2025 - 19 February 2025</v>
       </c>
-      <c r="B18" s="273" t="s">
+      <c r="B18" s="275" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A19" s="275" t="str">
+      <c r="A19" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,10),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*10)+10,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,11)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*11)+10),"dd mmmm yyyy"))</f>
         <v>20 February 2025 - 19 March 2025</v>
       </c>
-      <c r="B19" s="287"/>
+      <c r="B19" s="289"/>
     </row>
     <row r="20" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A20" s="289" t="str">
+      <c r="A20" s="291" t="str">
         <f>IF(B2,TEXT(EDATE(B3,11),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*11)+11,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,12)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*12)+11),"dd mmmm yyyy"))</f>
         <v>20 March 2025 - 19 April 2025</v>
       </c>
-      <c r="B20" s="288"/>
+      <c r="B20" s="290"/>
     </row>
     <row r="21" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A21" s="290" t="str">
+      <c r="A21" s="292" t="str">
         <f>IF(B2,TEXT(EDATE(B3,12),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*12)+12,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,13)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*13)+12),"dd mmmm yyyy"))</f>
         <v>20 April 2025 - 19 May 2025</v>
       </c>
-      <c r="B21" s="275" t="s">
+      <c r="B21" s="277" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A22" s="290" t="str">
+      <c r="A22" s="292" t="str">
         <f>IF(B2,TEXT(EDATE(B3,13),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*13)+13,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,14)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*14)+13),"dd mmmm yyyy"))</f>
         <v>20 May 2025 - 19 June 2025</v>
       </c>
-      <c r="B22" s="275"/>
+      <c r="B22" s="277"/>
     </row>
     <row r="23" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A23" s="289" t="str">
+      <c r="A23" s="291" t="str">
         <f>IF(B2,TEXT(EDATE(B3,14),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*14)+14,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,15)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*15)+14),"dd mmmm yyyy"))</f>
         <v>20 June 2025 - 19 July 2025</v>
       </c>
-      <c r="B23" s="273"/>
+      <c r="B23" s="275"/>
     </row>
     <row r="24" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A24" s="275" t="str">
+      <c r="A24" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,15),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*15)+15,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,16)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*16)+15),"dd mmmm yyyy"))</f>
         <v>20 July 2025 - 19 August 2025</v>
       </c>
-      <c r="B24" s="275" t="s">
+      <c r="B24" s="277" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="25" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A25" s="275" t="str">
+      <c r="A25" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,16),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*16)+16,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,17)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*17)+16),"dd mmmm yyyy"))</f>
         <v>20 August 2025 - 19 September 2025</v>
       </c>
-      <c r="B25" s="275"/>
+      <c r="B25" s="277"/>
     </row>
     <row r="26" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A26" s="273" t="str">
+      <c r="A26" s="275" t="str">
         <f>IF(B2,TEXT(EDATE(B3,17),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*17)+17,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,18)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*18)+17),"dd mmmm yyyy"))</f>
         <v>20 September 2025 - 19 October 2025</v>
       </c>
-      <c r="B26" s="273"/>
+      <c r="B26" s="275"/>
     </row>
     <row r="27" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A27" s="275" t="str">
+      <c r="A27" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,18),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*18)+18,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,19)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*19)+18),"dd mmmm yyyy"))</f>
         <v>20 October 2025 - 19 November 2025</v>
       </c>
-      <c r="B27" s="275" t="s">
+      <c r="B27" s="277" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="28" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A28" s="275" t="str">
+      <c r="A28" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,19),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*19)+19,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,20)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*20)+19),"dd mmmm yyyy"))</f>
         <v>20 November 2025 - 19 December 2025</v>
       </c>
-      <c r="B28" s="275"/>
+      <c r="B28" s="277"/>
     </row>
     <row r="29" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A29" s="273" t="str">
+      <c r="A29" s="275" t="str">
         <f>IF(B2,TEXT(EDATE(B3,20),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*20)+20,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,21)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*21)+20),"dd mmmm yyyy"))</f>
         <v>20 December 2025 - 19 January 2026</v>
       </c>
-      <c r="B29" s="273"/>
+      <c r="B29" s="275"/>
     </row>
     <row r="30" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A30" s="275" t="str">
+      <c r="A30" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,21),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*21)+21,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,22)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*22)+21),"dd mmmm yyyy"))</f>
         <v>20 January 2026 - 19 February 2026</v>
       </c>
-      <c r="B30" s="275" t="s">
+      <c r="B30" s="277" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="31" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A31" s="275" t="str">
+      <c r="A31" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,22),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*22)+22,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,23)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*23)+22),"dd mmmm yyyy"))</f>
         <v>20 February 2026 - 19 March 2026</v>
       </c>
-      <c r="B31" s="275"/>
+      <c r="B31" s="277"/>
     </row>
     <row r="32" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A32" s="273" t="str">
+      <c r="A32" s="275" t="str">
         <f>IF(B2,TEXT(EDATE(B3,23),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*23)+23,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,24)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*24)+23),"dd mmmm yyyy"))</f>
         <v>20 March 2026 - 19 April 2026</v>
       </c>
-      <c r="B32" s="273"/>
+      <c r="B32" s="275"/>
     </row>
     <row r="33" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A33" s="275" t="str">
+      <c r="A33" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,24),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*24)+24,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,25)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*25)+24),"dd mmmm yyyy"))</f>
         <v>20 April 2026 - 19 May 2026</v>
       </c>
-      <c r="B33" s="275" t="s">
+      <c r="B33" s="277" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="34" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A34" s="275" t="str">
+      <c r="A34" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,25),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*25)+25,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,26)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*26)+25),"dd mmmm yyyy"))</f>
         <v>20 May 2026 - 19 June 2026</v>
       </c>
-      <c r="B34" s="275"/>
+      <c r="B34" s="277"/>
     </row>
     <row r="35" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A35" s="273" t="str">
+      <c r="A35" s="275" t="str">
         <f>IF(B2,TEXT(EDATE(B3,26),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*26)+26,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,27)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*27)+26),"dd mmmm yyyy"))</f>
         <v>20 June 2026 - 19 July 2026</v>
       </c>
-      <c r="B35" s="273"/>
+      <c r="B35" s="275"/>
     </row>
     <row r="36" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A36" s="275" t="str">
+      <c r="A36" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,27),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*27)+27,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,28)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*28)+27),"dd mmmm yyyy"))</f>
         <v>20 July 2026 - 19 August 2026</v>
       </c>
-      <c r="B36" s="275" t="s">
+      <c r="B36" s="277" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="37" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A37" s="275" t="str">
+      <c r="A37" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,28),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*28)+28,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,29)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*29)+28),"dd mmmm yyyy"))</f>
         <v>20 August 2026 - 19 September 2026</v>
       </c>
-      <c r="B37" s="275"/>
+      <c r="B37" s="277"/>
     </row>
     <row r="38" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A38" s="273" t="str">
+      <c r="A38" s="275" t="str">
         <f>IF(B2,TEXT(EDATE(B3,29),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*29)+29,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,30)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*30)+29),"dd mmmm yyyy"))</f>
         <v>20 September 2026 - 19 October 2026</v>
       </c>
-      <c r="B38" s="273"/>
+      <c r="B38" s="275"/>
     </row>
     <row r="39" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A39" s="275" t="str">
+      <c r="A39" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,30),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*30)+30,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,31)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*31)+30),"dd mmmm yyyy"))</f>
         <v>20 October 2026 - 19 November 2026</v>
       </c>
-      <c r="B39" s="275" t="s">
+      <c r="B39" s="277" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="40" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A40" s="275" t="str">
+      <c r="A40" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,31),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*31)+31,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,32)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*32)+31),"dd mmmm yyyy"))</f>
         <v>20 November 2026 - 19 December 2026</v>
       </c>
-      <c r="B40" s="275"/>
+      <c r="B40" s="277"/>
     </row>
     <row r="41" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A41" s="273" t="str">
+      <c r="A41" s="275" t="str">
         <f>IF(B2,TEXT(EDATE(B3,32),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*32)+32,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,33)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*33)+32),"dd mmmm yyyy"))</f>
         <v>20 December 2026 - 19 January 2027</v>
       </c>
-      <c r="B41" s="273"/>
+      <c r="B41" s="275"/>
     </row>
     <row r="42" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A42" s="275" t="str">
+      <c r="A42" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,33),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*33)+33,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,34)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*34)+33),"dd mmmm yyyy"))</f>
         <v>20 January 2027 - 19 February 2027</v>
       </c>
-      <c r="B42" s="275" t="s">
+      <c r="B42" s="277" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="43" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A43" s="275" t="str">
+      <c r="A43" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,34),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*34)+34,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,35)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*35)+34),"dd mmmm yyyy"))</f>
         <v>20 February 2027 - 19 March 2027</v>
       </c>
-      <c r="B43" s="275"/>
+      <c r="B43" s="277"/>
     </row>
     <row r="44" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A44" s="273" t="str">
+      <c r="A44" s="275" t="str">
         <f>IF(B2,TEXT(EDATE(B3,35),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*35)+35,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,36)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*36)+35),"dd mmmm yyyy"))</f>
         <v>20 March 2027 - 19 April 2027</v>
       </c>
-      <c r="B44" s="273"/>
+      <c r="B44" s="275"/>
     </row>
     <row r="45" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A45" s="275" t="str">
+      <c r="A45" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,36),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*36)+36,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,37)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*37)+36),"dd mmmm yyyy"))</f>
         <v>20 April 2027 - 19 May 2027</v>
       </c>
-      <c r="B45" s="275" t="s">
+      <c r="B45" s="277" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="46" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A46" s="275" t="str">
+      <c r="A46" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,37),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*37)+37,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,38)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*38)+37),"dd mmmm yyyy"))</f>
         <v>20 May 2027 - 19 June 2027</v>
       </c>
-      <c r="B46" s="275"/>
+      <c r="B46" s="277"/>
     </row>
     <row r="47" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A47" s="273" t="str">
+      <c r="A47" s="275" t="str">
         <f>IF(B2,TEXT(EDATE(B3,38),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*38)+38,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,39)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*39)+38),"dd mmmm yyyy"))</f>
         <v>20 June 2027 - 19 July 2027</v>
       </c>
-      <c r="B47" s="273"/>
+      <c r="B47" s="275"/>
     </row>
     <row r="48" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A48" s="275" t="str">
+      <c r="A48" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,39),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*39)+39,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,40)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*40)+39),"dd mmmm yyyy"))</f>
         <v>20 July 2027 - 19 August 2027</v>
       </c>
-      <c r="B48" s="275" t="s">
+      <c r="B48" s="277" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="49" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A49" s="275" t="str">
+      <c r="A49" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,40),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*40)+40,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,41)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*41)+40),"dd mmmm yyyy"))</f>
         <v>20 August 2027 - 19 September 2027</v>
       </c>
-      <c r="B49" s="275"/>
+      <c r="B49" s="277"/>
     </row>
     <row r="50" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A50" s="273" t="str">
+      <c r="A50" s="275" t="str">
         <f>IF(B2,TEXT(EDATE(B3,41),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*41)+41,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,42)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*42)+41),"dd mmmm yyyy"))</f>
         <v>20 September 2027 - 19 October 2027</v>
       </c>
-      <c r="B50" s="273"/>
+      <c r="B50" s="275"/>
     </row>
     <row r="51" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A51" s="275" t="str">
+      <c r="A51" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,42),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*42)+42,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,43)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*43)+42),"dd mmmm yyyy"))</f>
         <v>20 October 2027 - 19 November 2027</v>
       </c>
-      <c r="B51" s="275" t="s">
+      <c r="B51" s="277" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="52" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A52" s="275" t="str">
+      <c r="A52" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,43),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*43)+43,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,44)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*44)+43),"dd mmmm yyyy"))</f>
         <v>20 November 2027 - 19 December 2027</v>
       </c>
-      <c r="B52" s="275"/>
+      <c r="B52" s="277"/>
     </row>
     <row r="53" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A53" s="273" t="str">
+      <c r="A53" s="275" t="str">
         <f>IF(B2,TEXT(EDATE(B3,44),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*44)+44,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,45)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*45)+44),"dd mmmm yyyy"))</f>
         <v>20 December 2027 - 19 January 2028</v>
       </c>
-      <c r="B53" s="273"/>
+      <c r="B53" s="275"/>
     </row>
     <row r="54" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A54" s="275" t="str">
+      <c r="A54" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,45),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*45)+45,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,46)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*46)+45),"dd mmmm yyyy"))</f>
         <v>20 January 2028 - 19 February 2028</v>
       </c>
-      <c r="B54" s="275" t="s">
+      <c r="B54" s="277" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="55" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A55" s="275" t="str">
+      <c r="A55" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,46),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*46)+46,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,47)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*47)+46),"dd mmmm yyyy"))</f>
         <v>20 February 2028 - 19 March 2028</v>
       </c>
-      <c r="B55" s="275"/>
+      <c r="B55" s="277"/>
     </row>
     <row r="56" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A56" s="275" t="str">
+      <c r="A56" s="277" t="str">
         <f>IF(B2,TEXT(EDATE(B3,47),"dd mmmm yyyy"),TEXT(B3+((B5-B3)*47)+47,"dd mmmm yyyy"))&amp;" - "&amp;IF(B2,TEXT(EDATE(B3,48)-1,"dd mmmm yyyy"),TEXT(B3+(((B5-B3)*48)+47),"dd mmmm yyyy"))</f>
         <v>20 March 2028 - 19 April 2028</v>
       </c>
-      <c r="B56" s="275"/>
+      <c r="B56" s="277"/>
     </row>
     <row r="57" ht="20.25" customHeight="1"/>
     <row r="58" ht="20.25" customHeight="1"/>
@@ -33398,75 +33410,75 @@
     <row r="62" ht="20.25" customHeight="1"/>
     <row r="63" ht="20.25" customHeight="1"/>
     <row r="64" ht="20.25" customHeight="1"/>
-    <row r="65" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="66" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="67" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="68" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="69" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="70" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="71" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="72" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="73" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="74" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="75" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="76" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="77" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="78" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="79" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="80" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="81" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="82" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="83" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="84" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="85" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="86" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="87" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="88" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="89" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="90" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="91" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="92" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="93" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="94" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="95" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="96" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="97" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="98" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="99" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="100" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="101" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="102" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="103" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="104" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="105" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="106" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="107" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="108" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="109" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="110" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="111" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="112" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="113" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="114" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="115" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="116" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="117" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="118" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="119" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="120" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="121" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="122" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="123" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="124" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="125" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="126" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="127" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="129" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="130" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="131" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="132" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="133" s="271" customFormat="1" ht="20.25" customHeight="1"/>
-    <row r="134" s="271" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="65" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="66" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="67" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="68" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="69" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="70" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="71" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="72" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="73" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="74" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="75" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="76" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="77" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="78" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="79" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="80" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="81" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="82" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="83" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="84" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="85" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="86" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="87" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="88" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="89" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="90" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="91" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="92" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="93" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="94" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="95" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="96" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="97" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="98" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="99" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="100" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="101" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="102" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="103" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="104" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="105" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="106" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="107" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="108" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="109" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="110" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="111" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="112" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="113" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="114" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="115" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="116" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="117" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="118" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="119" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="120" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="121" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="122" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="123" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="124" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="125" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="126" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="127" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="129" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="130" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="131" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="132" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="133" s="273" customFormat="1" ht="20.25" customHeight="1"/>
+    <row r="134" s="273" customFormat="1" ht="20.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="19">
     <mergeCell ref="A8:B8"/>
@@ -33499,8 +33511,8 @@
   <sheetPr/>
   <dimension ref="A2:P211"/>
   <sheetViews>
-    <sheetView topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:C26"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -33558,7 +33570,7 @@
       <c r="J3" s="241" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="250" t="s">
+      <c r="M3" s="252" t="s">
         <v>31</v>
       </c>
       <c r="N3" s="241" t="s">
@@ -33665,7 +33677,7 @@
         <f>'October 2024 - December 2024'!C5</f>
         <v>-10683</v>
       </c>
-      <c r="P6" s="251"/>
+      <c r="P6" s="253"/>
     </row>
     <row r="7" ht="35.25" customHeight="1" spans="1:14">
       <c r="A7" s="206"/>
@@ -33755,7 +33767,7 @@
         <f>'July 2024 - September 2024'!E202</f>
         <v>502.709999999998</v>
       </c>
-      <c r="M9" s="252" t="str">
+      <c r="M9" s="254" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,15),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*15+15),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,18)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*18+17),"dd mmmm yyyy"))</f>
         <v>20 July 2025 - 19 October 2025</v>
       </c>
@@ -33791,7 +33803,7 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,18),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*18+18),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,21)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*21+20),"dd mmmm yyyy"))</f>
         <v>20 October 2025 - 19 January 2026</v>
       </c>
-      <c r="N10" s="253">
+      <c r="N10" s="255">
         <f>'October 2025 - December 2025'!C5</f>
         <v>0</v>
       </c>
@@ -33819,7 +33831,7 @@
         <f>'October 2024 - December 2024'!E174</f>
         <v>229.399999999998</v>
       </c>
-      <c r="M11" s="254" t="str">
+      <c r="M11" s="256" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,21),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*21+21),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,24)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*24+23),"dd mmmm yyyy"))</f>
         <v>20 January 2026 - 19 April 2026</v>
       </c>
@@ -34060,7 +34072,7 @@
       </c>
     </row>
     <row r="20" ht="33" customHeight="1" spans="9:10">
-      <c r="I20" s="248" t="str">
+      <c r="I20" s="249" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,16),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*16)+16,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,17)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*17+16),"dd mmmm yyyy"))</f>
         <v>20 August 2025 - 19 September 2025</v>
       </c>
@@ -34070,7 +34082,7 @@
       </c>
     </row>
     <row r="21" ht="35.25" customHeight="1" spans="9:10">
-      <c r="I21" s="248" t="str">
+      <c r="I21" s="250" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,17),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*17)+17,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,18)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*18+17),"dd mmmm yyyy"))</f>
         <v>20 September 2025 - 19 October 2025</v>
       </c>
@@ -34271,7 +34283,7 @@
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,27),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*27)+27,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,28)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*28+27),"dd mmmm yyyy"))</f>
         <v>20 July 2026 - 19 August 2026</v>
       </c>
-      <c r="J31" s="249">
+      <c r="J31" s="251">
         <f>Forecast_10!E136</f>
         <v>6361.8</v>
       </c>
@@ -34823,7 +34835,7 @@
       <c r="B71" s="111" t="s">
         <v>77</v>
       </c>
-      <c r="C71" s="255">
+      <c r="C71" s="257">
         <f>SUM(C63:C70)</f>
         <v>443</v>
       </c>
@@ -34840,7 +34852,7 @@
         <v>79</v>
       </c>
       <c r="B73" s="36"/>
-      <c r="C73" s="255">
+      <c r="C73" s="257">
         <v>0</v>
       </c>
     </row>
@@ -34849,7 +34861,7 @@
         <v>80</v>
       </c>
       <c r="B74" s="36"/>
-      <c r="C74" s="255">
+      <c r="C74" s="257">
         <v>0</v>
       </c>
     </row>
@@ -34858,7 +34870,7 @@
         <v>81</v>
       </c>
       <c r="B75" s="36"/>
-      <c r="C75" s="255">
+      <c r="C75" s="257">
         <v>0</v>
       </c>
     </row>
@@ -34867,57 +34879,57 @@
         <v>82</v>
       </c>
       <c r="B76" s="36"/>
-      <c r="C76" s="255">
+      <c r="C76" s="257">
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="35"/>
       <c r="B77" s="36"/>
-      <c r="C77" s="255">
+      <c r="C77" s="257">
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="35"/>
       <c r="B78" s="36"/>
-      <c r="C78" s="255">
+      <c r="C78" s="257">
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="35"/>
       <c r="B79" s="36"/>
-      <c r="C79" s="255">
+      <c r="C79" s="257">
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="35"/>
       <c r="B80" s="36"/>
-      <c r="C80" s="255">
+      <c r="C80" s="257">
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="35"/>
       <c r="B81" s="36"/>
-      <c r="C81" s="255">
+      <c r="C81" s="257">
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="256"/>
-      <c r="B82" s="257" t="s">
+      <c r="A82" s="258"/>
+      <c r="B82" s="259" t="s">
         <v>77</v>
       </c>
-      <c r="C82" s="255">
+      <c r="C82" s="257">
         <f>SUM(C73:C81)</f>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="258" t="s">
+      <c r="A83" s="260" t="s">
         <v>83</v>
       </c>
       <c r="B83" s="232"/>
@@ -34935,7 +34947,7 @@
       </c>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="259" t="s">
+      <c r="A85" s="261" t="s">
         <v>86</v>
       </c>
       <c r="B85" s="36" t="s">
@@ -34981,8 +34993,8 @@
       </c>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="256"/>
-      <c r="B91" s="257" t="s">
+      <c r="A91" s="258"/>
+      <c r="B91" s="259" t="s">
         <v>88</v>
       </c>
       <c r="C91" s="37">
@@ -34998,60 +35010,60 @@
       <c r="C92" s="233"/>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="260" t="s">
+      <c r="A93" s="262" t="s">
         <v>90</v>
       </c>
-      <c r="B93" s="261"/>
-      <c r="C93" s="255">
+      <c r="B93" s="263"/>
+      <c r="C93" s="257">
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="35"/>
       <c r="B94" s="36"/>
-      <c r="C94" s="255">
+      <c r="C94" s="257">
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="35"/>
       <c r="B95" s="36"/>
-      <c r="C95" s="255">
+      <c r="C95" s="257">
         <v>0</v>
       </c>
     </row>
     <row r="96" ht="15.75" customHeight="1" spans="1:3">
       <c r="A96" s="35"/>
       <c r="B96" s="36"/>
-      <c r="C96" s="255">
+      <c r="C96" s="257">
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="35"/>
       <c r="B97" s="36"/>
-      <c r="C97" s="255">
+      <c r="C97" s="257">
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="35"/>
       <c r="B98" s="36"/>
-      <c r="C98" s="255">
+      <c r="C98" s="257">
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="35"/>
       <c r="B99" s="36"/>
-      <c r="C99" s="255">
+      <c r="C99" s="257">
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="35"/>
       <c r="B100" s="36"/>
-      <c r="C100" s="255">
+      <c r="C100" s="257">
         <v>0</v>
       </c>
     </row>
@@ -35149,7 +35161,7 @@
       <c r="B111" s="111" t="s">
         <v>77</v>
       </c>
-      <c r="C111" s="255">
+      <c r="C111" s="257">
         <f>SUM(C103:C110)</f>
         <v>1060</v>
       </c>
@@ -35159,24 +35171,24 @@
       <c r="B112" s="111" t="s">
         <v>101</v>
       </c>
-      <c r="C112" s="255">
+      <c r="C112" s="257">
         <f>C71+C82+C91+C101+C111</f>
         <v>1503</v>
       </c>
     </row>
     <row r="113" spans="1:3">
-      <c r="A113" s="262" t="s">
+      <c r="A113" s="264" t="s">
         <v>102</v>
       </c>
-      <c r="B113" s="263"/>
-      <c r="C113" s="264"/>
+      <c r="B113" s="265"/>
+      <c r="C113" s="266"/>
     </row>
     <row r="114" spans="1:8">
       <c r="A114" s="118" t="s">
         <v>103</v>
       </c>
-      <c r="B114" s="265"/>
-      <c r="C114" s="266">
+      <c r="B114" s="267"/>
+      <c r="C114" s="268">
         <v>16033</v>
       </c>
       <c r="D114" s="14"/>
@@ -35190,7 +35202,7 @@
         <v>104</v>
       </c>
       <c r="B115" s="36"/>
-      <c r="C115" s="267">
+      <c r="C115" s="269">
         <f>5000</f>
         <v>5000</v>
       </c>
@@ -35205,7 +35217,7 @@
         <v>105</v>
       </c>
       <c r="B116" s="36"/>
-      <c r="C116" s="268">
+      <c r="C116" s="270">
         <f>3300</f>
         <v>3300</v>
       </c>
@@ -35220,7 +35232,7 @@
         <v>106</v>
       </c>
       <c r="B117" s="36"/>
-      <c r="C117" s="268">
+      <c r="C117" s="270">
         <v>0</v>
       </c>
       <c r="D117" s="14"/>
@@ -35234,7 +35246,7 @@
         <v>107</v>
       </c>
       <c r="B118" s="36"/>
-      <c r="C118" s="268">
+      <c r="C118" s="270">
         <v>0</v>
       </c>
       <c r="D118" s="14"/>
@@ -35304,30 +35316,30 @@
       <c r="H123" s="14"/>
     </row>
     <row r="124" spans="1:3">
-      <c r="A124" s="256"/>
-      <c r="B124" s="257" t="s">
+      <c r="A124" s="258"/>
+      <c r="B124" s="259" t="s">
         <v>108</v>
       </c>
-      <c r="C124" s="255">
+      <c r="C124" s="257">
         <f>SUM(C113:C123)</f>
         <v>24333</v>
       </c>
     </row>
     <row r="125" spans="1:3">
-      <c r="A125" s="256"/>
-      <c r="B125" s="257" t="s">
+      <c r="A125" s="258"/>
+      <c r="B125" s="259" t="s">
         <v>109</v>
       </c>
-      <c r="C125" s="255">
+      <c r="C125" s="257">
         <f>ABS(C112+ABS(C124))</f>
         <v>25836</v>
       </c>
     </row>
     <row r="126" spans="5:5">
-      <c r="E126" s="269"/>
+      <c r="E126" s="271"/>
     </row>
     <row r="127" spans="5:5">
-      <c r="E127" s="269"/>
+      <c r="E127" s="271"/>
     </row>
     <row r="129" ht="45" customHeight="1"/>
     <row r="130" ht="45" customHeight="1" spans="1:5">
@@ -35600,8 +35612,8 @@
         <v>Balance Brought Forward From May 2024</v>
       </c>
       <c r="B158" s="57"/>
-      <c r="C158" s="270"/>
-      <c r="D158" s="270"/>
+      <c r="C158" s="272"/>
+      <c r="D158" s="272"/>
       <c r="E158" s="94">
         <f>E151</f>
         <v>0</v>
@@ -35867,8 +35879,8 @@
         <v>Balance Brought Forward From June 2024</v>
       </c>
       <c r="B185" s="57"/>
-      <c r="C185" s="270"/>
-      <c r="D185" s="270"/>
+      <c r="C185" s="272"/>
+      <c r="D185" s="272"/>
       <c r="E185" s="97">
         <f>E178</f>
         <v>-416.68</v>

</xml_diff>

<commit_message>
docs: 1. Document Updated
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -1449,7 +1449,11 @@
 - Best Mart 360 and 759 Store ~ $65.6
 - Market Chicken Chops ~ $17
 - Market Kwun Kee ~ $21
-- Transport Fee to East Kowloon Hospital $4</t>
+- Transport Fee to East Kowloon Hospital $4
+- Transport Fee Round Trip to Mong Kok $4
+- Transport Fee from Kowloon Tong To WTS $2
+- Ngan Lung Restaurant $55
+- Oat meal $19</t>
   </si>
   <si>
     <t>3.. Food And Transport Expenses
@@ -6163,7 +6167,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>18.9</v>
+        <v>12.9</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -6179,7 +6183,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>11286.8</v>
+        <v>11206.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -6195,7 +6199,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>11305.7</v>
+        <v>11219.7</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -7800,7 +7804,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'October 2025 - December 2025'!E190</f>
-        <v>6357.8</v>
+        <v>6277.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -8072,7 +8076,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>8052.8</v>
+        <v>7972.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -8164,7 +8168,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>8052.8</v>
+        <v>7972.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -8436,7 +8440,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>9591.8</v>
+        <v>9511.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -8528,7 +8532,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>9591.8</v>
+        <v>9511.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -8800,7 +8804,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>11286.8</v>
+        <v>11206.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -9319,7 +9323,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>18.9</v>
+        <v>12.9</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -9335,7 +9339,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>16109.8</v>
+        <v>16029.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -9351,7 +9355,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>16128.7</v>
+        <v>16042.7</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -10956,7 +10960,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'January 2026 - March 2026'!E190</f>
-        <v>11286.8</v>
+        <v>11206.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -11256,7 +11260,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>12875.8</v>
+        <v>12795.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -11348,7 +11352,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>12875.8</v>
+        <v>12795.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -11648,7 +11652,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>14520.8</v>
+        <v>14440.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -11740,7 +11744,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>14520.8</v>
+        <v>14440.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -12040,7 +12044,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>16109.8</v>
+        <v>16029.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -12552,7 +12556,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>18.9</v>
+        <v>12.9</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -12568,7 +12572,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>21038.8</v>
+        <v>20958.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -12584,7 +12588,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>21057.7</v>
+        <v>20971.7</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -14189,7 +14193,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'April 2026 - June 2026'!E190</f>
-        <v>16109.8</v>
+        <v>16029.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -14461,7 +14465,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>17804.8</v>
+        <v>17724.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -14553,7 +14557,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>17804.8</v>
+        <v>17724.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -14825,7 +14829,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>19343.8</v>
+        <v>19263.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -14917,7 +14921,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>19343.8</v>
+        <v>19263.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -15189,7 +15193,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>21038.8</v>
+        <v>20958.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -15699,7 +15703,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>18.9</v>
+        <v>12.9</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -15715,7 +15719,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>25861.8</v>
+        <v>25781.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -15731,7 +15735,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>25880.7</v>
+        <v>25794.7</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -17336,7 +17340,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'July 2026 - September 2026'!E190</f>
-        <v>21038.8</v>
+        <v>20958.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -17608,7 +17612,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>22627.8</v>
+        <v>22547.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -17700,7 +17704,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>22627.8</v>
+        <v>22547.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -17972,7 +17976,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>24272.8</v>
+        <v>24192.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -18064,7 +18068,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>24272.8</v>
+        <v>24192.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -18336,7 +18340,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>25861.8</v>
+        <v>25781.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -18856,7 +18860,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>18.9</v>
+        <v>12.9</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -18872,7 +18876,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>30790.8</v>
+        <v>30710.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -18888,7 +18892,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>30809.7</v>
+        <v>30723.7</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -20493,7 +20497,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'October 2026 - December 2026'!E190</f>
-        <v>25861.8</v>
+        <v>25781.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -20765,7 +20769,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>27556.8</v>
+        <v>27476.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -20857,7 +20861,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>27556.8</v>
+        <v>27476.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -21129,7 +21133,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>29095.8</v>
+        <v>29015.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -21221,7 +21225,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>29095.8</v>
+        <v>29015.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -21493,7 +21497,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>30790.8</v>
+        <v>30710.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -22011,7 +22015,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>18.9</v>
+        <v>12.9</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -22027,7 +22031,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -22043,7 +22047,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35632.7</v>
+        <v>35546.7</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -23648,7 +23652,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'January 2027 - March 2027'!E190</f>
-        <v>30790.8</v>
+        <v>30710.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -23920,7 +23924,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>32379.8</v>
+        <v>32299.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -24012,7 +24016,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>32379.8</v>
+        <v>32299.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -24284,7 +24288,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>34024.8</v>
+        <v>33944.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -24376,7 +24380,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>34024.8</v>
+        <v>33944.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -24648,7 +24652,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -25159,7 +25163,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>18.9</v>
+        <v>12.9</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -25175,7 +25179,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -25191,7 +25195,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35632.7</v>
+        <v>35546.7</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -26700,7 +26704,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'April 2027 - June 2027'!E190</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -26968,7 +26972,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -27060,7 +27064,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -27328,7 +27332,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -27420,7 +27424,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -27688,7 +27692,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -28139,7 +28143,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>18.9</v>
+        <v>12.9</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -28155,7 +28159,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -28171,7 +28175,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35632.7</v>
+        <v>35546.7</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -29680,7 +29684,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>Forecast_14!E190</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -29948,7 +29952,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -30040,7 +30044,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -30308,7 +30312,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -30400,7 +30404,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -30668,7 +30672,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -31121,7 +31125,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>18.9</v>
+        <v>12.9</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -31137,7 +31141,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -31153,7 +31157,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35632.7</v>
+        <v>35546.7</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -32662,7 +32666,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>Forecast_15!E190</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -32930,7 +32934,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -33022,7 +33026,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -33290,7 +33294,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -33382,7 +33386,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -33650,7 +33654,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -34685,7 +34689,7 @@
         <v>34</v>
       </c>
       <c r="C4" s="211">
-        <v>226</v>
+        <v>126</v>
       </c>
       <c r="D4" s="212" t="s">
         <v>33</v>
@@ -34719,7 +34723,7 @@
         <v>35</v>
       </c>
       <c r="C5" s="211">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D5" s="213"/>
       <c r="E5" s="5" t="s">
@@ -34945,7 +34949,7 @@
         <v>42</v>
       </c>
       <c r="C12" s="211">
-        <v>51.3</v>
+        <v>57.3</v>
       </c>
       <c r="D12" s="213"/>
       <c r="E12" s="5" t="s">
@@ -35025,7 +35029,7 @@
       </c>
       <c r="J14" s="246">
         <f>'January 2025 - March 2025'!E168</f>
-        <v>441.199999999998</v>
+        <v>361.199999999998</v>
       </c>
       <c r="M14" s="247" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,30),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*30+30),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,33)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+32),"dd mmmm yyyy"))</f>
@@ -35042,14 +35046,14 @@
         <v>45</v>
       </c>
       <c r="C15" s="211">
-        <v>18.9</v>
+        <v>12.9</v>
       </c>
       <c r="D15" s="213"/>
       <c r="E15" s="239" t="s">
         <v>45</v>
       </c>
       <c r="F15" s="237">
-        <v>22.9</v>
+        <v>18.9</v>
       </c>
       <c r="I15" s="249" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,11),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*11)+11,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,12)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*12+11),"dd mmmm yyyy"))</f>
@@ -35057,7 +35061,7 @@
       </c>
       <c r="J15" s="250">
         <f>'January 2025 - March 2025'!E195</f>
-        <v>855.199999999998</v>
+        <v>775.199999999998</v>
       </c>
       <c r="M15" s="247" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,33),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+33),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,36)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+35),"dd mmmm yyyy"))</f>
@@ -35089,7 +35093,7 @@
       </c>
       <c r="J16" s="250">
         <f>'April 2025 - June 2025'!E136</f>
-        <v>944.199999999998</v>
+        <v>864.199999999998</v>
       </c>
       <c r="M16" s="247" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,36),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+36),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,39)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+38),"dd mmmm yyyy"))</f>
@@ -35107,7 +35111,7 @@
       </c>
       <c r="C17" s="217">
         <f>SUM(C4:C16)</f>
-        <v>441.2</v>
+        <v>361.2</v>
       </c>
       <c r="D17" s="218"/>
       <c r="E17" s="216" t="s">
@@ -35115,7 +35119,7 @@
       </c>
       <c r="F17" s="240">
         <f>SUM(F4:F16)</f>
-        <v>445.2</v>
+        <v>441.2</v>
       </c>
       <c r="I17" s="251" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,13),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*13)+13,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,14)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*14+13),"dd mmmm yyyy"))</f>
@@ -35123,7 +35127,7 @@
       </c>
       <c r="J17" s="250">
         <f>'April 2025 - June 2025'!E163</f>
-        <v>1024.2</v>
+        <v>944.199999999998</v>
       </c>
       <c r="M17" s="247" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+39),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
@@ -35141,7 +35145,7 @@
       </c>
       <c r="J18" s="250">
         <f>'April 2025 - June 2025'!E190</f>
-        <v>1188.5</v>
+        <v>1108.5</v>
       </c>
       <c r="M18" s="247" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+42),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
@@ -35159,7 +35163,7 @@
       </c>
       <c r="J19" s="250">
         <f>'July 2025 - September 2025'!E136</f>
-        <v>1283.5</v>
+        <v>1203.5</v>
       </c>
       <c r="M19" s="247" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+45),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
@@ -35177,7 +35181,7 @@
       </c>
       <c r="J20" s="250">
         <f>'July 2025 - September 2025'!E163</f>
-        <v>1422.5</v>
+        <v>1342.5</v>
       </c>
     </row>
     <row r="21" ht="35.25" customHeight="1" spans="9:10">
@@ -35187,7 +35191,7 @@
       </c>
       <c r="J21" s="250">
         <f>'July 2025 - September 2025'!E190</f>
-        <v>1434.5</v>
+        <v>1354.5</v>
       </c>
     </row>
     <row r="22" ht="35.25" customHeight="1" spans="9:10">
@@ -35197,7 +35201,7 @@
       </c>
       <c r="J22" s="250">
         <f>'October 2025 - December 2025'!E136</f>
-        <v>3023.5</v>
+        <v>2943.5</v>
       </c>
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:10">
@@ -35217,7 +35221,7 @@
       </c>
       <c r="J23" s="250">
         <f>'October 2025 - December 2025'!E163</f>
-        <v>4668.5</v>
+        <v>4588.5</v>
       </c>
     </row>
     <row r="24" ht="24.75" customHeight="1" spans="1:10">
@@ -35242,7 +35246,7 @@
       </c>
       <c r="J24" s="250">
         <f>'October 2025 - December 2025'!E190</f>
-        <v>6357.8</v>
+        <v>6277.8</v>
       </c>
     </row>
     <row r="25" ht="34.5" customHeight="1" spans="1:10">
@@ -35267,7 +35271,7 @@
       </c>
       <c r="J25" s="250">
         <f>'January 2026 - March 2026'!E136</f>
-        <v>8052.8</v>
+        <v>7972.8</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1" spans="1:10">
@@ -35286,7 +35290,7 @@
       </c>
       <c r="J26" s="250">
         <f>'January 2026 - March 2026'!E163</f>
-        <v>9591.8</v>
+        <v>9511.8</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1" spans="1:10">
@@ -35305,7 +35309,7 @@
       </c>
       <c r="J27" s="250">
         <f>'January 2026 - March 2026'!E190</f>
-        <v>11286.8</v>
+        <v>11206.8</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:10">
@@ -35324,7 +35328,7 @@
       </c>
       <c r="J28" s="250">
         <f>'April 2026 - June 2026'!E136</f>
-        <v>12875.8</v>
+        <v>12795.8</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:10">
@@ -35343,7 +35347,7 @@
       </c>
       <c r="J29" s="250">
         <f>'April 2026 - June 2026'!E163</f>
-        <v>14520.8</v>
+        <v>14440.8</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1" spans="1:10">
@@ -35362,7 +35366,7 @@
       </c>
       <c r="J30" s="246">
         <f>'April 2026 - June 2026'!E190</f>
-        <v>16109.8</v>
+        <v>16029.8</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1" spans="1:10">
@@ -35384,7 +35388,7 @@
       </c>
       <c r="J31" s="254">
         <f>'July 2026 - September 2026'!E136</f>
-        <v>17804.8</v>
+        <v>17724.8</v>
       </c>
     </row>
     <row r="32" ht="30" customHeight="1" spans="9:10">
@@ -35394,7 +35398,7 @@
       </c>
       <c r="J32" s="250">
         <f>'July 2026 - September 2026'!E163</f>
-        <v>19343.8</v>
+        <v>19263.8</v>
       </c>
     </row>
     <row r="33" ht="27.75" customHeight="1" spans="9:10">
@@ -35404,7 +35408,7 @@
       </c>
       <c r="J33" s="250">
         <f>'July 2026 - September 2026'!E190</f>
-        <v>21038.8</v>
+        <v>20958.8</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1" spans="9:10">
@@ -35414,7 +35418,7 @@
       </c>
       <c r="J34" s="250">
         <f>'October 2026 - December 2026'!E136</f>
-        <v>22627.8</v>
+        <v>22547.8</v>
       </c>
     </row>
     <row r="35" ht="30" customHeight="1" spans="1:10">
@@ -35434,7 +35438,7 @@
       </c>
       <c r="J35" s="250">
         <f>'October 2026 - December 2026'!E163</f>
-        <v>24272.8</v>
+        <v>24192.8</v>
       </c>
     </row>
     <row r="36" ht="24.75" customHeight="1" spans="1:10">
@@ -35459,7 +35463,7 @@
       </c>
       <c r="J36" s="250">
         <f>'October 2026 - December 2026'!E190</f>
-        <v>25861.8</v>
+        <v>25781.8</v>
       </c>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:10">
@@ -35484,7 +35488,7 @@
       </c>
       <c r="J37" s="250">
         <f>'January 2027 - March 2027'!E136</f>
-        <v>27556.8</v>
+        <v>27476.8</v>
       </c>
     </row>
     <row r="38" ht="24.75" customHeight="1" spans="1:10">
@@ -35509,7 +35513,7 @@
       </c>
       <c r="J38" s="250">
         <f>'January 2027 - March 2027'!E163</f>
-        <v>29095.8</v>
+        <v>29015.8</v>
       </c>
     </row>
     <row r="39" ht="20.25" customHeight="1" spans="1:10">
@@ -35534,7 +35538,7 @@
       </c>
       <c r="J39" s="250">
         <f>'January 2027 - March 2027'!E190</f>
-        <v>30790.8</v>
+        <v>30710.8</v>
       </c>
     </row>
     <row r="40" ht="24.75" customHeight="1" spans="1:10">
@@ -35553,7 +35557,7 @@
       </c>
       <c r="J40" s="250">
         <f>'April 2027 - June 2027'!E136</f>
-        <v>32379.8</v>
+        <v>32299.8</v>
       </c>
     </row>
     <row r="41" ht="24.75" customHeight="1" spans="1:10">
@@ -35572,7 +35576,7 @@
       </c>
       <c r="J41" s="250">
         <f>'April 2027 - June 2027'!E163</f>
-        <v>34024.8</v>
+        <v>33944.8</v>
       </c>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:10">
@@ -35591,7 +35595,7 @@
       </c>
       <c r="J42" s="250">
         <f>'April 2027 - June 2027'!E190</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="1:10">
@@ -35613,7 +35617,7 @@
       </c>
       <c r="J43" s="250">
         <f>Forecast_14!E136</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
     </row>
     <row r="44" ht="24.75" customHeight="1" spans="9:10">
@@ -35623,7 +35627,7 @@
       </c>
       <c r="J44" s="250">
         <f>Forecast_14!E163</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
     </row>
     <row r="45" ht="24.75" customHeight="1" spans="9:10">
@@ -35633,7 +35637,7 @@
       </c>
       <c r="J45" s="250">
         <f>Forecast_14!E190</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
     </row>
     <row r="46" ht="24.75" customHeight="1" spans="9:10">
@@ -35643,7 +35647,7 @@
       </c>
       <c r="J46" s="250">
         <f>Forecast_15!E136</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
     </row>
     <row r="47" ht="24.75" customHeight="1" spans="1:10">
@@ -35663,7 +35667,7 @@
       </c>
       <c r="J47" s="250">
         <f>Forecast_15!E163</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
     </row>
     <row r="48" ht="24.75" customHeight="1" spans="1:10">
@@ -35688,7 +35692,7 @@
       </c>
       <c r="J48" s="250">
         <f>Forecast_15!E190</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
     </row>
     <row r="49" ht="24.75" customHeight="1" spans="1:10">
@@ -35713,7 +35717,7 @@
       </c>
       <c r="J49" s="250">
         <f>Forecast_16!E136</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
     </row>
     <row r="50" ht="24.75" customHeight="1" spans="1:10">
@@ -35738,7 +35742,7 @@
       </c>
       <c r="J50" s="250">
         <f>Forecast_16!E163</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
     </row>
     <row r="51" ht="50" customHeight="1" spans="1:10">
@@ -35763,7 +35767,7 @@
       </c>
       <c r="J51" s="246">
         <f>Forecast_16!E190</f>
-        <v>35613.8</v>
+        <v>35533.8</v>
       </c>
     </row>
     <row r="52" ht="24.75" customHeight="1" spans="1:7">
@@ -37717,7 +37721,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>18.9</v>
+        <v>12.9</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -37725,7 +37729,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="43" cm="1">
         <f ca="1" t="array" ref="H2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>18.9</v>
+        <v>12.9</v>
       </c>
     </row>
     <row r="3" ht="42" customHeight="1" spans="1:7">
@@ -37749,7 +37753,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>521.609999999998</v>
+        <v>515.609999999998</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -41136,7 +41140,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>18.9</v>
+        <v>12.9</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -41164,7 +41168,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>192.239999999998</v>
+        <v>186.239999999998</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -44654,8 +44658,8 @@
   <sheetPr/>
   <dimension ref="A1:I198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
-      <selection activeCell="A149" sqref="A149:B166"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="F162" sqref="F162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -44689,7 +44693,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>18.9</v>
+        <v>12.9</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -44705,7 +44709,7 @@
       </c>
       <c r="C3" s="7">
         <f>E195</f>
-        <v>855.199999999998</v>
+        <v>775.199999999998</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -44721,7 +44725,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>874.099999999998</v>
+        <v>788.099999999998</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -47009,7 +47013,7 @@
       <c r="H161" s="14"/>
       <c r="I161" s="50"/>
     </row>
-    <row r="162" ht="273" customHeight="1" spans="1:9">
+    <row r="162" ht="328" customHeight="1" spans="1:9">
       <c r="A162" s="89"/>
       <c r="B162" s="90"/>
       <c r="C162" s="102" t="s">
@@ -47017,7 +47021,7 @@
       </c>
       <c r="D162" s="102"/>
       <c r="E162" s="110">
-        <v>447.3</v>
+        <v>527.3</v>
       </c>
       <c r="F162" s="14"/>
       <c r="G162" s="14"/>
@@ -47103,7 +47107,7 @@
       <c r="D168" s="82"/>
       <c r="E168" s="97">
         <f>(F33+E148)-(SUM(E150:E159)+SUM(E161:E167))</f>
-        <v>441.199999999998</v>
+        <v>361.199999999998</v>
       </c>
       <c r="F168" s="14"/>
       <c r="G168" s="14"/>
@@ -47195,7 +47199,7 @@
       <c r="D175" s="58"/>
       <c r="E175" s="97">
         <f>E168</f>
-        <v>441.199999999998</v>
+        <v>361.199999999998</v>
       </c>
       <c r="F175" s="14"/>
       <c r="G175" s="14"/>
@@ -47471,7 +47475,7 @@
       <c r="D195" s="82"/>
       <c r="E195" s="97">
         <f>(F45+E175)-(SUM(E177:E186)+SUM(E188:E194))</f>
-        <v>855.199999999998</v>
+        <v>775.199999999998</v>
       </c>
       <c r="F195" s="14"/>
       <c r="G195" s="14"/>
@@ -48017,7 +48021,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>18.9</v>
+        <v>12.9</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -48033,7 +48037,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>1188.5</v>
+        <v>1108.5</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -48049,7 +48053,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1207.4</v>
+        <v>1121.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -49658,7 +49662,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'January 2025 - March 2025'!E195</f>
-        <v>855.199999999998</v>
+        <v>775.199999999998</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -49932,7 +49936,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>944.199999999998</v>
+        <v>864.199999999998</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -50024,7 +50028,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>944.199999999998</v>
+        <v>864.199999999998</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -50298,7 +50302,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>1024.2</v>
+        <v>944.199999999998</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -50390,7 +50394,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="134">
         <f>E163</f>
-        <v>1024.2</v>
+        <v>944.199999999998</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -50664,7 +50668,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>1188.5</v>
+        <v>1108.5</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -51179,7 +51183,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>18.9</v>
+        <v>12.9</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -51195,7 +51199,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>1434.5</v>
+        <v>1354.5</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -51211,7 +51215,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1453.4</v>
+        <v>1367.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -52812,7 +52816,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'April 2025 - June 2025'!E190</f>
-        <v>1188.5</v>
+        <v>1108.5</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -53086,7 +53090,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>1283.5</v>
+        <v>1203.5</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -53178,7 +53182,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>1283.5</v>
+        <v>1203.5</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -53454,7 +53458,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>1422.5</v>
+        <v>1342.5</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -53546,7 +53550,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>1422.5</v>
+        <v>1342.5</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -53820,7 +53824,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>1434.5</v>
+        <v>1354.5</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -54333,7 +54337,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>18.9</v>
+        <v>12.9</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -54349,7 +54353,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>6357.8</v>
+        <v>6277.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -54365,7 +54369,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>6376.7</v>
+        <v>6290.7</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -55966,7 +55970,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'July 2025 - September 2025'!E190</f>
-        <v>1434.5</v>
+        <v>1354.5</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -56238,7 +56242,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>3023.5</v>
+        <v>2943.5</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -56330,7 +56334,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>3023.5</v>
+        <v>2943.5</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -56602,7 +56606,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>4668.5</v>
+        <v>4588.5</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -56694,7 +56698,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>4668.5</v>
+        <v>4588.5</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -56966,7 +56970,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>6357.8</v>
+        <v>6277.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>

</xml_diff>

<commit_message>
docs: 1. Fix the Overall bug for each forecasts.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -6132,8 +6132,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="A102" sqref="A98:A102"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -6166,8 +6166,8 @@
         <v>132</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>12.9</v>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
+        <v>361.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -6199,7 +6199,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>11219.7</v>
+        <v>11568</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -9288,8 +9288,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="E130" sqref="C130:E130"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -9322,8 +9322,8 @@
         <v>132</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>12.9</v>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
+        <v>361.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -9355,7 +9355,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>16042.7</v>
+        <v>16391</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -12520,8 +12520,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="E130" sqref="C130:E130"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -12555,8 +12555,8 @@
         <v>132</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>12.9</v>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
+        <v>361.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -12588,7 +12588,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>20971.7</v>
+        <v>21320</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -15669,8 +15669,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="E184" sqref="C184:E184"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -15702,8 +15702,8 @@
         <v>132</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>12.9</v>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
+        <v>361.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -15735,7 +15735,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>25794.7</v>
+        <v>26143</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -18824,8 +18824,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E130" sqref="C130:E130"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -18859,8 +18859,8 @@
         <v>132</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>12.9</v>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
+        <v>361.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -18892,7 +18892,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>30723.7</v>
+        <v>31072</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -21981,8 +21981,8 @@
   <sheetPr/>
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C184" sqref="C184:D184"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -22014,8 +22014,8 @@
         <v>132</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>12.9</v>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
+        <v>361.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -22047,7 +22047,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35546.7</v>
+        <v>35895</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -25162,8 +25162,8 @@
         <v>132</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>12.9</v>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
+        <v>361.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -25195,7 +25195,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35546.7</v>
+        <v>35895</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -28110,7 +28110,7 @@
   <dimension ref="A1:I193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C188" sqref="C183:D188"/>
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -28142,8 +28142,8 @@
         <v>132</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>12.9</v>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
+        <v>361.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -28175,7 +28175,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35546.7</v>
+        <v>35895</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -31089,8 +31089,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C188" sqref="C183:D188"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -31124,8 +31124,8 @@
         <v>132</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>12.9</v>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
+        <v>361.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -31157,7 +31157,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35546.7</v>
+        <v>35895</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -34615,7 +34615,7 @@
   <dimension ref="A2:P211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D17"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -37685,8 +37685,8 @@
   <sheetPr/>
   <dimension ref="A1:I205"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -37720,8 +37720,8 @@
         <v>132</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>12.9</v>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
+        <v>361.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -37753,7 +37753,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>515.609999999998</v>
+        <v>863.909999999998</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -41105,8 +41105,8 @@
   <sheetPr/>
   <dimension ref="A1:I203"/>
   <sheetViews>
-    <sheetView topLeftCell="A194" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97:C97"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -41139,8 +41139,8 @@
         <v>132</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>12.9</v>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
+        <v>361.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -41168,7 +41168,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>186.239999999998</v>
+        <v>534.539999999998</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -44658,8 +44658,8 @@
   <sheetPr/>
   <dimension ref="A1:I198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="F162" sqref="F162"/>
+    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -44692,8 +44692,8 @@
         <v>132</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>12.9</v>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
+        <v>361.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -44725,7 +44725,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>788.099999999998</v>
+        <v>1136.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -48020,8 +48020,8 @@
         <v>132</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>12.9</v>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
+        <v>361.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -48053,7 +48053,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1121.4</v>
+        <v>1469.7</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -51149,8 +51149,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -51182,8 +51182,8 @@
         <v>132</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>12.9</v>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
+        <v>361.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -51215,7 +51215,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1367.4</v>
+        <v>1715.7</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -54303,8 +54303,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -54336,8 +54336,8 @@
         <v>132</v>
       </c>
       <c r="C2" s="4" cm="1">
-        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>12.9</v>
+        <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
+        <v>361.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -54369,7 +54369,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>6290.7</v>
+        <v>6639</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>

</xml_diff>

<commit_message>
docs: 1. Complete Forecast for March 2025 2. Expenses Updated
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -1435,7 +1435,7 @@
    include.)</t>
   </si>
   <si>
-    <t>2. Food And Transport Expenses
+    <t xml:space="preserve">2. Food And Transport Expenses
 - Chicken 6 piecies ~ $63
 - Tangerines 9 ones ~ $20
 - Milk 1 Litre 7 ~ $118.3
@@ -1453,7 +1453,9 @@
 - Transport Fee Round Trip to Mong Kok $4
 - Transport Fee from Kowloon Tong To WTS $2
 - Ngan Lung Restaurant $55
-- Oat meal $19</t>
+- Oat meal $19
+- Transport Fee to WTS Temple Mall $2
+- Transport Fee to Prince Edward And Back $4 </t>
   </si>
   <si>
     <t>3.. Food And Transport Expenses
@@ -6167,7 +6169,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>361.2</v>
+        <v>355.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -6183,7 +6185,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>11206.8</v>
+        <v>11200.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -6199,7 +6201,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>11568</v>
+        <v>11556</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -7804,7 +7806,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'October 2025 - December 2025'!E190</f>
-        <v>6277.8</v>
+        <v>6271.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -8076,7 +8078,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>7972.8</v>
+        <v>7966.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -8168,7 +8170,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>7972.8</v>
+        <v>7966.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -8440,7 +8442,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>9511.8</v>
+        <v>9505.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -8532,7 +8534,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>9511.8</v>
+        <v>9505.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -8804,7 +8806,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>11206.8</v>
+        <v>11200.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -9323,7 +9325,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>361.2</v>
+        <v>355.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -9339,7 +9341,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>16029.8</v>
+        <v>16023.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -9355,7 +9357,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>16391</v>
+        <v>16379</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -10960,7 +10962,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'January 2026 - March 2026'!E190</f>
-        <v>11206.8</v>
+        <v>11200.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -11260,7 +11262,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>12795.8</v>
+        <v>12789.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -11352,7 +11354,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>12795.8</v>
+        <v>12789.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -11652,7 +11654,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>14440.8</v>
+        <v>14434.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -11744,7 +11746,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>14440.8</v>
+        <v>14434.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -12044,7 +12046,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>16029.8</v>
+        <v>16023.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -12556,7 +12558,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>361.2</v>
+        <v>355.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -12572,7 +12574,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>20958.8</v>
+        <v>20952.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -12588,7 +12590,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>21320</v>
+        <v>21308</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -14193,7 +14195,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'April 2026 - June 2026'!E190</f>
-        <v>16029.8</v>
+        <v>16023.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -14465,7 +14467,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>17724.8</v>
+        <v>17718.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -14557,7 +14559,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>17724.8</v>
+        <v>17718.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -14829,7 +14831,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>19263.8</v>
+        <v>19257.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -14921,7 +14923,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>19263.8</v>
+        <v>19257.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -15193,7 +15195,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>20958.8</v>
+        <v>20952.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -15703,7 +15705,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>361.2</v>
+        <v>355.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -15719,7 +15721,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>25781.8</v>
+        <v>25775.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -15735,7 +15737,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>26143</v>
+        <v>26131</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -17340,7 +17342,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'July 2026 - September 2026'!E190</f>
-        <v>20958.8</v>
+        <v>20952.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -17612,7 +17614,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>22547.8</v>
+        <v>22541.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -17704,7 +17706,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>22547.8</v>
+        <v>22541.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -17976,7 +17978,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>24192.8</v>
+        <v>24186.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -18068,7 +18070,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>24192.8</v>
+        <v>24186.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -18340,7 +18342,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>25781.8</v>
+        <v>25775.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -18860,7 +18862,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>361.2</v>
+        <v>355.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -18876,7 +18878,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>30710.8</v>
+        <v>30704.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -18892,7 +18894,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>31072</v>
+        <v>31060</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -20497,7 +20499,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'October 2026 - December 2026'!E190</f>
-        <v>25781.8</v>
+        <v>25775.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -20769,7 +20771,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>27476.8</v>
+        <v>27470.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -20861,7 +20863,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>27476.8</v>
+        <v>27470.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -21133,7 +21135,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>29015.8</v>
+        <v>29009.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -21225,7 +21227,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>29015.8</v>
+        <v>29009.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -21497,7 +21499,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>30710.8</v>
+        <v>30704.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -22015,7 +22017,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>361.2</v>
+        <v>355.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -22031,7 +22033,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -22047,7 +22049,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35895</v>
+        <v>35883</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -23652,7 +23654,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'January 2027 - March 2027'!E190</f>
-        <v>30710.8</v>
+        <v>30704.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -23924,7 +23926,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>32299.8</v>
+        <v>32293.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -24016,7 +24018,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>32299.8</v>
+        <v>32293.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -24288,7 +24290,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>33944.8</v>
+        <v>33938.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -24380,7 +24382,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>33944.8</v>
+        <v>33938.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -24652,7 +24654,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -25163,7 +25165,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>361.2</v>
+        <v>355.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -25179,7 +25181,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -25195,7 +25197,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35895</v>
+        <v>35883</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -26704,7 +26706,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'April 2027 - June 2027'!E190</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -26972,7 +26974,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -27064,7 +27066,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -27332,7 +27334,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -27424,7 +27426,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -27692,7 +27694,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -28143,7 +28145,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>361.2</v>
+        <v>355.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -28159,7 +28161,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -28175,7 +28177,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35895</v>
+        <v>35883</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -29684,7 +29686,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>Forecast_14!E190</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -29952,7 +29954,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -30044,7 +30046,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -30312,7 +30314,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -30404,7 +30406,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -30672,7 +30674,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -31125,7 +31127,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>361.2</v>
+        <v>355.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -31141,7 +31143,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -31157,7 +31159,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35895</v>
+        <v>35883</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -32666,7 +32668,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>Forecast_15!E190</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -32934,7 +32936,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -33026,7 +33028,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -33294,7 +33296,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -33386,7 +33388,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -33654,7 +33656,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -34615,7 +34617,7 @@
   <dimension ref="A2:P211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D4" sqref="D4:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -34698,7 +34700,7 @@
         <v>34</v>
       </c>
       <c r="F4" s="237">
-        <v>226</v>
+        <v>126</v>
       </c>
       <c r="I4" s="245" t="str">
         <f>TEXT(Main!B3,"dd mmmm yyyy")&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,1)-1,"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)*1,"dd mmmm yyyy"))</f>
@@ -34730,7 +34732,7 @@
         <v>35</v>
       </c>
       <c r="F5" s="237">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I5" s="247" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,1),"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)+1,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,2)-1,"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)*2+1,"dd mmmm yyyy"))</f>
@@ -34956,7 +34958,7 @@
         <v>42</v>
       </c>
       <c r="F12" s="237">
-        <v>51.3</v>
+        <v>57.3</v>
       </c>
       <c r="H12" s="238"/>
       <c r="I12" s="247" t="str">
@@ -35029,7 +35031,7 @@
       </c>
       <c r="J14" s="246">
         <f>'January 2025 - March 2025'!E168</f>
-        <v>361.199999999998</v>
+        <v>355.199999999998</v>
       </c>
       <c r="M14" s="247" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,30),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*30+30),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,33)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+32),"dd mmmm yyyy"))</f>
@@ -35046,14 +35048,14 @@
         <v>45</v>
       </c>
       <c r="C15" s="211">
-        <v>12.9</v>
+        <v>6.9</v>
       </c>
       <c r="D15" s="213"/>
       <c r="E15" s="239" t="s">
         <v>45</v>
       </c>
       <c r="F15" s="237">
-        <v>18.9</v>
+        <v>12.9</v>
       </c>
       <c r="I15" s="249" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,11),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*11)+11,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,12)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*12+11),"dd mmmm yyyy"))</f>
@@ -35061,7 +35063,7 @@
       </c>
       <c r="J15" s="250">
         <f>'January 2025 - March 2025'!E195</f>
-        <v>775.199999999998</v>
+        <v>769.199999999998</v>
       </c>
       <c r="M15" s="247" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,33),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+33),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,36)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+35),"dd mmmm yyyy"))</f>
@@ -35093,7 +35095,7 @@
       </c>
       <c r="J16" s="250">
         <f>'April 2025 - June 2025'!E136</f>
-        <v>864.199999999998</v>
+        <v>858.199999999998</v>
       </c>
       <c r="M16" s="247" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,36),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+36),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,39)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+38),"dd mmmm yyyy"))</f>
@@ -35111,7 +35113,7 @@
       </c>
       <c r="C17" s="217">
         <f>SUM(C4:C16)</f>
-        <v>361.2</v>
+        <v>355.2</v>
       </c>
       <c r="D17" s="218"/>
       <c r="E17" s="216" t="s">
@@ -35119,7 +35121,7 @@
       </c>
       <c r="F17" s="240">
         <f>SUM(F4:F16)</f>
-        <v>441.2</v>
+        <v>361.2</v>
       </c>
       <c r="I17" s="251" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,13),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*13)+13,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,14)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*14+13),"dd mmmm yyyy"))</f>
@@ -35127,7 +35129,7 @@
       </c>
       <c r="J17" s="250">
         <f>'April 2025 - June 2025'!E163</f>
-        <v>944.199999999998</v>
+        <v>938.199999999998</v>
       </c>
       <c r="M17" s="247" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+39),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
@@ -35145,7 +35147,7 @@
       </c>
       <c r="J18" s="250">
         <f>'April 2025 - June 2025'!E190</f>
-        <v>1108.5</v>
+        <v>1102.5</v>
       </c>
       <c r="M18" s="247" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+42),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
@@ -35163,7 +35165,7 @@
       </c>
       <c r="J19" s="250">
         <f>'July 2025 - September 2025'!E136</f>
-        <v>1203.5</v>
+        <v>1197.5</v>
       </c>
       <c r="M19" s="247" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+45),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
@@ -35181,7 +35183,7 @@
       </c>
       <c r="J20" s="250">
         <f>'July 2025 - September 2025'!E163</f>
-        <v>1342.5</v>
+        <v>1336.5</v>
       </c>
     </row>
     <row r="21" ht="35.25" customHeight="1" spans="9:10">
@@ -35191,7 +35193,7 @@
       </c>
       <c r="J21" s="250">
         <f>'July 2025 - September 2025'!E190</f>
-        <v>1354.5</v>
+        <v>1348.5</v>
       </c>
     </row>
     <row r="22" ht="35.25" customHeight="1" spans="9:10">
@@ -35201,7 +35203,7 @@
       </c>
       <c r="J22" s="250">
         <f>'October 2025 - December 2025'!E136</f>
-        <v>2943.5</v>
+        <v>2937.5</v>
       </c>
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:10">
@@ -35221,7 +35223,7 @@
       </c>
       <c r="J23" s="250">
         <f>'October 2025 - December 2025'!E163</f>
-        <v>4588.5</v>
+        <v>4582.5</v>
       </c>
     </row>
     <row r="24" ht="24.75" customHeight="1" spans="1:10">
@@ -35246,7 +35248,7 @@
       </c>
       <c r="J24" s="250">
         <f>'October 2025 - December 2025'!E190</f>
-        <v>6277.8</v>
+        <v>6271.8</v>
       </c>
     </row>
     <row r="25" ht="34.5" customHeight="1" spans="1:10">
@@ -35271,7 +35273,7 @@
       </c>
       <c r="J25" s="250">
         <f>'January 2026 - March 2026'!E136</f>
-        <v>7972.8</v>
+        <v>7966.8</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1" spans="1:10">
@@ -35290,7 +35292,7 @@
       </c>
       <c r="J26" s="250">
         <f>'January 2026 - March 2026'!E163</f>
-        <v>9511.8</v>
+        <v>9505.8</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1" spans="1:10">
@@ -35309,7 +35311,7 @@
       </c>
       <c r="J27" s="250">
         <f>'January 2026 - March 2026'!E190</f>
-        <v>11206.8</v>
+        <v>11200.8</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:10">
@@ -35328,7 +35330,7 @@
       </c>
       <c r="J28" s="250">
         <f>'April 2026 - June 2026'!E136</f>
-        <v>12795.8</v>
+        <v>12789.8</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:10">
@@ -35347,7 +35349,7 @@
       </c>
       <c r="J29" s="250">
         <f>'April 2026 - June 2026'!E163</f>
-        <v>14440.8</v>
+        <v>14434.8</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1" spans="1:10">
@@ -35366,7 +35368,7 @@
       </c>
       <c r="J30" s="246">
         <f>'April 2026 - June 2026'!E190</f>
-        <v>16029.8</v>
+        <v>16023.8</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1" spans="1:10">
@@ -35388,7 +35390,7 @@
       </c>
       <c r="J31" s="254">
         <f>'July 2026 - September 2026'!E136</f>
-        <v>17724.8</v>
+        <v>17718.8</v>
       </c>
     </row>
     <row r="32" ht="30" customHeight="1" spans="9:10">
@@ -35398,7 +35400,7 @@
       </c>
       <c r="J32" s="250">
         <f>'July 2026 - September 2026'!E163</f>
-        <v>19263.8</v>
+        <v>19257.8</v>
       </c>
     </row>
     <row r="33" ht="27.75" customHeight="1" spans="9:10">
@@ -35408,7 +35410,7 @@
       </c>
       <c r="J33" s="250">
         <f>'July 2026 - September 2026'!E190</f>
-        <v>20958.8</v>
+        <v>20952.8</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1" spans="9:10">
@@ -35418,7 +35420,7 @@
       </c>
       <c r="J34" s="250">
         <f>'October 2026 - December 2026'!E136</f>
-        <v>22547.8</v>
+        <v>22541.8</v>
       </c>
     </row>
     <row r="35" ht="30" customHeight="1" spans="1:10">
@@ -35438,7 +35440,7 @@
       </c>
       <c r="J35" s="250">
         <f>'October 2026 - December 2026'!E163</f>
-        <v>24192.8</v>
+        <v>24186.8</v>
       </c>
     </row>
     <row r="36" ht="24.75" customHeight="1" spans="1:10">
@@ -35463,7 +35465,7 @@
       </c>
       <c r="J36" s="250">
         <f>'October 2026 - December 2026'!E190</f>
-        <v>25781.8</v>
+        <v>25775.8</v>
       </c>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:10">
@@ -35488,7 +35490,7 @@
       </c>
       <c r="J37" s="250">
         <f>'January 2027 - March 2027'!E136</f>
-        <v>27476.8</v>
+        <v>27470.8</v>
       </c>
     </row>
     <row r="38" ht="24.75" customHeight="1" spans="1:10">
@@ -35513,7 +35515,7 @@
       </c>
       <c r="J38" s="250">
         <f>'January 2027 - March 2027'!E163</f>
-        <v>29015.8</v>
+        <v>29009.8</v>
       </c>
     </row>
     <row r="39" ht="20.25" customHeight="1" spans="1:10">
@@ -35538,7 +35540,7 @@
       </c>
       <c r="J39" s="250">
         <f>'January 2027 - March 2027'!E190</f>
-        <v>30710.8</v>
+        <v>30704.8</v>
       </c>
     </row>
     <row r="40" ht="24.75" customHeight="1" spans="1:10">
@@ -35557,7 +35559,7 @@
       </c>
       <c r="J40" s="250">
         <f>'April 2027 - June 2027'!E136</f>
-        <v>32299.8</v>
+        <v>32293.8</v>
       </c>
     </row>
     <row r="41" ht="24.75" customHeight="1" spans="1:10">
@@ -35576,7 +35578,7 @@
       </c>
       <c r="J41" s="250">
         <f>'April 2027 - June 2027'!E163</f>
-        <v>33944.8</v>
+        <v>33938.8</v>
       </c>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:10">
@@ -35595,7 +35597,7 @@
       </c>
       <c r="J42" s="250">
         <f>'April 2027 - June 2027'!E190</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="1:10">
@@ -35617,7 +35619,7 @@
       </c>
       <c r="J43" s="250">
         <f>Forecast_14!E136</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
     </row>
     <row r="44" ht="24.75" customHeight="1" spans="9:10">
@@ -35627,7 +35629,7 @@
       </c>
       <c r="J44" s="250">
         <f>Forecast_14!E163</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
     </row>
     <row r="45" ht="24.75" customHeight="1" spans="9:10">
@@ -35637,7 +35639,7 @@
       </c>
       <c r="J45" s="250">
         <f>Forecast_14!E190</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
     </row>
     <row r="46" ht="24.75" customHeight="1" spans="9:10">
@@ -35647,7 +35649,7 @@
       </c>
       <c r="J46" s="250">
         <f>Forecast_15!E136</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
     </row>
     <row r="47" ht="24.75" customHeight="1" spans="1:10">
@@ -35667,7 +35669,7 @@
       </c>
       <c r="J47" s="250">
         <f>Forecast_15!E163</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
     </row>
     <row r="48" ht="24.75" customHeight="1" spans="1:10">
@@ -35692,7 +35694,7 @@
       </c>
       <c r="J48" s="250">
         <f>Forecast_15!E190</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
     </row>
     <row r="49" ht="24.75" customHeight="1" spans="1:10">
@@ -35717,7 +35719,7 @@
       </c>
       <c r="J49" s="250">
         <f>Forecast_16!E136</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
     </row>
     <row r="50" ht="24.75" customHeight="1" spans="1:10">
@@ -35742,7 +35744,7 @@
       </c>
       <c r="J50" s="250">
         <f>Forecast_16!E163</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
     </row>
     <row r="51" ht="50" customHeight="1" spans="1:10">
@@ -35767,7 +35769,7 @@
       </c>
       <c r="J51" s="246">
         <f>Forecast_16!E190</f>
-        <v>35533.8</v>
+        <v>35527.8</v>
       </c>
     </row>
     <row r="52" ht="24.75" customHeight="1" spans="1:7">
@@ -37721,7 +37723,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>361.2</v>
+        <v>355.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -37729,7 +37731,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="43" cm="1">
         <f ca="1" t="array" ref="H2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>12.9</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="3" ht="42" customHeight="1" spans="1:7">
@@ -37753,7 +37755,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>863.909999999998</v>
+        <v>857.909999999998</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -41140,7 +41142,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>361.2</v>
+        <v>355.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -41168,7 +41170,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>534.539999999998</v>
+        <v>528.539999999998</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -44658,8 +44660,8 @@
   <sheetPr/>
   <dimension ref="A1:I198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E162" sqref="E162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -44693,7 +44695,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>361.2</v>
+        <v>355.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -44709,7 +44711,7 @@
       </c>
       <c r="C3" s="7">
         <f>E195</f>
-        <v>775.199999999998</v>
+        <v>769.199999999998</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -44725,7 +44727,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1136.4</v>
+        <v>1124.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -47013,7 +47015,7 @@
       <c r="H161" s="14"/>
       <c r="I161" s="50"/>
     </row>
-    <row r="162" ht="328" customHeight="1" spans="1:9">
+    <row r="162" ht="362" customHeight="1" spans="1:9">
       <c r="A162" s="89"/>
       <c r="B162" s="90"/>
       <c r="C162" s="102" t="s">
@@ -47021,7 +47023,7 @@
       </c>
       <c r="D162" s="102"/>
       <c r="E162" s="110">
-        <v>527.3</v>
+        <v>533.3</v>
       </c>
       <c r="F162" s="14"/>
       <c r="G162" s="14"/>
@@ -47107,7 +47109,7 @@
       <c r="D168" s="82"/>
       <c r="E168" s="97">
         <f>(F33+E148)-(SUM(E150:E159)+SUM(E161:E167))</f>
-        <v>361.199999999998</v>
+        <v>355.199999999998</v>
       </c>
       <c r="F168" s="14"/>
       <c r="G168" s="14"/>
@@ -47199,7 +47201,7 @@
       <c r="D175" s="58"/>
       <c r="E175" s="97">
         <f>E168</f>
-        <v>361.199999999998</v>
+        <v>355.199999999998</v>
       </c>
       <c r="F175" s="14"/>
       <c r="G175" s="14"/>
@@ -47475,7 +47477,7 @@
       <c r="D195" s="82"/>
       <c r="E195" s="97">
         <f>(F45+E175)-(SUM(E177:E186)+SUM(E188:E194))</f>
-        <v>775.199999999998</v>
+        <v>769.199999999998</v>
       </c>
       <c r="F195" s="14"/>
       <c r="G195" s="14"/>
@@ -48021,7 +48023,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>361.2</v>
+        <v>355.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -48037,7 +48039,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>1108.5</v>
+        <v>1102.5</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -48053,7 +48055,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1469.7</v>
+        <v>1457.7</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -49662,7 +49664,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'January 2025 - March 2025'!E195</f>
-        <v>775.199999999998</v>
+        <v>769.199999999998</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -49936,7 +49938,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>864.199999999998</v>
+        <v>858.199999999998</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -50028,7 +50030,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>864.199999999998</v>
+        <v>858.199999999998</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -50302,7 +50304,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>944.199999999998</v>
+        <v>938.199999999998</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -50394,7 +50396,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="134">
         <f>E163</f>
-        <v>944.199999999998</v>
+        <v>938.199999999998</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -50668,7 +50670,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>1108.5</v>
+        <v>1102.5</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -51183,7 +51185,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>361.2</v>
+        <v>355.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -51199,7 +51201,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>1354.5</v>
+        <v>1348.5</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -51215,7 +51217,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1715.7</v>
+        <v>1703.7</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -52816,7 +52818,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'April 2025 - June 2025'!E190</f>
-        <v>1108.5</v>
+        <v>1102.5</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -53090,7 +53092,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>1203.5</v>
+        <v>1197.5</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -53182,7 +53184,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>1203.5</v>
+        <v>1197.5</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -53458,7 +53460,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>1342.5</v>
+        <v>1336.5</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -53550,7 +53552,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>1342.5</v>
+        <v>1336.5</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -53824,7 +53826,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>1354.5</v>
+        <v>1348.5</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -54337,7 +54339,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>361.2</v>
+        <v>355.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -54353,7 +54355,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>6277.8</v>
+        <v>6271.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -54369,7 +54371,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>6639</v>
+        <v>6627</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -55970,7 +55972,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'July 2025 - September 2025'!E190</f>
-        <v>1354.5</v>
+        <v>1348.5</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -56242,7 +56244,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>2943.5</v>
+        <v>2937.5</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -56334,7 +56336,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>2943.5</v>
+        <v>2937.5</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -56606,7 +56608,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>4588.5</v>
+        <v>4582.5</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -56698,7 +56700,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>4588.5</v>
+        <v>4582.5</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -56970,7 +56972,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>6277.8</v>
+        <v>6271.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>

</xml_diff>

<commit_message>
docs: 1. Add in value $50 for octopus. 2. Update Expenses.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560" firstSheet="10" activeTab="17"/>
+    <workbookView windowHeight="21560" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1998" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1998" uniqueCount="364">
   <si>
     <t>Income Forecast</t>
   </si>
@@ -1469,18 +1469,20 @@
     <t>Payback $800 to Lawrence</t>
   </si>
   <si>
-    <t>Additional Expense
+    <t>1. Additional Expense
     - Cigarette Egg - $0</t>
   </si>
   <si>
-    <t>Food And Transport Expenses
+    <t>2. Food And Transport Expenses
 Health Diet (Without Milk)
 - Oats 1.5kg  ~ $27
 - Chicken 15 piecies ~ $165
 - Marie Biscuit 2 Packets ~ $36
 - Vegetables 6kg ~ $48
 - Apples 30 ones ~ $43
-- Rice 5kg ~ $55</t>
+- Rice 5kg ~ $55
+- Ice Cream $30
+- Fanta soft drinks $16</t>
   </si>
   <si>
     <t>30th April 2025</t>
@@ -1507,6 +1509,16 @@
     <t>Additional Expense
     - Cigarette Egg - $800
     - See the psycharitic Doctor ~ $125</t>
+  </si>
+  <si>
+    <t>Food And Transport Expenses
+Health Diet (Without Milk)
+- Oats 1.5kg  ~ $27
+- Chicken 15 piecies ~ $165
+- Marie Biscuit 2 Packets ~ $36
+- Vegetables 6kg ~ $48
+- Apples 30 ones ~ $43
+- Rice 5kg ~ $55</t>
   </si>
   <si>
     <t>Payback $2600 to Mom</t>
@@ -6175,7 +6187,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>1195.2</v>
+        <v>1149.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -6191,7 +6203,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>11574.8</v>
+        <v>11528.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -6207,7 +6219,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>12770</v>
+        <v>12678</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -6306,7 +6318,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="98" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B11" s="99" t="s">
         <v>66</v>
@@ -6480,7 +6492,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="98" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B23" s="99" t="s">
         <v>66</v>
@@ -6654,7 +6666,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="98" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B35" s="99" t="s">
         <v>66</v>
@@ -7814,7 +7826,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'October 2025 - December 2025'!E190</f>
-        <v>6645.8</v>
+        <v>6599.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -7983,7 +7995,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="108" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D129" s="108"/>
       <c r="E129" s="109">
@@ -8086,7 +8098,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>8340.8</v>
+        <v>8294.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -8178,7 +8190,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>8340.8</v>
+        <v>8294.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -8347,7 +8359,7 @@
       <c r="A156" s="89"/>
       <c r="B156" s="90"/>
       <c r="C156" s="108" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D156" s="111"/>
       <c r="E156" s="109">
@@ -8450,7 +8462,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>9879.8</v>
+        <v>9833.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -8542,7 +8554,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>9879.8</v>
+        <v>9833.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -8711,7 +8723,7 @@
       <c r="A183" s="89"/>
       <c r="B183" s="90"/>
       <c r="C183" s="108" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D183" s="108"/>
       <c r="E183" s="109">
@@ -8814,7 +8826,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>11574.8</v>
+        <v>11528.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -9333,7 +9345,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>1195.2</v>
+        <v>1149.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -9349,7 +9361,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>16397.8</v>
+        <v>16351.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -9365,7 +9377,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>17593</v>
+        <v>17501</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -9464,7 +9476,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="98" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B11" s="99" t="s">
         <v>66</v>
@@ -9638,7 +9650,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="98" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B23" s="99" t="s">
         <v>66</v>
@@ -9812,7 +9824,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="98" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B35" s="99" t="s">
         <v>66</v>
@@ -10972,7 +10984,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'January 2026 - March 2026'!E190</f>
-        <v>11574.8</v>
+        <v>11528.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -10998,7 +11010,7 @@
       <c r="A118" s="63"/>
       <c r="B118" s="64"/>
       <c r="C118" s="65" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D118" s="66"/>
       <c r="E118" s="37">
@@ -11028,7 +11040,7 @@
       <c r="A120" s="63"/>
       <c r="B120" s="64"/>
       <c r="C120" s="65" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D120" s="66"/>
       <c r="E120" s="37">
@@ -11161,7 +11173,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="108" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D129" s="108"/>
       <c r="E129" s="109">
@@ -11206,7 +11218,7 @@
       <c r="A132" s="63"/>
       <c r="B132" s="64"/>
       <c r="C132" s="65" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D132" s="66"/>
       <c r="E132" s="93">
@@ -11272,7 +11284,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>13163.8</v>
+        <v>13117.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -11364,7 +11376,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>13163.8</v>
+        <v>13117.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -11390,7 +11402,7 @@
       <c r="A145" s="89"/>
       <c r="B145" s="90"/>
       <c r="C145" s="65" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D145" s="66"/>
       <c r="E145" s="37">
@@ -11420,7 +11432,7 @@
       <c r="A147" s="89"/>
       <c r="B147" s="90"/>
       <c r="C147" s="65" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D147" s="66"/>
       <c r="E147" s="37">
@@ -11553,7 +11565,7 @@
       <c r="A156" s="89"/>
       <c r="B156" s="90"/>
       <c r="C156" s="108" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D156" s="108"/>
       <c r="E156" s="109">
@@ -11598,7 +11610,7 @@
       <c r="A159" s="89"/>
       <c r="B159" s="90"/>
       <c r="C159" s="65" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D159" s="66"/>
       <c r="E159" s="93">
@@ -11664,7 +11676,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>14808.8</v>
+        <v>14762.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -11756,7 +11768,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>14808.8</v>
+        <v>14762.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -11782,7 +11794,7 @@
       <c r="A172" s="89"/>
       <c r="B172" s="90"/>
       <c r="C172" s="65" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D172" s="66"/>
       <c r="E172" s="37">
@@ -11812,7 +11824,7 @@
       <c r="A174" s="89"/>
       <c r="B174" s="90"/>
       <c r="C174" s="65" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D174" s="66"/>
       <c r="E174" s="37">
@@ -11945,7 +11957,7 @@
       <c r="A183" s="89"/>
       <c r="B183" s="90"/>
       <c r="C183" s="108" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D183" s="111"/>
       <c r="E183" s="109">
@@ -11990,7 +12002,7 @@
       <c r="A186" s="89"/>
       <c r="B186" s="90"/>
       <c r="C186" s="65" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D186" s="66"/>
       <c r="E186" s="93">
@@ -12056,7 +12068,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>16397.8</v>
+        <v>16351.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -12568,7 +12580,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>1195.2</v>
+        <v>1149.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -12584,7 +12596,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>21326.8</v>
+        <v>21280.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -12600,7 +12612,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>22522</v>
+        <v>22430</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -12699,7 +12711,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="98" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B11" s="99" t="s">
         <v>66</v>
@@ -12873,7 +12885,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="98" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B23" s="99" t="s">
         <v>66</v>
@@ -13047,7 +13059,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="98" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B35" s="99" t="s">
         <v>66</v>
@@ -14207,7 +14219,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'April 2026 - June 2026'!E190</f>
-        <v>16397.8</v>
+        <v>16351.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -14376,7 +14388,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="108" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D129" s="108"/>
       <c r="E129" s="109">
@@ -14479,7 +14491,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>18092.8</v>
+        <v>18046.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -14571,7 +14583,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>18092.8</v>
+        <v>18046.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -14740,7 +14752,7 @@
       <c r="A156" s="89"/>
       <c r="B156" s="90"/>
       <c r="C156" s="108" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D156" s="111"/>
       <c r="E156" s="109">
@@ -14843,7 +14855,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>19631.8</v>
+        <v>19585.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -14935,7 +14947,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>19631.8</v>
+        <v>19585.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -15104,7 +15116,7 @@
       <c r="A183" s="89"/>
       <c r="B183" s="90"/>
       <c r="C183" s="108" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D183" s="108"/>
       <c r="E183" s="109">
@@ -15207,7 +15219,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>21326.8</v>
+        <v>21280.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -15717,7 +15729,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>1195.2</v>
+        <v>1149.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -15733,7 +15745,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>26149.8</v>
+        <v>26103.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -15749,7 +15761,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>27345</v>
+        <v>27253</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -15848,7 +15860,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="98" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B11" s="99" t="s">
         <v>66</v>
@@ -16022,7 +16034,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="98" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B23" s="99" t="s">
         <v>66</v>
@@ -16196,7 +16208,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="98" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B35" s="99" t="s">
         <v>66</v>
@@ -17356,7 +17368,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'July 2026 - September 2026'!E190</f>
-        <v>21326.8</v>
+        <v>21280.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -17525,7 +17537,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="108" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D129" s="108"/>
       <c r="E129" s="109">
@@ -17628,7 +17640,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>22915.8</v>
+        <v>22869.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -17720,7 +17732,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>22915.8</v>
+        <v>22869.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -17889,7 +17901,7 @@
       <c r="A156" s="89"/>
       <c r="B156" s="90"/>
       <c r="C156" s="108" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D156" s="108"/>
       <c r="E156" s="109">
@@ -17992,7 +18004,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>24560.8</v>
+        <v>24514.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -18084,7 +18096,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>24560.8</v>
+        <v>24514.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -18253,7 +18265,7 @@
       <c r="A183" s="89"/>
       <c r="B183" s="90"/>
       <c r="C183" s="108" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D183" s="108"/>
       <c r="E183" s="109">
@@ -18356,7 +18368,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>26149.8</v>
+        <v>26103.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -18876,7 +18888,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>1195.2</v>
+        <v>1149.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -18892,7 +18904,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>31078.8</v>
+        <v>31032.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -18908,7 +18920,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>32274</v>
+        <v>32182</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -19007,7 +19019,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="98" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B11" s="99" t="s">
         <v>66</v>
@@ -19181,7 +19193,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="98" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B23" s="99" t="s">
         <v>66</v>
@@ -19355,7 +19367,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="98" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B35" s="99" t="s">
         <v>66</v>
@@ -20515,7 +20527,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'October 2026 - December 2026'!E190</f>
-        <v>26149.8</v>
+        <v>26103.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -20684,7 +20696,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="108" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D129" s="108"/>
       <c r="E129" s="109">
@@ -20787,7 +20799,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>27844.8</v>
+        <v>27798.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -20879,7 +20891,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>27844.8</v>
+        <v>27798.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -21048,7 +21060,7 @@
       <c r="A156" s="89"/>
       <c r="B156" s="90"/>
       <c r="C156" s="108" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D156" s="108"/>
       <c r="E156" s="109">
@@ -21151,7 +21163,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>29383.8</v>
+        <v>29337.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -21243,7 +21255,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>29383.8</v>
+        <v>29337.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -21412,7 +21424,7 @@
       <c r="A183" s="89"/>
       <c r="B183" s="90"/>
       <c r="C183" s="108" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D183" s="108"/>
       <c r="E183" s="109">
@@ -21515,7 +21527,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>31078.8</v>
+        <v>31032.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -22033,7 +22045,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>1195.2</v>
+        <v>1149.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -22049,7 +22061,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -22065,7 +22077,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>37097</v>
+        <v>37005</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -22164,7 +22176,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="98" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B11" s="99" t="s">
         <v>66</v>
@@ -22338,7 +22350,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="98" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B23" s="99" t="s">
         <v>66</v>
@@ -22512,7 +22524,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="98" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B35" s="99" t="s">
         <v>66</v>
@@ -23672,7 +23684,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'January 2027 - March 2027'!E190</f>
-        <v>31078.8</v>
+        <v>31032.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -23841,7 +23853,7 @@
       <c r="A129" s="63"/>
       <c r="B129" s="64"/>
       <c r="C129" s="108" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D129" s="108"/>
       <c r="E129" s="109">
@@ -23944,7 +23956,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>32667.8</v>
+        <v>32621.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -24036,7 +24048,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>32667.8</v>
+        <v>32621.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -24205,7 +24217,7 @@
       <c r="A156" s="89"/>
       <c r="B156" s="90"/>
       <c r="C156" s="108" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D156" s="108"/>
       <c r="E156" s="109">
@@ -24308,7 +24320,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>34312.8</v>
+        <v>34266.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -24400,7 +24412,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>34312.8</v>
+        <v>34266.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -24569,7 +24581,7 @@
       <c r="A183" s="89"/>
       <c r="B183" s="90"/>
       <c r="C183" s="108" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D183" s="108"/>
       <c r="E183" s="109">
@@ -24672,7 +24684,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -25183,7 +25195,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>1195.2</v>
+        <v>1149.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -25199,7 +25211,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -25215,7 +25227,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>37097</v>
+        <v>37005</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -26724,7 +26736,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'April 2027 - June 2027'!E190</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -26992,7 +27004,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -27084,7 +27096,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -27352,7 +27364,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -27444,7 +27456,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -27712,7 +27724,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -28163,7 +28175,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>1195.2</v>
+        <v>1149.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -28179,7 +28191,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -28195,7 +28207,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>37097</v>
+        <v>37005</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -29704,7 +29716,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>Forecast_14!E190</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -29972,7 +29984,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -30064,7 +30076,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -30332,7 +30344,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -30424,7 +30436,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -30692,7 +30704,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -31109,7 +31121,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+    <sheetView topLeftCell="A68" workbookViewId="0">
       <selection activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
@@ -31145,7 +31157,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>1195.2</v>
+        <v>1149.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -31161,7 +31173,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -31177,7 +31189,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>37097</v>
+        <v>37005</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -32686,7 +32698,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>Forecast_15!E190</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -32954,7 +32966,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -33046,7 +33058,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -33314,7 +33326,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -33406,7 +33418,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -33674,7 +33686,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -34634,8 +34646,8 @@
   <sheetPr/>
   <dimension ref="A2:P211"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -34709,7 +34721,7 @@
         <v>34</v>
       </c>
       <c r="C4" s="211">
-        <v>1034</v>
+        <v>1004</v>
       </c>
       <c r="D4" s="212" t="s">
         <v>33</v>
@@ -34718,7 +34730,7 @@
         <v>34</v>
       </c>
       <c r="F4" s="237">
-        <v>126</v>
+        <v>1034</v>
       </c>
       <c r="I4" s="245" t="str">
         <f>TEXT(Main!B3,"dd mmmm yyyy")&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,1)-1,"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)*1,"dd mmmm yyyy"))</f>
@@ -34743,7 +34755,7 @@
         <v>35</v>
       </c>
       <c r="C5" s="211">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D5" s="213"/>
       <c r="E5" s="5" t="s">
@@ -34969,7 +34981,7 @@
         <v>42</v>
       </c>
       <c r="C12" s="211">
-        <v>57.3</v>
+        <v>11.3</v>
       </c>
       <c r="D12" s="213"/>
       <c r="E12" s="5" t="s">
@@ -35009,7 +35021,7 @@
         <v>43</v>
       </c>
       <c r="F13" s="237">
-        <v>138</v>
+        <v>70</v>
       </c>
       <c r="I13" s="247" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,9),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*9)+9,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,10)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*10+9),"dd mmmm yyyy"))</f>
@@ -35066,7 +35078,7 @@
         <v>45</v>
       </c>
       <c r="C15" s="211">
-        <v>6.9</v>
+        <v>56.9</v>
       </c>
       <c r="D15" s="213"/>
       <c r="E15" s="239" t="s">
@@ -35081,7 +35093,7 @@
       </c>
       <c r="J15" s="250">
         <f>'January 2025 - March 2025'!E195</f>
-        <v>1143.2</v>
+        <v>1097.2</v>
       </c>
       <c r="M15" s="247" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,33),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+33),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,36)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+35),"dd mmmm yyyy"))</f>
@@ -35113,7 +35125,7 @@
       </c>
       <c r="J16" s="250">
         <f>'April 2025 - June 2025'!E136</f>
-        <v>1232.2</v>
+        <v>1186.2</v>
       </c>
       <c r="M16" s="247" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,36),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+36),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,39)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+38),"dd mmmm yyyy"))</f>
@@ -35131,7 +35143,7 @@
       </c>
       <c r="C17" s="217">
         <f>SUM(C4:C16)</f>
-        <v>1195.2</v>
+        <v>1149.2</v>
       </c>
       <c r="D17" s="218"/>
       <c r="E17" s="216" t="s">
@@ -35139,7 +35151,7 @@
       </c>
       <c r="F17" s="240">
         <f>SUM(F4:F16)</f>
-        <v>355.2</v>
+        <v>1195.2</v>
       </c>
       <c r="I17" s="251" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,13),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*13)+13,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,14)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*14+13),"dd mmmm yyyy"))</f>
@@ -35147,7 +35159,7 @@
       </c>
       <c r="J17" s="250">
         <f>'April 2025 - June 2025'!E163</f>
-        <v>1312.2</v>
+        <v>1266.2</v>
       </c>
       <c r="M17" s="247" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+39),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
@@ -35165,7 +35177,7 @@
       </c>
       <c r="J18" s="250">
         <f>'April 2025 - June 2025'!E190</f>
-        <v>1476.5</v>
+        <v>1430.5</v>
       </c>
       <c r="M18" s="247" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+42),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
@@ -35183,7 +35195,7 @@
       </c>
       <c r="J19" s="250">
         <f>'July 2025 - September 2025'!E136</f>
-        <v>1571.5</v>
+        <v>1525.5</v>
       </c>
       <c r="M19" s="247" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+45),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
@@ -35201,7 +35213,7 @@
       </c>
       <c r="J20" s="250">
         <f>'July 2025 - September 2025'!E163</f>
-        <v>1710.5</v>
+        <v>1664.5</v>
       </c>
     </row>
     <row r="21" ht="35.25" customHeight="1" spans="9:10">
@@ -35211,7 +35223,7 @@
       </c>
       <c r="J21" s="250">
         <f>'July 2025 - September 2025'!E190</f>
-        <v>1722.5</v>
+        <v>1676.5</v>
       </c>
     </row>
     <row r="22" ht="35.25" customHeight="1" spans="9:10">
@@ -35221,7 +35233,7 @@
       </c>
       <c r="J22" s="250">
         <f>'October 2025 - December 2025'!E136</f>
-        <v>3311.5</v>
+        <v>3265.5</v>
       </c>
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:10">
@@ -35241,7 +35253,7 @@
       </c>
       <c r="J23" s="250">
         <f>'October 2025 - December 2025'!E163</f>
-        <v>4956.5</v>
+        <v>4910.5</v>
       </c>
     </row>
     <row r="24" ht="24.75" customHeight="1" spans="1:10">
@@ -35266,7 +35278,7 @@
       </c>
       <c r="J24" s="250">
         <f>'October 2025 - December 2025'!E190</f>
-        <v>6645.8</v>
+        <v>6599.8</v>
       </c>
     </row>
     <row r="25" ht="34.5" customHeight="1" spans="1:10">
@@ -35291,7 +35303,7 @@
       </c>
       <c r="J25" s="250">
         <f>'January 2026 - March 2026'!E136</f>
-        <v>8340.8</v>
+        <v>8294.8</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1" spans="1:10">
@@ -35310,7 +35322,7 @@
       </c>
       <c r="J26" s="250">
         <f>'January 2026 - March 2026'!E163</f>
-        <v>9879.8</v>
+        <v>9833.8</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1" spans="1:10">
@@ -35329,7 +35341,7 @@
       </c>
       <c r="J27" s="250">
         <f>'January 2026 - March 2026'!E190</f>
-        <v>11574.8</v>
+        <v>11528.8</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:10">
@@ -35348,7 +35360,7 @@
       </c>
       <c r="J28" s="250">
         <f>'April 2026 - June 2026'!E136</f>
-        <v>13163.8</v>
+        <v>13117.8</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:10">
@@ -35367,7 +35379,7 @@
       </c>
       <c r="J29" s="250">
         <f>'April 2026 - June 2026'!E163</f>
-        <v>14808.8</v>
+        <v>14762.8</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1" spans="1:10">
@@ -35386,7 +35398,7 @@
       </c>
       <c r="J30" s="246">
         <f>'April 2026 - June 2026'!E190</f>
-        <v>16397.8</v>
+        <v>16351.8</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1" spans="1:10">
@@ -35408,7 +35420,7 @@
       </c>
       <c r="J31" s="254">
         <f>'July 2026 - September 2026'!E136</f>
-        <v>18092.8</v>
+        <v>18046.8</v>
       </c>
     </row>
     <row r="32" ht="30" customHeight="1" spans="9:10">
@@ -35418,7 +35430,7 @@
       </c>
       <c r="J32" s="250">
         <f>'July 2026 - September 2026'!E163</f>
-        <v>19631.8</v>
+        <v>19585.8</v>
       </c>
     </row>
     <row r="33" ht="27.75" customHeight="1" spans="9:10">
@@ -35428,7 +35440,7 @@
       </c>
       <c r="J33" s="250">
         <f>'July 2026 - September 2026'!E190</f>
-        <v>21326.8</v>
+        <v>21280.8</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1" spans="9:10">
@@ -35438,7 +35450,7 @@
       </c>
       <c r="J34" s="250">
         <f>'October 2026 - December 2026'!E136</f>
-        <v>22915.8</v>
+        <v>22869.8</v>
       </c>
     </row>
     <row r="35" ht="30" customHeight="1" spans="1:10">
@@ -35458,7 +35470,7 @@
       </c>
       <c r="J35" s="250">
         <f>'October 2026 - December 2026'!E163</f>
-        <v>24560.8</v>
+        <v>24514.8</v>
       </c>
     </row>
     <row r="36" ht="24.75" customHeight="1" spans="1:10">
@@ -35483,7 +35495,7 @@
       </c>
       <c r="J36" s="250">
         <f>'October 2026 - December 2026'!E190</f>
-        <v>26149.8</v>
+        <v>26103.8</v>
       </c>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:10">
@@ -35508,7 +35520,7 @@
       </c>
       <c r="J37" s="250">
         <f>'January 2027 - March 2027'!E136</f>
-        <v>27844.8</v>
+        <v>27798.8</v>
       </c>
     </row>
     <row r="38" ht="24.75" customHeight="1" spans="1:10">
@@ -35533,7 +35545,7 @@
       </c>
       <c r="J38" s="250">
         <f>'January 2027 - March 2027'!E163</f>
-        <v>29383.8</v>
+        <v>29337.8</v>
       </c>
     </row>
     <row r="39" ht="20.25" customHeight="1" spans="1:10">
@@ -35558,7 +35570,7 @@
       </c>
       <c r="J39" s="250">
         <f>'January 2027 - March 2027'!E190</f>
-        <v>31078.8</v>
+        <v>31032.8</v>
       </c>
     </row>
     <row r="40" ht="24.75" customHeight="1" spans="1:10">
@@ -35577,7 +35589,7 @@
       </c>
       <c r="J40" s="250">
         <f>'April 2027 - June 2027'!E136</f>
-        <v>32667.8</v>
+        <v>32621.8</v>
       </c>
     </row>
     <row r="41" ht="24.75" customHeight="1" spans="1:10">
@@ -35596,7 +35608,7 @@
       </c>
       <c r="J41" s="250">
         <f>'April 2027 - June 2027'!E163</f>
-        <v>34312.8</v>
+        <v>34266.8</v>
       </c>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:10">
@@ -35615,7 +35627,7 @@
       </c>
       <c r="J42" s="250">
         <f>'April 2027 - June 2027'!E190</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="1:10">
@@ -35637,7 +35649,7 @@
       </c>
       <c r="J43" s="250">
         <f>Forecast_14!E136</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
     </row>
     <row r="44" ht="24.75" customHeight="1" spans="9:10">
@@ -35647,7 +35659,7 @@
       </c>
       <c r="J44" s="250">
         <f>Forecast_14!E163</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
     </row>
     <row r="45" ht="24.75" customHeight="1" spans="9:10">
@@ -35657,7 +35669,7 @@
       </c>
       <c r="J45" s="250">
         <f>Forecast_14!E190</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
     </row>
     <row r="46" ht="24.75" customHeight="1" spans="9:10">
@@ -35667,7 +35679,7 @@
       </c>
       <c r="J46" s="250">
         <f>Forecast_15!E136</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
     </row>
     <row r="47" ht="24.75" customHeight="1" spans="1:10">
@@ -35687,7 +35699,7 @@
       </c>
       <c r="J47" s="250">
         <f>Forecast_15!E163</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
     </row>
     <row r="48" ht="24.75" customHeight="1" spans="1:10">
@@ -35712,7 +35724,7 @@
       </c>
       <c r="J48" s="250">
         <f>Forecast_15!E190</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
     </row>
     <row r="49" ht="24.75" customHeight="1" spans="1:10">
@@ -35737,7 +35749,7 @@
       </c>
       <c r="J49" s="250">
         <f>Forecast_16!E136</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
     </row>
     <row r="50" ht="24.75" customHeight="1" spans="1:10">
@@ -35762,7 +35774,7 @@
       </c>
       <c r="J50" s="250">
         <f>Forecast_16!E163</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
     </row>
     <row r="51" ht="50" customHeight="1" spans="1:10">
@@ -35787,7 +35799,7 @@
       </c>
       <c r="J51" s="246">
         <f>Forecast_16!E190</f>
-        <v>35901.8</v>
+        <v>35855.8</v>
       </c>
     </row>
     <row r="52" ht="24.75" customHeight="1" spans="1:7">
@@ -37743,7 +37755,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>1195.2</v>
+        <v>1149.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -37751,7 +37763,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="43" cm="1">
         <f ca="1" t="array" ref="H2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>6.9</v>
+        <v>56.9</v>
       </c>
     </row>
     <row r="3" ht="42" customHeight="1" spans="1:7">
@@ -37775,7 +37787,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1697.91</v>
+        <v>1651.91</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -41164,7 +41176,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>1195.2</v>
+        <v>1149.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -41192,7 +41204,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1368.54</v>
+        <v>1322.54</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -44684,8 +44696,8 @@
   <sheetPr/>
   <dimension ref="A1:I198"/>
   <sheetViews>
-    <sheetView topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="F189" sqref="F189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -44719,7 +44731,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>1195.2</v>
+        <v>1149.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -44735,7 +44747,7 @@
       </c>
       <c r="C3" s="7">
         <f>E195</f>
-        <v>1143.2</v>
+        <v>1097.2</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -44751,7 +44763,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>2338.4</v>
+        <v>2246.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -47411,7 +47423,7 @@
       <c r="H188" s="14"/>
       <c r="I188" s="50"/>
     </row>
-    <row r="189" ht="158" customHeight="1" spans="1:9">
+    <row r="189" ht="204" customHeight="1" spans="1:9">
       <c r="A189" s="89"/>
       <c r="B189" s="90"/>
       <c r="C189" s="102" t="s">
@@ -47419,7 +47431,7 @@
       </c>
       <c r="D189" s="102"/>
       <c r="E189" s="110">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="F189" s="14"/>
       <c r="G189" s="14"/>
@@ -47503,7 +47515,7 @@
       <c r="D195" s="82"/>
       <c r="E195" s="97">
         <f>(F45+E175)-(SUM(E177:E186)+SUM(E188:E194))</f>
-        <v>1143.2</v>
+        <v>1097.2</v>
       </c>
       <c r="F195" s="14"/>
       <c r="G195" s="14"/>
@@ -48049,7 +48061,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>1195.2</v>
+        <v>1149.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -48065,7 +48077,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>1476.5</v>
+        <v>1430.5</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -48081,7 +48093,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>2671.7</v>
+        <v>2579.7</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -49692,7 +49704,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'January 2025 - March 2025'!E195</f>
-        <v>1143.2</v>
+        <v>1097.2</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -49878,7 +49890,7 @@
       <c r="A130" s="89"/>
       <c r="B130" s="124"/>
       <c r="C130" s="132" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="D130" s="133"/>
       <c r="E130" s="103">
@@ -49966,7 +49978,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>1232.2</v>
+        <v>1186.2</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -50058,7 +50070,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>1232.2</v>
+        <v>1186.2</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -50084,7 +50096,7 @@
       <c r="A145" s="89"/>
       <c r="B145" s="90"/>
       <c r="C145" s="128" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D145" s="128"/>
       <c r="E145" s="103">
@@ -50229,7 +50241,7 @@
       <c r="A156" s="89"/>
       <c r="B156" s="90"/>
       <c r="C156" s="102" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D156" s="102"/>
       <c r="E156" s="103">
@@ -50244,7 +50256,7 @@
       <c r="A157" s="89"/>
       <c r="B157" s="90"/>
       <c r="C157" s="102" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="D157" s="102"/>
       <c r="E157" s="103">
@@ -50332,7 +50344,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>1312.2</v>
+        <v>1266.2</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -50424,7 +50436,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="134">
         <f>E163</f>
-        <v>1312.2</v>
+        <v>1266.2</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -50450,7 +50462,7 @@
       <c r="A172" s="89"/>
       <c r="B172" s="90"/>
       <c r="C172" s="128" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D172" s="128"/>
       <c r="E172" s="103">
@@ -50610,7 +50622,7 @@
       <c r="A184" s="89"/>
       <c r="B184" s="90"/>
       <c r="C184" s="102" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D184" s="102"/>
       <c r="E184" s="103">
@@ -50698,7 +50710,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>1476.5</v>
+        <v>1430.5</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -51213,7 +51225,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>1195.2</v>
+        <v>1149.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -51229,7 +51241,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>1722.5</v>
+        <v>1676.5</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -51245,7 +51257,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>2917.7</v>
+        <v>2825.7</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -51344,7 +51356,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="98" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B11" s="99" t="s">
         <v>66</v>
@@ -51364,11 +51376,11 @@
     <row r="12" ht="24.75" customHeight="1" spans="1:9">
       <c r="A12" s="98"/>
       <c r="B12" s="99" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C12" s="99"/>
       <c r="D12" s="100" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E12" s="100"/>
       <c r="F12" s="7">
@@ -51518,7 +51530,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="98" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B23" s="99" t="s">
         <v>66</v>
@@ -51690,7 +51702,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="98" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B35" s="99" t="s">
         <v>66</v>
@@ -52388,7 +52400,7 @@
     <row r="85" ht="24.75" customHeight="1" spans="1:9">
       <c r="A85" s="52"/>
       <c r="B85" s="121" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C85" s="37">
         <f>SUM(C77:C84)</f>
@@ -52436,7 +52448,7 @@
         <v>95</v>
       </c>
       <c r="B88" s="106" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C88" s="103">
         <v>68</v>
@@ -52848,7 +52860,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'April 2025 - June 2025'!E190</f>
-        <v>1476.5</v>
+        <v>1430.5</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -52874,7 +52886,7 @@
       <c r="A118" s="89"/>
       <c r="B118" s="124"/>
       <c r="C118" s="128" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D118" s="128"/>
       <c r="E118" s="103">
@@ -53019,7 +53031,7 @@
       <c r="A129" s="89"/>
       <c r="B129" s="124"/>
       <c r="C129" s="102" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D129" s="102"/>
       <c r="E129" s="103">
@@ -53034,7 +53046,7 @@
       <c r="A130" s="89"/>
       <c r="B130" s="124"/>
       <c r="C130" s="102" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="D130" s="102"/>
       <c r="E130" s="103">
@@ -53122,7 +53134,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>1571.5</v>
+        <v>1525.5</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -53214,7 +53226,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>1571.5</v>
+        <v>1525.5</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -53240,7 +53252,7 @@
       <c r="A145" s="89"/>
       <c r="B145" s="90"/>
       <c r="C145" s="128" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D145" s="128"/>
       <c r="E145" s="103">
@@ -53268,7 +53280,7 @@
       <c r="A147" s="89"/>
       <c r="B147" s="90"/>
       <c r="C147" s="65" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D147" s="66"/>
       <c r="E147" s="37">
@@ -53309,7 +53321,7 @@
       <c r="A150" s="89"/>
       <c r="B150" s="90"/>
       <c r="C150" s="65" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D150" s="66"/>
       <c r="E150" s="37">
@@ -53389,7 +53401,7 @@
       <c r="A156" s="89"/>
       <c r="B156" s="90"/>
       <c r="C156" s="102" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D156" s="102"/>
       <c r="E156" s="103">
@@ -53404,7 +53416,7 @@
       <c r="A157" s="89"/>
       <c r="B157" s="90"/>
       <c r="C157" s="102" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="D157" s="102"/>
       <c r="E157" s="103">
@@ -53492,7 +53504,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>1710.5</v>
+        <v>1664.5</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -53584,7 +53596,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>1710.5</v>
+        <v>1664.5</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -53675,7 +53687,7 @@
       <c r="A177" s="89"/>
       <c r="B177" s="90"/>
       <c r="C177" s="65" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D177" s="66"/>
       <c r="E177" s="37">
@@ -53755,7 +53767,7 @@
       <c r="A183" s="89"/>
       <c r="B183" s="90"/>
       <c r="C183" s="102" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D183" s="102"/>
       <c r="E183" s="103">
@@ -53770,7 +53782,7 @@
       <c r="A184" s="89"/>
       <c r="B184" s="90"/>
       <c r="C184" s="102" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="D184" s="102"/>
       <c r="E184" s="103">
@@ -53858,7 +53870,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>1722.5</v>
+        <v>1676.5</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -54371,7 +54383,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>1195.2</v>
+        <v>1149.2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -54387,7 +54399,7 @@
       </c>
       <c r="C3" s="7">
         <f>E190</f>
-        <v>6645.8</v>
+        <v>6599.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -54403,7 +54415,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>7841</v>
+        <v>7749</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -54502,7 +54514,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="98" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B11" s="99" t="s">
         <v>66</v>
@@ -54676,7 +54688,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="98" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B23" s="99" t="s">
         <v>66</v>
@@ -54846,7 +54858,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="98" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B35" s="99" t="s">
         <v>66</v>
@@ -56006,7 +56018,7 @@
       <c r="D116" s="58"/>
       <c r="E116" s="71">
         <f>'July 2025 - September 2025'!E190</f>
-        <v>1722.5</v>
+        <v>1676.5</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -56175,7 +56187,7 @@
       <c r="A129" s="89"/>
       <c r="B129" s="124"/>
       <c r="C129" s="102" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D129" s="102"/>
       <c r="E129" s="103">
@@ -56278,7 +56290,7 @@
       <c r="D136" s="82"/>
       <c r="E136" s="94">
         <f>(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>3311.5</v>
+        <v>3265.5</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -56370,7 +56382,7 @@
       <c r="D143" s="58"/>
       <c r="E143" s="94">
         <f>E136</f>
-        <v>3311.5</v>
+        <v>3265.5</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -56539,7 +56551,7 @@
       <c r="A156" s="89"/>
       <c r="B156" s="90"/>
       <c r="C156" s="102" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D156" s="102"/>
       <c r="E156" s="110">
@@ -56642,7 +56654,7 @@
       <c r="D163" s="82"/>
       <c r="E163" s="97">
         <f>(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>4956.5</v>
+        <v>4910.5</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -56734,7 +56746,7 @@
       <c r="D170" s="58"/>
       <c r="E170" s="97">
         <f>E163</f>
-        <v>4956.5</v>
+        <v>4910.5</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -56903,7 +56915,7 @@
       <c r="A183" s="89"/>
       <c r="B183" s="90"/>
       <c r="C183" s="102" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D183" s="102"/>
       <c r="E183" s="103">
@@ -57006,7 +57018,7 @@
       <c r="D190" s="82"/>
       <c r="E190" s="97">
         <f>(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>6645.8</v>
+        <v>6599.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>

</xml_diff>

<commit_message>
docs: Update Octopus value.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560" activeTab="5"/>
+    <workbookView windowHeight="21560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -6196,7 +6196,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>961.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -6228,7 +6228,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>12039.8</v>
+        <v>11987.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -9354,7 +9354,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>961.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -9386,7 +9386,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>16784.8</v>
+        <v>16732.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -12589,7 +12589,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>961.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -12621,7 +12621,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>21635.8</v>
+        <v>21583.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -15738,7 +15738,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>961.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -15770,7 +15770,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>26380.8</v>
+        <v>26328.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -18897,7 +18897,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>961.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -18929,7 +18929,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>31231.8</v>
+        <v>31179.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -22054,7 +22054,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>961.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -22086,7 +22086,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35976.8</v>
+        <v>35924.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -25204,7 +25204,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>961.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -25236,7 +25236,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35976.8</v>
+        <v>35924.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -28184,7 +28184,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>961.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -28216,7 +28216,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35976.8</v>
+        <v>35924.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -31166,7 +31166,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>961.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -31198,7 +31198,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35976.8</v>
+        <v>35924.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -34655,8 +34655,8 @@
   <sheetPr/>
   <dimension ref="A2:P211"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -35087,7 +35087,7 @@
         <v>45</v>
       </c>
       <c r="C15" s="211">
-        <v>56.9</v>
+        <v>4.9</v>
       </c>
       <c r="D15" s="213"/>
       <c r="E15" s="239" t="s">
@@ -35152,7 +35152,7 @@
       </c>
       <c r="C17" s="217">
         <f>SUM(C4:C16)</f>
-        <v>961.4</v>
+        <v>909.4</v>
       </c>
       <c r="D17" s="218"/>
       <c r="E17" s="216" t="s">
@@ -37764,7 +37764,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>961.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -37772,7 +37772,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="43" cm="1">
         <f ca="1" t="array" ref="H2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$15")</f>
-        <v>56.9</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="3" ht="42" customHeight="1" spans="1:7">
@@ -37796,7 +37796,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1464.11</v>
+        <v>1412.11</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -41185,7 +41185,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>961.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -41213,7 +41213,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1134.74</v>
+        <v>1082.74</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -44705,8 +44705,8 @@
   <sheetPr/>
   <dimension ref="A1:I198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="C189" sqref="C189:D189"/>
+    <sheetView topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="E195" sqref="E195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -44740,7 +44740,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>961.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -44772,7 +44772,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1870.8</v>
+        <v>1818.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -48070,7 +48070,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>961.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -48102,7 +48102,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>2150.8</v>
+        <v>2098.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -51234,7 +51234,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>961.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -51266,7 +51266,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>2318.8</v>
+        <v>2266.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -54392,7 +54392,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$17")</f>
-        <v>961.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -54424,7 +54424,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>7188.8</v>
+        <v>7136.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>

</xml_diff>

<commit_message>
docs: 1. Update Cash Received from Mom.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560"/>
+    <workbookView windowHeight="21560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -3867,7 +3867,7 @@
   <sheetPr/>
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="AB12" sqref="AB12"/>
     </sheetView>
   </sheetViews>
@@ -5664,7 +5664,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>629.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -5696,7 +5696,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>11582.8</v>
+        <v>11862.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -9094,7 +9094,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>629.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -9126,7 +9126,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>16327.8</v>
+        <v>16607.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -12525,7 +12525,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>629.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -12557,7 +12557,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>21178.8</v>
+        <v>21458.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -15954,7 +15954,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>629.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -15986,7 +15986,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>25923.8</v>
+        <v>26203.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -19385,7 +19385,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>629.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -19417,7 +19417,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>30774.8</v>
+        <v>31054.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -22814,7 +22814,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>629.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -22846,7 +22846,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35519.8</v>
+        <v>35799.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -26244,7 +26244,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>629.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -26276,7 +26276,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35519.8</v>
+        <v>35799.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -29567,7 +29567,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>629.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -29599,7 +29599,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35519.8</v>
+        <v>35799.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -32893,7 +32893,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>629.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -32925,7 +32925,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35519.8</v>
+        <v>35799.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -36721,8 +36721,8 @@
   <sheetPr/>
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="F104" sqref="F104"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -36827,7 +36827,7 @@
         <v>35</v>
       </c>
       <c r="C4" s="164">
-        <v>0</v>
+        <v>280</v>
       </c>
       <c r="D4" s="166"/>
       <c r="E4" s="5" t="s">
@@ -37214,7 +37214,7 @@
       </c>
       <c r="C16" s="170">
         <f>SUM(C3:C15)</f>
-        <v>629.4</v>
+        <v>909.4</v>
       </c>
       <c r="D16" s="171"/>
       <c r="E16" s="169" t="s">
@@ -39831,7 +39831,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>629.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -39859,7 +39859,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1132.11</v>
+        <v>1412.11</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -43297,7 +43297,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>629.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -43325,7 +43325,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>802.740000000001</v>
+        <v>1082.74</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -46864,7 +46864,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>629.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -46896,7 +46896,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1538.8</v>
+        <v>1818.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -50381,7 +50381,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>629.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -50413,7 +50413,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1818.8</v>
+        <v>2098.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -53832,7 +53832,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>629.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -53864,7 +53864,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1986.8</v>
+        <v>2266.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -57282,7 +57282,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>629.4</v>
+        <v>909.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -57314,7 +57314,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>6731.8</v>
+        <v>7011.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>

</xml_diff>

<commit_message>
docs: 1. Update Expenses.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560" activeTab="2"/>
+    <workbookView windowHeight="21560" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -1147,7 +1147,8 @@
 - Edo Pack Oat Biscuit x 3 ~  $39 
 - Longevity Filled Evaporated 3 cans $24
 - Ice Cream $30
-- Fanta soft drinks $16</t>
+- Fanta soft drinks $16
+- Best Mart 360 pepsi ~ $20</t>
   </si>
   <si>
     <t>30th April 2025</t>
@@ -5664,7 +5665,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>909.4</v>
+        <v>889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -5680,7 +5681,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>10953.4</v>
+        <v>10933.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -5696,7 +5697,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>11862.8</v>
+        <v>11822.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -7547,7 +7548,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!E190")</f>
-        <v>6102.4</v>
+        <v>6082.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -7819,7 +7820,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>7771.4</v>
+        <v>7751.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -7911,7 +7912,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>7771.4</v>
+        <v>7751.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -8183,7 +8184,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>9284.4</v>
+        <v>9264.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -8275,7 +8276,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>9284.4</v>
+        <v>9264.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -8547,7 +8548,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>10953.4</v>
+        <v>10933.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -9094,7 +9095,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>909.4</v>
+        <v>889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -9110,7 +9111,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>15698.4</v>
+        <v>15678.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -9126,7 +9127,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>16607.8</v>
+        <v>16567.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -10977,7 +10978,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!E190")</f>
-        <v>10953.4</v>
+        <v>10933.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -11249,7 +11250,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>12516.4</v>
+        <v>12496.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -11341,7 +11342,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>12516.4</v>
+        <v>12496.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -11613,7 +11614,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>14135.4</v>
+        <v>14115.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -11705,7 +11706,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>14135.4</v>
+        <v>14115.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -11977,7 +11978,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>15698.4</v>
+        <v>15678.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -12525,7 +12526,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>909.4</v>
+        <v>889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -12541,7 +12542,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>20549.4</v>
+        <v>20529.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -12557,7 +12558,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>21458.8</v>
+        <v>21418.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -14408,7 +14409,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!E190")</f>
-        <v>15698.4</v>
+        <v>15678.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -14680,7 +14681,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>17367.4</v>
+        <v>17347.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -14772,7 +14773,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>17367.4</v>
+        <v>17347.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -15044,7 +15045,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>18880.4</v>
+        <v>18860.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -15136,7 +15137,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>18880.4</v>
+        <v>18860.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -15408,7 +15409,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>20549.4</v>
+        <v>20529.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -15954,7 +15955,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>909.4</v>
+        <v>889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -15970,7 +15971,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>25294.4</v>
+        <v>25274.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -15986,7 +15987,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>26203.8</v>
+        <v>26163.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -17837,7 +17838,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!E190")</f>
-        <v>20549.4</v>
+        <v>20529.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -18109,7 +18110,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>22112.4</v>
+        <v>22092.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -18201,7 +18202,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>22112.4</v>
+        <v>22092.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -18473,7 +18474,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>23731.4</v>
+        <v>23711.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -18565,7 +18566,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>23731.4</v>
+        <v>23711.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -18837,7 +18838,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>25294.4</v>
+        <v>25274.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -19385,7 +19386,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>909.4</v>
+        <v>889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -19401,7 +19402,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>30145.4</v>
+        <v>30125.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -19417,7 +19418,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>31054.8</v>
+        <v>31014.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -21268,7 +21269,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!E190")</f>
-        <v>25294.4</v>
+        <v>25274.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -21540,7 +21541,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>26963.4</v>
+        <v>26943.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -21632,7 +21633,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>26963.4</v>
+        <v>26943.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -21904,7 +21905,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>28476.4</v>
+        <v>28456.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -21996,7 +21997,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>28476.4</v>
+        <v>28456.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -22268,7 +22269,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>30145.4</v>
+        <v>30125.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -22814,7 +22815,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>909.4</v>
+        <v>889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -22830,7 +22831,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -22846,7 +22847,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35799.8</v>
+        <v>35759.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -24697,7 +24698,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!E190")</f>
-        <v>30145.4</v>
+        <v>30125.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -24969,7 +24970,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>31708.4</v>
+        <v>31688.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -25061,7 +25062,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>31708.4</v>
+        <v>31688.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -25333,7 +25334,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>33327.4</v>
+        <v>33307.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -25425,7 +25426,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>33327.4</v>
+        <v>33307.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -25697,7 +25698,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -26244,7 +26245,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>909.4</v>
+        <v>889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -26260,7 +26261,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -26276,7 +26277,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35799.8</v>
+        <v>35759.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -28085,7 +28086,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!E190")</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -28353,7 +28354,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -28445,7 +28446,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -28713,7 +28714,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -28805,7 +28806,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -29073,7 +29074,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -29567,7 +29568,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>909.4</v>
+        <v>889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -29583,7 +29584,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -29599,7 +29600,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35799.8</v>
+        <v>35759.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -31407,7 +31408,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!E190")</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -31675,7 +31676,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -31767,7 +31768,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -32035,7 +32036,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -32127,7 +32128,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -32395,7 +32396,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -32893,7 +32894,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>909.4</v>
+        <v>889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -32909,7 +32910,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -32925,7 +32926,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35799.8</v>
+        <v>35759.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -34734,7 +34735,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!E190")</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -35002,7 +35003,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -35094,7 +35095,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -35362,7 +35363,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -35454,7 +35455,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -35722,7 +35723,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -36721,8 +36722,8 @@
   <sheetPr/>
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -36802,7 +36803,7 @@
         <v>34</v>
       </c>
       <c r="F3" s="192">
-        <v>816</v>
+        <v>536</v>
       </c>
       <c r="I3" s="200" t="str">
         <f>TEXT(Main!B3,"dd mmmm yyyy")&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,1)-1,"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)*1,"dd mmmm yyyy"))</f>
@@ -36827,14 +36828,14 @@
         <v>35</v>
       </c>
       <c r="C4" s="164">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="D4" s="166"/>
       <c r="E4" s="5" t="s">
         <v>35</v>
       </c>
       <c r="F4" s="192">
-        <v>0</v>
+        <v>280</v>
       </c>
       <c r="I4" s="202" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,1),"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)+1,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,2)-1,"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)*2+1,"dd mmmm yyyy"))</f>
@@ -37164,7 +37165,7 @@
       </c>
       <c r="J14" s="205">
         <f ca="1">'January 2025 - March 2025'!E190</f>
-        <v>909.400000000001</v>
+        <v>889.400000000001</v>
       </c>
       <c r="M14" s="202" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,33),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+33),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,36)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+35),"dd mmmm yyyy"))</f>
@@ -37196,7 +37197,7 @@
       </c>
       <c r="J15" s="205">
         <f ca="1">'April 2025 - June 2025'!E136</f>
-        <v>972.400000000001</v>
+        <v>952.400000000001</v>
       </c>
       <c r="M15" s="202" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,36),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+36),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,39)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+38),"dd mmmm yyyy"))</f>
@@ -37214,7 +37215,7 @@
       </c>
       <c r="C16" s="170">
         <f>SUM(C3:C15)</f>
-        <v>909.4</v>
+        <v>889.4</v>
       </c>
       <c r="D16" s="171"/>
       <c r="E16" s="169" t="s">
@@ -37230,7 +37231,7 @@
       </c>
       <c r="J16" s="205">
         <f ca="1">'April 2025 - June 2025'!E163</f>
-        <v>1026.4</v>
+        <v>1006.4</v>
       </c>
       <c r="M16" s="202" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+39),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
@@ -37248,7 +37249,7 @@
       </c>
       <c r="J17" s="205">
         <f ca="1">'April 2025 - June 2025'!E190</f>
-        <v>1189.4</v>
+        <v>1169.4</v>
       </c>
       <c r="M17" s="202" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+42),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
@@ -37266,7 +37267,7 @@
       </c>
       <c r="J18" s="205">
         <f ca="1">'July 2025 - September 2025'!E136</f>
-        <v>1258.4</v>
+        <v>1238.4</v>
       </c>
       <c r="M18" s="202" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+45),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
@@ -37284,7 +37285,7 @@
       </c>
       <c r="J19" s="205">
         <f ca="1">'July 2025 - September 2025'!E163</f>
-        <v>1371.4</v>
+        <v>1351.4</v>
       </c>
     </row>
     <row r="20" ht="35.25" customHeight="1" spans="9:10">
@@ -37294,7 +37295,7 @@
       </c>
       <c r="J20" s="205">
         <f ca="1">'July 2025 - September 2025'!E190</f>
-        <v>1357.4</v>
+        <v>1337.4</v>
       </c>
     </row>
     <row r="21" ht="35.25" customHeight="1" spans="9:10">
@@ -37304,7 +37305,7 @@
       </c>
       <c r="J21" s="205">
         <f ca="1">'October 2025 - December 2025'!E136</f>
-        <v>2920.4</v>
+        <v>2900.4</v>
       </c>
     </row>
     <row r="22" ht="24.75" customHeight="1" spans="1:10">
@@ -37324,7 +37325,7 @@
       </c>
       <c r="J22" s="205">
         <f ca="1">'October 2025 - December 2025'!E163</f>
-        <v>4539.4</v>
+        <v>4519.4</v>
       </c>
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:10">
@@ -37349,7 +37350,7 @@
       </c>
       <c r="J23" s="205">
         <f ca="1">'October 2025 - December 2025'!E190</f>
-        <v>6102.4</v>
+        <v>6082.4</v>
       </c>
     </row>
     <row r="24" ht="52.5" customHeight="1" spans="1:10">
@@ -37374,7 +37375,7 @@
       </c>
       <c r="J24" s="205">
         <f ca="1">'January 2026 - March 2026'!E136</f>
-        <v>7771.4</v>
+        <v>7751.4</v>
       </c>
     </row>
     <row r="25" ht="30" customHeight="1" spans="1:10">
@@ -37393,7 +37394,7 @@
       </c>
       <c r="J25" s="205">
         <f ca="1">'January 2026 - March 2026'!E163</f>
-        <v>9284.4</v>
+        <v>9264.4</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1" spans="1:10">
@@ -37412,7 +37413,7 @@
       </c>
       <c r="J26" s="205">
         <f ca="1">'January 2026 - March 2026'!E190</f>
-        <v>10953.4</v>
+        <v>10933.4</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1" spans="1:10">
@@ -37431,7 +37432,7 @@
       </c>
       <c r="J27" s="205">
         <f ca="1">'April 2026 - June 2026'!E136</f>
-        <v>12516.4</v>
+        <v>12496.4</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:10">
@@ -37450,7 +37451,7 @@
       </c>
       <c r="J28" s="205">
         <f ca="1">'April 2026 - June 2026'!E163</f>
-        <v>14135.4</v>
+        <v>14115.4</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:10">
@@ -37469,7 +37470,7 @@
       </c>
       <c r="J29" s="201">
         <f ca="1">'April 2026 - June 2026'!E190</f>
-        <v>15698.4</v>
+        <v>15678.4</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1" spans="1:10">
@@ -37491,7 +37492,7 @@
       </c>
       <c r="J30" s="207">
         <f ca="1">'July 2026 - September 2026'!E136</f>
-        <v>17367.4</v>
+        <v>17347.4</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1" spans="9:10">
@@ -37501,7 +37502,7 @@
       </c>
       <c r="J31" s="205">
         <f ca="1">'July 2026 - September 2026'!E163</f>
-        <v>18880.4</v>
+        <v>18860.4</v>
       </c>
     </row>
     <row r="32" ht="27.75" customHeight="1" spans="9:10">
@@ -37511,7 +37512,7 @@
       </c>
       <c r="J32" s="205">
         <f ca="1">'July 2026 - September 2026'!E190</f>
-        <v>20549.4</v>
+        <v>20529.4</v>
       </c>
     </row>
     <row r="33" ht="30" customHeight="1" spans="9:10">
@@ -37521,7 +37522,7 @@
       </c>
       <c r="J33" s="205">
         <f ca="1">'October 2026 - December 2026'!E136</f>
-        <v>22112.4</v>
+        <v>22092.4</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1" spans="1:10">
@@ -37541,7 +37542,7 @@
       </c>
       <c r="J34" s="205">
         <f ca="1">'October 2026 - December 2026'!E163</f>
-        <v>23731.4</v>
+        <v>23711.4</v>
       </c>
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:10">
@@ -37566,7 +37567,7 @@
       </c>
       <c r="J35" s="205">
         <f ca="1">'October 2026 - December 2026'!E190</f>
-        <v>25294.4</v>
+        <v>25274.4</v>
       </c>
     </row>
     <row r="36" ht="54.75" customHeight="1" spans="1:10">
@@ -37591,7 +37592,7 @@
       </c>
       <c r="J36" s="205">
         <f ca="1">'January 2027 - March 2027'!E136</f>
-        <v>26963.4</v>
+        <v>26943.4</v>
       </c>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:10">
@@ -37616,7 +37617,7 @@
       </c>
       <c r="J37" s="205">
         <f ca="1">'January 2027 - March 2027'!E163</f>
-        <v>28476.4</v>
+        <v>28456.4</v>
       </c>
     </row>
     <row r="38" ht="20.25" customHeight="1" spans="1:10">
@@ -37641,7 +37642,7 @@
       </c>
       <c r="J38" s="205">
         <f ca="1">'January 2027 - March 2027'!E190</f>
-        <v>30145.4</v>
+        <v>30125.4</v>
       </c>
     </row>
     <row r="39" ht="24.75" customHeight="1" spans="1:10">
@@ -37660,7 +37661,7 @@
       </c>
       <c r="J39" s="205">
         <f ca="1">'April 2027 - June 2027'!E136</f>
-        <v>31708.4</v>
+        <v>31688.4</v>
       </c>
     </row>
     <row r="40" ht="24.75" customHeight="1" spans="1:10">
@@ -37679,7 +37680,7 @@
       </c>
       <c r="J40" s="205">
         <f ca="1">'April 2027 - June 2027'!E163</f>
-        <v>33327.4</v>
+        <v>33307.4</v>
       </c>
     </row>
     <row r="41" ht="24.75" customHeight="1" spans="1:10">
@@ -37698,7 +37699,7 @@
       </c>
       <c r="J41" s="205">
         <f ca="1">'April 2027 - June 2027'!E190</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:10">
@@ -37720,7 +37721,7 @@
       </c>
       <c r="J42" s="205">
         <f ca="1">Forecast_14!E136</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="9:10">
@@ -37730,7 +37731,7 @@
       </c>
       <c r="J43" s="205">
         <f ca="1">Forecast_14!E163</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
     </row>
     <row r="44" ht="24.75" customHeight="1" spans="9:10">
@@ -37740,7 +37741,7 @@
       </c>
       <c r="J44" s="205">
         <f ca="1">Forecast_14!E190</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
     </row>
     <row r="45" ht="24.75" customHeight="1" spans="9:10">
@@ -37750,7 +37751,7 @@
       </c>
       <c r="J45" s="205">
         <f ca="1">Forecast_15!E136</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
     </row>
     <row r="46" ht="24.75" customHeight="1" spans="1:10">
@@ -37770,7 +37771,7 @@
       </c>
       <c r="J46" s="205">
         <f ca="1">Forecast_15!E163</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
     </row>
     <row r="47" ht="24.75" customHeight="1" spans="1:10">
@@ -37795,7 +37796,7 @@
       </c>
       <c r="J47" s="205">
         <f ca="1">Forecast_15!E190</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
     </row>
     <row r="48" ht="24.75" customHeight="1" spans="1:10">
@@ -37820,7 +37821,7 @@
       </c>
       <c r="J48" s="205">
         <f ca="1">Forecast_16!E136</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
     </row>
     <row r="49" ht="24.75" customHeight="1" spans="1:10">
@@ -37845,7 +37846,7 @@
       </c>
       <c r="J49" s="205">
         <f ca="1">Forecast_16!E163</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
     </row>
     <row r="50" ht="24.75" customHeight="1" spans="1:10">
@@ -37870,7 +37871,7 @@
       </c>
       <c r="J50" s="201">
         <f ca="1">Forecast_16!E190</f>
-        <v>34890.4</v>
+        <v>34870.4</v>
       </c>
     </row>
     <row r="51" ht="41" customHeight="1" spans="1:7">
@@ -39831,7 +39832,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>909.4</v>
+        <v>889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -39859,7 +39860,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1412.11</v>
+        <v>1392.11</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -43297,7 +43298,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>909.4</v>
+        <v>889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -43325,7 +43326,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1082.74</v>
+        <v>1062.74</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -46829,8 +46830,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="F184" sqref="F184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -46864,7 +46865,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>909.4</v>
+        <v>889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -46880,7 +46881,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>909.400000000001</v>
+        <v>889.400000000001</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -46896,7 +46897,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1818.8</v>
+        <v>1778.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -49705,7 +49706,7 @@
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="102">
-        <v>233.8</v>
+        <v>253.8</v>
       </c>
       <c r="F184" s="14"/>
       <c r="G184" s="14"/>
@@ -49789,7 +49790,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>909.400000000001</v>
+        <v>889.400000000001</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -50381,7 +50382,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>909.4</v>
+        <v>889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -50397,7 +50398,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>1189.4</v>
+        <v>1169.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -50413,7 +50414,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>2098.8</v>
+        <v>2058.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -52268,7 +52269,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!E190")</f>
-        <v>909.400000000001</v>
+        <v>889.400000000001</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -52542,7 +52543,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>972.400000000001</v>
+        <v>952.400000000001</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -52634,7 +52635,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>972.400000000001</v>
+        <v>952.400000000001</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -52908,7 +52909,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>1026.4</v>
+        <v>1006.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -53000,7 +53001,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>1026.4</v>
+        <v>1006.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -53274,7 +53275,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>1189.4</v>
+        <v>1169.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -53832,7 +53833,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>909.4</v>
+        <v>889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -53848,7 +53849,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>1357.4</v>
+        <v>1337.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -53864,7 +53865,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>2266.8</v>
+        <v>2226.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -55711,7 +55712,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!E190")</f>
-        <v>1189.4</v>
+        <v>1169.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -55985,7 +55986,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>1258.4</v>
+        <v>1238.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -56077,7 +56078,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>1258.4</v>
+        <v>1238.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -56355,7 +56356,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>1371.4</v>
+        <v>1351.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -56447,7 +56448,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>1371.4</v>
+        <v>1351.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -56721,7 +56722,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>1357.4</v>
+        <v>1337.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -57282,7 +57283,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>909.4</v>
+        <v>889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -57298,7 +57299,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>6102.4</v>
+        <v>6082.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -57314,7 +57315,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>7011.8</v>
+        <v>6971.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -59161,7 +59162,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!E190")</f>
-        <v>1357.4</v>
+        <v>1337.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -59433,7 +59434,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>2920.4</v>
+        <v>2900.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -59525,7 +59526,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>2920.4</v>
+        <v>2900.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -59797,7 +59798,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>4539.4</v>
+        <v>4519.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -59889,7 +59890,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>4539.4</v>
+        <v>4519.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -60161,7 +60162,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>6102.4</v>
+        <v>6082.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>

</xml_diff>

<commit_message>
docs: Removed all the non protected cell.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560" activeTab="5"/>
+    <workbookView windowHeight="21560"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="294">
   <si>
     <t>Income Forecast</t>
   </si>
@@ -1012,6 +1012,12 @@
   </si>
   <si>
     <t>31st March 2025</t>
+  </si>
+  <si>
+    <t>22th March 2025</t>
+  </si>
+  <si>
+    <t>Lawrence give me $1000 as a gift</t>
   </si>
   <si>
     <t xml:space="preserve">Payback $1400 to Mom including $900 borrowed </t>
@@ -3865,8 +3871,8 @@
   <sheetPr/>
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="AC22" sqref="AC22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="17.6"/>
@@ -5662,7 +5668,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>889.4</v>
+        <v>1889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -5678,7 +5684,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>10933.4</v>
+        <v>11933.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -5694,7 +5700,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>11822.8</v>
+        <v>13822.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -5793,7 +5799,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -5967,7 +5973,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -6141,7 +6147,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -7545,7 +7551,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!E190")</f>
-        <v>6082.4</v>
+        <v>7082.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -7714,7 +7720,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -7817,7 +7823,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>7751.4</v>
+        <v>8751.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -7909,7 +7915,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>7751.4</v>
+        <v>8751.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -8078,7 +8084,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D156" s="103"/>
       <c r="E156" s="101">
@@ -8181,7 +8187,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>9264.4</v>
+        <v>10264.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -8273,7 +8279,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>9264.4</v>
+        <v>10264.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -8442,7 +8448,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -8545,7 +8551,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>10933.4</v>
+        <v>11933.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -8587,23 +8593,6 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
-  <protectedRanges>
-    <protectedRange sqref="A10:G15" name="R1"/>
-    <protectedRange sqref="A22:G27" name="R2"/>
-    <protectedRange sqref="A34:G39" name="R3"/>
-    <protectedRange sqref="A46:C46 C47:C54" name="F1"/>
-    <protectedRange sqref="C56:C65" name="F2"/>
-    <protectedRange sqref="C67:C74" name="F3"/>
-    <protectedRange sqref="C76:C84" name="F4"/>
-    <protectedRange sqref="C86:C95" name="F5"/>
-    <protectedRange sqref="C117:E134" name="E1"/>
-    <protectedRange sqref="C144:E161" name="E2"/>
-    <protectedRange sqref="C171:E188" name="E3"/>
-    <protectedRange sqref="A56:B56" name="F2_1"/>
-    <protectedRange sqref="A67:B67" name="F3_1"/>
-    <protectedRange sqref="A76:B76" name="F4_1"/>
-    <protectedRange sqref="A86:B86" name="F5_1"/>
-  </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C2:G2"/>
@@ -9092,7 +9081,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>889.4</v>
+        <v>1889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -9108,7 +9097,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>15678.4</v>
+        <v>16678.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -9124,7 +9113,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>16567.8</v>
+        <v>18567.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -9223,7 +9212,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -9397,7 +9386,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -9571,7 +9560,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -10975,7 +10964,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!E190")</f>
-        <v>10933.4</v>
+        <v>11933.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -11144,7 +11133,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -11247,7 +11236,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>12496.4</v>
+        <v>13496.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -11339,7 +11328,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>12496.4</v>
+        <v>13496.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -11508,7 +11497,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
@@ -11611,7 +11600,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>14115.4</v>
+        <v>15115.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -11703,7 +11692,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>14115.4</v>
+        <v>15115.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -11872,7 +11861,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D183" s="103"/>
       <c r="E183" s="101">
@@ -11975,7 +11964,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>15678.4</v>
+        <v>16678.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -12017,23 +12006,6 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
-  <protectedRanges>
-    <protectedRange sqref="A10:G15" name="R1"/>
-    <protectedRange sqref="A22:G27" name="R2"/>
-    <protectedRange sqref="A34:G39" name="R3"/>
-    <protectedRange sqref="A46:C46 C47:C54" name="F1"/>
-    <protectedRange sqref="C56:C65" name="F2"/>
-    <protectedRange sqref="C67:C74" name="F3"/>
-    <protectedRange sqref="C76:C84" name="F4"/>
-    <protectedRange sqref="C86:C94" name="F5"/>
-    <protectedRange sqref="C117:E134" name="E1"/>
-    <protectedRange sqref="C144:E161" name="E2"/>
-    <protectedRange sqref="C171:E188" name="E3"/>
-    <protectedRange sqref="A56:B56" name="F2_1"/>
-    <protectedRange sqref="A67:B67" name="F3_1"/>
-    <protectedRange sqref="A76:B76" name="F4_1"/>
-    <protectedRange sqref="A86:B86" name="F5_1"/>
-  </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C2:G2"/>
@@ -12487,7 +12459,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="A46" sqref="A46:C46"/>
     </sheetView>
   </sheetViews>
@@ -12523,7 +12495,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>889.4</v>
+        <v>1889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -12539,7 +12511,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>20529.4</v>
+        <v>21529.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -12555,7 +12527,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>21418.8</v>
+        <v>23418.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -12654,7 +12626,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -12828,7 +12800,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -13002,7 +12974,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -14406,7 +14378,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!E190")</f>
-        <v>15678.4</v>
+        <v>16678.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -14575,7 +14547,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -14678,7 +14650,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>17347.4</v>
+        <v>18347.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -14770,7 +14742,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>17347.4</v>
+        <v>18347.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -14939,7 +14911,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D156" s="103"/>
       <c r="E156" s="101">
@@ -15042,7 +15014,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>18860.4</v>
+        <v>19860.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -15134,7 +15106,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>18860.4</v>
+        <v>19860.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -15303,7 +15275,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -15406,7 +15378,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>20529.4</v>
+        <v>21529.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -15448,23 +15420,6 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
-  <protectedRanges>
-    <protectedRange sqref="A10:G15" name="R1"/>
-    <protectedRange sqref="A22:G27" name="R2"/>
-    <protectedRange sqref="A34:G39" name="R3"/>
-    <protectedRange sqref="C47:C54" name="F1"/>
-    <protectedRange sqref="C56:C65" name="F2"/>
-    <protectedRange sqref="C67:C74" name="F3"/>
-    <protectedRange sqref="C76:C84" name="F4"/>
-    <protectedRange sqref="C86:C94" name="F5"/>
-    <protectedRange sqref="C117:E134" name="E1"/>
-    <protectedRange sqref="C144:E161" name="E2"/>
-    <protectedRange sqref="C171:E188" name="E3"/>
-    <protectedRange sqref="A56:B56" name="F2_1"/>
-    <protectedRange sqref="A67:B67" name="F3_1"/>
-    <protectedRange sqref="A76:B76" name="F4_1"/>
-    <protectedRange sqref="A86:B86" name="F5_1"/>
-  </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C2:G2"/>
@@ -15952,7 +15907,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>889.4</v>
+        <v>1889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -15968,7 +15923,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>25274.4</v>
+        <v>26274.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -15984,7 +15939,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>26163.8</v>
+        <v>28163.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -16083,7 +16038,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -16257,7 +16212,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -16431,7 +16386,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -17835,7 +17790,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!E190")</f>
-        <v>20529.4</v>
+        <v>21529.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -18004,7 +17959,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -18107,7 +18062,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>22092.4</v>
+        <v>23092.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -18199,7 +18154,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>22092.4</v>
+        <v>23092.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -18368,7 +18323,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
@@ -18471,7 +18426,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>23711.4</v>
+        <v>24711.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -18563,7 +18518,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>23711.4</v>
+        <v>24711.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -18732,7 +18687,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -18835,7 +18790,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>25274.4</v>
+        <v>26274.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -18877,23 +18832,6 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
-  <protectedRanges>
-    <protectedRange sqref="A10:G15" name="R1"/>
-    <protectedRange sqref="A22:G27" name="R2"/>
-    <protectedRange sqref="A34:G39" name="R3"/>
-    <protectedRange sqref="A46:C46 C47:C54" name="F1"/>
-    <protectedRange sqref="C56:C65" name="F2"/>
-    <protectedRange sqref="C67:C74" name="F3"/>
-    <protectedRange sqref="C76:C84" name="F4"/>
-    <protectedRange sqref="C86:C94" name="F5"/>
-    <protectedRange sqref="C117:E134" name="E1"/>
-    <protectedRange sqref="C144:E161" name="E2"/>
-    <protectedRange sqref="C171:E188" name="E3"/>
-    <protectedRange sqref="A56:B56" name="F2_1"/>
-    <protectedRange sqref="A67:B67" name="F3_1"/>
-    <protectedRange sqref="A76:B76" name="F4_1"/>
-    <protectedRange sqref="A86:B86" name="F5_1"/>
-  </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C2:G2"/>
@@ -19383,7 +19321,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>889.4</v>
+        <v>1889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -19399,7 +19337,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>30125.4</v>
+        <v>31125.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -19415,7 +19353,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>31014.8</v>
+        <v>33014.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -19514,7 +19452,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -19688,7 +19626,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -19862,7 +19800,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -21266,7 +21204,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!E190")</f>
-        <v>25274.4</v>
+        <v>26274.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -21435,7 +21373,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -21538,7 +21476,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>26943.4</v>
+        <v>27943.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -21630,7 +21568,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>26943.4</v>
+        <v>27943.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -21799,7 +21737,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
@@ -21902,7 +21840,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>28456.4</v>
+        <v>29456.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -21994,7 +21932,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>28456.4</v>
+        <v>29456.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -22163,7 +22101,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -22266,7 +22204,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>30125.4</v>
+        <v>31125.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -22308,23 +22246,6 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
-  <protectedRanges>
-    <protectedRange sqref="A10:G15" name="R1"/>
-    <protectedRange sqref="A22:G27" name="R2"/>
-    <protectedRange sqref="A34:G39" name="R3"/>
-    <protectedRange sqref="A46:C46 C47:C54" name="F1"/>
-    <protectedRange sqref="C67:C74" name="F3"/>
-    <protectedRange sqref="C76:C84" name="F4"/>
-    <protectedRange sqref="C56:C65" name="F2"/>
-    <protectedRange sqref="C86:C94" name="F5"/>
-    <protectedRange sqref="C117:E134" name="E1"/>
-    <protectedRange sqref="C144:E161" name="E2"/>
-    <protectedRange sqref="C171:E188" name="E3"/>
-    <protectedRange sqref="A56:B56" name="F2_1"/>
-    <protectedRange sqref="A67:B67" name="F3_1"/>
-    <protectedRange sqref="A76:B76" name="F4_1"/>
-    <protectedRange sqref="A86:B86" name="F5_1"/>
-  </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C2:G2"/>
@@ -22778,7 +22699,7 @@
   <sheetPr/>
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView topLeftCell="A171" workbookViewId="0">
+    <sheetView topLeftCell="A170" workbookViewId="0">
       <selection activeCell="F184" sqref="F184"/>
     </sheetView>
   </sheetViews>
@@ -22812,7 +22733,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>889.4</v>
+        <v>1889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -22828,7 +22749,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -22844,7 +22765,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35759.8</v>
+        <v>37759.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -22943,7 +22864,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -23117,7 +23038,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -23291,7 +23212,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -24695,7 +24616,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!E190")</f>
-        <v>30125.4</v>
+        <v>31125.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -24864,7 +24785,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -24967,7 +24888,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>31688.4</v>
+        <v>32688.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -25059,7 +24980,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>31688.4</v>
+        <v>32688.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -25228,7 +25149,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
@@ -25331,7 +25252,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>33307.4</v>
+        <v>34307.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -25423,7 +25344,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>33307.4</v>
+        <v>34307.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -25592,7 +25513,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -25695,7 +25616,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -25738,23 +25659,6 @@
     <row r="194" ht="24.75" customHeight="1"/>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
-  <protectedRanges>
-    <protectedRange sqref="A10:G15" name="R1"/>
-    <protectedRange sqref="A22:G27" name="R2"/>
-    <protectedRange sqref="A34:G39" name="R3"/>
-    <protectedRange sqref="A46:C46 C47:C54" name="F1"/>
-    <protectedRange sqref="C56:C65" name="F2"/>
-    <protectedRange sqref="C76:C84" name="F3"/>
-    <protectedRange sqref="C86:C94" name="F5"/>
-    <protectedRange sqref="C117:E134" name="E1"/>
-    <protectedRange sqref="C144:E161" name="E2"/>
-    <protectedRange sqref="C171:E188" name="E3"/>
-    <protectedRange sqref="C68:C74" name="F4"/>
-    <protectedRange sqref="A56:B56" name="F2_1"/>
-    <protectedRange sqref="A67:B67" name="F3_1"/>
-    <protectedRange sqref="A76:B76" name="F4_1"/>
-    <protectedRange sqref="A86:B86" name="F5_1"/>
-  </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C2:G2"/>
@@ -26242,7 +26146,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>889.4</v>
+        <v>1889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -26258,7 +26162,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -26274,7 +26178,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35759.8</v>
+        <v>37759.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -28083,7 +27987,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!E190")</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -28351,7 +28255,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -28443,7 +28347,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -28711,7 +28615,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -28803,7 +28707,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -29071,7 +28975,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -29113,23 +29017,6 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
-  <protectedRanges>
-    <protectedRange sqref="A10:G15" name="R1"/>
-    <protectedRange sqref="A22:G27" name="R2"/>
-    <protectedRange sqref="A34:G39" name="R3"/>
-    <protectedRange sqref="A46:C46 C47:C54" name="F1"/>
-    <protectedRange sqref="C56:C65" name="F2"/>
-    <protectedRange sqref="C67:C74" name="F3"/>
-    <protectedRange sqref="C76:C84" name="F4"/>
-    <protectedRange sqref="C86:C94" name="F5"/>
-    <protectedRange sqref="C117:E134" name="E1"/>
-    <protectedRange sqref="C144:E161" name="E2"/>
-    <protectedRange sqref="C171:E188" name="E3"/>
-    <protectedRange sqref="A56:B56" name="F2_1"/>
-    <protectedRange sqref="A67:B67" name="F3_1"/>
-    <protectedRange sqref="A76:B76" name="F4_1"/>
-    <protectedRange sqref="A86:B86" name="F5_1"/>
-  </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C2:G2"/>
@@ -29531,7 +29418,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
+    <sheetView topLeftCell="A70" workbookViewId="0">
       <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
@@ -29565,7 +29452,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>889.4</v>
+        <v>1889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -29581,7 +29468,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -29597,7 +29484,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35759.8</v>
+        <v>37759.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -31175,7 +31062,7 @@
         <v>Bankruptcy Department / Bank</v>
       </c>
       <c r="B102" s="37" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C102" s="36" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C102")+SUM(E122+E149+E176)</f>
@@ -31405,7 +31292,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!E190")</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -31673,7 +31560,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -31765,7 +31652,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -32033,7 +31920,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -32125,7 +32012,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -32393,7 +32280,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -32435,25 +32322,6 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
-  <protectedRanges>
-    <protectedRange sqref="A10:G15" name="R1"/>
-    <protectedRange sqref="A22:G27" name="R2"/>
-    <protectedRange sqref="A34:G39" name="R3"/>
-    <protectedRange sqref="A46:C46 C47:C54" name="F1"/>
-    <protectedRange sqref="C56:C65" name="F2"/>
-    <protectedRange sqref="C67:C74" name="F3"/>
-    <protectedRange sqref="C76:C84" name="F4"/>
-    <protectedRange sqref="C86:C94" name="F5"/>
-    <protectedRange sqref="C117:E134" name="E1"/>
-    <protectedRange sqref="C144:E161" name="E2"/>
-    <protectedRange sqref="C171:E188" name="E3"/>
-    <protectedRange sqref="A56:B56" name="F2_1"/>
-    <protectedRange sqref="A76:B76" name="F4_1"/>
-    <protectedRange sqref="A56:B56" name="F2_2"/>
-    <protectedRange sqref="A67:B67" name="F3_1"/>
-    <protectedRange sqref="A76:B76" name="F4_2"/>
-    <protectedRange sqref="A86:B86" name="F5_1"/>
-  </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C2:G2"/>
@@ -32891,7 +32759,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>889.4</v>
+        <v>1889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -32907,7 +32775,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -32923,7 +32791,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>35759.8</v>
+        <v>37759.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -34732,7 +34600,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!E190")</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -35000,7 +34868,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -35092,7 +34960,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -35360,7 +35228,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -35452,7 +35320,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -35720,7 +35588,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -35762,19 +35630,6 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
-  <protectedRanges>
-    <protectedRange sqref="A10:G15" name="R1"/>
-    <protectedRange sqref="A22:G27" name="R2"/>
-    <protectedRange sqref="A34:G39" name="R3"/>
-    <protectedRange sqref="A46:C46 C47:C54" name="F1"/>
-    <protectedRange sqref="A56:C56 C57:C65" name="F2"/>
-    <protectedRange sqref="A67:C67 C68:C74" name="F3"/>
-    <protectedRange sqref="A76:C76 C77:C84" name="F4"/>
-    <protectedRange sqref="A86:C86 C87:C94" name="F5"/>
-    <protectedRange sqref="C117:E134" name="E1"/>
-    <protectedRange sqref="C144:E161" name="E2"/>
-    <protectedRange sqref="C171:E188" name="E3"/>
-  </protectedRanges>
   <mergeCells count="169">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C2:G2"/>
@@ -36715,8 +36570,8 @@
   <sheetPr/>
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60:C60"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -36821,14 +36676,14 @@
         <v>35</v>
       </c>
       <c r="C4" s="162">
-        <v>260</v>
+        <v>1260</v>
       </c>
       <c r="D4" s="164"/>
       <c r="E4" s="5" t="s">
         <v>35</v>
       </c>
       <c r="F4" s="190">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="I4" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,1),"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)+1,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,2)-1,"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)*2+1,"dd mmmm yyyy"))</f>
@@ -37158,7 +37013,7 @@
       </c>
       <c r="J14" s="203">
         <f ca="1">'January 2025 - March 2025'!E190</f>
-        <v>889.400000000001</v>
+        <v>1889.4</v>
       </c>
       <c r="M14" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,33),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+33),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,36)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+35),"dd mmmm yyyy"))</f>
@@ -37190,7 +37045,7 @@
       </c>
       <c r="J15" s="203">
         <f ca="1">'April 2025 - June 2025'!E136</f>
-        <v>952.400000000001</v>
+        <v>1952.4</v>
       </c>
       <c r="M15" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,36),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+36),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,39)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+38),"dd mmmm yyyy"))</f>
@@ -37208,7 +37063,7 @@
       </c>
       <c r="C16" s="168">
         <f>SUM(C3:C15)</f>
-        <v>889.4</v>
+        <v>1889.4</v>
       </c>
       <c r="D16" s="169"/>
       <c r="E16" s="167" t="s">
@@ -37216,7 +37071,7 @@
       </c>
       <c r="F16" s="193">
         <f>SUM(F3:F15)</f>
-        <v>909.4</v>
+        <v>889.4</v>
       </c>
       <c r="I16" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,13),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*13)+13,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,14)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*14+13),"dd mmmm yyyy"))</f>
@@ -37224,7 +37079,7 @@
       </c>
       <c r="J16" s="203">
         <f ca="1">'April 2025 - June 2025'!E163</f>
-        <v>1006.4</v>
+        <v>2006.4</v>
       </c>
       <c r="M16" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+39),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
@@ -37242,7 +37097,7 @@
       </c>
       <c r="J17" s="203">
         <f ca="1">'April 2025 - June 2025'!E190</f>
-        <v>1169.4</v>
+        <v>2169.4</v>
       </c>
       <c r="M17" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+42),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
@@ -37260,7 +37115,7 @@
       </c>
       <c r="J18" s="203">
         <f ca="1">'July 2025 - September 2025'!E136</f>
-        <v>1238.4</v>
+        <v>2238.4</v>
       </c>
       <c r="M18" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+45),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
@@ -37278,7 +37133,7 @@
       </c>
       <c r="J19" s="203">
         <f ca="1">'July 2025 - September 2025'!E163</f>
-        <v>1351.4</v>
+        <v>2351.4</v>
       </c>
     </row>
     <row r="20" ht="35.25" customHeight="1" spans="9:10">
@@ -37288,7 +37143,7 @@
       </c>
       <c r="J20" s="203">
         <f ca="1">'July 2025 - September 2025'!E190</f>
-        <v>1337.4</v>
+        <v>2337.4</v>
       </c>
     </row>
     <row r="21" ht="35.25" customHeight="1" spans="9:10">
@@ -37298,7 +37153,7 @@
       </c>
       <c r="J21" s="203">
         <f ca="1">'October 2025 - December 2025'!E136</f>
-        <v>2900.4</v>
+        <v>3900.4</v>
       </c>
     </row>
     <row r="22" ht="24.75" customHeight="1" spans="1:10">
@@ -37318,7 +37173,7 @@
       </c>
       <c r="J22" s="203">
         <f ca="1">'October 2025 - December 2025'!E163</f>
-        <v>4519.4</v>
+        <v>5519.4</v>
       </c>
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:10">
@@ -37343,7 +37198,7 @@
       </c>
       <c r="J23" s="203">
         <f ca="1">'October 2025 - December 2025'!E190</f>
-        <v>6082.4</v>
+        <v>7082.4</v>
       </c>
     </row>
     <row r="24" ht="52.5" customHeight="1" spans="1:10">
@@ -37368,7 +37223,7 @@
       </c>
       <c r="J24" s="203">
         <f ca="1">'January 2026 - March 2026'!E136</f>
-        <v>7751.4</v>
+        <v>8751.4</v>
       </c>
     </row>
     <row r="25" ht="30" customHeight="1" spans="1:10">
@@ -37387,7 +37242,7 @@
       </c>
       <c r="J25" s="203">
         <f ca="1">'January 2026 - March 2026'!E163</f>
-        <v>9264.4</v>
+        <v>10264.4</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1" spans="1:10">
@@ -37406,7 +37261,7 @@
       </c>
       <c r="J26" s="203">
         <f ca="1">'January 2026 - March 2026'!E190</f>
-        <v>10933.4</v>
+        <v>11933.4</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1" spans="1:10">
@@ -37425,7 +37280,7 @@
       </c>
       <c r="J27" s="203">
         <f ca="1">'April 2026 - June 2026'!E136</f>
-        <v>12496.4</v>
+        <v>13496.4</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:10">
@@ -37444,7 +37299,7 @@
       </c>
       <c r="J28" s="203">
         <f ca="1">'April 2026 - June 2026'!E163</f>
-        <v>14115.4</v>
+        <v>15115.4</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:10">
@@ -37463,7 +37318,7 @@
       </c>
       <c r="J29" s="199">
         <f ca="1">'April 2026 - June 2026'!E190</f>
-        <v>15678.4</v>
+        <v>16678.4</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1" spans="1:10">
@@ -37485,7 +37340,7 @@
       </c>
       <c r="J30" s="205">
         <f ca="1">'July 2026 - September 2026'!E136</f>
-        <v>17347.4</v>
+        <v>18347.4</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1" spans="9:10">
@@ -37495,7 +37350,7 @@
       </c>
       <c r="J31" s="203">
         <f ca="1">'July 2026 - September 2026'!E163</f>
-        <v>18860.4</v>
+        <v>19860.4</v>
       </c>
     </row>
     <row r="32" ht="27.75" customHeight="1" spans="9:10">
@@ -37505,7 +37360,7 @@
       </c>
       <c r="J32" s="203">
         <f ca="1">'July 2026 - September 2026'!E190</f>
-        <v>20529.4</v>
+        <v>21529.4</v>
       </c>
     </row>
     <row r="33" ht="30" customHeight="1" spans="9:10">
@@ -37515,7 +37370,7 @@
       </c>
       <c r="J33" s="203">
         <f ca="1">'October 2026 - December 2026'!E136</f>
-        <v>22092.4</v>
+        <v>23092.4</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1" spans="1:10">
@@ -37535,7 +37390,7 @@
       </c>
       <c r="J34" s="203">
         <f ca="1">'October 2026 - December 2026'!E163</f>
-        <v>23711.4</v>
+        <v>24711.4</v>
       </c>
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:10">
@@ -37560,7 +37415,7 @@
       </c>
       <c r="J35" s="203">
         <f ca="1">'October 2026 - December 2026'!E190</f>
-        <v>25274.4</v>
+        <v>26274.4</v>
       </c>
     </row>
     <row r="36" ht="54.75" customHeight="1" spans="1:10">
@@ -37585,7 +37440,7 @@
       </c>
       <c r="J36" s="203">
         <f ca="1">'January 2027 - March 2027'!E136</f>
-        <v>26943.4</v>
+        <v>27943.4</v>
       </c>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:10">
@@ -37610,7 +37465,7 @@
       </c>
       <c r="J37" s="203">
         <f ca="1">'January 2027 - March 2027'!E163</f>
-        <v>28456.4</v>
+        <v>29456.4</v>
       </c>
     </row>
     <row r="38" ht="20.25" customHeight="1" spans="1:10">
@@ -37635,7 +37490,7 @@
       </c>
       <c r="J38" s="203">
         <f ca="1">'January 2027 - March 2027'!E190</f>
-        <v>30125.4</v>
+        <v>31125.4</v>
       </c>
     </row>
     <row r="39" ht="24.75" customHeight="1" spans="1:10">
@@ -37654,7 +37509,7 @@
       </c>
       <c r="J39" s="203">
         <f ca="1">'April 2027 - June 2027'!E136</f>
-        <v>31688.4</v>
+        <v>32688.4</v>
       </c>
     </row>
     <row r="40" ht="24.75" customHeight="1" spans="1:10">
@@ -37673,7 +37528,7 @@
       </c>
       <c r="J40" s="203">
         <f ca="1">'April 2027 - June 2027'!E163</f>
-        <v>33307.4</v>
+        <v>34307.4</v>
       </c>
     </row>
     <row r="41" ht="24.75" customHeight="1" spans="1:10">
@@ -37692,7 +37547,7 @@
       </c>
       <c r="J41" s="203">
         <f ca="1">'April 2027 - June 2027'!E190</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:10">
@@ -37714,7 +37569,7 @@
       </c>
       <c r="J42" s="203">
         <f ca="1">Forecast_14!E136</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="9:10">
@@ -37724,7 +37579,7 @@
       </c>
       <c r="J43" s="203">
         <f ca="1">Forecast_14!E163</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
     </row>
     <row r="44" ht="24.75" customHeight="1" spans="9:10">
@@ -37734,7 +37589,7 @@
       </c>
       <c r="J44" s="203">
         <f ca="1">Forecast_14!E190</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
     </row>
     <row r="45" ht="24.75" customHeight="1" spans="9:10">
@@ -37744,7 +37599,7 @@
       </c>
       <c r="J45" s="203">
         <f ca="1">Forecast_15!E136</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
     </row>
     <row r="46" ht="24.75" customHeight="1" spans="1:10">
@@ -37764,7 +37619,7 @@
       </c>
       <c r="J46" s="203">
         <f ca="1">Forecast_15!E163</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
     </row>
     <row r="47" ht="24.75" customHeight="1" spans="1:10">
@@ -37789,7 +37644,7 @@
       </c>
       <c r="J47" s="203">
         <f ca="1">Forecast_15!E190</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
     </row>
     <row r="48" ht="24.75" customHeight="1" spans="1:10">
@@ -37814,7 +37669,7 @@
       </c>
       <c r="J48" s="203">
         <f ca="1">Forecast_16!E136</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
     </row>
     <row r="49" ht="24.75" customHeight="1" spans="1:10">
@@ -37839,7 +37694,7 @@
       </c>
       <c r="J49" s="203">
         <f ca="1">Forecast_16!E163</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
     </row>
     <row r="50" ht="24.75" customHeight="1" spans="1:10">
@@ -37864,7 +37719,7 @@
       </c>
       <c r="J50" s="199">
         <f ca="1">Forecast_16!E190</f>
-        <v>34870.4</v>
+        <v>35870.4</v>
       </c>
     </row>
     <row r="51" ht="41" customHeight="1" spans="1:7">
@@ -39809,7 +39664,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>889.4</v>
+        <v>1889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -39837,7 +39692,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1392.11</v>
+        <v>2392.11</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -43262,7 +43117,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>889.4</v>
+        <v>1889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -43290,7 +43145,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1062.74</v>
+        <v>2062.74</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -46777,8 +46632,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="G183" sqref="G183"/>
+    <sheetView topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="G157" sqref="G157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -46812,7 +46667,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>889.4</v>
+        <v>1889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -46828,7 +46683,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>889.400000000001</v>
+        <v>1889.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -46844,7 +46699,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1778.8</v>
+        <v>3778.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -47180,7 +47035,7 @@
       <c r="H25" s="14"/>
       <c r="I25" s="47"/>
     </row>
-    <row r="26" ht="24.75" customHeight="1" spans="1:9">
+    <row r="26" ht="71" customHeight="1" spans="1:9">
       <c r="A26" s="19" t="s">
         <v>226</v>
       </c>
@@ -47354,13 +47209,19 @@
       <c r="I36" s="48"/>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:9">
-      <c r="A37" s="19"/>
-      <c r="B37" s="21"/>
+      <c r="A37" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>104</v>
+      </c>
       <c r="C37" s="22"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="43"/>
+      <c r="D37" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="E37" s="22"/>
       <c r="F37" s="41">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="G37" s="42"/>
       <c r="H37" s="14"/>
@@ -47402,7 +47263,7 @@
       <c r="E40" s="44"/>
       <c r="F40" s="45">
         <f>SUM(F34:G39)</f>
-        <v>2485</v>
+        <v>3485</v>
       </c>
       <c r="G40" s="46"/>
       <c r="H40" s="14"/>
@@ -48749,7 +48610,7 @@
       <c r="A118" s="62"/>
       <c r="B118" s="63"/>
       <c r="C118" s="109" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D118" s="109"/>
       <c r="E118" s="102">
@@ -48896,7 +48757,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="100" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D129" s="100"/>
       <c r="E129" s="102">
@@ -48911,7 +48772,7 @@
       <c r="A130" s="62"/>
       <c r="B130" s="63"/>
       <c r="C130" s="100" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D130" s="100"/>
       <c r="E130" s="102">
@@ -48926,7 +48787,7 @@
       <c r="A131" s="62"/>
       <c r="B131" s="63"/>
       <c r="C131" s="113" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D131" s="114"/>
       <c r="E131" s="102">
@@ -49119,7 +48980,7 @@
       <c r="A145" s="62"/>
       <c r="B145" s="63"/>
       <c r="C145" s="100" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D145" s="100"/>
       <c r="E145" s="102">
@@ -49264,7 +49125,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="100" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D156" s="100"/>
       <c r="E156" s="102">
@@ -49279,7 +49140,7 @@
       <c r="A157" s="62"/>
       <c r="B157" s="63"/>
       <c r="C157" s="100" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D157" s="100"/>
       <c r="E157" s="102">
@@ -49294,7 +49155,7 @@
       <c r="A158" s="62"/>
       <c r="B158" s="63"/>
       <c r="C158" s="72" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D158" s="65"/>
       <c r="E158" s="86">
@@ -49487,7 +49348,7 @@
       <c r="A172" s="62"/>
       <c r="B172" s="63"/>
       <c r="C172" s="109" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D172" s="109"/>
       <c r="E172" s="102">
@@ -49515,7 +49376,7 @@
       <c r="A174" s="62"/>
       <c r="B174" s="63"/>
       <c r="C174" s="64" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D174" s="65"/>
       <c r="E174" s="36">
@@ -49634,7 +49495,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="100" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D183" s="100"/>
       <c r="E183" s="36">
@@ -49649,7 +49510,7 @@
       <c r="A184" s="62"/>
       <c r="B184" s="63"/>
       <c r="C184" s="100" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="102">
@@ -49737,7 +49598,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>889.400000000001</v>
+        <v>1889.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -49779,23 +49640,6 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
-  <protectedRanges>
-    <protectedRange sqref="A10:G15" name="R1"/>
-    <protectedRange sqref="A22:G29" name="R2"/>
-    <protectedRange sqref="A34:G39" name="R3"/>
-    <protectedRange sqref="A46:C46 C47:C54" name="F1"/>
-    <protectedRange sqref="C56:C65" name="F2"/>
-    <protectedRange sqref="C67:C74" name="F3"/>
-    <protectedRange sqref="C76:C84" name="F4"/>
-    <protectedRange sqref="C86:C94" name="F5"/>
-    <protectedRange sqref="C117:E134" name="E1"/>
-    <protectedRange sqref="C144:E161" name="E2"/>
-    <protectedRange sqref="C171:E188" name="E3"/>
-    <protectedRange sqref="A56:B56" name="F2_1"/>
-    <protectedRange sqref="A67:B67" name="F3_1"/>
-    <protectedRange sqref="A76:B76" name="F4_1"/>
-    <protectedRange sqref="A86:B86" name="F5_1"/>
-  </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C2:G2"/>
@@ -50329,7 +50173,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>889.4</v>
+        <v>1889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -50345,7 +50189,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>1169.4</v>
+        <v>2169.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -50361,7 +50205,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>2058.8</v>
+        <v>4058.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -50477,7 +50321,7 @@
     </row>
     <row r="12" ht="24.75" customHeight="1" spans="1:9">
       <c r="A12" s="95" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B12" s="96" t="s">
         <v>66</v>
@@ -50497,11 +50341,11 @@
     <row r="13" ht="24.75" customHeight="1" spans="1:9">
       <c r="A13" s="95"/>
       <c r="B13" s="96" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C13" s="96"/>
       <c r="D13" s="97" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E13" s="97"/>
       <c r="F13" s="7">
@@ -50638,7 +50482,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -50662,7 +50506,7 @@
       </c>
       <c r="C24" s="110"/>
       <c r="D24" s="111" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E24" s="111"/>
       <c r="F24" s="112">
@@ -50812,7 +50656,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -52216,7 +52060,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!E190")</f>
-        <v>889.400000000001</v>
+        <v>1889.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -52242,7 +52086,7 @@
       <c r="A118" s="62"/>
       <c r="B118" s="63"/>
       <c r="C118" s="109" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D118" s="109"/>
       <c r="E118" s="98">
@@ -52387,7 +52231,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="100" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D129" s="109"/>
       <c r="E129" s="98">
@@ -52402,7 +52246,7 @@
       <c r="A130" s="62"/>
       <c r="B130" s="63"/>
       <c r="C130" s="113" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D130" s="114"/>
       <c r="E130" s="98">
@@ -52490,7 +52334,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>952.400000000001</v>
+        <v>1952.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -52582,7 +52426,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>952.400000000001</v>
+        <v>1952.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -52608,7 +52452,7 @@
       <c r="A145" s="62"/>
       <c r="B145" s="63"/>
       <c r="C145" s="109" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D145" s="109"/>
       <c r="E145" s="98">
@@ -52753,7 +52597,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="100" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D156" s="100"/>
       <c r="E156" s="98">
@@ -52768,7 +52612,7 @@
       <c r="A157" s="62"/>
       <c r="B157" s="63"/>
       <c r="C157" s="100" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D157" s="100"/>
       <c r="E157" s="98">
@@ -52856,7 +52700,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>1006.4</v>
+        <v>2006.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -52948,7 +52792,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>1006.4</v>
+        <v>2006.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -52974,7 +52818,7 @@
       <c r="A172" s="62"/>
       <c r="B172" s="63"/>
       <c r="C172" s="109" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D172" s="109"/>
       <c r="E172" s="98">
@@ -53119,7 +52963,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="100" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D183" s="100"/>
       <c r="E183" s="98">
@@ -53134,7 +52978,7 @@
       <c r="A184" s="62"/>
       <c r="B184" s="63"/>
       <c r="C184" s="100" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="98">
@@ -53222,7 +53066,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>1169.4</v>
+        <v>2169.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -53264,23 +53108,6 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
-  <protectedRanges>
-    <protectedRange sqref="A10:G15" name="R1"/>
-    <protectedRange sqref="A22:G27" name="R2"/>
-    <protectedRange sqref="A34:G39" name="R3"/>
-    <protectedRange sqref="A46:C46 C47:C54" name="F1"/>
-    <protectedRange sqref="C56:C65" name="F2"/>
-    <protectedRange sqref="C67:C74" name="F3"/>
-    <protectedRange sqref="C76:C84" name="F4"/>
-    <protectedRange sqref="C86:C94" name="F5"/>
-    <protectedRange sqref="C117:E134" name="E1"/>
-    <protectedRange sqref="C144:E161" name="E2"/>
-    <protectedRange sqref="C171:E188" name="E3"/>
-    <protectedRange sqref="A56:B56" name="F2_1"/>
-    <protectedRange sqref="A67:B67" name="F3_1"/>
-    <protectedRange sqref="A76:B76" name="F4_1"/>
-    <protectedRange sqref="A86:B86" name="F5_1"/>
-  </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C2:G2"/>
@@ -53747,7 +53574,7 @@
   <dimension ref="A1:I193"/>
   <sheetViews>
     <sheetView topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="F184" sqref="F184"/>
+      <selection activeCell="F183" sqref="F183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -53780,7 +53607,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>889.4</v>
+        <v>1889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -53796,7 +53623,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>1337.4</v>
+        <v>2337.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -53812,7 +53639,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>2226.8</v>
+        <v>4226.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -53911,7 +53738,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -53931,11 +53758,11 @@
     <row r="12" ht="24.75" customHeight="1" spans="1:9">
       <c r="A12" s="95"/>
       <c r="B12" s="96" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C12" s="96"/>
       <c r="D12" s="97" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E12" s="97"/>
       <c r="F12" s="7">
@@ -54085,7 +53912,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -54259,7 +54086,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -55659,7 +55486,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!E190")</f>
-        <v>1169.4</v>
+        <v>2169.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -55685,7 +55512,7 @@
       <c r="A118" s="62"/>
       <c r="B118" s="63"/>
       <c r="C118" s="109" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D118" s="109"/>
       <c r="E118" s="98">
@@ -55830,7 +55657,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="100" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D129" s="100"/>
       <c r="E129" s="98">
@@ -55845,7 +55672,7 @@
       <c r="A130" s="62"/>
       <c r="B130" s="63"/>
       <c r="C130" s="100" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D130" s="100"/>
       <c r="E130" s="98">
@@ -55933,7 +55760,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>1238.4</v>
+        <v>2238.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -56025,7 +55852,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>1238.4</v>
+        <v>2238.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -56051,7 +55878,7 @@
       <c r="A145" s="62"/>
       <c r="B145" s="63"/>
       <c r="C145" s="109" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D145" s="109"/>
       <c r="E145" s="98">
@@ -56079,7 +55906,7 @@
       <c r="A147" s="62"/>
       <c r="B147" s="63"/>
       <c r="C147" s="64" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D147" s="65"/>
       <c r="E147" s="36">
@@ -56120,7 +55947,7 @@
       <c r="A150" s="62"/>
       <c r="B150" s="63"/>
       <c r="C150" s="64" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D150" s="65"/>
       <c r="E150" s="36">
@@ -56200,7 +56027,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="100" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D156" s="100"/>
       <c r="E156" s="98">
@@ -56215,7 +56042,7 @@
       <c r="A157" s="62"/>
       <c r="B157" s="63"/>
       <c r="C157" s="100" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D157" s="100"/>
       <c r="E157" s="98">
@@ -56303,7 +56130,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>1351.4</v>
+        <v>2351.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -56395,7 +56222,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>1351.4</v>
+        <v>2351.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -56486,7 +56313,7 @@
       <c r="A177" s="62"/>
       <c r="B177" s="63"/>
       <c r="C177" s="64" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D177" s="65"/>
       <c r="E177" s="36">
@@ -56566,7 +56393,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="100" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D183" s="100"/>
       <c r="E183" s="98">
@@ -56581,7 +56408,7 @@
       <c r="A184" s="62"/>
       <c r="B184" s="63"/>
       <c r="C184" s="100" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="98">
@@ -56669,7 +56496,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>1337.4</v>
+        <v>2337.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -56711,23 +56538,6 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
-  <protectedRanges>
-    <protectedRange sqref="A10:G15" name="R1"/>
-    <protectedRange sqref="A22:G27" name="R2"/>
-    <protectedRange sqref="A34:G39" name="R3"/>
-    <protectedRange sqref="A46:C46 C47:C54" name="F1"/>
-    <protectedRange sqref="C56:C65" name="F2"/>
-    <protectedRange sqref="C67:C74" name="F3"/>
-    <protectedRange sqref="C76:C84" name="F4"/>
-    <protectedRange sqref="C86:C94" name="F5"/>
-    <protectedRange sqref="C117:E134" name="E1"/>
-    <protectedRange sqref="C144:E161" name="E2"/>
-    <protectedRange sqref="C171:E188" name="E3"/>
-    <protectedRange sqref="A56:B56" name="F2_1"/>
-    <protectedRange sqref="A67:B67" name="F3_1"/>
-    <protectedRange sqref="A76:B76" name="F4_1"/>
-    <protectedRange sqref="A86:B86" name="F5_1"/>
-  </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C2:G2"/>
@@ -57230,7 +57040,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>889.4</v>
+        <v>1889.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -57246,7 +57056,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>6082.4</v>
+        <v>7082.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -57262,7 +57072,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>6971.8</v>
+        <v>8971.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -57361,7 +57171,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -57535,7 +57345,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -57705,7 +57515,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -59109,7 +58919,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!E190")</f>
-        <v>1337.4</v>
+        <v>2337.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -59278,7 +59088,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="100" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D129" s="100"/>
       <c r="E129" s="98">
@@ -59381,7 +59191,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>2900.4</v>
+        <v>3900.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -59473,7 +59283,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>2900.4</v>
+        <v>3900.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -59642,7 +59452,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="100" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D156" s="100"/>
       <c r="E156" s="102">
@@ -59745,7 +59555,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>4519.4</v>
+        <v>5519.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -59837,7 +59647,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>4519.4</v>
+        <v>5519.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -60006,7 +59816,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="100" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D183" s="100"/>
       <c r="E183" s="98">
@@ -60109,7 +59919,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>6082.4</v>
+        <v>7082.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -60151,23 +59961,6 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
-  <protectedRanges>
-    <protectedRange sqref="A10:G15" name="R1"/>
-    <protectedRange sqref="A22:G27" name="R2"/>
-    <protectedRange sqref="A34:G39" name="R3"/>
-    <protectedRange sqref="A46:C46 C47:C54" name="F1"/>
-    <protectedRange sqref="C56:C65" name="F2"/>
-    <protectedRange sqref="C67:C74" name="F3"/>
-    <protectedRange sqref="C76:C84" name="F4"/>
-    <protectedRange sqref="C86:C94" name="F5"/>
-    <protectedRange sqref="C117:E134" name="E1"/>
-    <protectedRange sqref="C144:E161" name="E2"/>
-    <protectedRange sqref="C171:E188" name="E3"/>
-    <protectedRange sqref="A56:B56" name="F2_1"/>
-    <protectedRange sqref="A67:B67" name="F3_1"/>
-    <protectedRange sqref="A76:B76" name="F4_1"/>
-    <protectedRange sqref="A86:B86" name="F5_1"/>
-  </protectedRanges>
   <mergeCells count="174">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C2:G2"/>
@@ -60623,225 +60416,19 @@
   <rangeList sheetStid="1" master="" otherUserPermission="visible"/>
   <rangeList sheetStid="2" master="" otherUserPermission="visible"/>
   <rangeList sheetStid="4" master="" otherUserPermission="visible"/>
-  <rangeList sheetStid="5" master="" otherUserPermission="visible">
-    <arrUserId title="R1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5_1" rangeCreator="" othersAccessPermission="edit"/>
-  </rangeList>
-  <rangeList sheetStid="6" master="" otherUserPermission="visible">
-    <arrUserId title="R1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5_1" rangeCreator="" othersAccessPermission="edit"/>
-  </rangeList>
-  <rangeList sheetStid="7" master="" otherUserPermission="visible">
-    <arrUserId title="R1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5_1" rangeCreator="" othersAccessPermission="edit"/>
-  </rangeList>
-  <rangeList sheetStid="8" master="" otherUserPermission="visible">
-    <arrUserId title="R1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5_1" rangeCreator="" othersAccessPermission="edit"/>
-  </rangeList>
-  <rangeList sheetStid="9" master="" otherUserPermission="visible">
-    <arrUserId title="R1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5_1" rangeCreator="" othersAccessPermission="edit"/>
-  </rangeList>
-  <rangeList sheetStid="10" master="" otherUserPermission="visible">
-    <arrUserId title="R1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5_1" rangeCreator="" othersAccessPermission="edit"/>
-  </rangeList>
-  <rangeList sheetStid="11" master="" otherUserPermission="visible">
-    <arrUserId title="R1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5_1" rangeCreator="" othersAccessPermission="edit"/>
-  </rangeList>
-  <rangeList sheetStid="12" master="" otherUserPermission="visible">
-    <arrUserId title="R1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5_1" rangeCreator="" othersAccessPermission="edit"/>
-  </rangeList>
-  <rangeList sheetStid="13" master="" otherUserPermission="visible">
-    <arrUserId title="R1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5_1" rangeCreator="" othersAccessPermission="edit"/>
-  </rangeList>
-  <rangeList sheetStid="14" master="" otherUserPermission="visible">
-    <arrUserId title="R1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5_1" rangeCreator="" othersAccessPermission="edit"/>
-  </rangeList>
-  <rangeList sheetStid="15" master="" otherUserPermission="visible">
-    <arrUserId title="R1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5_1" rangeCreator="" othersAccessPermission="edit"/>
-  </rangeList>
-  <rangeList sheetStid="16" master="" otherUserPermission="visible">
-    <arrUserId title="R1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2_2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3_1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4_2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5_1" rangeCreator="" othersAccessPermission="edit"/>
-  </rangeList>
-  <rangeList sheetStid="17" master="" otherUserPermission="visible">
-    <arrUserId title="R1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="R3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F3" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F4" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="F5" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E1" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E2" rangeCreator="" othersAccessPermission="edit"/>
-    <arrUserId title="E3" rangeCreator="" othersAccessPermission="edit"/>
-  </rangeList>
+  <rangeList sheetStid="5" master="" otherUserPermission="visible"/>
+  <rangeList sheetStid="6" master="" otherUserPermission="visible"/>
+  <rangeList sheetStid="7" master="" otherUserPermission="visible"/>
+  <rangeList sheetStid="8" master="" otherUserPermission="visible"/>
+  <rangeList sheetStid="9" master="" otherUserPermission="visible"/>
+  <rangeList sheetStid="10" master="" otherUserPermission="visible"/>
+  <rangeList sheetStid="11" master="" otherUserPermission="visible"/>
+  <rangeList sheetStid="12" master="" otherUserPermission="visible"/>
+  <rangeList sheetStid="13" master="" otherUserPermission="visible"/>
+  <rangeList sheetStid="14" master="" otherUserPermission="visible"/>
+  <rangeList sheetStid="15" master="" otherUserPermission="visible"/>
+  <rangeList sheetStid="16" master="" otherUserPermission="visible"/>
+  <rangeList sheetStid="17" master="" otherUserPermission="visible"/>
 </allowEditUser>
 </file>
 

</xml_diff>

<commit_message>
docs: 1. Update buying printer expenses.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560"/>
+    <workbookView windowHeight="21560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="295">
   <si>
     <t>Income Forecast</t>
   </si>
@@ -1158,6 +1158,9 @@
 - Ice Cream $30
 - Fanta soft drinks $16
 - Best Mart 360 pepsi ~ $20</t>
+  </si>
+  <si>
+    <t>3. Brought a Brother Printer For $999</t>
   </si>
   <si>
     <t>30th April 2025</t>
@@ -3871,7 +3874,7 @@
   <sheetPr/>
   <dimension ref="A1:Z62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
@@ -5668,7 +5671,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1889.4</v>
+        <v>890.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -5684,7 +5687,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>11933.4</v>
+        <v>10934.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -5700,7 +5703,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>13822.8</v>
+        <v>11824.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -5799,7 +5802,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -5973,7 +5976,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -6147,7 +6150,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -7551,7 +7554,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!E190")</f>
-        <v>7082.4</v>
+        <v>6083.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -7720,7 +7723,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -7823,7 +7826,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>8751.4</v>
+        <v>7752.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -7915,7 +7918,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>8751.4</v>
+        <v>7752.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -8084,7 +8087,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D156" s="103"/>
       <c r="E156" s="101">
@@ -8187,7 +8190,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>10264.4</v>
+        <v>9265.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -8279,7 +8282,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>10264.4</v>
+        <v>9265.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -8448,7 +8451,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -8551,7 +8554,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>11933.4</v>
+        <v>10934.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -9081,7 +9084,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1889.4</v>
+        <v>890.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -9097,7 +9100,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>16678.4</v>
+        <v>15679.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -9113,7 +9116,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>18567.8</v>
+        <v>16569.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -9212,7 +9215,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -9386,7 +9389,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -9560,7 +9563,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -10964,7 +10967,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!E190")</f>
-        <v>11933.4</v>
+        <v>10934.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -11133,7 +11136,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -11236,7 +11239,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>13496.4</v>
+        <v>12497.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -11328,7 +11331,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>13496.4</v>
+        <v>12497.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -11497,7 +11500,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
@@ -11600,7 +11603,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>15115.4</v>
+        <v>14116.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -11692,7 +11695,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>15115.4</v>
+        <v>14116.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -11861,7 +11864,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D183" s="103"/>
       <c r="E183" s="101">
@@ -11964,7 +11967,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>16678.4</v>
+        <v>15679.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -12495,7 +12498,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1889.4</v>
+        <v>890.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -12511,7 +12514,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>21529.4</v>
+        <v>20530.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -12527,7 +12530,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>23418.8</v>
+        <v>21420.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -12626,7 +12629,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -12800,7 +12803,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -12974,7 +12977,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -14378,7 +14381,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!E190")</f>
-        <v>16678.4</v>
+        <v>15679.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -14547,7 +14550,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -14650,7 +14653,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>18347.4</v>
+        <v>17348.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -14742,7 +14745,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>18347.4</v>
+        <v>17348.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -14911,7 +14914,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D156" s="103"/>
       <c r="E156" s="101">
@@ -15014,7 +15017,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>19860.4</v>
+        <v>18861.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -15106,7 +15109,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>19860.4</v>
+        <v>18861.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -15275,7 +15278,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -15378,7 +15381,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>21529.4</v>
+        <v>20530.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -15907,7 +15910,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1889.4</v>
+        <v>890.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -15923,7 +15926,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>26274.4</v>
+        <v>25275.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -15939,7 +15942,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>28163.8</v>
+        <v>26165.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -16038,7 +16041,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -16212,7 +16215,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -16386,7 +16389,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -17790,7 +17793,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!E190")</f>
-        <v>21529.4</v>
+        <v>20530.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -17959,7 +17962,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -18062,7 +18065,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>23092.4</v>
+        <v>22093.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -18154,7 +18157,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>23092.4</v>
+        <v>22093.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -18323,7 +18326,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
@@ -18426,7 +18429,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>24711.4</v>
+        <v>23712.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -18518,7 +18521,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>24711.4</v>
+        <v>23712.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -18687,7 +18690,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -18790,7 +18793,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>26274.4</v>
+        <v>25275.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -19321,7 +19324,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1889.4</v>
+        <v>890.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -19337,7 +19340,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>31125.4</v>
+        <v>30126.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -19353,7 +19356,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>33014.8</v>
+        <v>31016.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -19452,7 +19455,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -19626,7 +19629,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -19800,7 +19803,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -21204,7 +21207,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!E190")</f>
-        <v>26274.4</v>
+        <v>25275.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -21373,7 +21376,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -21476,7 +21479,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>27943.4</v>
+        <v>26944.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -21568,7 +21571,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>27943.4</v>
+        <v>26944.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -21737,7 +21740,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
@@ -21840,7 +21843,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>29456.4</v>
+        <v>28457.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -21932,7 +21935,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>29456.4</v>
+        <v>28457.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -22101,7 +22104,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -22204,7 +22207,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>31125.4</v>
+        <v>30126.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -22733,7 +22736,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1889.4</v>
+        <v>890.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -22749,7 +22752,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -22765,7 +22768,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>37759.8</v>
+        <v>35761.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -22864,7 +22867,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -23038,7 +23041,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -23212,7 +23215,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -24616,7 +24619,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!E190")</f>
-        <v>31125.4</v>
+        <v>30126.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -24785,7 +24788,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -24888,7 +24891,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>32688.4</v>
+        <v>31689.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -24980,7 +24983,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>32688.4</v>
+        <v>31689.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -25149,7 +25152,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
@@ -25252,7 +25255,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>34307.4</v>
+        <v>33308.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -25344,7 +25347,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>34307.4</v>
+        <v>33308.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -25513,7 +25516,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -25616,7 +25619,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -26146,7 +26149,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1889.4</v>
+        <v>890.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -26162,7 +26165,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -26178,7 +26181,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>37759.8</v>
+        <v>35761.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -27987,7 +27990,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!E190")</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -28255,7 +28258,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -28347,7 +28350,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -28615,7 +28618,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -28707,7 +28710,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -28975,7 +28978,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -29452,7 +29455,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1889.4</v>
+        <v>890.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -29468,7 +29471,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -29484,7 +29487,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>37759.8</v>
+        <v>35761.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -31062,7 +31065,7 @@
         <v>Bankruptcy Department / Bank</v>
       </c>
       <c r="B102" s="37" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C102" s="36" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C102")+SUM(E122+E149+E176)</f>
@@ -31292,7 +31295,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!E190")</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -31560,7 +31563,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -31652,7 +31655,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -31920,7 +31923,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -32012,7 +32015,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -32280,7 +32283,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -32759,7 +32762,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1889.4</v>
+        <v>890.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -32775,7 +32778,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -32791,7 +32794,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>37759.8</v>
+        <v>35761.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -34600,7 +34603,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!E190")</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -34868,7 +34871,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -34960,7 +34963,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -35228,7 +35231,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -35320,7 +35323,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -35588,7 +35591,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -36570,8 +36573,8 @@
   <sheetPr/>
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -36642,7 +36645,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="162">
-        <v>536</v>
+        <v>737.2</v>
       </c>
       <c r="D3" s="163" t="s">
         <v>33</v>
@@ -36676,7 +36679,7 @@
         <v>35</v>
       </c>
       <c r="C4" s="162">
-        <v>1260</v>
+        <v>60</v>
       </c>
       <c r="D4" s="164"/>
       <c r="E4" s="5" t="s">
@@ -36772,7 +36775,7 @@
         <v>38</v>
       </c>
       <c r="C7" s="162">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="D7" s="164"/>
       <c r="E7" s="5" t="s">
@@ -37013,7 +37016,7 @@
       </c>
       <c r="J14" s="203">
         <f ca="1">'January 2025 - March 2025'!E190</f>
-        <v>1889.4</v>
+        <v>890.400000000001</v>
       </c>
       <c r="M14" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,33),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+33),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,36)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+35),"dd mmmm yyyy"))</f>
@@ -37045,7 +37048,7 @@
       </c>
       <c r="J15" s="203">
         <f ca="1">'April 2025 - June 2025'!E136</f>
-        <v>1952.4</v>
+        <v>953.400000000001</v>
       </c>
       <c r="M15" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,36),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+36),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,39)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+38),"dd mmmm yyyy"))</f>
@@ -37063,7 +37066,7 @@
       </c>
       <c r="C16" s="168">
         <f>SUM(C3:C15)</f>
-        <v>1889.4</v>
+        <v>890.4</v>
       </c>
       <c r="D16" s="169"/>
       <c r="E16" s="167" t="s">
@@ -37079,7 +37082,7 @@
       </c>
       <c r="J16" s="203">
         <f ca="1">'April 2025 - June 2025'!E163</f>
-        <v>2006.4</v>
+        <v>1007.4</v>
       </c>
       <c r="M16" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+39),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
@@ -37097,7 +37100,7 @@
       </c>
       <c r="J17" s="203">
         <f ca="1">'April 2025 - June 2025'!E190</f>
-        <v>2169.4</v>
+        <v>1170.4</v>
       </c>
       <c r="M17" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+42),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
@@ -37115,7 +37118,7 @@
       </c>
       <c r="J18" s="203">
         <f ca="1">'July 2025 - September 2025'!E136</f>
-        <v>2238.4</v>
+        <v>1239.4</v>
       </c>
       <c r="M18" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+45),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
@@ -37133,7 +37136,7 @@
       </c>
       <c r="J19" s="203">
         <f ca="1">'July 2025 - September 2025'!E163</f>
-        <v>2351.4</v>
+        <v>1352.4</v>
       </c>
     </row>
     <row r="20" ht="35.25" customHeight="1" spans="9:10">
@@ -37143,7 +37146,7 @@
       </c>
       <c r="J20" s="203">
         <f ca="1">'July 2025 - September 2025'!E190</f>
-        <v>2337.4</v>
+        <v>1338.4</v>
       </c>
     </row>
     <row r="21" ht="35.25" customHeight="1" spans="9:10">
@@ -37153,7 +37156,7 @@
       </c>
       <c r="J21" s="203">
         <f ca="1">'October 2025 - December 2025'!E136</f>
-        <v>3900.4</v>
+        <v>2901.4</v>
       </c>
     </row>
     <row r="22" ht="24.75" customHeight="1" spans="1:10">
@@ -37173,7 +37176,7 @@
       </c>
       <c r="J22" s="203">
         <f ca="1">'October 2025 - December 2025'!E163</f>
-        <v>5519.4</v>
+        <v>4520.4</v>
       </c>
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:10">
@@ -37198,7 +37201,7 @@
       </c>
       <c r="J23" s="203">
         <f ca="1">'October 2025 - December 2025'!E190</f>
-        <v>7082.4</v>
+        <v>6083.4</v>
       </c>
     </row>
     <row r="24" ht="52.5" customHeight="1" spans="1:10">
@@ -37223,7 +37226,7 @@
       </c>
       <c r="J24" s="203">
         <f ca="1">'January 2026 - March 2026'!E136</f>
-        <v>8751.4</v>
+        <v>7752.4</v>
       </c>
     </row>
     <row r="25" ht="30" customHeight="1" spans="1:10">
@@ -37242,7 +37245,7 @@
       </c>
       <c r="J25" s="203">
         <f ca="1">'January 2026 - March 2026'!E163</f>
-        <v>10264.4</v>
+        <v>9265.4</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1" spans="1:10">
@@ -37261,7 +37264,7 @@
       </c>
       <c r="J26" s="203">
         <f ca="1">'January 2026 - March 2026'!E190</f>
-        <v>11933.4</v>
+        <v>10934.4</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1" spans="1:10">
@@ -37280,7 +37283,7 @@
       </c>
       <c r="J27" s="203">
         <f ca="1">'April 2026 - June 2026'!E136</f>
-        <v>13496.4</v>
+        <v>12497.4</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:10">
@@ -37299,7 +37302,7 @@
       </c>
       <c r="J28" s="203">
         <f ca="1">'April 2026 - June 2026'!E163</f>
-        <v>15115.4</v>
+        <v>14116.4</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:10">
@@ -37318,7 +37321,7 @@
       </c>
       <c r="J29" s="199">
         <f ca="1">'April 2026 - June 2026'!E190</f>
-        <v>16678.4</v>
+        <v>15679.4</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1" spans="1:10">
@@ -37340,7 +37343,7 @@
       </c>
       <c r="J30" s="205">
         <f ca="1">'July 2026 - September 2026'!E136</f>
-        <v>18347.4</v>
+        <v>17348.4</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1" spans="9:10">
@@ -37350,7 +37353,7 @@
       </c>
       <c r="J31" s="203">
         <f ca="1">'July 2026 - September 2026'!E163</f>
-        <v>19860.4</v>
+        <v>18861.4</v>
       </c>
     </row>
     <row r="32" ht="27.75" customHeight="1" spans="9:10">
@@ -37360,7 +37363,7 @@
       </c>
       <c r="J32" s="203">
         <f ca="1">'July 2026 - September 2026'!E190</f>
-        <v>21529.4</v>
+        <v>20530.4</v>
       </c>
     </row>
     <row r="33" ht="30" customHeight="1" spans="9:10">
@@ -37370,7 +37373,7 @@
       </c>
       <c r="J33" s="203">
         <f ca="1">'October 2026 - December 2026'!E136</f>
-        <v>23092.4</v>
+        <v>22093.4</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1" spans="1:10">
@@ -37390,7 +37393,7 @@
       </c>
       <c r="J34" s="203">
         <f ca="1">'October 2026 - December 2026'!E163</f>
-        <v>24711.4</v>
+        <v>23712.4</v>
       </c>
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:10">
@@ -37415,7 +37418,7 @@
       </c>
       <c r="J35" s="203">
         <f ca="1">'October 2026 - December 2026'!E190</f>
-        <v>26274.4</v>
+        <v>25275.4</v>
       </c>
     </row>
     <row r="36" ht="54.75" customHeight="1" spans="1:10">
@@ -37440,7 +37443,7 @@
       </c>
       <c r="J36" s="203">
         <f ca="1">'January 2027 - March 2027'!E136</f>
-        <v>27943.4</v>
+        <v>26944.4</v>
       </c>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:10">
@@ -37465,7 +37468,7 @@
       </c>
       <c r="J37" s="203">
         <f ca="1">'January 2027 - March 2027'!E163</f>
-        <v>29456.4</v>
+        <v>28457.4</v>
       </c>
     </row>
     <row r="38" ht="20.25" customHeight="1" spans="1:10">
@@ -37490,7 +37493,7 @@
       </c>
       <c r="J38" s="203">
         <f ca="1">'January 2027 - March 2027'!E190</f>
-        <v>31125.4</v>
+        <v>30126.4</v>
       </c>
     </row>
     <row r="39" ht="24.75" customHeight="1" spans="1:10">
@@ -37509,7 +37512,7 @@
       </c>
       <c r="J39" s="203">
         <f ca="1">'April 2027 - June 2027'!E136</f>
-        <v>32688.4</v>
+        <v>31689.4</v>
       </c>
     </row>
     <row r="40" ht="24.75" customHeight="1" spans="1:10">
@@ -37528,7 +37531,7 @@
       </c>
       <c r="J40" s="203">
         <f ca="1">'April 2027 - June 2027'!E163</f>
-        <v>34307.4</v>
+        <v>33308.4</v>
       </c>
     </row>
     <row r="41" ht="24.75" customHeight="1" spans="1:10">
@@ -37547,7 +37550,7 @@
       </c>
       <c r="J41" s="203">
         <f ca="1">'April 2027 - June 2027'!E190</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:10">
@@ -37569,7 +37572,7 @@
       </c>
       <c r="J42" s="203">
         <f ca="1">Forecast_14!E136</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="9:10">
@@ -37579,7 +37582,7 @@
       </c>
       <c r="J43" s="203">
         <f ca="1">Forecast_14!E163</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
     </row>
     <row r="44" ht="24.75" customHeight="1" spans="9:10">
@@ -37589,7 +37592,7 @@
       </c>
       <c r="J44" s="203">
         <f ca="1">Forecast_14!E190</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
     </row>
     <row r="45" ht="24.75" customHeight="1" spans="9:10">
@@ -37599,7 +37602,7 @@
       </c>
       <c r="J45" s="203">
         <f ca="1">Forecast_15!E136</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
     </row>
     <row r="46" ht="24.75" customHeight="1" spans="1:10">
@@ -37619,7 +37622,7 @@
       </c>
       <c r="J46" s="203">
         <f ca="1">Forecast_15!E163</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
     </row>
     <row r="47" ht="24.75" customHeight="1" spans="1:10">
@@ -37644,7 +37647,7 @@
       </c>
       <c r="J47" s="203">
         <f ca="1">Forecast_15!E190</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
     </row>
     <row r="48" ht="24.75" customHeight="1" spans="1:10">
@@ -37669,7 +37672,7 @@
       </c>
       <c r="J48" s="203">
         <f ca="1">Forecast_16!E136</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
     </row>
     <row r="49" ht="24.75" customHeight="1" spans="1:10">
@@ -37694,7 +37697,7 @@
       </c>
       <c r="J49" s="203">
         <f ca="1">Forecast_16!E163</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
     </row>
     <row r="50" ht="24.75" customHeight="1" spans="1:10">
@@ -37719,7 +37722,7 @@
       </c>
       <c r="J50" s="199">
         <f ca="1">Forecast_16!E190</f>
-        <v>35870.4</v>
+        <v>34871.4</v>
       </c>
     </row>
     <row r="51" ht="41" customHeight="1" spans="1:7">
@@ -39664,7 +39667,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1889.4</v>
+        <v>890.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -39692,7 +39695,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>2392.11</v>
+        <v>1393.11</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -43117,7 +43120,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1889.4</v>
+        <v>890.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -43145,7 +43148,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>2062.74</v>
+        <v>1063.74</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -46632,8 +46635,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="G157" sqref="G157"/>
+    <sheetView topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="F185" sqref="F185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -46667,7 +46670,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1889.4</v>
+        <v>890.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -46683,7 +46686,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>1889.4</v>
+        <v>890.400000000001</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -46699,7 +46702,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>3778.8</v>
+        <v>1780.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -49524,10 +49527,12 @@
     <row r="185" ht="24.75" customHeight="1" spans="1:9">
       <c r="A185" s="62"/>
       <c r="B185" s="63"/>
-      <c r="C185" s="64"/>
+      <c r="C185" s="64" t="s">
+        <v>244</v>
+      </c>
       <c r="D185" s="65"/>
       <c r="E185" s="86">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="F185" s="14"/>
       <c r="G185" s="14"/>
@@ -49598,7 +49603,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>1889.4</v>
+        <v>890.400000000001</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -50137,8 +50142,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A168" workbookViewId="0">
-      <selection activeCell="E188" sqref="E188"/>
+    <sheetView topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -50173,7 +50178,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1889.4</v>
+        <v>890.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -50189,7 +50194,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>2169.4</v>
+        <v>1170.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -50205,7 +50210,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>4058.8</v>
+        <v>2060.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -50321,7 +50326,7 @@
     </row>
     <row r="12" ht="24.75" customHeight="1" spans="1:9">
       <c r="A12" s="95" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B12" s="96" t="s">
         <v>66</v>
@@ -50341,11 +50346,11 @@
     <row r="13" ht="24.75" customHeight="1" spans="1:9">
       <c r="A13" s="95"/>
       <c r="B13" s="96" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C13" s="96"/>
       <c r="D13" s="97" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E13" s="97"/>
       <c r="F13" s="7">
@@ -50482,7 +50487,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -50506,7 +50511,7 @@
       </c>
       <c r="C24" s="110"/>
       <c r="D24" s="111" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E24" s="111"/>
       <c r="F24" s="112">
@@ -50656,7 +50661,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -52060,7 +52065,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!E190")</f>
-        <v>1889.4</v>
+        <v>890.400000000001</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -52086,7 +52091,7 @@
       <c r="A118" s="62"/>
       <c r="B118" s="63"/>
       <c r="C118" s="109" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D118" s="109"/>
       <c r="E118" s="98">
@@ -52231,7 +52236,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="100" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D129" s="109"/>
       <c r="E129" s="98">
@@ -52246,7 +52251,7 @@
       <c r="A130" s="62"/>
       <c r="B130" s="63"/>
       <c r="C130" s="113" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D130" s="114"/>
       <c r="E130" s="98">
@@ -52334,7 +52339,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>1952.4</v>
+        <v>953.400000000001</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -52426,7 +52431,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>1952.4</v>
+        <v>953.400000000001</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -52452,7 +52457,7 @@
       <c r="A145" s="62"/>
       <c r="B145" s="63"/>
       <c r="C145" s="109" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D145" s="109"/>
       <c r="E145" s="98">
@@ -52597,7 +52602,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="100" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D156" s="100"/>
       <c r="E156" s="98">
@@ -52612,7 +52617,7 @@
       <c r="A157" s="62"/>
       <c r="B157" s="63"/>
       <c r="C157" s="100" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D157" s="100"/>
       <c r="E157" s="98">
@@ -52700,7 +52705,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>2006.4</v>
+        <v>1007.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -52792,7 +52797,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>2006.4</v>
+        <v>1007.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -52818,7 +52823,7 @@
       <c r="A172" s="62"/>
       <c r="B172" s="63"/>
       <c r="C172" s="109" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D172" s="109"/>
       <c r="E172" s="98">
@@ -52963,7 +52968,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="100" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D183" s="100"/>
       <c r="E183" s="98">
@@ -52978,7 +52983,7 @@
       <c r="A184" s="62"/>
       <c r="B184" s="63"/>
       <c r="C184" s="100" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="98">
@@ -53066,7 +53071,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>2169.4</v>
+        <v>1170.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -53607,7 +53612,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1889.4</v>
+        <v>890.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -53623,7 +53628,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>2337.4</v>
+        <v>1338.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -53639,7 +53644,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>4226.8</v>
+        <v>2228.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -53738,7 +53743,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -53758,11 +53763,11 @@
     <row r="12" ht="24.75" customHeight="1" spans="1:9">
       <c r="A12" s="95"/>
       <c r="B12" s="96" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C12" s="96"/>
       <c r="D12" s="97" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E12" s="97"/>
       <c r="F12" s="7">
@@ -53912,7 +53917,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -54086,7 +54091,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -55486,7 +55491,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!E190")</f>
-        <v>2169.4</v>
+        <v>1170.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -55512,7 +55517,7 @@
       <c r="A118" s="62"/>
       <c r="B118" s="63"/>
       <c r="C118" s="109" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D118" s="109"/>
       <c r="E118" s="98">
@@ -55657,7 +55662,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="100" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D129" s="100"/>
       <c r="E129" s="98">
@@ -55672,7 +55677,7 @@
       <c r="A130" s="62"/>
       <c r="B130" s="63"/>
       <c r="C130" s="100" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D130" s="100"/>
       <c r="E130" s="98">
@@ -55760,7 +55765,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>2238.4</v>
+        <v>1239.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -55852,7 +55857,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>2238.4</v>
+        <v>1239.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -55878,7 +55883,7 @@
       <c r="A145" s="62"/>
       <c r="B145" s="63"/>
       <c r="C145" s="109" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D145" s="109"/>
       <c r="E145" s="98">
@@ -55906,7 +55911,7 @@
       <c r="A147" s="62"/>
       <c r="B147" s="63"/>
       <c r="C147" s="64" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D147" s="65"/>
       <c r="E147" s="36">
@@ -55947,7 +55952,7 @@
       <c r="A150" s="62"/>
       <c r="B150" s="63"/>
       <c r="C150" s="64" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D150" s="65"/>
       <c r="E150" s="36">
@@ -56027,7 +56032,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="100" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D156" s="100"/>
       <c r="E156" s="98">
@@ -56042,7 +56047,7 @@
       <c r="A157" s="62"/>
       <c r="B157" s="63"/>
       <c r="C157" s="100" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D157" s="100"/>
       <c r="E157" s="98">
@@ -56130,7 +56135,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>2351.4</v>
+        <v>1352.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -56222,7 +56227,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>2351.4</v>
+        <v>1352.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -56313,7 +56318,7 @@
       <c r="A177" s="62"/>
       <c r="B177" s="63"/>
       <c r="C177" s="64" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D177" s="65"/>
       <c r="E177" s="36">
@@ -56393,7 +56398,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="100" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D183" s="100"/>
       <c r="E183" s="98">
@@ -56408,7 +56413,7 @@
       <c r="A184" s="62"/>
       <c r="B184" s="63"/>
       <c r="C184" s="100" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="98">
@@ -56496,7 +56501,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>2337.4</v>
+        <v>1338.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -57040,7 +57045,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>1889.4</v>
+        <v>890.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -57056,7 +57061,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>7082.4</v>
+        <v>6083.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -57072,7 +57077,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>8971.8</v>
+        <v>6973.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -57171,7 +57176,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -57345,7 +57350,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -57515,7 +57520,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -58919,7 +58924,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!E190")</f>
-        <v>2337.4</v>
+        <v>1338.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -59088,7 +59093,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="100" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D129" s="100"/>
       <c r="E129" s="98">
@@ -59191,7 +59196,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>3900.4</v>
+        <v>2901.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -59283,7 +59288,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>3900.4</v>
+        <v>2901.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -59452,7 +59457,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="100" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D156" s="100"/>
       <c r="E156" s="102">
@@ -59555,7 +59560,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>5519.4</v>
+        <v>4520.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -59647,7 +59652,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>5519.4</v>
+        <v>4520.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -59816,7 +59821,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="100" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D183" s="100"/>
       <c r="E183" s="98">
@@ -59919,7 +59924,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>7082.4</v>
+        <v>6083.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>

</xml_diff>

<commit_message>
docs: 1. Expenses Updated.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560" firstSheet="4" activeTab="9"/>
+    <workbookView windowHeight="21560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -1163,7 +1163,11 @@
 - Best Mart 360 ~ $39.9
 - A1 Bakery ~ $34
 - U Mart Miggi Seasoning ~ $14.9
-- OK Store soft drinks ~ $22</t>
+- OK Store soft drinks ~ $22
+- Kwun Kee Food Store ~ $34
+- Trip to Eldery Center ~ $9.5
+- Market Vegetable 1 Kg ~ $12
+- U Mart Instant Noodles ~ $9.9</t>
   </si>
   <si>
     <t>3. Brought a Brother Printer For $999</t>
@@ -5654,7 +5658,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+    <sheetView topLeftCell="A163" workbookViewId="0">
       <selection activeCell="F157" sqref="F157"/>
     </sheetView>
   </sheetViews>
@@ -5689,7 +5693,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>754.1</v>
+        <v>688.7</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -5705,7 +5709,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>6294.1</v>
+        <v>6228.7</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -5721,7 +5725,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>7048.2</v>
+        <v>6917.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -7572,7 +7576,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!E190")</f>
-        <v>3490.1</v>
+        <v>3424.7</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -7844,7 +7848,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>4575.1</v>
+        <v>4509.7</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -7936,7 +7940,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>4575.1</v>
+        <v>4509.7</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -8208,7 +8212,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>5209.1</v>
+        <v>5143.7</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -8300,7 +8304,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>5209.1</v>
+        <v>5143.7</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -8572,7 +8576,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>6294.1</v>
+        <v>6228.7</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -9102,7 +9106,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>754.1</v>
+        <v>688.7</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -9118,7 +9122,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>8807.1</v>
+        <v>8741.7</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -9134,7 +9138,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>9561.2</v>
+        <v>9430.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -10985,7 +10989,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!E190")</f>
-        <v>6294.1</v>
+        <v>6228.7</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -11257,7 +11261,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>7088.1</v>
+        <v>7022.7</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -11349,7 +11353,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>7088.1</v>
+        <v>7022.7</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -11621,7 +11625,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>8013.1</v>
+        <v>7947.7</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -11713,7 +11717,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>8013.1</v>
+        <v>7947.7</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -11985,7 +11989,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>8807.1</v>
+        <v>8741.7</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -12516,7 +12520,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>754.1</v>
+        <v>688.7</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -12532,7 +12536,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>11611.1</v>
+        <v>11545.7</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -12548,7 +12552,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>12365.2</v>
+        <v>12234.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -14399,7 +14403,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!E190")</f>
-        <v>8807.1</v>
+        <v>8741.7</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -14671,7 +14675,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>9892.1</v>
+        <v>9826.7</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -14763,7 +14767,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>9892.1</v>
+        <v>9826.7</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -15035,7 +15039,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>10526.1</v>
+        <v>10460.7</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -15127,7 +15131,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>10526.1</v>
+        <v>10460.7</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -15399,7 +15403,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>11611.1</v>
+        <v>11545.7</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -15928,7 +15932,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>754.1</v>
+        <v>688.7</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -15944,7 +15948,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>14124.1</v>
+        <v>14058.7</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -15960,7 +15964,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>14878.2</v>
+        <v>14747.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -17811,7 +17815,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!E190")</f>
-        <v>11611.1</v>
+        <v>11545.7</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -18083,7 +18087,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>12405.1</v>
+        <v>12339.7</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -18175,7 +18179,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>12405.1</v>
+        <v>12339.7</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -18447,7 +18451,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>13330.1</v>
+        <v>13264.7</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -18539,7 +18543,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>13330.1</v>
+        <v>13264.7</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -18811,7 +18815,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>14124.1</v>
+        <v>14058.7</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -19342,7 +19346,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>754.1</v>
+        <v>688.7</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -19358,7 +19362,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>16928.1</v>
+        <v>16862.7</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -19374,7 +19378,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>17682.2</v>
+        <v>17551.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -21225,7 +21229,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!E190")</f>
-        <v>14124.1</v>
+        <v>14058.7</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -21497,7 +21501,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>15209.1</v>
+        <v>15143.7</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -21589,7 +21593,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>15209.1</v>
+        <v>15143.7</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -21861,7 +21865,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>15843.1</v>
+        <v>15777.7</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -21953,7 +21957,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>15843.1</v>
+        <v>15777.7</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -22225,7 +22229,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>16928.1</v>
+        <v>16862.7</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -22720,7 +22724,7 @@
   <sheetPr/>
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView topLeftCell="A164" workbookViewId="0">
+    <sheetView topLeftCell="A162" workbookViewId="0">
       <selection activeCell="F184" sqref="F184"/>
     </sheetView>
   </sheetViews>
@@ -22754,7 +22758,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>754.1</v>
+        <v>688.7</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -22770,7 +22774,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -22786,7 +22790,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>20195.2</v>
+        <v>20064.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -24637,7 +24641,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!E190")</f>
-        <v>16928.1</v>
+        <v>16862.7</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -24909,7 +24913,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>17722.1</v>
+        <v>17656.7</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -25001,7 +25005,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>17722.1</v>
+        <v>17656.7</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -25273,7 +25277,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>18647.1</v>
+        <v>18581.7</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -25365,7 +25369,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>18647.1</v>
+        <v>18581.7</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -25637,7 +25641,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -26167,7 +26171,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>754.1</v>
+        <v>688.7</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -26183,7 +26187,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -26199,7 +26203,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>20195.2</v>
+        <v>20064.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -28008,7 +28012,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!E190")</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -28276,7 +28280,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -28368,7 +28372,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -28636,7 +28640,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -28728,7 +28732,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -28996,7 +29000,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -29473,7 +29477,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>754.1</v>
+        <v>688.7</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -29489,7 +29493,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -29505,7 +29509,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>20195.2</v>
+        <v>20064.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -31313,7 +31317,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!E190")</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -31581,7 +31585,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -31673,7 +31677,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -31941,7 +31945,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -32033,7 +32037,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -32301,7 +32305,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -32780,7 +32784,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>754.1</v>
+        <v>688.7</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -32796,7 +32800,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -32812,7 +32816,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>20195.2</v>
+        <v>20064.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -34621,7 +34625,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!E190")</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -34889,7 +34893,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -34981,7 +34985,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -35249,7 +35253,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -35341,7 +35345,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -35609,7 +35613,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -36591,8 +36595,8 @@
   <sheetPr/>
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16:I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -36663,7 +36667,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="162">
-        <v>626.4</v>
+        <v>526.4</v>
       </c>
       <c r="D3" s="163" t="s">
         <v>33</v>
@@ -36672,7 +36676,7 @@
         <v>34</v>
       </c>
       <c r="F3" s="190">
-        <v>648.4</v>
+        <v>626.4</v>
       </c>
       <c r="I3" s="198" t="str">
         <f>TEXT(Main!B3,"dd mmmm yyyy")&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,1)-1,"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)*1,"dd mmmm yyyy"))</f>
@@ -36697,7 +36701,7 @@
         <v>35</v>
       </c>
       <c r="C4" s="162">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D4" s="164"/>
       <c r="E4" s="5" t="s">
@@ -36922,7 +36926,7 @@
         <v>42</v>
       </c>
       <c r="C11" s="162">
-        <v>7.3</v>
+        <v>11.4</v>
       </c>
       <c r="D11" s="164"/>
       <c r="E11" s="5" t="s">
@@ -37019,7 +37023,7 @@
         <v>45</v>
       </c>
       <c r="C14" s="162">
-        <v>43.4</v>
+        <v>33.9</v>
       </c>
       <c r="D14" s="164"/>
       <c r="E14" s="192" t="s">
@@ -37034,7 +37038,7 @@
       </c>
       <c r="J14" s="203">
         <f ca="1">'January 2025 - March 2025'!E190</f>
-        <v>754.100000000001</v>
+        <v>688.700000000001</v>
       </c>
       <c r="M14" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,33),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+33),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,36)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+35),"dd mmmm yyyy"))</f>
@@ -37066,7 +37070,7 @@
       </c>
       <c r="J15" s="203">
         <f ca="1">'April 2025 - June 2025'!E136</f>
-        <v>1733.1</v>
+        <v>1667.7</v>
       </c>
       <c r="M15" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,36),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+36),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,39)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+38),"dd mmmm yyyy"))</f>
@@ -37084,7 +37088,7 @@
       </c>
       <c r="C16" s="168">
         <f>SUM(C3:C15)</f>
-        <v>754.1</v>
+        <v>688.7</v>
       </c>
       <c r="D16" s="169"/>
       <c r="E16" s="167" t="s">
@@ -37092,7 +37096,7 @@
       </c>
       <c r="F16" s="193">
         <f>SUM(F3:F15)</f>
-        <v>776.1</v>
+        <v>754.1</v>
       </c>
       <c r="I16" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,13),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*13)+13,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,14)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*14+13),"dd mmmm yyyy"))</f>
@@ -37100,7 +37104,7 @@
       </c>
       <c r="J16" s="203">
         <f ca="1">'April 2025 - June 2025'!E163</f>
-        <v>3803.1</v>
+        <v>3737.7</v>
       </c>
       <c r="M16" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+39),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
@@ -37118,7 +37122,7 @@
       </c>
       <c r="J17" s="203">
         <f ca="1">'April 2025 - June 2025'!E190</f>
-        <v>4782.1</v>
+        <v>4716.7</v>
       </c>
       <c r="M17" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+42),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
@@ -37136,7 +37140,7 @@
       </c>
       <c r="J18" s="203">
         <f ca="1">'July 2025 - September 2025'!E136</f>
-        <v>4651.1</v>
+        <v>4585.7</v>
       </c>
       <c r="M18" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+45),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
@@ -37154,7 +37158,7 @@
       </c>
       <c r="J19" s="203">
         <f ca="1">'July 2025 - September 2025'!E163</f>
-        <v>4580.1</v>
+        <v>4514.7</v>
       </c>
     </row>
     <row r="20" ht="35.25" customHeight="1" spans="9:10">
@@ -37164,7 +37168,7 @@
       </c>
       <c r="J20" s="203">
         <f ca="1">'July 2025 - September 2025'!E190</f>
-        <v>4665.1</v>
+        <v>4599.7</v>
       </c>
     </row>
     <row r="21" ht="35.25" customHeight="1" spans="9:10">
@@ -37174,7 +37178,7 @@
       </c>
       <c r="J21" s="203">
         <f ca="1">'October 2025 - December 2025'!E136</f>
-        <v>4644.1</v>
+        <v>4578.7</v>
       </c>
     </row>
     <row r="22" ht="24.75" customHeight="1" spans="1:10">
@@ -37194,7 +37198,7 @@
       </c>
       <c r="J22" s="203">
         <f ca="1">'October 2025 - December 2025'!E163</f>
-        <v>4179.1</v>
+        <v>4113.7</v>
       </c>
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:10">
@@ -37219,7 +37223,7 @@
       </c>
       <c r="J23" s="203">
         <f ca="1">'October 2025 - December 2025'!E190</f>
-        <v>3490.1</v>
+        <v>3424.7</v>
       </c>
     </row>
     <row r="24" ht="52.5" customHeight="1" spans="1:10">
@@ -37244,7 +37248,7 @@
       </c>
       <c r="J24" s="203">
         <f ca="1">'January 2026 - March 2026'!E136</f>
-        <v>4575.1</v>
+        <v>4509.7</v>
       </c>
     </row>
     <row r="25" ht="30" customHeight="1" spans="1:10">
@@ -37263,7 +37267,7 @@
       </c>
       <c r="J25" s="203">
         <f ca="1">'January 2026 - March 2026'!E163</f>
-        <v>5209.1</v>
+        <v>5143.7</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1" spans="1:10">
@@ -37282,7 +37286,7 @@
       </c>
       <c r="J26" s="203">
         <f ca="1">'January 2026 - March 2026'!E190</f>
-        <v>6294.1</v>
+        <v>6228.7</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1" spans="1:10">
@@ -37301,7 +37305,7 @@
       </c>
       <c r="J27" s="203">
         <f ca="1">'April 2026 - June 2026'!E136</f>
-        <v>7088.1</v>
+        <v>7022.7</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:10">
@@ -37320,7 +37324,7 @@
       </c>
       <c r="J28" s="203">
         <f ca="1">'April 2026 - June 2026'!E163</f>
-        <v>8013.1</v>
+        <v>7947.7</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:10">
@@ -37339,7 +37343,7 @@
       </c>
       <c r="J29" s="199">
         <f ca="1">'April 2026 - June 2026'!E190</f>
-        <v>8807.1</v>
+        <v>8741.7</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1" spans="1:10">
@@ -37361,7 +37365,7 @@
       </c>
       <c r="J30" s="206">
         <f ca="1">'July 2026 - September 2026'!E136</f>
-        <v>9892.1</v>
+        <v>9826.7</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1" spans="9:10">
@@ -37371,7 +37375,7 @@
       </c>
       <c r="J31" s="203">
         <f ca="1">'July 2026 - September 2026'!E163</f>
-        <v>10526.1</v>
+        <v>10460.7</v>
       </c>
     </row>
     <row r="32" ht="27.75" customHeight="1" spans="9:10">
@@ -37381,7 +37385,7 @@
       </c>
       <c r="J32" s="203">
         <f ca="1">'July 2026 - September 2026'!E190</f>
-        <v>11611.1</v>
+        <v>11545.7</v>
       </c>
     </row>
     <row r="33" ht="30" customHeight="1" spans="9:10">
@@ -37391,7 +37395,7 @@
       </c>
       <c r="J33" s="203">
         <f ca="1">'October 2026 - December 2026'!E136</f>
-        <v>12405.1</v>
+        <v>12339.7</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1" spans="1:10">
@@ -37411,7 +37415,7 @@
       </c>
       <c r="J34" s="203">
         <f ca="1">'October 2026 - December 2026'!E163</f>
-        <v>13330.1</v>
+        <v>13264.7</v>
       </c>
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:10">
@@ -37436,7 +37440,7 @@
       </c>
       <c r="J35" s="203">
         <f ca="1">'October 2026 - December 2026'!E190</f>
-        <v>14124.1</v>
+        <v>14058.7</v>
       </c>
     </row>
     <row r="36" ht="54.75" customHeight="1" spans="1:10">
@@ -37461,7 +37465,7 @@
       </c>
       <c r="J36" s="203">
         <f ca="1">'January 2027 - March 2027'!E136</f>
-        <v>15209.1</v>
+        <v>15143.7</v>
       </c>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:10">
@@ -37486,7 +37490,7 @@
       </c>
       <c r="J37" s="203">
         <f ca="1">'January 2027 - March 2027'!E163</f>
-        <v>15843.1</v>
+        <v>15777.7</v>
       </c>
     </row>
     <row r="38" ht="20.25" customHeight="1" spans="1:10">
@@ -37511,7 +37515,7 @@
       </c>
       <c r="J38" s="203">
         <f ca="1">'January 2027 - March 2027'!E190</f>
-        <v>16928.1</v>
+        <v>16862.7</v>
       </c>
     </row>
     <row r="39" ht="24.75" customHeight="1" spans="1:10">
@@ -37530,7 +37534,7 @@
       </c>
       <c r="J39" s="203">
         <f ca="1">'April 2027 - June 2027'!E136</f>
-        <v>17722.1</v>
+        <v>17656.7</v>
       </c>
     </row>
     <row r="40" ht="24.75" customHeight="1" spans="1:10">
@@ -37549,7 +37553,7 @@
       </c>
       <c r="J40" s="203">
         <f ca="1">'April 2027 - June 2027'!E163</f>
-        <v>18647.1</v>
+        <v>18581.7</v>
       </c>
     </row>
     <row r="41" ht="24.75" customHeight="1" spans="1:10">
@@ -37568,7 +37572,7 @@
       </c>
       <c r="J41" s="203">
         <f ca="1">'April 2027 - June 2027'!E190</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:10">
@@ -37590,7 +37594,7 @@
       </c>
       <c r="J42" s="203">
         <f ca="1">Forecast_14!E136</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="9:10">
@@ -37600,7 +37604,7 @@
       </c>
       <c r="J43" s="203">
         <f ca="1">Forecast_14!E163</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
     </row>
     <row r="44" ht="24.75" customHeight="1" spans="9:10">
@@ -37610,7 +37614,7 @@
       </c>
       <c r="J44" s="203">
         <f ca="1">Forecast_14!E190</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
     </row>
     <row r="45" ht="24.75" customHeight="1" spans="9:10">
@@ -37620,7 +37624,7 @@
       </c>
       <c r="J45" s="203">
         <f ca="1">Forecast_15!E136</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
     </row>
     <row r="46" ht="24.75" customHeight="1" spans="1:10">
@@ -37640,7 +37644,7 @@
       </c>
       <c r="J46" s="203">
         <f ca="1">Forecast_15!E163</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
     </row>
     <row r="47" ht="24.75" customHeight="1" spans="1:10">
@@ -37665,7 +37669,7 @@
       </c>
       <c r="J47" s="203">
         <f ca="1">Forecast_15!E190</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
     </row>
     <row r="48" ht="24.75" customHeight="1" spans="1:10">
@@ -37690,7 +37694,7 @@
       </c>
       <c r="J48" s="203">
         <f ca="1">Forecast_16!E136</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
     </row>
     <row r="49" ht="24.75" customHeight="1" spans="1:10">
@@ -37715,7 +37719,7 @@
       </c>
       <c r="J49" s="203">
         <f ca="1">Forecast_16!E163</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
     </row>
     <row r="50" ht="24.75" customHeight="1" spans="1:10">
@@ -37740,7 +37744,7 @@
       </c>
       <c r="J50" s="199">
         <f ca="1">Forecast_16!E190</f>
-        <v>19441.1</v>
+        <v>19375.7</v>
       </c>
     </row>
     <row r="51" ht="41" customHeight="1" spans="1:7">
@@ -39690,7 +39694,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>754.1</v>
+        <v>688.7</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -39718,7 +39722,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1256.81</v>
+        <v>1191.41</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -43143,7 +43147,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>754.1</v>
+        <v>688.7</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -43171,7 +43175,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>927.440000000001</v>
+        <v>862.040000000001</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -46658,8 +46662,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A173" workbookViewId="0">
-      <selection activeCell="G186" sqref="G186"/>
+    <sheetView topLeftCell="A176" workbookViewId="0">
+      <selection activeCell="F184" sqref="F184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -46693,7 +46697,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>754.1</v>
+        <v>688.7</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -46709,7 +46713,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>754.100000000001</v>
+        <v>688.700000000001</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -46725,7 +46729,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1508.2</v>
+        <v>1377.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -49532,7 +49536,7 @@
       <c r="H183" s="14"/>
       <c r="I183" s="47"/>
     </row>
-    <row r="184" ht="301" customHeight="1" spans="1:9">
+    <row r="184" ht="356" customHeight="1" spans="1:9">
       <c r="A184" s="62"/>
       <c r="B184" s="63"/>
       <c r="C184" s="100" t="s">
@@ -49540,7 +49544,7 @@
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="102">
-        <v>390.1</v>
+        <v>455.5</v>
       </c>
       <c r="F184" s="14"/>
       <c r="G184" s="14"/>
@@ -49626,7 +49630,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>754.100000000001</v>
+        <v>688.700000000001</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -49667,7 +49671,7 @@
       <c r="I193" s="40"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" objects="1"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="174">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C2:G2"/>
@@ -50201,7 +50205,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>754.1</v>
+        <v>688.7</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -50217,7 +50221,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>4782.1</v>
+        <v>4716.7</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -50233,7 +50237,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>5536.2</v>
+        <v>5405.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -52088,7 +52092,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!E190")</f>
-        <v>754.100000000001</v>
+        <v>688.700000000001</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -52362,7 +52366,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>1733.1</v>
+        <v>1667.7</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -52454,7 +52458,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>1733.1</v>
+        <v>1667.7</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -52728,7 +52732,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>3803.1</v>
+        <v>3737.7</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -52820,7 +52824,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>3803.1</v>
+        <v>3737.7</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -53094,7 +53098,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>4782.1</v>
+        <v>4716.7</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -53644,7 +53648,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>754.1</v>
+        <v>688.7</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -53660,7 +53664,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>4665.1</v>
+        <v>4599.7</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -53676,7 +53680,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>5419.2</v>
+        <v>5288.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -55523,7 +55527,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!E190")</f>
-        <v>4782.1</v>
+        <v>4716.7</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -55797,7 +55801,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>4651.1</v>
+        <v>4585.7</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -55889,7 +55893,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>4651.1</v>
+        <v>4585.7</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -56163,7 +56167,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>4580.1</v>
+        <v>4514.7</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -56255,7 +56259,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>4580.1</v>
+        <v>4514.7</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -56529,7 +56533,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>4665.1</v>
+        <v>4599.7</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -57073,7 +57077,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>754.1</v>
+        <v>688.7</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -57089,7 +57093,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>3490.1</v>
+        <v>3424.7</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -57105,7 +57109,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>4244.2</v>
+        <v>4113.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -58952,7 +58956,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!E190")</f>
-        <v>4665.1</v>
+        <v>4599.7</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -59226,7 +59230,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>4644.1</v>
+        <v>4578.7</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -59318,7 +59322,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>4644.1</v>
+        <v>4578.7</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -59594,7 +59598,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>4179.1</v>
+        <v>4113.7</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -59686,7 +59690,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>4179.1</v>
+        <v>4113.7</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -59962,7 +59966,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>3490.1</v>
+        <v>3424.7</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>

</xml_diff>

<commit_message>
docs: 1. Updated Expenses
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560" activeTab="5"/>
+    <workbookView windowHeight="21560" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -1113,7 +1113,7 @@
    include.)</t>
   </si>
   <si>
-    <t xml:space="preserve">2. Food And Transport Expenses
+    <t>2. Food And Transport Expenses
 - Chicken 6 piecies ~ $63
 - Tangerines 9 ones ~ $20
 - Milk 1 Litre 7 ~ $118.3
@@ -1133,7 +1133,7 @@
 - Ngan Lung Restaurant $55
 - Oat meal $19
 - Transport Fee to WTS Temple Mall $2
-- Transport Fee to Prince Edward And Back $4 </t>
+- Transport Fee to Prince Edward And Back $4</t>
   </si>
   <si>
     <t>3.. Food And Transport Expenses
@@ -1168,7 +1168,8 @@
 - Trip to Eldery Center ~ $9.5
 - Market Vegetable 1 Kg ~ $12
 - U Mart Instant Noodles ~ $9.9
-- Market Vegetable 1 Kg ~ $12</t>
+- Market Vegetable 1 Kg ~ $12
+- OK Store soft drinks ~ $21.4</t>
   </si>
   <si>
     <t>3. Brought a Brother Printer For $999</t>
@@ -5694,7 +5695,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>635.7</v>
+        <v>614.3</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -5710,7 +5711,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>6175.7</v>
+        <v>6154.3</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -5726,7 +5727,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>6811.4</v>
+        <v>6768.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -7577,7 +7578,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!E190")</f>
-        <v>3371.7</v>
+        <v>3350.3</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -7849,7 +7850,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>4456.7</v>
+        <v>4435.3</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -7941,7 +7942,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>4456.7</v>
+        <v>4435.3</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -8213,7 +8214,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>5090.7</v>
+        <v>5069.3</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -8305,7 +8306,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>5090.7</v>
+        <v>5069.3</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -8577,7 +8578,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>6175.7</v>
+        <v>6154.3</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -9107,7 +9108,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>635.7</v>
+        <v>614.3</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -9123,7 +9124,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>8688.7</v>
+        <v>8667.3</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -9139,7 +9140,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>9324.4</v>
+        <v>9281.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -10990,7 +10991,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!E190")</f>
-        <v>6175.7</v>
+        <v>6154.3</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -11262,7 +11263,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>6969.7</v>
+        <v>6948.3</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -11354,7 +11355,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>6969.7</v>
+        <v>6948.3</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -11626,7 +11627,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>7894.7</v>
+        <v>7873.3</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -11718,7 +11719,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>7894.7</v>
+        <v>7873.3</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -11990,7 +11991,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>8688.7</v>
+        <v>8667.3</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -12521,7 +12522,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>635.7</v>
+        <v>614.3</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -12537,7 +12538,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>11492.7</v>
+        <v>11471.3</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -12553,7 +12554,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>12128.4</v>
+        <v>12085.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -14404,7 +14405,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!E190")</f>
-        <v>8688.7</v>
+        <v>8667.3</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -14676,7 +14677,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>9773.7</v>
+        <v>9752.3</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -14768,7 +14769,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>9773.7</v>
+        <v>9752.3</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -15040,7 +15041,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>10407.7</v>
+        <v>10386.3</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -15132,7 +15133,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>10407.7</v>
+        <v>10386.3</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -15404,7 +15405,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>11492.7</v>
+        <v>11471.3</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -15933,7 +15934,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>635.7</v>
+        <v>614.3</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -15949,7 +15950,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>14005.7</v>
+        <v>13984.3</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -15965,7 +15966,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>14641.4</v>
+        <v>14598.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -17816,7 +17817,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!E190")</f>
-        <v>11492.7</v>
+        <v>11471.3</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -18088,7 +18089,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>12286.7</v>
+        <v>12265.3</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -18180,7 +18181,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>12286.7</v>
+        <v>12265.3</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -18452,7 +18453,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>13211.7</v>
+        <v>13190.3</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -18544,7 +18545,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>13211.7</v>
+        <v>13190.3</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -18816,7 +18817,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>14005.7</v>
+        <v>13984.3</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -19347,7 +19348,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>635.7</v>
+        <v>614.3</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -19363,7 +19364,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>16809.7</v>
+        <v>16788.3</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -19379,7 +19380,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>17445.4</v>
+        <v>17402.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -21230,7 +21231,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!E190")</f>
-        <v>14005.7</v>
+        <v>13984.3</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -21502,7 +21503,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>15090.7</v>
+        <v>15069.3</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -21594,7 +21595,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>15090.7</v>
+        <v>15069.3</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -21866,7 +21867,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>15724.7</v>
+        <v>15703.3</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -21958,7 +21959,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>15724.7</v>
+        <v>15703.3</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -22230,7 +22231,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>16809.7</v>
+        <v>16788.3</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -22759,7 +22760,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>635.7</v>
+        <v>614.3</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -22775,7 +22776,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -22791,7 +22792,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>19958.4</v>
+        <v>19915.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -24642,7 +24643,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!E190")</f>
-        <v>16809.7</v>
+        <v>16788.3</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -24914,7 +24915,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>17603.7</v>
+        <v>17582.3</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -25006,7 +25007,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>17603.7</v>
+        <v>17582.3</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -25278,7 +25279,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>18528.7</v>
+        <v>18507.3</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -25370,7 +25371,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>18528.7</v>
+        <v>18507.3</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -25642,7 +25643,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -26172,7 +26173,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>635.7</v>
+        <v>614.3</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -26188,7 +26189,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -26204,7 +26205,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>19958.4</v>
+        <v>19915.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -28013,7 +28014,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!E190")</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -28281,7 +28282,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -28373,7 +28374,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -28641,7 +28642,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -28733,7 +28734,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -29001,7 +29002,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -29478,7 +29479,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>635.7</v>
+        <v>614.3</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -29494,7 +29495,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -29510,7 +29511,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>19958.4</v>
+        <v>19915.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -31318,7 +31319,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!E190")</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -31586,7 +31587,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -31678,7 +31679,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -31946,7 +31947,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -32038,7 +32039,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -32306,7 +32307,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -32785,7 +32786,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>635.7</v>
+        <v>614.3</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -32801,7 +32802,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -32817,7 +32818,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>19958.4</v>
+        <v>19915.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -34626,7 +34627,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!E190")</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -34894,7 +34895,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -34986,7 +34987,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -35254,7 +35255,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -35346,7 +35347,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -35614,7 +35615,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -36597,7 +36598,7 @@
   <dimension ref="A1:N204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D3" sqref="D3:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -36677,7 +36678,7 @@
         <v>34</v>
       </c>
       <c r="F3" s="190">
-        <v>526.4</v>
+        <v>485.4</v>
       </c>
       <c r="I3" s="198" t="str">
         <f>TEXT(Main!B3,"dd mmmm yyyy")&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,1)-1,"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)*1,"dd mmmm yyyy"))</f>
@@ -36702,14 +36703,14 @@
         <v>35</v>
       </c>
       <c r="C4" s="162">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D4" s="164"/>
       <c r="E4" s="5" t="s">
         <v>35</v>
       </c>
       <c r="F4" s="190">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="I4" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,1),"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)+1,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,2)-1,"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)*2+1,"dd mmmm yyyy"))</f>
@@ -36927,14 +36928,14 @@
         <v>42</v>
       </c>
       <c r="C11" s="162">
-        <v>19.4</v>
+        <v>18</v>
       </c>
       <c r="D11" s="164"/>
       <c r="E11" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F11" s="190">
-        <v>11.4</v>
+        <v>19.4</v>
       </c>
       <c r="H11" s="191"/>
       <c r="I11" s="200" t="str">
@@ -37039,7 +37040,7 @@
       </c>
       <c r="J14" s="203">
         <f ca="1">'January 2025 - March 2025'!E190</f>
-        <v>635.700000000001</v>
+        <v>614.300000000001</v>
       </c>
       <c r="M14" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,33),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+33),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,36)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+35),"dd mmmm yyyy"))</f>
@@ -37071,7 +37072,7 @@
       </c>
       <c r="J15" s="203">
         <f ca="1">'April 2025 - June 2025'!E136</f>
-        <v>1614.7</v>
+        <v>1593.3</v>
       </c>
       <c r="M15" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,36),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+36),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,39)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+38),"dd mmmm yyyy"))</f>
@@ -37089,7 +37090,7 @@
       </c>
       <c r="C16" s="168">
         <f>SUM(C3:C15)</f>
-        <v>635.7</v>
+        <v>614.3</v>
       </c>
       <c r="D16" s="169"/>
       <c r="E16" s="167" t="s">
@@ -37097,7 +37098,7 @@
       </c>
       <c r="F16" s="193">
         <f>SUM(F3:F15)</f>
-        <v>688.7</v>
+        <v>635.7</v>
       </c>
       <c r="I16" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,13),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*13)+13,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,14)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*14+13),"dd mmmm yyyy"))</f>
@@ -37105,7 +37106,7 @@
       </c>
       <c r="J16" s="203">
         <f ca="1">'April 2025 - June 2025'!E163</f>
-        <v>3684.7</v>
+        <v>3663.3</v>
       </c>
       <c r="M16" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+39),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
@@ -37123,7 +37124,7 @@
       </c>
       <c r="J17" s="203">
         <f ca="1">'April 2025 - June 2025'!E190</f>
-        <v>4663.7</v>
+        <v>4642.3</v>
       </c>
       <c r="M17" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+42),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
@@ -37141,7 +37142,7 @@
       </c>
       <c r="J18" s="203">
         <f ca="1">'July 2025 - September 2025'!E136</f>
-        <v>4532.7</v>
+        <v>4511.3</v>
       </c>
       <c r="M18" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+45),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
@@ -37159,7 +37160,7 @@
       </c>
       <c r="J19" s="203">
         <f ca="1">'July 2025 - September 2025'!E163</f>
-        <v>4461.7</v>
+        <v>4440.3</v>
       </c>
     </row>
     <row r="20" ht="35.25" customHeight="1" spans="9:10">
@@ -37169,7 +37170,7 @@
       </c>
       <c r="J20" s="203">
         <f ca="1">'July 2025 - September 2025'!E190</f>
-        <v>4546.7</v>
+        <v>4525.3</v>
       </c>
     </row>
     <row r="21" ht="35.25" customHeight="1" spans="9:10">
@@ -37179,7 +37180,7 @@
       </c>
       <c r="J21" s="203">
         <f ca="1">'October 2025 - December 2025'!E136</f>
-        <v>4525.7</v>
+        <v>4504.3</v>
       </c>
     </row>
     <row r="22" ht="24.75" customHeight="1" spans="1:10">
@@ -37199,7 +37200,7 @@
       </c>
       <c r="J22" s="203">
         <f ca="1">'October 2025 - December 2025'!E163</f>
-        <v>4060.7</v>
+        <v>4039.3</v>
       </c>
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:10">
@@ -37224,7 +37225,7 @@
       </c>
       <c r="J23" s="203">
         <f ca="1">'October 2025 - December 2025'!E190</f>
-        <v>3371.7</v>
+        <v>3350.3</v>
       </c>
     </row>
     <row r="24" ht="52.5" customHeight="1" spans="1:10">
@@ -37249,7 +37250,7 @@
       </c>
       <c r="J24" s="203">
         <f ca="1">'January 2026 - March 2026'!E136</f>
-        <v>4456.7</v>
+        <v>4435.3</v>
       </c>
     </row>
     <row r="25" ht="30" customHeight="1" spans="1:10">
@@ -37268,7 +37269,7 @@
       </c>
       <c r="J25" s="203">
         <f ca="1">'January 2026 - March 2026'!E163</f>
-        <v>5090.7</v>
+        <v>5069.3</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1" spans="1:10">
@@ -37287,7 +37288,7 @@
       </c>
       <c r="J26" s="203">
         <f ca="1">'January 2026 - March 2026'!E190</f>
-        <v>6175.7</v>
+        <v>6154.3</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1" spans="1:10">
@@ -37306,7 +37307,7 @@
       </c>
       <c r="J27" s="203">
         <f ca="1">'April 2026 - June 2026'!E136</f>
-        <v>6969.7</v>
+        <v>6948.3</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:10">
@@ -37325,7 +37326,7 @@
       </c>
       <c r="J28" s="203">
         <f ca="1">'April 2026 - June 2026'!E163</f>
-        <v>7894.7</v>
+        <v>7873.3</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:10">
@@ -37344,7 +37345,7 @@
       </c>
       <c r="J29" s="199">
         <f ca="1">'April 2026 - June 2026'!E190</f>
-        <v>8688.7</v>
+        <v>8667.3</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1" spans="1:10">
@@ -37366,7 +37367,7 @@
       </c>
       <c r="J30" s="206">
         <f ca="1">'July 2026 - September 2026'!E136</f>
-        <v>9773.7</v>
+        <v>9752.3</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1" spans="9:10">
@@ -37376,7 +37377,7 @@
       </c>
       <c r="J31" s="203">
         <f ca="1">'July 2026 - September 2026'!E163</f>
-        <v>10407.7</v>
+        <v>10386.3</v>
       </c>
     </row>
     <row r="32" ht="27.75" customHeight="1" spans="9:10">
@@ -37386,7 +37387,7 @@
       </c>
       <c r="J32" s="203">
         <f ca="1">'July 2026 - September 2026'!E190</f>
-        <v>11492.7</v>
+        <v>11471.3</v>
       </c>
     </row>
     <row r="33" ht="30" customHeight="1" spans="9:10">
@@ -37396,7 +37397,7 @@
       </c>
       <c r="J33" s="203">
         <f ca="1">'October 2026 - December 2026'!E136</f>
-        <v>12286.7</v>
+        <v>12265.3</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1" spans="1:10">
@@ -37416,7 +37417,7 @@
       </c>
       <c r="J34" s="203">
         <f ca="1">'October 2026 - December 2026'!E163</f>
-        <v>13211.7</v>
+        <v>13190.3</v>
       </c>
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:10">
@@ -37441,7 +37442,7 @@
       </c>
       <c r="J35" s="203">
         <f ca="1">'October 2026 - December 2026'!E190</f>
-        <v>14005.7</v>
+        <v>13984.3</v>
       </c>
     </row>
     <row r="36" ht="54.75" customHeight="1" spans="1:10">
@@ -37466,7 +37467,7 @@
       </c>
       <c r="J36" s="203">
         <f ca="1">'January 2027 - March 2027'!E136</f>
-        <v>15090.7</v>
+        <v>15069.3</v>
       </c>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:10">
@@ -37491,7 +37492,7 @@
       </c>
       <c r="J37" s="203">
         <f ca="1">'January 2027 - March 2027'!E163</f>
-        <v>15724.7</v>
+        <v>15703.3</v>
       </c>
     </row>
     <row r="38" ht="20.25" customHeight="1" spans="1:10">
@@ -37516,7 +37517,7 @@
       </c>
       <c r="J38" s="203">
         <f ca="1">'January 2027 - March 2027'!E190</f>
-        <v>16809.7</v>
+        <v>16788.3</v>
       </c>
     </row>
     <row r="39" ht="24.75" customHeight="1" spans="1:10">
@@ -37535,7 +37536,7 @@
       </c>
       <c r="J39" s="203">
         <f ca="1">'April 2027 - June 2027'!E136</f>
-        <v>17603.7</v>
+        <v>17582.3</v>
       </c>
     </row>
     <row r="40" ht="24.75" customHeight="1" spans="1:10">
@@ -37554,7 +37555,7 @@
       </c>
       <c r="J40" s="203">
         <f ca="1">'April 2027 - June 2027'!E163</f>
-        <v>18528.7</v>
+        <v>18507.3</v>
       </c>
     </row>
     <row r="41" ht="24.75" customHeight="1" spans="1:10">
@@ -37573,7 +37574,7 @@
       </c>
       <c r="J41" s="203">
         <f ca="1">'April 2027 - June 2027'!E190</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:10">
@@ -37595,7 +37596,7 @@
       </c>
       <c r="J42" s="203">
         <f ca="1">Forecast_14!E136</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="9:10">
@@ -37605,7 +37606,7 @@
       </c>
       <c r="J43" s="203">
         <f ca="1">Forecast_14!E163</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
     </row>
     <row r="44" ht="24.75" customHeight="1" spans="9:10">
@@ -37615,7 +37616,7 @@
       </c>
       <c r="J44" s="203">
         <f ca="1">Forecast_14!E190</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
     </row>
     <row r="45" ht="24.75" customHeight="1" spans="9:10">
@@ -37625,7 +37626,7 @@
       </c>
       <c r="J45" s="203">
         <f ca="1">Forecast_15!E136</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
     </row>
     <row r="46" ht="24.75" customHeight="1" spans="1:10">
@@ -37645,7 +37646,7 @@
       </c>
       <c r="J46" s="203">
         <f ca="1">Forecast_15!E163</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
     </row>
     <row r="47" ht="24.75" customHeight="1" spans="1:10">
@@ -37670,7 +37671,7 @@
       </c>
       <c r="J47" s="203">
         <f ca="1">Forecast_15!E190</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
     </row>
     <row r="48" ht="24.75" customHeight="1" spans="1:10">
@@ -37695,7 +37696,7 @@
       </c>
       <c r="J48" s="203">
         <f ca="1">Forecast_16!E136</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
     </row>
     <row r="49" ht="24.75" customHeight="1" spans="1:10">
@@ -37720,7 +37721,7 @@
       </c>
       <c r="J49" s="203">
         <f ca="1">Forecast_16!E163</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
     </row>
     <row r="50" ht="24.75" customHeight="1" spans="1:10">
@@ -37745,7 +37746,7 @@
       </c>
       <c r="J50" s="199">
         <f ca="1">Forecast_16!E190</f>
-        <v>19322.7</v>
+        <v>19301.3</v>
       </c>
     </row>
     <row r="51" ht="41" customHeight="1" spans="1:7">
@@ -39695,7 +39696,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>635.7</v>
+        <v>614.3</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -39723,7 +39724,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1138.41</v>
+        <v>1117.01</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -43148,7 +43149,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>635.7</v>
+        <v>614.3</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -43176,7 +43177,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>809.040000000001</v>
+        <v>787.640000000001</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -46663,8 +46664,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G184" sqref="G184"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="E194" sqref="E194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -46698,7 +46699,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>635.7</v>
+        <v>614.3</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -46714,7 +46715,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>635.700000000001</v>
+        <v>614.300000000001</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -46730,7 +46731,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1271.4</v>
+        <v>1228.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -49167,7 +49168,7 @@
       <c r="H156" s="14"/>
       <c r="I156" s="47"/>
     </row>
-    <row r="157" ht="389" customHeight="1" spans="1:9">
+    <row r="157" ht="379" customHeight="1" spans="1:9">
       <c r="A157" s="62"/>
       <c r="B157" s="63"/>
       <c r="C157" s="100" t="s">
@@ -49537,7 +49538,7 @@
       <c r="H183" s="14"/>
       <c r="I183" s="47"/>
     </row>
-    <row r="184" ht="408" customHeight="1" spans="1:9">
+    <row r="184" ht="380" customHeight="1" spans="1:9">
       <c r="A184" s="62"/>
       <c r="B184" s="63"/>
       <c r="C184" s="100" t="s">
@@ -49545,7 +49546,7 @@
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="102">
-        <v>508.5</v>
+        <v>529.9</v>
       </c>
       <c r="F184" s="14"/>
       <c r="G184" s="14"/>
@@ -49631,7 +49632,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>635.700000000001</v>
+        <v>614.300000000001</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -50170,8 +50171,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="C156" sqref="C156:D156"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="C130" sqref="C130:D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -50206,7 +50207,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>635.7</v>
+        <v>614.3</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -50222,7 +50223,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>4663.7</v>
+        <v>4642.3</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -50238,7 +50239,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>5299.4</v>
+        <v>5256.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -52093,7 +52094,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!E190")</f>
-        <v>635.700000000001</v>
+        <v>614.300000000001</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -52367,7 +52368,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>1614.7</v>
+        <v>1593.3</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -52459,7 +52460,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>1614.7</v>
+        <v>1593.3</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -52733,7 +52734,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>3684.7</v>
+        <v>3663.3</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -52825,7 +52826,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>3684.7</v>
+        <v>3663.3</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -53099,7 +53100,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>4663.7</v>
+        <v>4642.3</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -53649,7 +53650,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>635.7</v>
+        <v>614.3</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -53665,7 +53666,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>4546.7</v>
+        <v>4525.3</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -53681,7 +53682,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>5182.4</v>
+        <v>5139.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -55528,7 +55529,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!E190")</f>
-        <v>4663.7</v>
+        <v>4642.3</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -55802,7 +55803,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>4532.7</v>
+        <v>4511.3</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -55894,7 +55895,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>4532.7</v>
+        <v>4511.3</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -56168,7 +56169,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>4461.7</v>
+        <v>4440.3</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -56260,7 +56261,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>4461.7</v>
+        <v>4440.3</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -56534,7 +56535,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>4546.7</v>
+        <v>4525.3</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -57078,7 +57079,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>635.7</v>
+        <v>614.3</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -57094,7 +57095,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>3371.7</v>
+        <v>3350.3</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -57110,7 +57111,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>4007.4</v>
+        <v>3964.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -58957,7 +58958,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!E190")</f>
-        <v>4546.7</v>
+        <v>4525.3</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -59231,7 +59232,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>4525.7</v>
+        <v>4504.3</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -59323,7 +59324,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>4525.7</v>
+        <v>4504.3</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -59599,7 +59600,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>4060.7</v>
+        <v>4039.3</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -59691,7 +59692,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>4060.7</v>
+        <v>4039.3</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -59967,7 +59968,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>3371.7</v>
+        <v>3350.3</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>

</xml_diff>

<commit_message>
docs: 1. Update Cigarette Buds to Original Value.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560" activeTab="5"/>
+    <workbookView windowHeight="21560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="292">
   <si>
     <t>Income Forecast</t>
   </si>
@@ -1197,7 +1197,7 @@
   </si>
   <si>
     <t>Additional Expense
-    - Cigarette Egg - $584
+    - Cigarette Egg - $650
     - See the psycharitic Doctor ~ $125</t>
   </si>
   <si>
@@ -1212,7 +1212,7 @@
   </si>
   <si>
     <t>Additional Expense
-    - Cigarette Egg - $584
+    - Cigarette Egg - $650
     - See the psycharitic Doctor For Injection ~ $19
     - See the high blood pressure Doctor ~ $50</t>
   </si>
@@ -1242,7 +1242,7 @@
   </si>
   <si>
     <t>Additional Expense
-    - Cigarette Egg - $800
+    - Cigarette Egg - $650
     - See the psycharitic Doctor For Injection ~ $19
     - Add In value for Google Play ~ $150 (don't need to
    include.)</t>
@@ -1259,16 +1259,9 @@
   </si>
   <si>
     <t>Additional Expense
-    - Cigarette Egg - $584
+    - Cigarette Egg - $650
     - See the psycharitic Doctor ~ $125
     - See the high blood pressure Doctor ~ $50</t>
-  </si>
-  <si>
-    <t>Additional Expense
-    - Cigarette Egg - $584
-    - See the psycharitic Doctor For Injection ~ $19
-    - Add In value for Google Play ~ $150 (don't need to
-   include.)</t>
   </si>
   <si>
     <t>31st October 2025</t>
@@ -1284,7 +1277,7 @@
   </si>
   <si>
     <t>Additional Expense
-    - Cigarette Egg - $584
+    - Cigarette Egg - $650
     - Add In value for Google Play ~ $150 (don't need to
    include.)
     - See the psycharitic Doctor For Injection ~ $19
@@ -1298,7 +1291,7 @@
   </si>
   <si>
     <t>Additional Expense
-    - Cigarette Egg - $584
+    - Cigarette Egg - $650
     - See the psycharitic Doctor ~ $310</t>
   </si>
   <si>
@@ -1312,20 +1305,20 @@
   </si>
   <si>
     <t>Additional Expense
-    - Cigarette Egg - $584
+    - Cigarette Egg - $650
     - Add In value for Google Play ~ $150  (don't need to
    include.)
     - See the psycharitic Doctor For Injection ~ $19</t>
   </si>
   <si>
     <t>Additional Expense
-    - Cigarette Egg - $584
+    - Cigarette Egg - $650
     - See the psycharitic Doctor ~ $310
     - See the high blood pressure Doctor ~ $160</t>
   </si>
   <si>
     <t>Additional Expense
-    - Cigarette Egg - $584
+    - Cigarette Egg - $650
     - See the psycharitic Doctor For Injection ~ $19</t>
   </si>
   <si>
@@ -1341,18 +1334,18 @@
     <t>Additional Expense
     - Add In value for Google Play ~ $150 (don't need to
    include.)
-    - Cigarette Egg - $584
+    - Cigarette Egg - $650
     - See the psycharitic Doctor ~ $310</t>
   </si>
   <si>
     <t>Additional Expense
-    - Cigarette Egg - $584
+    - Cigarette Egg - $650
     - See the psycharitic Doctor For Injection ~ $19
     - See the high blood pressure Doctor ~ $160</t>
   </si>
   <si>
     <t>1. Additional Expense
-    - Cigarette Egg - $584
+    - Cigarette Egg - $650
     - See the psycharitic Doctor ~ $310</t>
   </si>
   <si>
@@ -1366,7 +1359,7 @@
   </si>
   <si>
     <t>1. Additional Expense
-    - Cigarette Egg - $584
+    - Cigarette Egg - $650
     - See the psycharitic Doctor For Injection ~ $19</t>
   </si>
   <si>
@@ -5664,7 +5657,7 @@
   <dimension ref="A1:I193"/>
   <sheetViews>
     <sheetView topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="F157" sqref="F157"/>
+      <selection activeCell="F184" sqref="F184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -5714,7 +5707,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>6041.8</v>
+        <v>5465.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -5730,7 +5723,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>6543.6</v>
+        <v>5967.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -5829,7 +5822,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -6003,7 +5996,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -6177,7 +6170,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -7581,7 +7574,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!E190")</f>
-        <v>3237.8</v>
+        <v>2859.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -7750,11 +7743,11 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
-        <v>603</v>
+        <v>669</v>
       </c>
       <c r="F129" s="14"/>
       <c r="G129" s="14"/>
@@ -7853,7 +7846,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>4322.8</v>
+        <v>3878.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -7945,7 +7938,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>4322.8</v>
+        <v>3878.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -8114,11 +8107,11 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D156" s="103"/>
       <c r="E156" s="101">
-        <v>1054</v>
+        <v>1120</v>
       </c>
       <c r="F156" s="14"/>
       <c r="G156" s="14"/>
@@ -8217,7 +8210,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>4956.8</v>
+        <v>4446.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -8309,7 +8302,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>4956.8</v>
+        <v>4446.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -8478,11 +8471,11 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
-        <v>603</v>
+        <v>669</v>
       </c>
       <c r="F183" s="14"/>
       <c r="G183" s="14"/>
@@ -8581,7 +8574,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>6041.8</v>
+        <v>5465.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -9076,7 +9069,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A174" workbookViewId="0">
+    <sheetView topLeftCell="A165" workbookViewId="0">
       <selection activeCell="F184" sqref="F184"/>
     </sheetView>
   </sheetViews>
@@ -9127,7 +9120,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>8554.8</v>
+        <v>7780.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -9143,7 +9136,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>9056.6</v>
+        <v>8282.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -9242,7 +9235,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -9416,7 +9409,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -9590,7 +9583,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -10994,7 +10987,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!E190")</f>
-        <v>6041.8</v>
+        <v>5465.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -11163,11 +11156,11 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
-        <v>894</v>
+        <v>960</v>
       </c>
       <c r="F129" s="14"/>
       <c r="G129" s="14"/>
@@ -11266,7 +11259,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>6835.8</v>
+        <v>6193.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -11358,7 +11351,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>6835.8</v>
+        <v>6193.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -11527,11 +11520,11 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
-        <v>763</v>
+        <v>829</v>
       </c>
       <c r="F156" s="14"/>
       <c r="G156" s="14"/>
@@ -11630,7 +11623,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>7760.8</v>
+        <v>7052.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -11722,7 +11715,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>7760.8</v>
+        <v>7052.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -11891,11 +11884,11 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D183" s="103"/>
       <c r="E183" s="101">
-        <v>894</v>
+        <v>960</v>
       </c>
       <c r="F183" s="14"/>
       <c r="G183" s="14"/>
@@ -11994,7 +11987,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>8554.8</v>
+        <v>7780.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -12490,7 +12483,7 @@
   <dimension ref="A1:I193"/>
   <sheetViews>
     <sheetView topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="F157" sqref="F157"/>
+      <selection activeCell="F184" sqref="F184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -12541,7 +12534,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>11358.8</v>
+        <v>10386.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -12557,7 +12550,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>11860.6</v>
+        <v>10888.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -12656,7 +12649,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -12830,7 +12823,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -13004,7 +12997,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -14408,7 +14401,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!E190")</f>
-        <v>8554.8</v>
+        <v>7780.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -14577,11 +14570,11 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
-        <v>603</v>
+        <v>669</v>
       </c>
       <c r="F129" s="14"/>
       <c r="G129" s="14"/>
@@ -14680,7 +14673,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>9639.8</v>
+        <v>8799.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -14772,7 +14765,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>9639.8</v>
+        <v>8799.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -14941,11 +14934,11 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D156" s="103"/>
       <c r="E156" s="101">
-        <v>1054</v>
+        <v>1120</v>
       </c>
       <c r="F156" s="14"/>
       <c r="G156" s="14"/>
@@ -15044,7 +15037,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>10273.8</v>
+        <v>9367.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -15136,7 +15129,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>10273.8</v>
+        <v>9367.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -15305,11 +15298,11 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
-        <v>603</v>
+        <v>669</v>
       </c>
       <c r="F183" s="14"/>
       <c r="G183" s="14"/>
@@ -15408,7 +15401,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>11358.8</v>
+        <v>10386.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -15903,7 +15896,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A161" workbookViewId="0">
+    <sheetView topLeftCell="A163" workbookViewId="0">
       <selection activeCell="F184" sqref="F184"/>
     </sheetView>
   </sheetViews>
@@ -15953,7 +15946,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>13871.8</v>
+        <v>12701.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -15969,7 +15962,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>14373.6</v>
+        <v>13203.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -16068,7 +16061,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -16242,7 +16235,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -16416,7 +16409,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -17820,7 +17813,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!E190")</f>
-        <v>11358.8</v>
+        <v>10386.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -17989,11 +17982,11 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
-        <v>894</v>
+        <v>960</v>
       </c>
       <c r="F129" s="14"/>
       <c r="G129" s="14"/>
@@ -18092,7 +18085,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>12152.8</v>
+        <v>11114.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -18184,7 +18177,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>12152.8</v>
+        <v>11114.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -18353,11 +18346,11 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
-        <v>763</v>
+        <v>829</v>
       </c>
       <c r="F156" s="14"/>
       <c r="G156" s="14"/>
@@ -18456,7 +18449,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>13077.8</v>
+        <v>11973.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -18548,7 +18541,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>13077.8</v>
+        <v>11973.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -18717,11 +18710,11 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
-        <v>894</v>
+        <v>960</v>
       </c>
       <c r="F183" s="14"/>
       <c r="G183" s="14"/>
@@ -18820,7 +18813,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>13871.8</v>
+        <v>12701.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -19315,8 +19308,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="F157" sqref="F157"/>
+    <sheetView topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="F183" sqref="F183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -19367,7 +19360,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>16675.8</v>
+        <v>15307.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -19383,7 +19376,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>17177.6</v>
+        <v>15809.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -19482,7 +19475,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -19656,7 +19649,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -19830,7 +19823,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -21234,7 +21227,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!E190")</f>
-        <v>13871.8</v>
+        <v>12701.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -21403,11 +21396,11 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
-        <v>603</v>
+        <v>669</v>
       </c>
       <c r="F129" s="14"/>
       <c r="G129" s="14"/>
@@ -21506,7 +21499,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>14956.8</v>
+        <v>13720.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -21598,7 +21591,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>14956.8</v>
+        <v>13720.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -21767,11 +21760,11 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
-        <v>1054</v>
+        <v>1120</v>
       </c>
       <c r="F156" s="14"/>
       <c r="G156" s="14"/>
@@ -21870,7 +21863,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>15590.8</v>
+        <v>14288.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -21962,7 +21955,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>15590.8</v>
+        <v>14288.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -22131,11 +22124,11 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
-        <v>603</v>
+        <v>669</v>
       </c>
       <c r="F183" s="14"/>
       <c r="G183" s="14"/>
@@ -22234,7 +22227,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>16675.8</v>
+        <v>15307.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -22729,7 +22722,7 @@
   <sheetPr/>
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView topLeftCell="A162" workbookViewId="0">
+    <sheetView topLeftCell="A164" workbookViewId="0">
       <selection activeCell="F184" sqref="F184"/>
     </sheetView>
   </sheetViews>
@@ -22779,7 +22772,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -22795,7 +22788,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>19690.6</v>
+        <v>18124.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -22894,7 +22887,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -23068,7 +23061,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -23242,7 +23235,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -24646,7 +24639,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!E190")</f>
-        <v>16675.8</v>
+        <v>15307.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -24815,11 +24808,11 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
-        <v>894</v>
+        <v>960</v>
       </c>
       <c r="F129" s="14"/>
       <c r="G129" s="14"/>
@@ -24918,7 +24911,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>17469.8</v>
+        <v>16035.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -25010,7 +25003,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>17469.8</v>
+        <v>16035.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -25179,11 +25172,11 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
-        <v>763</v>
+        <v>829</v>
       </c>
       <c r="F156" s="14"/>
       <c r="G156" s="14"/>
@@ -25282,7 +25275,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>18394.8</v>
+        <v>16894.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -25374,7 +25367,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>18394.8</v>
+        <v>16894.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -25543,11 +25536,11 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
-        <v>894</v>
+        <v>960</v>
       </c>
       <c r="F183" s="14"/>
       <c r="G183" s="14"/>
@@ -25646,7 +25639,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -26192,7 +26185,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -26208,7 +26201,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>19690.6</v>
+        <v>18124.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -28017,7 +28010,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!E190")</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -28285,7 +28278,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -28377,7 +28370,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -28645,7 +28638,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -28737,7 +28730,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -29005,7 +28998,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -29498,7 +29491,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -29514,7 +29507,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>19690.6</v>
+        <v>18124.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -31092,7 +31085,7 @@
         <v>Bankruptcy Department / Bank</v>
       </c>
       <c r="B102" s="37" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C102" s="36" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C102")+SUM(E122+E149+E176)</f>
@@ -31322,7 +31315,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!E190")</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -31590,7 +31583,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -31682,7 +31675,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -31950,7 +31943,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -32042,7 +32035,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -32310,7 +32303,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -32805,7 +32798,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -32821,7 +32814,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>19690.6</v>
+        <v>18124.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -34630,7 +34623,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!E190")</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -34898,7 +34891,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -34990,7 +34983,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -35258,7 +35251,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -35350,7 +35343,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -35618,7 +35611,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -36600,8 +36593,8 @@
   <sheetPr/>
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -37075,7 +37068,7 @@
       </c>
       <c r="J15" s="203">
         <f ca="1">'April 2025 - June 2025'!E136</f>
-        <v>1480.8</v>
+        <v>1414.8</v>
       </c>
       <c r="M15" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,36),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+36),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,39)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+38),"dd mmmm yyyy"))</f>
@@ -37109,7 +37102,7 @@
       </c>
       <c r="J16" s="203">
         <f ca="1">'April 2025 - June 2025'!E163</f>
-        <v>3550.8</v>
+        <v>3418.8</v>
       </c>
       <c r="M16" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+39),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
@@ -37127,7 +37120,7 @@
       </c>
       <c r="J17" s="203">
         <f ca="1">'April 2025 - June 2025'!E190</f>
-        <v>4529.8</v>
+        <v>4331.8</v>
       </c>
       <c r="M17" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+42),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
@@ -37145,7 +37138,7 @@
       </c>
       <c r="J18" s="203">
         <f ca="1">'July 2025 - September 2025'!E136</f>
-        <v>4398.8</v>
+        <v>4350.8</v>
       </c>
       <c r="M18" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+45),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
@@ -37163,7 +37156,7 @@
       </c>
       <c r="J19" s="203">
         <f ca="1">'July 2025 - September 2025'!E163</f>
-        <v>4327.8</v>
+        <v>4213.8</v>
       </c>
     </row>
     <row r="20" ht="35.25" customHeight="1" spans="9:10">
@@ -37173,7 +37166,7 @@
       </c>
       <c r="J20" s="203">
         <f ca="1">'July 2025 - September 2025'!E190</f>
-        <v>4412.8</v>
+        <v>4232.8</v>
       </c>
     </row>
     <row r="21" ht="35.25" customHeight="1" spans="9:10">
@@ -37183,7 +37176,7 @@
       </c>
       <c r="J21" s="203">
         <f ca="1">'October 2025 - December 2025'!E136</f>
-        <v>4391.8</v>
+        <v>4145.8</v>
       </c>
     </row>
     <row r="22" ht="24.75" customHeight="1" spans="1:10">
@@ -37203,7 +37196,7 @@
       </c>
       <c r="J22" s="203">
         <f ca="1">'October 2025 - December 2025'!E163</f>
-        <v>3926.8</v>
+        <v>3614.8</v>
       </c>
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:10">
@@ -37228,7 +37221,7 @@
       </c>
       <c r="J23" s="203">
         <f ca="1">'October 2025 - December 2025'!E190</f>
-        <v>3237.8</v>
+        <v>2859.8</v>
       </c>
     </row>
     <row r="24" ht="52.5" customHeight="1" spans="1:10">
@@ -37253,7 +37246,7 @@
       </c>
       <c r="J24" s="203">
         <f ca="1">'January 2026 - March 2026'!E136</f>
-        <v>4322.8</v>
+        <v>3878.8</v>
       </c>
     </row>
     <row r="25" ht="30" customHeight="1" spans="1:10">
@@ -37272,7 +37265,7 @@
       </c>
       <c r="J25" s="203">
         <f ca="1">'January 2026 - March 2026'!E163</f>
-        <v>4956.8</v>
+        <v>4446.8</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1" spans="1:10">
@@ -37291,7 +37284,7 @@
       </c>
       <c r="J26" s="203">
         <f ca="1">'January 2026 - March 2026'!E190</f>
-        <v>6041.8</v>
+        <v>5465.8</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1" spans="1:10">
@@ -37310,7 +37303,7 @@
       </c>
       <c r="J27" s="203">
         <f ca="1">'April 2026 - June 2026'!E136</f>
-        <v>6835.8</v>
+        <v>6193.8</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:10">
@@ -37329,7 +37322,7 @@
       </c>
       <c r="J28" s="203">
         <f ca="1">'April 2026 - June 2026'!E163</f>
-        <v>7760.8</v>
+        <v>7052.8</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:10">
@@ -37348,7 +37341,7 @@
       </c>
       <c r="J29" s="199">
         <f ca="1">'April 2026 - June 2026'!E190</f>
-        <v>8554.8</v>
+        <v>7780.8</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1" spans="1:10">
@@ -37370,7 +37363,7 @@
       </c>
       <c r="J30" s="206">
         <f ca="1">'July 2026 - September 2026'!E136</f>
-        <v>9639.8</v>
+        <v>8799.8</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1" spans="9:10">
@@ -37380,7 +37373,7 @@
       </c>
       <c r="J31" s="203">
         <f ca="1">'July 2026 - September 2026'!E163</f>
-        <v>10273.8</v>
+        <v>9367.8</v>
       </c>
     </row>
     <row r="32" ht="27.75" customHeight="1" spans="9:10">
@@ -37390,7 +37383,7 @@
       </c>
       <c r="J32" s="203">
         <f ca="1">'July 2026 - September 2026'!E190</f>
-        <v>11358.8</v>
+        <v>10386.8</v>
       </c>
     </row>
     <row r="33" ht="30" customHeight="1" spans="9:10">
@@ -37400,7 +37393,7 @@
       </c>
       <c r="J33" s="203">
         <f ca="1">'October 2026 - December 2026'!E136</f>
-        <v>12152.8</v>
+        <v>11114.8</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1" spans="1:10">
@@ -37420,7 +37413,7 @@
       </c>
       <c r="J34" s="203">
         <f ca="1">'October 2026 - December 2026'!E163</f>
-        <v>13077.8</v>
+        <v>11973.8</v>
       </c>
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:10">
@@ -37445,7 +37438,7 @@
       </c>
       <c r="J35" s="203">
         <f ca="1">'October 2026 - December 2026'!E190</f>
-        <v>13871.8</v>
+        <v>12701.8</v>
       </c>
     </row>
     <row r="36" ht="54.75" customHeight="1" spans="1:10">
@@ -37470,7 +37463,7 @@
       </c>
       <c r="J36" s="203">
         <f ca="1">'January 2027 - March 2027'!E136</f>
-        <v>14956.8</v>
+        <v>13720.8</v>
       </c>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:10">
@@ -37495,7 +37488,7 @@
       </c>
       <c r="J37" s="203">
         <f ca="1">'January 2027 - March 2027'!E163</f>
-        <v>15590.8</v>
+        <v>14288.8</v>
       </c>
     </row>
     <row r="38" ht="20.25" customHeight="1" spans="1:10">
@@ -37520,7 +37513,7 @@
       </c>
       <c r="J38" s="203">
         <f ca="1">'January 2027 - March 2027'!E190</f>
-        <v>16675.8</v>
+        <v>15307.8</v>
       </c>
     </row>
     <row r="39" ht="24.75" customHeight="1" spans="1:10">
@@ -37539,7 +37532,7 @@
       </c>
       <c r="J39" s="203">
         <f ca="1">'April 2027 - June 2027'!E136</f>
-        <v>17469.8</v>
+        <v>16035.8</v>
       </c>
     </row>
     <row r="40" ht="24.75" customHeight="1" spans="1:10">
@@ -37558,7 +37551,7 @@
       </c>
       <c r="J40" s="203">
         <f ca="1">'April 2027 - June 2027'!E163</f>
-        <v>18394.8</v>
+        <v>16894.8</v>
       </c>
     </row>
     <row r="41" ht="24.75" customHeight="1" spans="1:10">
@@ -37577,7 +37570,7 @@
       </c>
       <c r="J41" s="203">
         <f ca="1">'April 2027 - June 2027'!E190</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:10">
@@ -37599,7 +37592,7 @@
       </c>
       <c r="J42" s="203">
         <f ca="1">Forecast_14!E136</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="9:10">
@@ -37609,7 +37602,7 @@
       </c>
       <c r="J43" s="203">
         <f ca="1">Forecast_14!E163</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
     </row>
     <row r="44" ht="24.75" customHeight="1" spans="9:10">
@@ -37619,7 +37612,7 @@
       </c>
       <c r="J44" s="203">
         <f ca="1">Forecast_14!E190</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
     </row>
     <row r="45" ht="24.75" customHeight="1" spans="9:10">
@@ -37629,7 +37622,7 @@
       </c>
       <c r="J45" s="203">
         <f ca="1">Forecast_15!E136</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
     </row>
     <row r="46" ht="24.75" customHeight="1" spans="1:10">
@@ -37649,7 +37642,7 @@
       </c>
       <c r="J46" s="203">
         <f ca="1">Forecast_15!E163</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
     </row>
     <row r="47" ht="24.75" customHeight="1" spans="1:10">
@@ -37674,7 +37667,7 @@
       </c>
       <c r="J47" s="203">
         <f ca="1">Forecast_15!E190</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
     </row>
     <row r="48" ht="24.75" customHeight="1" spans="1:10">
@@ -37699,7 +37692,7 @@
       </c>
       <c r="J48" s="203">
         <f ca="1">Forecast_16!E136</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
     </row>
     <row r="49" ht="24.75" customHeight="1" spans="1:10">
@@ -37724,7 +37717,7 @@
       </c>
       <c r="J49" s="203">
         <f ca="1">Forecast_16!E163</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
     </row>
     <row r="50" ht="24.75" customHeight="1" spans="1:10">
@@ -37749,7 +37742,7 @@
       </c>
       <c r="J50" s="199">
         <f ca="1">Forecast_16!E190</f>
-        <v>19188.8</v>
+        <v>17622.8</v>
       </c>
     </row>
     <row r="51" ht="41" customHeight="1" spans="1:7">
@@ -46667,8 +46660,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="C184" sqref="C184:D184"/>
+    <sheetView topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="G184" sqref="G184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -50174,8 +50167,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="E130" sqref="E130"/>
+    <sheetView topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="F184" sqref="F184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -50226,7 +50219,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>4529.8</v>
+        <v>4331.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -50242,7 +50235,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>5031.6</v>
+        <v>4833.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -52272,7 +52265,7 @@
       </c>
       <c r="D129" s="109"/>
       <c r="E129" s="98">
-        <v>709</v>
+        <v>775</v>
       </c>
       <c r="F129" s="14"/>
       <c r="G129" s="14"/>
@@ -52371,7 +52364,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>1480.8</v>
+        <v>1414.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -52463,7 +52456,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>1480.8</v>
+        <v>1414.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -52638,7 +52631,7 @@
       </c>
       <c r="D156" s="100"/>
       <c r="E156" s="98">
-        <v>653</v>
+        <v>719</v>
       </c>
       <c r="F156" s="14"/>
       <c r="G156" s="14"/>
@@ -52737,7 +52730,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>3550.8</v>
+        <v>3418.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -52829,7 +52822,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>3550.8</v>
+        <v>3418.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -53004,7 +52997,7 @@
       </c>
       <c r="D183" s="100"/>
       <c r="E183" s="98">
-        <v>709</v>
+        <v>775</v>
       </c>
       <c r="F183" s="14"/>
       <c r="G183" s="14"/>
@@ -53103,7 +53096,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>4529.8</v>
+        <v>4331.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -53619,7 +53612,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A168" workbookViewId="0">
+    <sheetView topLeftCell="A179" workbookViewId="0">
       <selection activeCell="F184" sqref="F184"/>
     </sheetView>
   </sheetViews>
@@ -53669,7 +53662,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>4412.8</v>
+        <v>4232.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -53685,7 +53678,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>4914.6</v>
+        <v>4734.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -55532,7 +55525,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!E190")</f>
-        <v>4529.8</v>
+        <v>4331.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -55707,7 +55700,7 @@
       </c>
       <c r="D129" s="100"/>
       <c r="E129" s="98">
-        <v>819</v>
+        <v>669</v>
       </c>
       <c r="F129" s="14"/>
       <c r="G129" s="14"/>
@@ -55806,7 +55799,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>4398.8</v>
+        <v>4350.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -55898,7 +55891,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>4398.8</v>
+        <v>4350.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -56073,7 +56066,7 @@
       </c>
       <c r="D156" s="100"/>
       <c r="E156" s="98">
-        <v>759</v>
+        <v>825</v>
       </c>
       <c r="F156" s="14"/>
       <c r="G156" s="14"/>
@@ -56172,7 +56165,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>4327.8</v>
+        <v>4213.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -56264,7 +56257,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>4327.8</v>
+        <v>4213.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -56435,11 +56428,11 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="100" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D183" s="100"/>
       <c r="E183" s="98">
-        <v>603</v>
+        <v>669</v>
       </c>
       <c r="F183" s="14"/>
       <c r="G183" s="14"/>
@@ -56538,7 +56531,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>4412.8</v>
+        <v>4232.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -57048,8 +57041,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="G182" sqref="G182"/>
+    <sheetView topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="F184" sqref="F184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -57098,7 +57091,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>3237.8</v>
+        <v>2859.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -57114,7 +57107,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>3739.6</v>
+        <v>3361.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -57213,7 +57206,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -57387,7 +57380,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -57557,7 +57550,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -58961,7 +58954,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!E190")</f>
-        <v>4412.8</v>
+        <v>4232.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -59136,7 +59129,7 @@
       </c>
       <c r="D129" s="100"/>
       <c r="E129" s="98">
-        <v>709</v>
+        <v>775</v>
       </c>
       <c r="F129" s="14"/>
       <c r="G129" s="14"/>
@@ -59235,7 +59228,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>4391.8</v>
+        <v>4145.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -59327,7 +59320,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>4391.8</v>
+        <v>4145.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -59420,7 +59413,7 @@
       <c r="A150" s="62"/>
       <c r="B150" s="63"/>
       <c r="C150" s="64" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D150" s="65"/>
       <c r="E150" s="36">
@@ -59500,11 +59493,11 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="100" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D156" s="100"/>
       <c r="E156" s="102">
-        <v>653</v>
+        <v>719</v>
       </c>
       <c r="F156" s="14"/>
       <c r="G156" s="14"/>
@@ -59603,7 +59596,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>3926.8</v>
+        <v>3614.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -59695,7 +59688,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>3926.8</v>
+        <v>3614.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -59721,7 +59714,7 @@
       <c r="A172" s="62"/>
       <c r="B172" s="63"/>
       <c r="C172" s="64" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D172" s="65"/>
       <c r="E172" s="36">
@@ -59788,7 +59781,7 @@
       <c r="A177" s="62"/>
       <c r="B177" s="63"/>
       <c r="C177" s="64" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D177" s="65"/>
       <c r="E177" s="36">
@@ -59868,11 +59861,11 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="100" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D183" s="100"/>
       <c r="E183" s="98">
-        <v>894</v>
+        <v>960</v>
       </c>
       <c r="F183" s="14"/>
       <c r="G183" s="14"/>
@@ -59971,7 +59964,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>3237.8</v>
+        <v>2859.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>

</xml_diff>

<commit_message>
docs: 1. Converted yuu points to money.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="295">
   <si>
     <t>Income Forecast</t>
   </si>
@@ -1018,6 +1018,15 @@
   </si>
   <si>
     <t>Lawrence give me $1000 as a gift for selling his house</t>
+  </si>
+  <si>
+    <t>1st April 2025</t>
+  </si>
+  <si>
+    <t>Yuu</t>
+  </si>
+  <si>
+    <t>Newly added / remain yuu points ~ $2</t>
   </si>
   <si>
     <t xml:space="preserve">Payback $1400 to Mom including $900 borrowed </t>
@@ -5691,7 +5700,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>501.8</v>
+        <v>503.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -5707,7 +5716,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>5465.8</v>
+        <v>5467.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -5723,7 +5732,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>5967.6</v>
+        <v>5971.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -5822,7 +5831,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -5996,7 +6005,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -6170,7 +6179,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -7574,7 +7583,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!E190")</f>
-        <v>2859.8</v>
+        <v>2861.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -7743,7 +7752,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -7846,7 +7855,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>3878.8</v>
+        <v>3880.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -7938,7 +7947,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>3878.8</v>
+        <v>3880.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -8107,7 +8116,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D156" s="103"/>
       <c r="E156" s="101">
@@ -8210,7 +8219,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>4446.8</v>
+        <v>4448.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -8302,7 +8311,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>4446.8</v>
+        <v>4448.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -8471,7 +8480,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -8574,7 +8583,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>5465.8</v>
+        <v>5467.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -9104,7 +9113,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>501.8</v>
+        <v>503.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -9120,7 +9129,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>7780.8</v>
+        <v>7782.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -9136,7 +9145,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>8282.6</v>
+        <v>8286.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -9235,7 +9244,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -9409,7 +9418,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -9583,7 +9592,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -10987,7 +10996,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!E190")</f>
-        <v>5465.8</v>
+        <v>5467.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -11156,7 +11165,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -11259,7 +11268,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>6193.8</v>
+        <v>6195.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -11351,7 +11360,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>6193.8</v>
+        <v>6195.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -11520,7 +11529,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
@@ -11623,7 +11632,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>7052.8</v>
+        <v>7054.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -11715,7 +11724,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>7052.8</v>
+        <v>7054.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -11884,7 +11893,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="D183" s="103"/>
       <c r="E183" s="101">
@@ -11987,7 +11996,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>7780.8</v>
+        <v>7782.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -12518,7 +12527,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>501.8</v>
+        <v>503.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -12534,7 +12543,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>10386.8</v>
+        <v>10388.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -12550,7 +12559,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>10888.6</v>
+        <v>10892.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -12649,7 +12658,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -12823,7 +12832,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -12997,7 +13006,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -14401,7 +14410,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!E190")</f>
-        <v>7780.8</v>
+        <v>7782.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -14570,7 +14579,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -14673,7 +14682,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>8799.8</v>
+        <v>8801.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -14765,7 +14774,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>8799.8</v>
+        <v>8801.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -14934,7 +14943,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D156" s="103"/>
       <c r="E156" s="101">
@@ -15037,7 +15046,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>9367.8</v>
+        <v>9369.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -15129,7 +15138,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>9367.8</v>
+        <v>9369.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -15298,7 +15307,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -15401,7 +15410,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>10386.8</v>
+        <v>10388.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -15930,7 +15939,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>501.8</v>
+        <v>503.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -15946,7 +15955,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>12701.8</v>
+        <v>12703.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -15962,7 +15971,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>13203.6</v>
+        <v>13207.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -16061,7 +16070,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -16235,7 +16244,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -16409,7 +16418,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -17813,7 +17822,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!E190")</f>
-        <v>10386.8</v>
+        <v>10388.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -17982,7 +17991,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -18085,7 +18094,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>11114.8</v>
+        <v>11116.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -18177,7 +18186,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>11114.8</v>
+        <v>11116.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -18346,7 +18355,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
@@ -18449,7 +18458,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>11973.8</v>
+        <v>11975.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -18541,7 +18550,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>11973.8</v>
+        <v>11975.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -18710,7 +18719,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -18813,7 +18822,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>12701.8</v>
+        <v>12703.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -19344,7 +19353,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>501.8</v>
+        <v>503.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -19360,7 +19369,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>15307.8</v>
+        <v>15309.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -19376,7 +19385,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>15809.6</v>
+        <v>15813.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -19475,7 +19484,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -19649,7 +19658,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -19823,7 +19832,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -21227,7 +21236,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!E190")</f>
-        <v>12701.8</v>
+        <v>12703.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -21396,7 +21405,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -21499,7 +21508,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>13720.8</v>
+        <v>13722.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -21591,7 +21600,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>13720.8</v>
+        <v>13722.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -21760,7 +21769,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
@@ -21863,7 +21872,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>14288.8</v>
+        <v>14290.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -21955,7 +21964,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>14288.8</v>
+        <v>14290.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -22124,7 +22133,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -22227,7 +22236,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>15307.8</v>
+        <v>15309.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -22756,7 +22765,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>501.8</v>
+        <v>503.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -22772,7 +22781,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -22788,7 +22797,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>18124.6</v>
+        <v>18128.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -22887,7 +22896,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -23061,7 +23070,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -23235,7 +23244,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -24639,7 +24648,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!E190")</f>
-        <v>15307.8</v>
+        <v>15309.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -24808,7 +24817,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -24911,7 +24920,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>16035.8</v>
+        <v>16037.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -25003,7 +25012,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>16035.8</v>
+        <v>16037.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -25172,7 +25181,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
@@ -25275,7 +25284,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>16894.8</v>
+        <v>16896.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -25367,7 +25376,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>16894.8</v>
+        <v>16896.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -25536,7 +25545,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -25639,7 +25648,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -26169,7 +26178,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>501.8</v>
+        <v>503.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -26185,7 +26194,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -26201,7 +26210,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>18124.6</v>
+        <v>18128.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -28010,7 +28019,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!E190")</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -28278,7 +28287,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -28370,7 +28379,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -28638,7 +28647,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -28730,7 +28739,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -28998,7 +29007,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -29475,7 +29484,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>501.8</v>
+        <v>503.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -29491,7 +29500,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -29507,7 +29516,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>18124.6</v>
+        <v>18128.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -31085,7 +31094,7 @@
         <v>Bankruptcy Department / Bank</v>
       </c>
       <c r="B102" s="37" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C102" s="36" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C102")+SUM(E122+E149+E176)</f>
@@ -31315,7 +31324,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!E190")</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -31583,7 +31592,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -31675,7 +31684,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -31943,7 +31952,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -32035,7 +32044,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -32303,7 +32312,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -32782,7 +32791,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>501.8</v>
+        <v>503.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -32798,7 +32807,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -32814,7 +32823,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>18124.6</v>
+        <v>18128.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -34623,7 +34632,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!E190")</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -34891,7 +34900,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -34983,7 +34992,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -35251,7 +35260,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -35343,7 +35352,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -35611,7 +35620,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -36594,7 +36603,7 @@
   <dimension ref="A1:N204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="D3" sqref="D3:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -36989,7 +36998,7 @@
         <v>44</v>
       </c>
       <c r="C13" s="162">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D13" s="164"/>
       <c r="E13" s="192" t="s">
@@ -37036,7 +37045,7 @@
       </c>
       <c r="J14" s="203">
         <f ca="1">'January 2025 - March 2025'!E190</f>
-        <v>501.800000000001</v>
+        <v>503.800000000001</v>
       </c>
       <c r="M14" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,33),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+33),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,36)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+35),"dd mmmm yyyy"))</f>
@@ -37068,7 +37077,7 @@
       </c>
       <c r="J15" s="203">
         <f ca="1">'April 2025 - June 2025'!E136</f>
-        <v>1414.8</v>
+        <v>1416.8</v>
       </c>
       <c r="M15" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,36),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+36),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,39)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+38),"dd mmmm yyyy"))</f>
@@ -37086,7 +37095,7 @@
       </c>
       <c r="C16" s="168">
         <f>SUM(C3:C15)</f>
-        <v>501.8</v>
+        <v>503.8</v>
       </c>
       <c r="D16" s="169"/>
       <c r="E16" s="167" t="s">
@@ -37102,7 +37111,7 @@
       </c>
       <c r="J16" s="203">
         <f ca="1">'April 2025 - June 2025'!E163</f>
-        <v>3418.8</v>
+        <v>3420.8</v>
       </c>
       <c r="M16" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+39),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
@@ -37120,7 +37129,7 @@
       </c>
       <c r="J17" s="203">
         <f ca="1">'April 2025 - June 2025'!E190</f>
-        <v>4331.8</v>
+        <v>4333.8</v>
       </c>
       <c r="M17" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+42),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
@@ -37138,7 +37147,7 @@
       </c>
       <c r="J18" s="203">
         <f ca="1">'July 2025 - September 2025'!E136</f>
-        <v>4350.8</v>
+        <v>4352.8</v>
       </c>
       <c r="M18" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+45),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
@@ -37156,7 +37165,7 @@
       </c>
       <c r="J19" s="203">
         <f ca="1">'July 2025 - September 2025'!E163</f>
-        <v>4213.8</v>
+        <v>4215.8</v>
       </c>
     </row>
     <row r="20" ht="35.25" customHeight="1" spans="9:10">
@@ -37166,7 +37175,7 @@
       </c>
       <c r="J20" s="203">
         <f ca="1">'July 2025 - September 2025'!E190</f>
-        <v>4232.8</v>
+        <v>4234.8</v>
       </c>
     </row>
     <row r="21" ht="35.25" customHeight="1" spans="9:10">
@@ -37176,7 +37185,7 @@
       </c>
       <c r="J21" s="203">
         <f ca="1">'October 2025 - December 2025'!E136</f>
-        <v>4145.8</v>
+        <v>4147.8</v>
       </c>
     </row>
     <row r="22" ht="24.75" customHeight="1" spans="1:10">
@@ -37196,7 +37205,7 @@
       </c>
       <c r="J22" s="203">
         <f ca="1">'October 2025 - December 2025'!E163</f>
-        <v>3614.8</v>
+        <v>3616.8</v>
       </c>
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:10">
@@ -37221,7 +37230,7 @@
       </c>
       <c r="J23" s="203">
         <f ca="1">'October 2025 - December 2025'!E190</f>
-        <v>2859.8</v>
+        <v>2861.8</v>
       </c>
     </row>
     <row r="24" ht="52.5" customHeight="1" spans="1:10">
@@ -37246,7 +37255,7 @@
       </c>
       <c r="J24" s="203">
         <f ca="1">'January 2026 - March 2026'!E136</f>
-        <v>3878.8</v>
+        <v>3880.8</v>
       </c>
     </row>
     <row r="25" ht="30" customHeight="1" spans="1:10">
@@ -37265,7 +37274,7 @@
       </c>
       <c r="J25" s="203">
         <f ca="1">'January 2026 - March 2026'!E163</f>
-        <v>4446.8</v>
+        <v>4448.8</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1" spans="1:10">
@@ -37284,7 +37293,7 @@
       </c>
       <c r="J26" s="203">
         <f ca="1">'January 2026 - March 2026'!E190</f>
-        <v>5465.8</v>
+        <v>5467.8</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1" spans="1:10">
@@ -37303,7 +37312,7 @@
       </c>
       <c r="J27" s="203">
         <f ca="1">'April 2026 - June 2026'!E136</f>
-        <v>6193.8</v>
+        <v>6195.8</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:10">
@@ -37322,7 +37331,7 @@
       </c>
       <c r="J28" s="203">
         <f ca="1">'April 2026 - June 2026'!E163</f>
-        <v>7052.8</v>
+        <v>7054.8</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:10">
@@ -37341,7 +37350,7 @@
       </c>
       <c r="J29" s="199">
         <f ca="1">'April 2026 - June 2026'!E190</f>
-        <v>7780.8</v>
+        <v>7782.8</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1" spans="1:10">
@@ -37363,7 +37372,7 @@
       </c>
       <c r="J30" s="206">
         <f ca="1">'July 2026 - September 2026'!E136</f>
-        <v>8799.8</v>
+        <v>8801.8</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1" spans="9:10">
@@ -37373,7 +37382,7 @@
       </c>
       <c r="J31" s="203">
         <f ca="1">'July 2026 - September 2026'!E163</f>
-        <v>9367.8</v>
+        <v>9369.8</v>
       </c>
     </row>
     <row r="32" ht="27.75" customHeight="1" spans="9:10">
@@ -37383,7 +37392,7 @@
       </c>
       <c r="J32" s="203">
         <f ca="1">'July 2026 - September 2026'!E190</f>
-        <v>10386.8</v>
+        <v>10388.8</v>
       </c>
     </row>
     <row r="33" ht="30" customHeight="1" spans="9:10">
@@ -37393,7 +37402,7 @@
       </c>
       <c r="J33" s="203">
         <f ca="1">'October 2026 - December 2026'!E136</f>
-        <v>11114.8</v>
+        <v>11116.8</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1" spans="1:10">
@@ -37413,7 +37422,7 @@
       </c>
       <c r="J34" s="203">
         <f ca="1">'October 2026 - December 2026'!E163</f>
-        <v>11973.8</v>
+        <v>11975.8</v>
       </c>
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:10">
@@ -37438,7 +37447,7 @@
       </c>
       <c r="J35" s="203">
         <f ca="1">'October 2026 - December 2026'!E190</f>
-        <v>12701.8</v>
+        <v>12703.8</v>
       </c>
     </row>
     <row r="36" ht="54.75" customHeight="1" spans="1:10">
@@ -37463,7 +37472,7 @@
       </c>
       <c r="J36" s="203">
         <f ca="1">'January 2027 - March 2027'!E136</f>
-        <v>13720.8</v>
+        <v>13722.8</v>
       </c>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:10">
@@ -37488,7 +37497,7 @@
       </c>
       <c r="J37" s="203">
         <f ca="1">'January 2027 - March 2027'!E163</f>
-        <v>14288.8</v>
+        <v>14290.8</v>
       </c>
     </row>
     <row r="38" ht="20.25" customHeight="1" spans="1:10">
@@ -37513,7 +37522,7 @@
       </c>
       <c r="J38" s="203">
         <f ca="1">'January 2027 - March 2027'!E190</f>
-        <v>15307.8</v>
+        <v>15309.8</v>
       </c>
     </row>
     <row r="39" ht="24.75" customHeight="1" spans="1:10">
@@ -37532,7 +37541,7 @@
       </c>
       <c r="J39" s="203">
         <f ca="1">'April 2027 - June 2027'!E136</f>
-        <v>16035.8</v>
+        <v>16037.8</v>
       </c>
     </row>
     <row r="40" ht="24.75" customHeight="1" spans="1:10">
@@ -37551,7 +37560,7 @@
       </c>
       <c r="J40" s="203">
         <f ca="1">'April 2027 - June 2027'!E163</f>
-        <v>16894.8</v>
+        <v>16896.8</v>
       </c>
     </row>
     <row r="41" ht="24.75" customHeight="1" spans="1:10">
@@ -37570,7 +37579,7 @@
       </c>
       <c r="J41" s="203">
         <f ca="1">'April 2027 - June 2027'!E190</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:10">
@@ -37592,7 +37601,7 @@
       </c>
       <c r="J42" s="203">
         <f ca="1">Forecast_14!E136</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="9:10">
@@ -37602,7 +37611,7 @@
       </c>
       <c r="J43" s="203">
         <f ca="1">Forecast_14!E163</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
     </row>
     <row r="44" ht="24.75" customHeight="1" spans="9:10">
@@ -37612,7 +37621,7 @@
       </c>
       <c r="J44" s="203">
         <f ca="1">Forecast_14!E190</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
     </row>
     <row r="45" ht="24.75" customHeight="1" spans="9:10">
@@ -37622,7 +37631,7 @@
       </c>
       <c r="J45" s="203">
         <f ca="1">Forecast_15!E136</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
     </row>
     <row r="46" ht="24.75" customHeight="1" spans="1:10">
@@ -37642,7 +37651,7 @@
       </c>
       <c r="J46" s="203">
         <f ca="1">Forecast_15!E163</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
     </row>
     <row r="47" ht="24.75" customHeight="1" spans="1:10">
@@ -37667,7 +37676,7 @@
       </c>
       <c r="J47" s="203">
         <f ca="1">Forecast_15!E190</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
     </row>
     <row r="48" ht="24.75" customHeight="1" spans="1:10">
@@ -37692,7 +37701,7 @@
       </c>
       <c r="J48" s="203">
         <f ca="1">Forecast_16!E136</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
     </row>
     <row r="49" ht="24.75" customHeight="1" spans="1:10">
@@ -37717,7 +37726,7 @@
       </c>
       <c r="J49" s="203">
         <f ca="1">Forecast_16!E163</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
     </row>
     <row r="50" ht="24.75" customHeight="1" spans="1:10">
@@ -37742,7 +37751,7 @@
       </c>
       <c r="J50" s="199">
         <f ca="1">Forecast_16!E190</f>
-        <v>17622.8</v>
+        <v>17624.8</v>
       </c>
     </row>
     <row r="51" ht="41" customHeight="1" spans="1:7">
@@ -39692,7 +39701,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>501.8</v>
+        <v>503.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -39720,7 +39729,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1004.51</v>
+        <v>1006.51</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -43145,7 +43154,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>501.8</v>
+        <v>503.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -43173,7 +43182,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>675.140000000001</v>
+        <v>677.140000000001</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -46660,8 +46669,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="G184" sqref="G184"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -46695,7 +46704,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>501.8</v>
+        <v>503.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -46711,7 +46720,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>501.800000000001</v>
+        <v>503.800000000001</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -46727,7 +46736,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1003.6</v>
+        <v>1007.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -47256,13 +47265,19 @@
       <c r="I37" s="47"/>
     </row>
     <row r="38" ht="24.75" customHeight="1" spans="1:9">
-      <c r="A38" s="19"/>
-      <c r="B38" s="21"/>
+      <c r="A38" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>234</v>
+      </c>
       <c r="C38" s="22"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="43"/>
+      <c r="D38" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="E38" s="22"/>
       <c r="F38" s="41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G38" s="42"/>
       <c r="H38" s="14"/>
@@ -47291,7 +47306,7 @@
       <c r="E40" s="44"/>
       <c r="F40" s="45">
         <f>SUM(F34:G39)</f>
-        <v>3485</v>
+        <v>3487</v>
       </c>
       <c r="G40" s="46"/>
       <c r="H40" s="14"/>
@@ -48638,7 +48653,7 @@
       <c r="A118" s="62"/>
       <c r="B118" s="63"/>
       <c r="C118" s="109" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D118" s="109"/>
       <c r="E118" s="102">
@@ -48785,7 +48800,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="100" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="D129" s="100"/>
       <c r="E129" s="102">
@@ -48800,7 +48815,7 @@
       <c r="A130" s="62"/>
       <c r="B130" s="63"/>
       <c r="C130" s="100" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D130" s="100"/>
       <c r="E130" s="102">
@@ -48815,7 +48830,7 @@
       <c r="A131" s="62"/>
       <c r="B131" s="63"/>
       <c r="C131" s="113" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D131" s="114"/>
       <c r="E131" s="102">
@@ -49008,7 +49023,7 @@
       <c r="A145" s="62"/>
       <c r="B145" s="63"/>
       <c r="C145" s="100" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D145" s="100"/>
       <c r="E145" s="102">
@@ -49153,7 +49168,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="100" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D156" s="100"/>
       <c r="E156" s="102">
@@ -49168,7 +49183,7 @@
       <c r="A157" s="62"/>
       <c r="B157" s="63"/>
       <c r="C157" s="100" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D157" s="100"/>
       <c r="E157" s="102">
@@ -49183,7 +49198,7 @@
       <c r="A158" s="62"/>
       <c r="B158" s="63"/>
       <c r="C158" s="72" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D158" s="65"/>
       <c r="E158" s="86">
@@ -49376,7 +49391,7 @@
       <c r="A172" s="62"/>
       <c r="B172" s="63"/>
       <c r="C172" s="109" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D172" s="109"/>
       <c r="E172" s="102">
@@ -49404,7 +49419,7 @@
       <c r="A174" s="62"/>
       <c r="B174" s="63"/>
       <c r="C174" s="64" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D174" s="65"/>
       <c r="E174" s="36">
@@ -49523,7 +49538,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="100" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="D183" s="100"/>
       <c r="E183" s="36">
@@ -49538,7 +49553,7 @@
       <c r="A184" s="62"/>
       <c r="B184" s="63"/>
       <c r="C184" s="100" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="102">
@@ -49553,7 +49568,7 @@
       <c r="A185" s="62"/>
       <c r="B185" s="63"/>
       <c r="C185" s="64" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D185" s="65"/>
       <c r="E185" s="86">
@@ -49628,7 +49643,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>501.800000000001</v>
+        <v>503.800000000001</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -50203,7 +50218,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>501.8</v>
+        <v>503.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -50219,7 +50234,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>4331.8</v>
+        <v>4333.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -50235,7 +50250,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>4833.6</v>
+        <v>4837.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -50351,7 +50366,7 @@
     </row>
     <row r="12" ht="24.75" customHeight="1" spans="1:9">
       <c r="A12" s="95" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B12" s="96" t="s">
         <v>66</v>
@@ -50371,11 +50386,11 @@
     <row r="13" ht="24.75" customHeight="1" spans="1:9">
       <c r="A13" s="95"/>
       <c r="B13" s="96" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C13" s="96"/>
       <c r="D13" s="97" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="E13" s="97"/>
       <c r="F13" s="7">
@@ -50512,7 +50527,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -50536,7 +50551,7 @@
       </c>
       <c r="C24" s="110"/>
       <c r="D24" s="111" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E24" s="111"/>
       <c r="F24" s="112">
@@ -50686,7 +50701,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -52090,7 +52105,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!E190")</f>
-        <v>501.800000000001</v>
+        <v>503.800000000001</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -52261,7 +52276,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="100" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D129" s="109"/>
       <c r="E129" s="98">
@@ -52276,7 +52291,7 @@
       <c r="A130" s="62"/>
       <c r="B130" s="63"/>
       <c r="C130" s="113" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D130" s="114"/>
       <c r="E130" s="98">
@@ -52364,7 +52379,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>1414.8</v>
+        <v>1416.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -52456,7 +52471,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>1414.8</v>
+        <v>1416.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -52627,7 +52642,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="100" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="D156" s="100"/>
       <c r="E156" s="98">
@@ -52642,7 +52657,7 @@
       <c r="A157" s="62"/>
       <c r="B157" s="63"/>
       <c r="C157" s="100" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D157" s="100"/>
       <c r="E157" s="98">
@@ -52730,7 +52745,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>3418.8</v>
+        <v>3420.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -52822,7 +52837,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>3418.8</v>
+        <v>3420.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -52993,7 +53008,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="100" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D183" s="100"/>
       <c r="E183" s="98">
@@ -53008,7 +53023,7 @@
       <c r="A184" s="62"/>
       <c r="B184" s="63"/>
       <c r="C184" s="100" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="98">
@@ -53096,7 +53111,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>4331.8</v>
+        <v>4333.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -53646,7 +53661,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>501.8</v>
+        <v>503.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -53662,7 +53677,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>4232.8</v>
+        <v>4234.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -53678,7 +53693,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>4734.6</v>
+        <v>4738.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -53777,7 +53792,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -53797,11 +53812,11 @@
     <row r="12" ht="24.75" customHeight="1" spans="1:9">
       <c r="A12" s="95"/>
       <c r="B12" s="96" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C12" s="96"/>
       <c r="D12" s="97" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="E12" s="97"/>
       <c r="F12" s="7">
@@ -53951,7 +53966,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -54125,7 +54140,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -55525,7 +55540,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!E190")</f>
-        <v>4331.8</v>
+        <v>4333.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -55696,7 +55711,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="100" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D129" s="100"/>
       <c r="E129" s="98">
@@ -55711,7 +55726,7 @@
       <c r="A130" s="62"/>
       <c r="B130" s="63"/>
       <c r="C130" s="100" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D130" s="100"/>
       <c r="E130" s="98">
@@ -55799,7 +55814,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>4350.8</v>
+        <v>4352.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -55891,7 +55906,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>4350.8</v>
+        <v>4352.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -56062,7 +56077,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="100" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D156" s="100"/>
       <c r="E156" s="98">
@@ -56077,7 +56092,7 @@
       <c r="A157" s="62"/>
       <c r="B157" s="63"/>
       <c r="C157" s="100" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D157" s="100"/>
       <c r="E157" s="98">
@@ -56165,7 +56180,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>4213.8</v>
+        <v>4215.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -56257,7 +56272,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>4213.8</v>
+        <v>4215.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -56428,7 +56443,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="100" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D183" s="100"/>
       <c r="E183" s="98">
@@ -56443,7 +56458,7 @@
       <c r="A184" s="62"/>
       <c r="B184" s="63"/>
       <c r="C184" s="100" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="98">
@@ -56531,7 +56546,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>4232.8</v>
+        <v>4234.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -57075,7 +57090,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>501.8</v>
+        <v>503.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -57091,7 +57106,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>2859.8</v>
+        <v>2861.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -57107,7 +57122,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>3361.6</v>
+        <v>3365.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -57206,7 +57221,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -57380,7 +57395,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -57550,7 +57565,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -58954,7 +58969,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!E190")</f>
-        <v>4232.8</v>
+        <v>4234.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -59125,7 +59140,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="100" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D129" s="100"/>
       <c r="E129" s="98">
@@ -59228,7 +59243,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>4145.8</v>
+        <v>4147.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -59320,7 +59335,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>4145.8</v>
+        <v>4147.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -59413,7 +59428,7 @@
       <c r="A150" s="62"/>
       <c r="B150" s="63"/>
       <c r="C150" s="64" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D150" s="65"/>
       <c r="E150" s="36">
@@ -59493,7 +59508,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="100" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D156" s="100"/>
       <c r="E156" s="102">
@@ -59596,7 +59611,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>3614.8</v>
+        <v>3616.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -59688,7 +59703,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>3614.8</v>
+        <v>3616.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -59714,7 +59729,7 @@
       <c r="A172" s="62"/>
       <c r="B172" s="63"/>
       <c r="C172" s="64" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D172" s="65"/>
       <c r="E172" s="36">
@@ -59781,7 +59796,7 @@
       <c r="A177" s="62"/>
       <c r="B177" s="63"/>
       <c r="C177" s="64" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D177" s="65"/>
       <c r="E177" s="36">
@@ -59861,7 +59876,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="100" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D183" s="100"/>
       <c r="E183" s="98">
@@ -59964,7 +59979,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>2859.8</v>
+        <v>2861.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>

</xml_diff>

<commit_message>
docs: 1. Update Starbucks Card Remain Value.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560" activeTab="2"/>
+    <workbookView windowHeight="21560" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -214,7 +214,7 @@
     <t>Octopus Remain Value</t>
   </si>
   <si>
-    <t>Other 5</t>
+    <t>Starbucks Card</t>
   </si>
   <si>
     <t>Total</t>
@@ -1023,10 +1023,12 @@
     <t>1st April 2025</t>
   </si>
   <si>
-    <t>Yuu</t>
+    <t>1. Yuu
+2. Starbucks</t>
   </si>
   <si>
-    <t>Newly added / remain yuu points ~ $2</t>
+    <t>1. Newly added / remain yuu points ~ $2
+2. Newly added Starbucks Card ~ $60</t>
   </si>
   <si>
     <t xml:space="preserve">Payback $1400 to Mom including $900 borrowed </t>
@@ -5700,7 +5702,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>503.8</v>
+        <v>563.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -5716,7 +5718,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>5467.8</v>
+        <v>5527.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -5732,7 +5734,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>5971.6</v>
+        <v>6091.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -7583,7 +7585,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!E190")</f>
-        <v>2861.8</v>
+        <v>2921.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -7855,7 +7857,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>3880.8</v>
+        <v>3940.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -7947,7 +7949,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>3880.8</v>
+        <v>3940.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -8219,7 +8221,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>4448.8</v>
+        <v>4508.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -8311,7 +8313,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>4448.8</v>
+        <v>4508.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -8583,7 +8585,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>5467.8</v>
+        <v>5527.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -9113,7 +9115,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>503.8</v>
+        <v>563.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -9129,7 +9131,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>7782.8</v>
+        <v>7842.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -9145,7 +9147,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>8286.6</v>
+        <v>8406.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -10996,7 +10998,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!E190")</f>
-        <v>5467.8</v>
+        <v>5527.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -11268,7 +11270,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>6195.8</v>
+        <v>6255.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -11360,7 +11362,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>6195.8</v>
+        <v>6255.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -11632,7 +11634,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>7054.8</v>
+        <v>7114.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -11724,7 +11726,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>7054.8</v>
+        <v>7114.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -11996,7 +11998,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>7782.8</v>
+        <v>7842.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -12527,7 +12529,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>503.8</v>
+        <v>563.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -12543,7 +12545,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>10388.8</v>
+        <v>10448.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -12559,7 +12561,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>10892.6</v>
+        <v>11012.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -14410,7 +14412,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!E190")</f>
-        <v>7782.8</v>
+        <v>7842.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -14682,7 +14684,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>8801.8</v>
+        <v>8861.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -14774,7 +14776,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>8801.8</v>
+        <v>8861.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -15046,7 +15048,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>9369.8</v>
+        <v>9429.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -15138,7 +15140,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>9369.8</v>
+        <v>9429.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -15410,7 +15412,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>10388.8</v>
+        <v>10448.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -15939,7 +15941,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>503.8</v>
+        <v>563.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -15955,7 +15957,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>12703.8</v>
+        <v>12763.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -15971,7 +15973,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>13207.6</v>
+        <v>13327.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -17822,7 +17824,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!E190")</f>
-        <v>10388.8</v>
+        <v>10448.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -18094,7 +18096,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>11116.8</v>
+        <v>11176.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -18186,7 +18188,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>11116.8</v>
+        <v>11176.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -18458,7 +18460,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>11975.8</v>
+        <v>12035.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -18550,7 +18552,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>11975.8</v>
+        <v>12035.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -18822,7 +18824,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>12703.8</v>
+        <v>12763.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -19353,7 +19355,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>503.8</v>
+        <v>563.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -19369,7 +19371,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>15309.8</v>
+        <v>15369.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -19385,7 +19387,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>15813.6</v>
+        <v>15933.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -21236,7 +21238,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!E190")</f>
-        <v>12703.8</v>
+        <v>12763.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -21508,7 +21510,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>13722.8</v>
+        <v>13782.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -21600,7 +21602,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>13722.8</v>
+        <v>13782.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -21872,7 +21874,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>14290.8</v>
+        <v>14350.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -21964,7 +21966,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>14290.8</v>
+        <v>14350.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -22236,7 +22238,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>15309.8</v>
+        <v>15369.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -22765,7 +22767,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>503.8</v>
+        <v>563.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -22781,7 +22783,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -22797,7 +22799,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>18128.6</v>
+        <v>18248.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -24648,7 +24650,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!E190")</f>
-        <v>15309.8</v>
+        <v>15369.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -24920,7 +24922,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>16037.8</v>
+        <v>16097.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -25012,7 +25014,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>16037.8</v>
+        <v>16097.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -25284,7 +25286,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>16896.8</v>
+        <v>16956.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -25376,7 +25378,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>16896.8</v>
+        <v>16956.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -25648,7 +25650,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -26178,7 +26180,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>503.8</v>
+        <v>563.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -26194,7 +26196,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -26210,7 +26212,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>18128.6</v>
+        <v>18248.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -28019,7 +28021,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!E190")</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -28287,7 +28289,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -28379,7 +28381,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -28647,7 +28649,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -28739,7 +28741,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -29007,7 +29009,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -29484,7 +29486,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>503.8</v>
+        <v>563.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -29500,7 +29502,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -29516,7 +29518,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>18128.6</v>
+        <v>18248.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -31324,7 +31326,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!E190")</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -31592,7 +31594,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -31684,7 +31686,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -31952,7 +31954,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -32044,7 +32046,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -32312,7 +32314,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -32791,7 +32793,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>503.8</v>
+        <v>563.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -32807,7 +32809,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -32823,7 +32825,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>18128.6</v>
+        <v>18248.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -34632,7 +34634,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!E190")</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -34900,7 +34902,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -34992,7 +34994,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -35260,7 +35262,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -35352,7 +35354,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -35620,7 +35622,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -36602,8 +36604,8 @@
   <sheetPr/>
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D16"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -37045,7 +37047,7 @@
       </c>
       <c r="J14" s="203">
         <f ca="1">'January 2025 - March 2025'!E190</f>
-        <v>503.800000000001</v>
+        <v>563.800000000001</v>
       </c>
       <c r="M14" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,33),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+33),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,36)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+35),"dd mmmm yyyy"))</f>
@@ -37062,14 +37064,14 @@
         <v>46</v>
       </c>
       <c r="C15" s="162">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D15" s="164"/>
       <c r="E15" s="192" t="s">
         <v>46</v>
       </c>
       <c r="F15" s="190">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="I15" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,12),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*12)+12,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,13)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*13+12),"dd mmmm yyyy"))</f>
@@ -37077,7 +37079,7 @@
       </c>
       <c r="J15" s="203">
         <f ca="1">'April 2025 - June 2025'!E136</f>
-        <v>1416.8</v>
+        <v>1476.8</v>
       </c>
       <c r="M15" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,36),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+36),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,39)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+38),"dd mmmm yyyy"))</f>
@@ -37095,7 +37097,7 @@
       </c>
       <c r="C16" s="168">
         <f>SUM(C3:C15)</f>
-        <v>503.8</v>
+        <v>563.8</v>
       </c>
       <c r="D16" s="169"/>
       <c r="E16" s="167" t="s">
@@ -37103,7 +37105,7 @@
       </c>
       <c r="F16" s="193">
         <f>SUM(F3:F15)</f>
-        <v>614.3</v>
+        <v>674.3</v>
       </c>
       <c r="I16" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,13),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*13)+13,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,14)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*14+13),"dd mmmm yyyy"))</f>
@@ -37111,7 +37113,7 @@
       </c>
       <c r="J16" s="203">
         <f ca="1">'April 2025 - June 2025'!E163</f>
-        <v>3420.8</v>
+        <v>3480.8</v>
       </c>
       <c r="M16" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+39),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
@@ -37129,7 +37131,7 @@
       </c>
       <c r="J17" s="203">
         <f ca="1">'April 2025 - June 2025'!E190</f>
-        <v>4333.8</v>
+        <v>4393.8</v>
       </c>
       <c r="M17" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+42),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
@@ -37147,7 +37149,7 @@
       </c>
       <c r="J18" s="203">
         <f ca="1">'July 2025 - September 2025'!E136</f>
-        <v>4352.8</v>
+        <v>4412.8</v>
       </c>
       <c r="M18" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+45),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
@@ -37165,7 +37167,7 @@
       </c>
       <c r="J19" s="203">
         <f ca="1">'July 2025 - September 2025'!E163</f>
-        <v>4215.8</v>
+        <v>4275.8</v>
       </c>
     </row>
     <row r="20" ht="35.25" customHeight="1" spans="9:10">
@@ -37175,7 +37177,7 @@
       </c>
       <c r="J20" s="203">
         <f ca="1">'July 2025 - September 2025'!E190</f>
-        <v>4234.8</v>
+        <v>4294.8</v>
       </c>
     </row>
     <row r="21" ht="35.25" customHeight="1" spans="9:10">
@@ -37185,7 +37187,7 @@
       </c>
       <c r="J21" s="203">
         <f ca="1">'October 2025 - December 2025'!E136</f>
-        <v>4147.8</v>
+        <v>4207.8</v>
       </c>
     </row>
     <row r="22" ht="24.75" customHeight="1" spans="1:10">
@@ -37205,7 +37207,7 @@
       </c>
       <c r="J22" s="203">
         <f ca="1">'October 2025 - December 2025'!E163</f>
-        <v>3616.8</v>
+        <v>3676.8</v>
       </c>
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:10">
@@ -37230,7 +37232,7 @@
       </c>
       <c r="J23" s="203">
         <f ca="1">'October 2025 - December 2025'!E190</f>
-        <v>2861.8</v>
+        <v>2921.8</v>
       </c>
     </row>
     <row r="24" ht="52.5" customHeight="1" spans="1:10">
@@ -37255,7 +37257,7 @@
       </c>
       <c r="J24" s="203">
         <f ca="1">'January 2026 - March 2026'!E136</f>
-        <v>3880.8</v>
+        <v>3940.8</v>
       </c>
     </row>
     <row r="25" ht="30" customHeight="1" spans="1:10">
@@ -37274,7 +37276,7 @@
       </c>
       <c r="J25" s="203">
         <f ca="1">'January 2026 - March 2026'!E163</f>
-        <v>4448.8</v>
+        <v>4508.8</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1" spans="1:10">
@@ -37293,7 +37295,7 @@
       </c>
       <c r="J26" s="203">
         <f ca="1">'January 2026 - March 2026'!E190</f>
-        <v>5467.8</v>
+        <v>5527.8</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1" spans="1:10">
@@ -37312,7 +37314,7 @@
       </c>
       <c r="J27" s="203">
         <f ca="1">'April 2026 - June 2026'!E136</f>
-        <v>6195.8</v>
+        <v>6255.8</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:10">
@@ -37331,7 +37333,7 @@
       </c>
       <c r="J28" s="203">
         <f ca="1">'April 2026 - June 2026'!E163</f>
-        <v>7054.8</v>
+        <v>7114.8</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:10">
@@ -37350,7 +37352,7 @@
       </c>
       <c r="J29" s="199">
         <f ca="1">'April 2026 - June 2026'!E190</f>
-        <v>7782.8</v>
+        <v>7842.8</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1" spans="1:10">
@@ -37372,7 +37374,7 @@
       </c>
       <c r="J30" s="206">
         <f ca="1">'July 2026 - September 2026'!E136</f>
-        <v>8801.8</v>
+        <v>8861.8</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1" spans="9:10">
@@ -37382,7 +37384,7 @@
       </c>
       <c r="J31" s="203">
         <f ca="1">'July 2026 - September 2026'!E163</f>
-        <v>9369.8</v>
+        <v>9429.8</v>
       </c>
     </row>
     <row r="32" ht="27.75" customHeight="1" spans="9:10">
@@ -37392,7 +37394,7 @@
       </c>
       <c r="J32" s="203">
         <f ca="1">'July 2026 - September 2026'!E190</f>
-        <v>10388.8</v>
+        <v>10448.8</v>
       </c>
     </row>
     <row r="33" ht="30" customHeight="1" spans="9:10">
@@ -37402,7 +37404,7 @@
       </c>
       <c r="J33" s="203">
         <f ca="1">'October 2026 - December 2026'!E136</f>
-        <v>11116.8</v>
+        <v>11176.8</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1" spans="1:10">
@@ -37422,7 +37424,7 @@
       </c>
       <c r="J34" s="203">
         <f ca="1">'October 2026 - December 2026'!E163</f>
-        <v>11975.8</v>
+        <v>12035.8</v>
       </c>
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:10">
@@ -37447,7 +37449,7 @@
       </c>
       <c r="J35" s="203">
         <f ca="1">'October 2026 - December 2026'!E190</f>
-        <v>12703.8</v>
+        <v>12763.8</v>
       </c>
     </row>
     <row r="36" ht="54.75" customHeight="1" spans="1:10">
@@ -37472,7 +37474,7 @@
       </c>
       <c r="J36" s="203">
         <f ca="1">'January 2027 - March 2027'!E136</f>
-        <v>13722.8</v>
+        <v>13782.8</v>
       </c>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:10">
@@ -37497,7 +37499,7 @@
       </c>
       <c r="J37" s="203">
         <f ca="1">'January 2027 - March 2027'!E163</f>
-        <v>14290.8</v>
+        <v>14350.8</v>
       </c>
     </row>
     <row r="38" ht="20.25" customHeight="1" spans="1:10">
@@ -37522,7 +37524,7 @@
       </c>
       <c r="J38" s="203">
         <f ca="1">'January 2027 - March 2027'!E190</f>
-        <v>15309.8</v>
+        <v>15369.8</v>
       </c>
     </row>
     <row r="39" ht="24.75" customHeight="1" spans="1:10">
@@ -37541,7 +37543,7 @@
       </c>
       <c r="J39" s="203">
         <f ca="1">'April 2027 - June 2027'!E136</f>
-        <v>16037.8</v>
+        <v>16097.8</v>
       </c>
     </row>
     <row r="40" ht="24.75" customHeight="1" spans="1:10">
@@ -37560,7 +37562,7 @@
       </c>
       <c r="J40" s="203">
         <f ca="1">'April 2027 - June 2027'!E163</f>
-        <v>16896.8</v>
+        <v>16956.8</v>
       </c>
     </row>
     <row r="41" ht="24.75" customHeight="1" spans="1:10">
@@ -37579,7 +37581,7 @@
       </c>
       <c r="J41" s="203">
         <f ca="1">'April 2027 - June 2027'!E190</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:10">
@@ -37601,7 +37603,7 @@
       </c>
       <c r="J42" s="203">
         <f ca="1">Forecast_14!E136</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="9:10">
@@ -37611,7 +37613,7 @@
       </c>
       <c r="J43" s="203">
         <f ca="1">Forecast_14!E163</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
     </row>
     <row r="44" ht="24.75" customHeight="1" spans="9:10">
@@ -37621,7 +37623,7 @@
       </c>
       <c r="J44" s="203">
         <f ca="1">Forecast_14!E190</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
     </row>
     <row r="45" ht="24.75" customHeight="1" spans="9:10">
@@ -37631,7 +37633,7 @@
       </c>
       <c r="J45" s="203">
         <f ca="1">Forecast_15!E136</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
     </row>
     <row r="46" ht="24.75" customHeight="1" spans="1:10">
@@ -37651,7 +37653,7 @@
       </c>
       <c r="J46" s="203">
         <f ca="1">Forecast_15!E163</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
     </row>
     <row r="47" ht="24.75" customHeight="1" spans="1:10">
@@ -37676,7 +37678,7 @@
       </c>
       <c r="J47" s="203">
         <f ca="1">Forecast_15!E190</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
     </row>
     <row r="48" ht="24.75" customHeight="1" spans="1:10">
@@ -37701,7 +37703,7 @@
       </c>
       <c r="J48" s="203">
         <f ca="1">Forecast_16!E136</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
     </row>
     <row r="49" ht="24.75" customHeight="1" spans="1:10">
@@ -37726,7 +37728,7 @@
       </c>
       <c r="J49" s="203">
         <f ca="1">Forecast_16!E163</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
     </row>
     <row r="50" ht="24.75" customHeight="1" spans="1:10">
@@ -37751,7 +37753,7 @@
       </c>
       <c r="J50" s="199">
         <f ca="1">Forecast_16!E190</f>
-        <v>17624.8</v>
+        <v>17684.8</v>
       </c>
     </row>
     <row r="51" ht="41" customHeight="1" spans="1:7">
@@ -39701,7 +39703,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>503.8</v>
+        <v>563.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -39729,7 +39731,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1006.51</v>
+        <v>1066.51</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -43154,7 +43156,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>503.8</v>
+        <v>563.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -43182,7 +43184,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>677.140000000001</v>
+        <v>737.140000000001</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -46669,8 +46671,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -46704,7 +46706,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>503.8</v>
+        <v>563.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -46720,7 +46722,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>503.800000000001</v>
+        <v>563.800000000001</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -46736,7 +46738,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1007.6</v>
+        <v>1127.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -47264,7 +47266,7 @@
       <c r="H37" s="14"/>
       <c r="I37" s="47"/>
     </row>
-    <row r="38" ht="24.75" customHeight="1" spans="1:9">
+    <row r="38" ht="51" customHeight="1" spans="1:9">
       <c r="A38" s="19" t="s">
         <v>233</v>
       </c>
@@ -47277,7 +47279,7 @@
       </c>
       <c r="E38" s="22"/>
       <c r="F38" s="41">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="G38" s="42"/>
       <c r="H38" s="14"/>
@@ -47306,7 +47308,7 @@
       <c r="E40" s="44"/>
       <c r="F40" s="45">
         <f>SUM(F34:G39)</f>
-        <v>3487</v>
+        <v>3547</v>
       </c>
       <c r="G40" s="46"/>
       <c r="H40" s="14"/>
@@ -49643,7 +49645,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>503.800000000001</v>
+        <v>563.800000000001</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -50218,7 +50220,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>503.8</v>
+        <v>563.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -50234,7 +50236,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>4333.8</v>
+        <v>4393.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -50250,7 +50252,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>4837.6</v>
+        <v>4957.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -52105,7 +52107,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!E190")</f>
-        <v>503.800000000001</v>
+        <v>563.800000000001</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -52379,7 +52381,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>1416.8</v>
+        <v>1476.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -52471,7 +52473,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>1416.8</v>
+        <v>1476.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -52745,7 +52747,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>3420.8</v>
+        <v>3480.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -52837,7 +52839,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>3420.8</v>
+        <v>3480.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -53111,7 +53113,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>4333.8</v>
+        <v>4393.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -53661,7 +53663,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>503.8</v>
+        <v>563.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -53677,7 +53679,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>4234.8</v>
+        <v>4294.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -53693,7 +53695,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>4738.6</v>
+        <v>4858.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -55540,7 +55542,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!E190")</f>
-        <v>4333.8</v>
+        <v>4393.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -55814,7 +55816,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>4352.8</v>
+        <v>4412.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -55906,7 +55908,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>4352.8</v>
+        <v>4412.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -56180,7 +56182,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>4215.8</v>
+        <v>4275.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -56272,7 +56274,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>4215.8</v>
+        <v>4275.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -56546,7 +56548,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>4234.8</v>
+        <v>4294.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -57090,7 +57092,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>503.8</v>
+        <v>563.8</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -57106,7 +57108,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>2861.8</v>
+        <v>2921.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -57122,7 +57124,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>3365.6</v>
+        <v>3485.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -58969,7 +58971,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!E190")</f>
-        <v>4234.8</v>
+        <v>4294.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -59243,7 +59245,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>4147.8</v>
+        <v>4207.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -59335,7 +59337,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>4147.8</v>
+        <v>4207.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -59611,7 +59613,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>3616.8</v>
+        <v>3676.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -59703,7 +59705,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>3616.8</v>
+        <v>3676.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -59979,7 +59981,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>2861.8</v>
+        <v>2921.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>

</xml_diff>

<commit_message>
docs: 1. Updated Expenses. 2. Updated Transport and Food Expenses.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560" activeTab="5"/>
+    <workbookView windowHeight="21560" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="293">
   <si>
     <t>Income Forecast</t>
   </si>
@@ -1184,7 +1184,9 @@
 - Trip to Eldery Center ~ $9.5
 - Quaker Oat ~ $20
 - Satay King Restaurant ~ $83
-- Best Mart 360 Chocolate ~ $30</t>
+- Best Mart 360 Chocolate ~ $30
+- Devondale Milk ParknShop ~ $107.4
+- Best Mart Granola 500gm ~ $36</t>
   </si>
   <si>
     <t>3. Brought a Brother Printer For $999</t>
@@ -1214,28 +1216,20 @@
   </si>
   <si>
     <t>Food And Transport Expenses
-- Oats 1.6kg  ~ $36
-- Chicken 15 piecies ~ $150
-- Vegetables 6kg ~ $48
+- Quaker Oats 1.6kg ~ $40
+- Chicken 21 piecies ~ $231
+- Vegetables 6kg ~ $60
 - Rice 5kg ~ $49
-- Edo Pack Biscuit $45
-- Edo Pack Oat Biscuit $39 
-- Longevity Filled Evaporated 3 cans $33</t>
+- Milk 1 Litre 8 boxes ~ $143.2
+- Nissan Granola 500gm ~ $36
+- Longevity Filled Evaporated Milk 3 cans ~ $27
+- Julie’s Lemond Cheese Biz (3 packets) ~ $53.7</t>
   </si>
   <si>
     <t>Additional Expense
     - Cigarette Egg - $650
     - See the psycharitic Doctor For Injection ~ $19
     - See the high blood pressure Doctor ~ $50</t>
-  </si>
-  <si>
-    <t>Food And Transport Expenses
-- Oats 1.5kg  ~ $27
-- Chicken 15 piecies ~ $165
-- Marie Biscuit 3 Packets ~ $49.7
-- Vegetables 6kg ~ $48
-- Apples 30 ones ~ $60
-- Rice 5kg ~ $49</t>
   </si>
   <si>
     <t>31st July 2025</t>
@@ -1258,16 +1252,6 @@
     - See the psycharitic Doctor For Injection ~ $19
     - Add In value for Google Play ~ $150 (don't need to
    include.)</t>
-  </si>
-  <si>
-    <t>Food And Transport Expenses
-Health Diet (Without Milk)
-- Oats 1.5kg  ~ $27
-- Chicken 15 piecies ~ $165
-- Marie Biscuit 2 Packets ~ $36
-- Vegetables 6kg ~ $48
-- Apples 30 ones ~ $43
-- Rice 5kg ~ $55</t>
   </si>
   <si>
     <t>Additional Expense
@@ -5668,7 +5652,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A163" workbookViewId="0">
+    <sheetView topLeftCell="A162" workbookViewId="0">
       <selection activeCell="F184" sqref="F184"/>
     </sheetView>
   </sheetViews>
@@ -5703,7 +5687,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>533.8</v>
+        <v>390.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -5719,7 +5703,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>5497.8</v>
+        <v>2475.6</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -5735,7 +5719,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>6031.6</v>
+        <v>2866</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -5834,7 +5818,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -6008,7 +5992,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -6182,7 +6166,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -7586,7 +7570,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!E190")</f>
-        <v>2891.8</v>
+        <v>589.300000000002</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -7755,7 +7739,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -7774,7 +7758,7 @@
       </c>
       <c r="D130" s="100"/>
       <c r="E130" s="102">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F130" s="14"/>
       <c r="G130" s="14"/>
@@ -7858,7 +7842,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>3910.8</v>
+        <v>1368.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -7950,7 +7934,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>3910.8</v>
+        <v>1368.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -8119,7 +8103,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D156" s="103"/>
       <c r="E156" s="101">
@@ -8138,7 +8122,7 @@
       </c>
       <c r="D157" s="100"/>
       <c r="E157" s="102">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F157" s="14"/>
       <c r="G157" s="14"/>
@@ -8222,7 +8206,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>4478.8</v>
+        <v>1696.5</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -8314,7 +8298,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>4478.8</v>
+        <v>1696.5</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -8483,7 +8467,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -8502,7 +8486,7 @@
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="102">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F184" s="14"/>
       <c r="G184" s="14"/>
@@ -8586,7 +8570,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>5497.8</v>
+        <v>2475.6</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -9081,7 +9065,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A165" workbookViewId="0">
+    <sheetView topLeftCell="A166" workbookViewId="0">
       <selection activeCell="F184" sqref="F184"/>
     </sheetView>
   </sheetViews>
@@ -9116,7 +9100,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>533.8</v>
+        <v>390.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -9132,7 +9116,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>7812.8</v>
+        <v>4070.9</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -9148,7 +9132,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>8346.6</v>
+        <v>4461.3</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -9247,7 +9231,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -9421,7 +9405,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -9595,7 +9579,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -10999,7 +10983,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!E190")</f>
-        <v>5497.8</v>
+        <v>2475.6</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -11168,7 +11152,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -11187,7 +11171,7 @@
       </c>
       <c r="D130" s="100"/>
       <c r="E130" s="102">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F130" s="14"/>
       <c r="G130" s="14"/>
@@ -11271,7 +11255,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>6225.8</v>
+        <v>2963.7</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -11363,7 +11347,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>6225.8</v>
+        <v>2963.7</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -11532,7 +11516,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
@@ -11551,7 +11535,7 @@
       </c>
       <c r="D157" s="100"/>
       <c r="E157" s="102">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F157" s="14"/>
       <c r="G157" s="14"/>
@@ -11635,7 +11619,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>7084.8</v>
+        <v>3582.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -11727,7 +11711,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>7084.8</v>
+        <v>3582.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -11896,7 +11880,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D183" s="103"/>
       <c r="E183" s="101">
@@ -11915,7 +11899,7 @@
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="102">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F184" s="14"/>
       <c r="G184" s="14"/>
@@ -11999,7 +11983,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>7812.8</v>
+        <v>4070.9</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -12494,8 +12478,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="F184" sqref="F184"/>
+    <sheetView topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="F130" sqref="F130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -12530,7 +12514,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>533.8</v>
+        <v>390.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -12546,7 +12530,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>10418.8</v>
+        <v>5957.2</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -12562,7 +12546,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>10952.6</v>
+        <v>6347.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -12661,7 +12645,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -12835,7 +12819,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -13009,7 +12993,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -14413,7 +14397,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!E190")</f>
-        <v>7812.8</v>
+        <v>4070.9</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -14582,7 +14566,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -14601,7 +14585,7 @@
       </c>
       <c r="D130" s="100"/>
       <c r="E130" s="102">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F130" s="14"/>
       <c r="G130" s="14"/>
@@ -14685,7 +14669,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>8831.8</v>
+        <v>4850</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -14777,7 +14761,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>8831.8</v>
+        <v>4850</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -14946,7 +14930,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D156" s="103"/>
       <c r="E156" s="101">
@@ -14965,7 +14949,7 @@
       </c>
       <c r="D157" s="100"/>
       <c r="E157" s="102">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F157" s="14"/>
       <c r="G157" s="14"/>
@@ -15049,7 +15033,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>9399.8</v>
+        <v>5178.1</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -15141,7 +15125,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>9399.8</v>
+        <v>5178.1</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -15310,7 +15294,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -15329,7 +15313,7 @@
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="102">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F184" s="14"/>
       <c r="G184" s="14"/>
@@ -15413,7 +15397,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>10418.8</v>
+        <v>5957.2</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -15908,8 +15892,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="F184" sqref="F184"/>
+    <sheetView topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="F191" sqref="F191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -15942,7 +15926,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>533.8</v>
+        <v>390.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -15958,7 +15942,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>12733.8</v>
+        <v>7552.50000000001</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -15974,7 +15958,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>13267.6</v>
+        <v>7942.90000000001</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -16073,7 +16057,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -16247,7 +16231,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -16421,7 +16405,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -17825,7 +17809,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!E190")</f>
-        <v>10418.8</v>
+        <v>5957.2</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -17994,7 +17978,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -18013,7 +17997,7 @@
       </c>
       <c r="D130" s="100"/>
       <c r="E130" s="102">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F130" s="14"/>
       <c r="G130" s="14"/>
@@ -18097,7 +18081,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>11146.8</v>
+        <v>6445.3</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -18189,7 +18173,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>11146.8</v>
+        <v>6445.3</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -18358,7 +18342,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
@@ -18377,7 +18361,7 @@
       </c>
       <c r="D157" s="100"/>
       <c r="E157" s="102">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F157" s="14"/>
       <c r="G157" s="14"/>
@@ -18461,7 +18445,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>12005.8</v>
+        <v>7064.40000000001</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -18553,7 +18537,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>12005.8</v>
+        <v>7064.40000000001</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -18722,7 +18706,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -18741,7 +18725,7 @@
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="102">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F184" s="14"/>
       <c r="G184" s="14"/>
@@ -18825,7 +18809,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>12733.8</v>
+        <v>7552.50000000001</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -19320,8 +19304,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="F183" sqref="F183"/>
+    <sheetView topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="F130" sqref="F130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -19356,7 +19340,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>533.8</v>
+        <v>390.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -19372,7 +19356,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>15339.8</v>
+        <v>9438.80000000001</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -19388,7 +19372,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>15873.6</v>
+        <v>9829.20000000001</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -19487,7 +19471,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -19661,7 +19645,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -19835,7 +19819,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -21239,7 +21223,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!E190")</f>
-        <v>12733.8</v>
+        <v>7552.50000000001</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -21408,7 +21392,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -21427,7 +21411,7 @@
       </c>
       <c r="D130" s="100"/>
       <c r="E130" s="102">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F130" s="14"/>
       <c r="G130" s="14"/>
@@ -21511,7 +21495,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>13752.8</v>
+        <v>8331.60000000001</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -21603,7 +21587,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>13752.8</v>
+        <v>8331.60000000001</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -21772,7 +21756,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
@@ -21791,7 +21775,7 @@
       </c>
       <c r="D157" s="100"/>
       <c r="E157" s="102">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F157" s="14"/>
       <c r="G157" s="14"/>
@@ -21875,7 +21859,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>14320.8</v>
+        <v>8659.70000000001</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -21967,7 +21951,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>14320.8</v>
+        <v>8659.70000000001</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -22136,7 +22120,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -22155,7 +22139,7 @@
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="102">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F184" s="14"/>
       <c r="G184" s="14"/>
@@ -22239,7 +22223,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>15339.8</v>
+        <v>9438.80000000001</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -22734,8 +22718,8 @@
   <sheetPr/>
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="F184" sqref="F184"/>
+    <sheetView topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="F185" sqref="F185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -22768,7 +22752,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>533.8</v>
+        <v>390.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -22784,7 +22768,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -22800,7 +22784,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>18188.6</v>
+        <v>11424.5</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -22899,7 +22883,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -23073,7 +23057,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -23247,7 +23231,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -24651,7 +24635,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!E190")</f>
-        <v>15339.8</v>
+        <v>9438.80000000001</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -24820,7 +24804,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -24839,7 +24823,7 @@
       </c>
       <c r="D130" s="100"/>
       <c r="E130" s="102">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F130" s="14"/>
       <c r="G130" s="14"/>
@@ -24923,7 +24907,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>16067.8</v>
+        <v>9926.90000000001</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -25015,7 +24999,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>16067.8</v>
+        <v>9926.90000000001</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -25184,7 +25168,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
@@ -25203,7 +25187,7 @@
       </c>
       <c r="D157" s="100"/>
       <c r="E157" s="102">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F157" s="14"/>
       <c r="G157" s="14"/>
@@ -25287,7 +25271,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>16926.8</v>
+        <v>10546</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -25379,7 +25363,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>16926.8</v>
+        <v>10546</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -25548,7 +25532,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -25567,7 +25551,7 @@
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="102">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F184" s="14"/>
       <c r="G184" s="14"/>
@@ -25651,7 +25635,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -26181,7 +26165,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>533.8</v>
+        <v>390.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -26197,7 +26181,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -26213,7 +26197,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>18188.6</v>
+        <v>11424.5</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -28022,7 +28006,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!E190")</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -28290,7 +28274,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -28382,7 +28366,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -28650,7 +28634,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -28742,7 +28726,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -29010,7 +28994,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -29487,7 +29471,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>533.8</v>
+        <v>390.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -29503,7 +29487,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -29519,7 +29503,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>18188.6</v>
+        <v>11424.5</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -31097,7 +31081,7 @@
         <v>Bankruptcy Department / Bank</v>
       </c>
       <c r="B102" s="37" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C102" s="36" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C102")+SUM(E122+E149+E176)</f>
@@ -31327,7 +31311,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!E190")</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -31595,7 +31579,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -31687,7 +31671,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -31955,7 +31939,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -32047,7 +32031,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -32315,7 +32299,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -32794,7 +32778,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>533.8</v>
+        <v>390.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -32810,7 +32794,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -32826,7 +32810,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>18188.6</v>
+        <v>11424.5</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -34635,7 +34619,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!E190")</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -34903,7 +34887,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -34995,7 +34979,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -35263,7 +35247,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -35355,7 +35339,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -35623,7 +35607,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -36606,7 +36590,7 @@
   <dimension ref="A1:N204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -36677,7 +36661,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="162">
-        <v>345.4</v>
+        <v>212</v>
       </c>
       <c r="D3" s="163" t="s">
         <v>33</v>
@@ -36686,7 +36670,7 @@
         <v>34</v>
       </c>
       <c r="F3" s="190">
-        <v>385.4</v>
+        <v>248</v>
       </c>
       <c r="I3" s="198" t="str">
         <f>TEXT(Main!B3,"dd mmmm yyyy")&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,1)-1,"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)*1,"dd mmmm yyyy"))</f>
@@ -36807,7 +36791,7 @@
         <v>38</v>
       </c>
       <c r="C7" s="162">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D7" s="164"/>
       <c r="E7" s="5" t="s">
@@ -37048,7 +37032,7 @@
       </c>
       <c r="J14" s="203">
         <f ca="1">'January 2025 - March 2025'!E190</f>
-        <v>533.800000000001</v>
+        <v>390.400000000001</v>
       </c>
       <c r="M14" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,33),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*33+33),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,36)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+35),"dd mmmm yyyy"))</f>
@@ -37080,7 +37064,7 @@
       </c>
       <c r="J15" s="203">
         <f ca="1">'April 2025 - June 2025'!E136</f>
-        <v>1446.8</v>
+        <v>1063.5</v>
       </c>
       <c r="M15" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,36),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*36+36),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,39)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+38),"dd mmmm yyyy"))</f>
@@ -37098,7 +37082,7 @@
       </c>
       <c r="C16" s="168">
         <f>SUM(C3:C15)</f>
-        <v>533.8</v>
+        <v>390.4</v>
       </c>
       <c r="D16" s="169"/>
       <c r="E16" s="167" t="s">
@@ -37106,7 +37090,7 @@
       </c>
       <c r="F16" s="193">
         <f>SUM(F3:F15)</f>
-        <v>563.8</v>
+        <v>426.4</v>
       </c>
       <c r="I16" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,13),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*13)+13,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,14)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*14+13),"dd mmmm yyyy"))</f>
@@ -37114,7 +37098,7 @@
       </c>
       <c r="J16" s="203">
         <f ca="1">'April 2025 - June 2025'!E163</f>
-        <v>3450.8</v>
+        <v>2827.6</v>
       </c>
       <c r="M16" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+39),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
@@ -37132,7 +37116,7 @@
       </c>
       <c r="J17" s="203">
         <f ca="1">'April 2025 - June 2025'!E190</f>
-        <v>4363.8</v>
+        <v>3500.7</v>
       </c>
       <c r="M17" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+42),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
@@ -37150,7 +37134,7 @@
       </c>
       <c r="J18" s="203">
         <f ca="1">'July 2025 - September 2025'!E136</f>
-        <v>4382.8</v>
+        <v>3279.8</v>
       </c>
       <c r="M18" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+45),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
@@ -37168,7 +37152,7 @@
       </c>
       <c r="J19" s="203">
         <f ca="1">'July 2025 - September 2025'!E163</f>
-        <v>4245.8</v>
+        <v>2902.9</v>
       </c>
     </row>
     <row r="20" ht="35.25" customHeight="1" spans="9:10">
@@ -37178,7 +37162,7 @@
       </c>
       <c r="J20" s="203">
         <f ca="1">'July 2025 - September 2025'!E190</f>
-        <v>4264.8</v>
+        <v>2682</v>
       </c>
     </row>
     <row r="21" ht="35.25" customHeight="1" spans="9:10">
@@ -37188,7 +37172,7 @@
       </c>
       <c r="J21" s="203">
         <f ca="1">'October 2025 - December 2025'!E136</f>
-        <v>4177.8</v>
+        <v>2355.1</v>
       </c>
     </row>
     <row r="22" ht="24.75" customHeight="1" spans="1:10">
@@ -37208,7 +37192,7 @@
       </c>
       <c r="J22" s="203">
         <f ca="1">'October 2025 - December 2025'!E163</f>
-        <v>3646.8</v>
+        <v>1584.2</v>
       </c>
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:10">
@@ -37233,7 +37217,7 @@
       </c>
       <c r="J23" s="203">
         <f ca="1">'October 2025 - December 2025'!E190</f>
-        <v>2891.8</v>
+        <v>589.300000000002</v>
       </c>
     </row>
     <row r="24" ht="52.5" customHeight="1" spans="1:10">
@@ -37258,7 +37242,7 @@
       </c>
       <c r="J24" s="203">
         <f ca="1">'January 2026 - March 2026'!E136</f>
-        <v>3910.8</v>
+        <v>1368.4</v>
       </c>
     </row>
     <row r="25" ht="30" customHeight="1" spans="1:10">
@@ -37277,7 +37261,7 @@
       </c>
       <c r="J25" s="203">
         <f ca="1">'January 2026 - March 2026'!E163</f>
-        <v>4478.8</v>
+        <v>1696.5</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1" spans="1:10">
@@ -37296,7 +37280,7 @@
       </c>
       <c r="J26" s="203">
         <f ca="1">'January 2026 - March 2026'!E190</f>
-        <v>5497.8</v>
+        <v>2475.6</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1" spans="1:10">
@@ -37315,7 +37299,7 @@
       </c>
       <c r="J27" s="203">
         <f ca="1">'April 2026 - June 2026'!E136</f>
-        <v>6225.8</v>
+        <v>2963.7</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1" spans="1:10">
@@ -37334,7 +37318,7 @@
       </c>
       <c r="J28" s="203">
         <f ca="1">'April 2026 - June 2026'!E163</f>
-        <v>7084.8</v>
+        <v>3582.8</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1" spans="1:10">
@@ -37353,7 +37337,7 @@
       </c>
       <c r="J29" s="199">
         <f ca="1">'April 2026 - June 2026'!E190</f>
-        <v>7812.8</v>
+        <v>4070.9</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1" spans="1:10">
@@ -37375,7 +37359,7 @@
       </c>
       <c r="J30" s="206">
         <f ca="1">'July 2026 - September 2026'!E136</f>
-        <v>8831.8</v>
+        <v>4850</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1" spans="9:10">
@@ -37385,7 +37369,7 @@
       </c>
       <c r="J31" s="203">
         <f ca="1">'July 2026 - September 2026'!E163</f>
-        <v>9399.8</v>
+        <v>5178.1</v>
       </c>
     </row>
     <row r="32" ht="27.75" customHeight="1" spans="9:10">
@@ -37395,7 +37379,7 @@
       </c>
       <c r="J32" s="203">
         <f ca="1">'July 2026 - September 2026'!E190</f>
-        <v>10418.8</v>
+        <v>5957.2</v>
       </c>
     </row>
     <row r="33" ht="30" customHeight="1" spans="9:10">
@@ -37405,7 +37389,7 @@
       </c>
       <c r="J33" s="203">
         <f ca="1">'October 2026 - December 2026'!E136</f>
-        <v>11146.8</v>
+        <v>6445.3</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1" spans="1:10">
@@ -37425,7 +37409,7 @@
       </c>
       <c r="J34" s="203">
         <f ca="1">'October 2026 - December 2026'!E163</f>
-        <v>12005.8</v>
+        <v>7064.40000000001</v>
       </c>
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:10">
@@ -37450,7 +37434,7 @@
       </c>
       <c r="J35" s="203">
         <f ca="1">'October 2026 - December 2026'!E190</f>
-        <v>12733.8</v>
+        <v>7552.50000000001</v>
       </c>
     </row>
     <row r="36" ht="54.75" customHeight="1" spans="1:10">
@@ -37475,7 +37459,7 @@
       </c>
       <c r="J36" s="203">
         <f ca="1">'January 2027 - March 2027'!E136</f>
-        <v>13752.8</v>
+        <v>8331.60000000001</v>
       </c>
     </row>
     <row r="37" ht="24.75" customHeight="1" spans="1:10">
@@ -37500,7 +37484,7 @@
       </c>
       <c r="J37" s="203">
         <f ca="1">'January 2027 - March 2027'!E163</f>
-        <v>14320.8</v>
+        <v>8659.70000000001</v>
       </c>
     </row>
     <row r="38" ht="20.25" customHeight="1" spans="1:10">
@@ -37525,7 +37509,7 @@
       </c>
       <c r="J38" s="203">
         <f ca="1">'January 2027 - March 2027'!E190</f>
-        <v>15339.8</v>
+        <v>9438.80000000001</v>
       </c>
     </row>
     <row r="39" ht="24.75" customHeight="1" spans="1:10">
@@ -37544,7 +37528,7 @@
       </c>
       <c r="J39" s="203">
         <f ca="1">'April 2027 - June 2027'!E136</f>
-        <v>16067.8</v>
+        <v>9926.90000000001</v>
       </c>
     </row>
     <row r="40" ht="24.75" customHeight="1" spans="1:10">
@@ -37563,7 +37547,7 @@
       </c>
       <c r="J40" s="203">
         <f ca="1">'April 2027 - June 2027'!E163</f>
-        <v>16926.8</v>
+        <v>10546</v>
       </c>
     </row>
     <row r="41" ht="24.75" customHeight="1" spans="1:10">
@@ -37582,7 +37566,7 @@
       </c>
       <c r="J41" s="203">
         <f ca="1">'April 2027 - June 2027'!E190</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
     </row>
     <row r="42" ht="24.75" customHeight="1" spans="1:10">
@@ -37604,7 +37588,7 @@
       </c>
       <c r="J42" s="203">
         <f ca="1">Forecast_14!E136</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
     </row>
     <row r="43" ht="24.75" customHeight="1" spans="9:10">
@@ -37614,7 +37598,7 @@
       </c>
       <c r="J43" s="203">
         <f ca="1">Forecast_14!E163</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
     </row>
     <row r="44" ht="24.75" customHeight="1" spans="9:10">
@@ -37624,7 +37608,7 @@
       </c>
       <c r="J44" s="203">
         <f ca="1">Forecast_14!E190</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
     </row>
     <row r="45" ht="24.75" customHeight="1" spans="9:10">
@@ -37634,7 +37618,7 @@
       </c>
       <c r="J45" s="203">
         <f ca="1">Forecast_15!E136</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
     </row>
     <row r="46" ht="24.75" customHeight="1" spans="1:10">
@@ -37654,7 +37638,7 @@
       </c>
       <c r="J46" s="203">
         <f ca="1">Forecast_15!E163</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
     </row>
     <row r="47" ht="24.75" customHeight="1" spans="1:10">
@@ -37679,7 +37663,7 @@
       </c>
       <c r="J47" s="203">
         <f ca="1">Forecast_15!E190</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
     </row>
     <row r="48" ht="24.75" customHeight="1" spans="1:10">
@@ -37704,7 +37688,7 @@
       </c>
       <c r="J48" s="203">
         <f ca="1">Forecast_16!E136</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
     </row>
     <row r="49" ht="24.75" customHeight="1" spans="1:10">
@@ -37729,7 +37713,7 @@
       </c>
       <c r="J49" s="203">
         <f ca="1">Forecast_16!E163</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
     </row>
     <row r="50" ht="24.75" customHeight="1" spans="1:10">
@@ -37754,7 +37738,7 @@
       </c>
       <c r="J50" s="199">
         <f ca="1">Forecast_16!E190</f>
-        <v>17654.8</v>
+        <v>11034.1</v>
       </c>
     </row>
     <row r="51" ht="41" customHeight="1" spans="1:7">
@@ -39704,7 +39688,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>533.8</v>
+        <v>390.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -39732,7 +39716,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1036.51</v>
+        <v>893.11</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -43157,7 +43141,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>533.8</v>
+        <v>390.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -43185,7 +43169,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>707.140000000001</v>
+        <v>563.740000000001</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -46672,8 +46656,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="C187" sqref="C187:D187"/>
+    <sheetView topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="F184" sqref="F184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -46707,7 +46691,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>533.8</v>
+        <v>390.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -46723,7 +46707,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>533.800000000001</v>
+        <v>390.400000000001</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -46739,7 +46723,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1067.6</v>
+        <v>780.800000000001</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -49560,7 +49544,7 @@
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="102">
-        <v>672.4</v>
+        <v>815.8</v>
       </c>
       <c r="F184" s="14"/>
       <c r="G184" s="14"/>
@@ -49646,7 +49630,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>533.800000000001</v>
+        <v>390.400000000001</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -50185,8 +50169,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A183" workbookViewId="0">
-      <selection activeCell="F130" sqref="F130"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="F157" sqref="F157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -50221,7 +50205,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>533.8</v>
+        <v>390.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -50237,7 +50221,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>4363.8</v>
+        <v>3500.7</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -50253,7 +50237,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>4897.6</v>
+        <v>3891.1</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -52108,7 +52092,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!E190")</f>
-        <v>533.800000000001</v>
+        <v>390.400000000001</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -52290,7 +52274,7 @@
       <c r="H129" s="14"/>
       <c r="I129" s="47"/>
     </row>
-    <row r="130" ht="148" customHeight="1" spans="1:9">
+    <row r="130" ht="197" customHeight="1" spans="1:9">
       <c r="A130" s="62"/>
       <c r="B130" s="63"/>
       <c r="C130" s="113" t="s">
@@ -52298,7 +52282,7 @@
       </c>
       <c r="D130" s="114"/>
       <c r="E130" s="98">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F130" s="14"/>
       <c r="G130" s="14"/>
@@ -52382,7 +52366,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>1446.8</v>
+        <v>1063.5</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -52474,7 +52458,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>1446.8</v>
+        <v>1063.5</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -52656,7 +52640,7 @@
       <c r="H156" s="14"/>
       <c r="I156" s="47"/>
     </row>
-    <row r="157" ht="145" customHeight="1" spans="1:9">
+    <row r="157" ht="185" customHeight="1" spans="1:9">
       <c r="A157" s="62"/>
       <c r="B157" s="63"/>
       <c r="C157" s="100" t="s">
@@ -52664,7 +52648,7 @@
       </c>
       <c r="D157" s="100"/>
       <c r="E157" s="98">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F157" s="14"/>
       <c r="G157" s="14"/>
@@ -52748,7 +52732,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>3450.8</v>
+        <v>2827.6</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -52840,7 +52824,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>3450.8</v>
+        <v>2827.6</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -53022,15 +53006,15 @@
       <c r="H183" s="14"/>
       <c r="I183" s="47"/>
     </row>
-    <row r="184" ht="135" customHeight="1" spans="1:9">
+    <row r="184" ht="184" customHeight="1" spans="1:9">
       <c r="A184" s="62"/>
       <c r="B184" s="63"/>
       <c r="C184" s="100" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="98">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F184" s="14"/>
       <c r="G184" s="14"/>
@@ -53114,7 +53098,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>4363.8</v>
+        <v>3500.7</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -53630,8 +53614,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="F184" sqref="F184"/>
+    <sheetView topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="E184" sqref="E184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -53664,7 +53648,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>533.8</v>
+        <v>390.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -53680,7 +53664,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>4264.8</v>
+        <v>2682</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -53696,7 +53680,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>4798.6</v>
+        <v>3072.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -53795,7 +53779,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -53815,11 +53799,11 @@
     <row r="12" ht="24.75" customHeight="1" spans="1:9">
       <c r="A12" s="95"/>
       <c r="B12" s="96" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C12" s="96"/>
       <c r="D12" s="97" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E12" s="97"/>
       <c r="F12" s="7">
@@ -53969,7 +53953,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -54143,7 +54127,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -55543,7 +55527,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!E190")</f>
-        <v>4363.8</v>
+        <v>3500.7</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -55714,7 +55698,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="100" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D129" s="100"/>
       <c r="E129" s="98">
@@ -55725,15 +55709,15 @@
       <c r="H129" s="14"/>
       <c r="I129" s="47"/>
     </row>
-    <row r="130" ht="149" customHeight="1" spans="1:9">
+    <row r="130" ht="208" customHeight="1" spans="1:9">
       <c r="A130" s="62"/>
       <c r="B130" s="63"/>
       <c r="C130" s="100" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="D130" s="100"/>
       <c r="E130" s="98">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F130" s="14"/>
       <c r="G130" s="14"/>
@@ -55817,7 +55801,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>4382.8</v>
+        <v>3279.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -55909,7 +55893,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>4382.8</v>
+        <v>3279.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -56080,7 +56064,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="100" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D156" s="100"/>
       <c r="E156" s="98">
@@ -56091,7 +56075,7 @@
       <c r="H156" s="14"/>
       <c r="I156" s="47"/>
     </row>
-    <row r="157" ht="156" customHeight="1" spans="1:9">
+    <row r="157" ht="180" customHeight="1" spans="1:9">
       <c r="A157" s="62"/>
       <c r="B157" s="63"/>
       <c r="C157" s="100" t="s">
@@ -56099,7 +56083,7 @@
       </c>
       <c r="D157" s="100"/>
       <c r="E157" s="98">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F157" s="14"/>
       <c r="G157" s="14"/>
@@ -56183,7 +56167,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>4245.8</v>
+        <v>2902.9</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -56275,7 +56259,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>4245.8</v>
+        <v>2902.9</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -56446,7 +56430,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="100" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D183" s="100"/>
       <c r="E183" s="98">
@@ -56457,7 +56441,7 @@
       <c r="H183" s="14"/>
       <c r="I183" s="47"/>
     </row>
-    <row r="184" ht="149" customHeight="1" spans="1:9">
+    <row r="184" ht="194" customHeight="1" spans="1:9">
       <c r="A184" s="62"/>
       <c r="B184" s="63"/>
       <c r="C184" s="100" t="s">
@@ -56465,7 +56449,7 @@
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="98">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F184" s="14"/>
       <c r="G184" s="14"/>
@@ -56549,7 +56533,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>4264.8</v>
+        <v>2682</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -57059,7 +57043,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A166" workbookViewId="0">
+    <sheetView topLeftCell="A165" workbookViewId="0">
       <selection activeCell="F184" sqref="F184"/>
     </sheetView>
   </sheetViews>
@@ -57093,7 +57077,7 @@
       </c>
       <c r="C2" s="4" cm="1">
         <f ca="1" t="array" ref="C2">INDIRECT("'"&amp;Main!B9&amp;"'!$C$16")</f>
-        <v>533.8</v>
+        <v>390.4</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -57109,7 +57093,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>2891.8</v>
+        <v>589.300000000002</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -57125,7 +57109,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>3425.6</v>
+        <v>979.700000000002</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -57224,7 +57208,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -57398,7 +57382,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -57568,7 +57552,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -58972,7 +58956,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!E190")</f>
-        <v>4264.8</v>
+        <v>2682</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -59162,7 +59146,7 @@
       </c>
       <c r="D130" s="100"/>
       <c r="E130" s="98">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F130" s="14"/>
       <c r="G130" s="14"/>
@@ -59246,7 +59230,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>4177.8</v>
+        <v>2355.1</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -59338,7 +59322,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>4177.8</v>
+        <v>2355.1</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -59431,7 +59415,7 @@
       <c r="A150" s="62"/>
       <c r="B150" s="63"/>
       <c r="C150" s="64" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D150" s="65"/>
       <c r="E150" s="36">
@@ -59511,7 +59495,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="100" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D156" s="100"/>
       <c r="E156" s="102">
@@ -59530,7 +59514,7 @@
       </c>
       <c r="D157" s="100"/>
       <c r="E157" s="102">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F157" s="14"/>
       <c r="G157" s="14"/>
@@ -59614,7 +59598,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>3646.8</v>
+        <v>1584.2</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -59706,7 +59690,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>3646.8</v>
+        <v>1584.2</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -59732,7 +59716,7 @@
       <c r="A172" s="62"/>
       <c r="B172" s="63"/>
       <c r="C172" s="64" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D172" s="65"/>
       <c r="E172" s="36">
@@ -59799,7 +59783,7 @@
       <c r="A177" s="62"/>
       <c r="B177" s="63"/>
       <c r="C177" s="64" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D177" s="65"/>
       <c r="E177" s="36">
@@ -59879,7 +59863,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="100" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D183" s="100"/>
       <c r="E183" s="98">
@@ -59898,7 +59882,7 @@
       </c>
       <c r="D184" s="100"/>
       <c r="E184" s="98">
-        <v>400</v>
+        <v>639.9</v>
       </c>
       <c r="F184" s="14"/>
       <c r="G184" s="14"/>
@@ -59982,7 +59966,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>2891.8</v>
+        <v>589.300000000002</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>

</xml_diff>

<commit_message>
docs: 1. Update Payback For Mom.
</commit_message>
<xml_diff>
--- a/Income And Expenses Forecast.xlsx
+++ b/Income And Expenses Forecast.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="21560" firstSheet="9" activeTab="14"/>
+    <workbookView windowHeight="21560" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="18" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1523" uniqueCount="290">
   <si>
     <t>Income Forecast</t>
   </si>
@@ -1268,21 +1268,12 @@
     <t>30th December 2025</t>
   </si>
   <si>
-    <t>Payback $500 to Mom For Air Ticket</t>
-  </si>
-  <si>
     <t>Additional Expense
     - Cigarette Egg - $650
     - Add In value for Google Play ~ $150 (don't need to
    include.)
     - See the psycharitic Doctor For Injection ~ $19
     - See the high blood pressure Doctor ~ $50</t>
-  </si>
-  <si>
-    <t>Payback $900 to Mom</t>
-  </si>
-  <si>
-    <t>Payback $583 to Mom For Air Ticket</t>
   </si>
   <si>
     <t>Additional Expense
@@ -1388,7 +1379,7 @@
     <numFmt numFmtId="179" formatCode="mmm\-yy"/>
     <numFmt numFmtId="180" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="47">
+  <fonts count="48">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1513,6 +1504,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
@@ -2545,31 +2542,28 @@
   </borders>
   <cellStyleXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2578,130 +2572,133 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="42" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="13" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="42" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="13" borderId="42" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="13" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="14" borderId="44" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="13" borderId="42" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="45" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="14" borderId="44" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="45" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="42" fillId="3" borderId="47">
+    <xf numFmtId="0" fontId="41" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="43" fillId="3" borderId="47">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="43" fillId="0" borderId="0" applyProtection="0">
+    <xf numFmtId="49" fontId="44" fillId="0" borderId="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="44" fillId="9" borderId="0" applyProtection="0">
+    <xf numFmtId="49" fontId="45" fillId="9" borderId="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="45" fillId="5" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="49" fontId="46" fillId="5" borderId="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" applyProtection="0">
@@ -3319,7 +3316,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="18" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3375,19 +3372,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="180" fontId="9" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3405,7 +3402,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3432,10 +3429,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -5651,7 +5648,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A134" workbookViewId="0">
+    <sheetView topLeftCell="A75" workbookViewId="0">
       <selection activeCell="F130" sqref="F130"/>
     </sheetView>
   </sheetViews>
@@ -5702,7 +5699,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>3120</v>
+        <v>5603</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -5718,7 +5715,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>3510.4</v>
+        <v>5993.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -5734,7 +5731,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -5817,7 +5814,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -5991,7 +5988,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -6165,7 +6162,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -7263,7 +7260,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>0</v>
+        <v>-1400</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -7363,7 +7360,7 @@
       </c>
       <c r="C103" s="36" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>0</v>
+        <v>-1083</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -7459,7 +7456,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -7475,7 +7472,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>-347</v>
+        <v>-2830</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -7569,7 +7566,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B27")&amp;"'!E190")</f>
-        <v>1072.6</v>
+        <v>3555.6</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -7738,7 +7735,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -7749,7 +7746,7 @@
       <c r="H129" s="14"/>
       <c r="I129" s="47"/>
     </row>
-    <row r="130" ht="96" customHeight="1" spans="1:9">
+    <row r="130" ht="28" customHeight="1" spans="1:9">
       <c r="A130" s="62"/>
       <c r="B130" s="63"/>
       <c r="C130" s="100" t="s">
@@ -7841,7 +7838,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>1905.4</v>
+        <v>4388.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -7933,7 +7930,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>1905.4</v>
+        <v>4388.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -8102,7 +8099,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D156" s="103"/>
       <c r="E156" s="101">
@@ -8205,7 +8202,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>2287.2</v>
+        <v>4770.2</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -8297,7 +8294,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>2287.2</v>
+        <v>4770.2</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -8466,7 +8463,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -8569,7 +8566,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>3120</v>
+        <v>5603</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -9115,7 +9112,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>4876.4</v>
+        <v>7359.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -9131,7 +9128,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>5266.8</v>
+        <v>7749.8</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -9147,7 +9144,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -9230,7 +9227,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -9404,7 +9401,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -9578,7 +9575,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -10676,7 +10673,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>0</v>
+        <v>-1400</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -10776,7 +10773,7 @@
       </c>
       <c r="C103" s="36" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>0</v>
+        <v>-1083</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -10872,7 +10869,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -10888,7 +10885,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>-347</v>
+        <v>-2830</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -10982,7 +10979,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B30")&amp;"'!E190")</f>
-        <v>3120</v>
+        <v>5603</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -11151,7 +11148,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -11254,7 +11251,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>3661.8</v>
+        <v>6144.8</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -11346,7 +11343,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>3661.8</v>
+        <v>6144.8</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -11515,7 +11512,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
@@ -11618,7 +11615,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>4334.6</v>
+        <v>6817.6</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -11710,7 +11707,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>4334.6</v>
+        <v>6817.6</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -11879,7 +11876,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D183" s="103"/>
       <c r="E183" s="101">
@@ -11982,7 +11979,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>4876.4</v>
+        <v>7359.4</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -12529,7 +12526,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>6923.8</v>
+        <v>9406.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -12545,7 +12542,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>7314.2</v>
+        <v>9797.2</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -12561,7 +12558,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -12644,7 +12641,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -12818,7 +12815,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -12992,7 +12989,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -14090,7 +14087,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>0</v>
+        <v>-1400</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -14190,7 +14187,7 @@
       </c>
       <c r="C103" s="36" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>0</v>
+        <v>-1083</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -14286,7 +14283,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -14302,7 +14299,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>-347</v>
+        <v>-2830</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -14396,7 +14393,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B33")&amp;"'!E190")</f>
-        <v>4876.4</v>
+        <v>7359.4</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -14565,7 +14562,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -14668,7 +14665,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>5709.2</v>
+        <v>8192.2</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -14760,7 +14757,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>5709.2</v>
+        <v>8192.2</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -14929,7 +14926,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D156" s="103"/>
       <c r="E156" s="101">
@@ -15032,7 +15029,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>6091</v>
+        <v>8574</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -15124,7 +15121,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>6091</v>
+        <v>8574</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -15293,7 +15290,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -15396,7 +15393,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>6923.8</v>
+        <v>9406.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -15891,7 +15888,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" workbookViewId="0">
+    <sheetView topLeftCell="A130" workbookViewId="0">
       <selection activeCell="F130" sqref="F130"/>
     </sheetView>
   </sheetViews>
@@ -15941,7 +15938,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>8680.2</v>
+        <v>11163.2</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -15957,7 +15954,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>9070.6</v>
+        <v>11553.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -15973,7 +15970,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -16056,7 +16053,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -16230,7 +16227,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -16404,7 +16401,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -17502,7 +17499,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>0</v>
+        <v>-1400</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -17602,7 +17599,7 @@
       </c>
       <c r="C103" s="36" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>0</v>
+        <v>-1083</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -17698,7 +17695,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -17714,7 +17711,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>-347</v>
+        <v>-2830</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -17808,7 +17805,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B36")&amp;"'!E190")</f>
-        <v>6923.8</v>
+        <v>9406.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -17977,7 +17974,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -18080,7 +18077,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>7465.6</v>
+        <v>9948.6</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -18172,7 +18169,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>7465.6</v>
+        <v>9948.6</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -18341,7 +18338,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
@@ -18444,7 +18441,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>8138.4</v>
+        <v>10621.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -18536,7 +18533,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>8138.4</v>
+        <v>10621.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -18705,7 +18702,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -18808,7 +18805,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>8680.2</v>
+        <v>11163.2</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -19303,7 +19300,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A117" workbookViewId="0">
+    <sheetView topLeftCell="A131" workbookViewId="0">
       <selection activeCell="F130" sqref="F130"/>
     </sheetView>
   </sheetViews>
@@ -19355,7 +19352,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>10727.6</v>
+        <v>13210.6</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -19371,7 +19368,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>11118</v>
+        <v>13601</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -19387,7 +19384,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -19470,7 +19467,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -19644,7 +19641,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -19818,7 +19815,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -20916,7 +20913,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>0</v>
+        <v>-1400</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -21016,7 +21013,7 @@
       </c>
       <c r="C103" s="36" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>0</v>
+        <v>-1083</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -21112,7 +21109,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -21128,7 +21125,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>-347</v>
+        <v>-2830</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -21222,7 +21219,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B39")&amp;"'!E190")</f>
-        <v>8680.2</v>
+        <v>11163.2</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -21391,7 +21388,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -21494,7 +21491,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>9513</v>
+        <v>11996</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -21586,7 +21583,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>9513</v>
+        <v>11996</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -21755,7 +21752,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
@@ -21858,7 +21855,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>9894.8</v>
+        <v>12377.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -21950,7 +21947,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>9894.8</v>
+        <v>12377.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -22119,7 +22116,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -22222,7 +22219,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>10727.6</v>
+        <v>13210.6</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -22717,7 +22714,7 @@
   <sheetPr/>
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+    <sheetView topLeftCell="A111" workbookViewId="0">
       <selection activeCell="F130" sqref="F130"/>
     </sheetView>
   </sheetViews>
@@ -22767,7 +22764,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -22783,7 +22780,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>12874.4</v>
+        <v>15357.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -22799,7 +22796,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -22882,7 +22879,7 @@
     </row>
     <row r="11" ht="24.75" customHeight="1" spans="1:9">
       <c r="A11" s="95" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B11" s="96" t="s">
         <v>66</v>
@@ -23056,7 +23053,7 @@
     </row>
     <row r="23" ht="24.75" customHeight="1" spans="1:9">
       <c r="A23" s="95" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B23" s="96" t="s">
         <v>66</v>
@@ -23230,7 +23227,7 @@
     </row>
     <row r="35" ht="24.75" customHeight="1" spans="1:9">
       <c r="A35" s="95" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B35" s="96" t="s">
         <v>66</v>
@@ -24328,7 +24325,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>0</v>
+        <v>-1400</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -24428,7 +24425,7 @@
       </c>
       <c r="C103" s="36" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>0</v>
+        <v>-1083</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -24524,7 +24521,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -24540,7 +24537,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>-347</v>
+        <v>-2830</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -24634,7 +24631,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B42")&amp;"'!E190")</f>
-        <v>10727.6</v>
+        <v>13210.6</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -24803,7 +24800,7 @@
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="99" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D129" s="99"/>
       <c r="E129" s="101">
@@ -24906,7 +24903,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>11269.4</v>
+        <v>13752.4</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -24998,7 +24995,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>11269.4</v>
+        <v>13752.4</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -25167,7 +25164,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="99" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D156" s="99"/>
       <c r="E156" s="101">
@@ -25270,7 +25267,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>11942.2</v>
+        <v>14425.2</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -25362,7 +25359,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>11942.2</v>
+        <v>14425.2</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -25531,7 +25528,7 @@
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="99" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D183" s="99"/>
       <c r="E183" s="101">
@@ -25634,7 +25631,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -26180,7 +26177,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -26196,7 +26193,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>12874.4</v>
+        <v>15357.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -26212,7 +26209,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -27699,7 +27696,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>0</v>
+        <v>-1400</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -27799,7 +27796,7 @@
       </c>
       <c r="C103" s="36" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>0</v>
+        <v>-1083</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -27895,7 +27892,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -27911,7 +27908,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -28005,7 +28002,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B45")&amp;"'!E190")</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -28273,7 +28270,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -28365,7 +28362,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -28633,7 +28630,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -28725,7 +28722,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -28993,7 +28990,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -29486,7 +29483,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -29502,7 +29499,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>12874.4</v>
+        <v>15357.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -29518,7 +29515,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -31005,7 +31002,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>0</v>
+        <v>-1400</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -31080,7 +31077,7 @@
         <v>Bankruptcy Department / Bank</v>
       </c>
       <c r="B102" s="37" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C102" s="36" cm="1">
         <f ca="1" t="array" ref="C102">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C102")+SUM(E122+E149+E176)</f>
@@ -31104,7 +31101,7 @@
       </c>
       <c r="C103" s="36" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>0</v>
+        <v>-1083</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -31200,7 +31197,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -31216,7 +31213,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -31310,7 +31307,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B48")&amp;"'!E190")</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -31578,7 +31575,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -31670,7 +31667,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -31938,7 +31935,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -32030,7 +32027,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -32298,7 +32295,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -32793,7 +32790,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -32809,7 +32806,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>12874.4</v>
+        <v>15357.4</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -32825,7 +32822,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -34312,7 +34309,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>0</v>
+        <v>-1400</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="68"/>
@@ -34412,7 +34409,7 @@
       </c>
       <c r="C103" s="36" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>0</v>
+        <v>-1083</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -34508,7 +34505,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -34524,7 +34521,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -34618,7 +34615,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B51")&amp;"'!E190")</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -34886,7 +34883,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -34978,7 +34975,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -35246,7 +35243,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -35338,7 +35335,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -35606,7 +35603,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>12484</v>
+        <v>14967</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -36588,8 +36585,8 @@
   <sheetPr/>
   <dimension ref="A1:N204"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -36609,7 +36606,7 @@
     <col min="15" max="16384" width="9" style="155"/>
   </cols>
   <sheetData>
-    <row r="1" ht="36.75" customHeight="1" spans="1:14">
+    <row r="1" ht="35" customHeight="1" spans="1:14">
       <c r="A1" s="156" t="str">
         <f>"Forecasts For the Year "&amp;TEXT(Main!B3,"mmmm yyyy")&amp;" to "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,3)-1,"mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*3+2),"mmmm yyyy"))</f>
         <v>Forecasts For the Year April 2024 to July 2024</v>
@@ -36628,7 +36625,7 @@
       </c>
       <c r="N1" s="195"/>
     </row>
-    <row r="2" ht="36" customHeight="1" spans="1:14">
+    <row r="2" ht="35" customHeight="1" spans="1:14">
       <c r="A2" s="157" t="s">
         <v>27</v>
       </c>
@@ -36652,7 +36649,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" ht="35.25" customHeight="1" spans="1:14">
+    <row r="3" ht="35" customHeight="1" spans="1:14">
       <c r="A3" s="160" t="s">
         <v>33</v>
       </c>
@@ -36688,7 +36685,7 @@
         <v>-24333</v>
       </c>
     </row>
-    <row r="4" ht="35.25" customHeight="1" spans="1:14">
+    <row r="4" ht="35" customHeight="1" spans="1:14">
       <c r="A4" s="160"/>
       <c r="B4" s="161" t="s">
         <v>35</v>
@@ -36720,7 +36717,7 @@
         <v>-11683</v>
       </c>
     </row>
-    <row r="5" ht="35.25" customHeight="1" spans="1:14">
+    <row r="5" ht="35" customHeight="1" spans="1:14">
       <c r="A5" s="160"/>
       <c r="B5" s="161" t="s">
         <v>36</v>
@@ -36752,7 +36749,7 @@
         <v>-10683</v>
       </c>
     </row>
-    <row r="6" ht="35.25" customHeight="1" spans="1:14">
+    <row r="6" ht="35" customHeight="1" spans="1:14">
       <c r="A6" s="160"/>
       <c r="B6" s="161" t="s">
         <v>37</v>
@@ -36784,7 +36781,7 @@
         <v>-6983</v>
       </c>
     </row>
-    <row r="7" ht="35.25" customHeight="1" spans="1:14">
+    <row r="7" ht="35" customHeight="1" spans="1:14">
       <c r="A7" s="160"/>
       <c r="B7" s="161" t="s">
         <v>38</v>
@@ -36813,10 +36810,10 @@
       </c>
       <c r="N7" s="199">
         <f ca="1">'April 2025 - June 2025'!C5</f>
-        <v>-6983</v>
-      </c>
-    </row>
-    <row r="8" ht="45" customHeight="1" spans="1:14">
+        <v>-5483</v>
+      </c>
+    </row>
+    <row r="8" ht="35" customHeight="1" spans="1:14">
       <c r="A8" s="160"/>
       <c r="B8" s="161" t="s">
         <v>39</v>
@@ -36846,10 +36843,10 @@
       </c>
       <c r="N8" s="199">
         <f ca="1">'July 2025 - September 2025'!C5</f>
-        <v>-3983</v>
-      </c>
-    </row>
-    <row r="9" ht="39.75" customHeight="1" spans="1:14">
+        <v>-2483</v>
+      </c>
+    </row>
+    <row r="9" ht="35" customHeight="1" spans="1:14">
       <c r="A9" s="160"/>
       <c r="B9" s="161" t="s">
         <v>40</v>
@@ -36878,10 +36875,10 @@
       </c>
       <c r="N9" s="209">
         <f ca="1">'October 2025 - December 2025'!C5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" ht="35.25" customHeight="1" spans="1:14">
+        <v>-2483</v>
+      </c>
+    </row>
+    <row r="10" ht="35" customHeight="1" spans="1:14">
       <c r="A10" s="160"/>
       <c r="B10" s="161" t="s">
         <v>41</v>
@@ -36910,10 +36907,10 @@
       </c>
       <c r="N10" s="199">
         <f ca="1">'January 2026 - March 2026'!C5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" ht="35.25" customHeight="1" spans="1:14">
+        <v>-2483</v>
+      </c>
+    </row>
+    <row r="11" ht="35" customHeight="1" spans="1:14">
       <c r="A11" s="160"/>
       <c r="B11" s="161" t="s">
         <v>42</v>
@@ -36943,10 +36940,10 @@
       </c>
       <c r="N11" s="203">
         <f ca="1">'April 2026 - June 2026'!C5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" ht="35.25" customHeight="1" spans="1:14">
+        <v>-2483</v>
+      </c>
+    </row>
+    <row r="12" ht="35" customHeight="1" spans="1:14">
       <c r="A12" s="160"/>
       <c r="B12" s="161" t="s">
         <v>43</v>
@@ -36975,10 +36972,10 @@
       </c>
       <c r="N12" s="203">
         <f ca="1">'July 2026 - September 2026'!C5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" ht="35.25" customHeight="1" spans="1:14">
+        <v>-2483</v>
+      </c>
+    </row>
+    <row r="13" ht="35" customHeight="1" spans="1:14">
       <c r="A13" s="160"/>
       <c r="B13" s="161" t="s">
         <v>44</v>
@@ -37007,10 +37004,10 @@
       </c>
       <c r="N13" s="203">
         <f ca="1">'October 2026 - December 2026'!C5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" ht="35.25" customHeight="1" spans="1:14">
+        <v>-2483</v>
+      </c>
+    </row>
+    <row r="14" ht="35" customHeight="1" spans="1:14">
       <c r="A14" s="160"/>
       <c r="B14" s="161" t="s">
         <v>45</v>
@@ -37039,10 +37036,10 @@
       </c>
       <c r="N14" s="203">
         <f ca="1">'January 2027 - March 2027'!C5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" ht="35.25" customHeight="1" spans="1:14">
+        <v>-2483</v>
+      </c>
+    </row>
+    <row r="15" ht="35" customHeight="1" spans="1:14">
       <c r="A15" s="160"/>
       <c r="B15" s="165" t="s">
         <v>46</v>
@@ -37071,10 +37068,10 @@
       </c>
       <c r="N15" s="203">
         <f ca="1">'April 2027 - June 2027'!C5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" ht="35.25" customHeight="1" spans="1:14">
+        <v>-2483</v>
+      </c>
+    </row>
+    <row r="16" ht="35" customHeight="1" spans="1:14">
       <c r="A16" s="166"/>
       <c r="B16" s="167" t="s">
         <v>47</v>
@@ -37097,7 +37094,7 @@
       </c>
       <c r="J16" s="203">
         <f ca="1">'April 2025 - June 2025'!E163</f>
-        <v>2935</v>
+        <v>1935</v>
       </c>
       <c r="M16" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,39),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*39+39),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
@@ -37105,17 +37102,17 @@
       </c>
       <c r="N16" s="203">
         <f ca="1">Forecast_14!C5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" ht="35.25" customHeight="1" spans="9:14">
+        <v>-2483</v>
+      </c>
+    </row>
+    <row r="17" ht="35" customHeight="1" spans="9:14">
       <c r="I17" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,14),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*14)+14,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,15)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*15+14),"dd mmmm yyyy"))</f>
         <v>20 June 2025 - 19 July 2025</v>
       </c>
       <c r="J17" s="203">
         <f ca="1">'April 2025 - June 2025'!E190</f>
-        <v>3661.8</v>
+        <v>2161.8</v>
       </c>
       <c r="M17" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+42),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,45)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+44),"dd mmmm yyyy"))</f>
@@ -37123,17 +37120,17 @@
       </c>
       <c r="N17" s="203">
         <f ca="1">Forecast_15!C5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" ht="35.25" customHeight="1" spans="9:14">
+        <v>-2483</v>
+      </c>
+    </row>
+    <row r="18" ht="35" customHeight="1" spans="9:14">
       <c r="I18" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,15),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*15)+15,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,16)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*16+15),"dd mmmm yyyy"))</f>
         <v>20 July 2025 - 19 August 2025</v>
       </c>
       <c r="J18" s="203">
         <f ca="1">'July 2025 - September 2025'!E136</f>
-        <v>3494.6</v>
+        <v>1994.6</v>
       </c>
       <c r="M18" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,45),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*45+45),"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,48)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*48+47),"dd mmmm yyyy"))</f>
@@ -37141,40 +37138,40 @@
       </c>
       <c r="N18" s="199">
         <f ca="1">Forecast_16!C5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" ht="33" customHeight="1" spans="9:10">
+        <v>-2483</v>
+      </c>
+    </row>
+    <row r="19" ht="35" customHeight="1" spans="9:10">
       <c r="I19" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,16),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*16)+16,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,17)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*17+16),"dd mmmm yyyy"))</f>
         <v>20 August 2025 - 19 September 2025</v>
       </c>
       <c r="J19" s="203">
         <f ca="1">'July 2025 - September 2025'!E163</f>
-        <v>3171.4</v>
-      </c>
-    </row>
-    <row r="20" ht="35.25" customHeight="1" spans="9:10">
+        <v>1671.4</v>
+      </c>
+    </row>
+    <row r="20" ht="35" customHeight="1" spans="9:10">
       <c r="I20" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,17),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*17)+17,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,18)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*18+17),"dd mmmm yyyy"))</f>
         <v>20 September 2025 - 19 October 2025</v>
       </c>
       <c r="J20" s="203">
         <f ca="1">'July 2025 - September 2025'!E190</f>
-        <v>3004.2</v>
-      </c>
-    </row>
-    <row r="21" ht="35.25" customHeight="1" spans="9:10">
+        <v>1504.2</v>
+      </c>
+    </row>
+    <row r="21" ht="35" customHeight="1" spans="9:10">
       <c r="I21" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,18),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*18)+18,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,19)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*19+18),"dd mmmm yyyy"))</f>
         <v>20 October 2025 - 19 November 2025</v>
       </c>
       <c r="J21" s="203">
         <f ca="1">'October 2025 - December 2025'!E136</f>
-        <v>2731</v>
-      </c>
-    </row>
-    <row r="22" ht="24.75" customHeight="1" spans="1:10">
+        <v>2231</v>
+      </c>
+    </row>
+    <row r="22" ht="35" customHeight="1" spans="1:10">
       <c r="A22" s="15" t="str">
         <f>TEXT(Main!B3,"dd mmmm yyyy")&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,1)-1,"dd mmmm yyyy"),TEXT(Main!B3+Main!B5-Main!B3,"dd mmmm yyyy"))&amp;" / "&amp;" (Revenue / Deferred Debts Or Expenses)"</f>
         <v>20 April 2024 - 19 May 2024 /  (Revenue / Deferred Debts Or Expenses)</v>
@@ -37185,16 +37182,16 @@
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
-      <c r="I22" s="204" t="str">
+      <c r="I22" s="205" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,19),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*19)+19,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,20)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*20+19),"dd mmmm yyyy"))</f>
         <v>20 November 2025 - 19 December 2025</v>
       </c>
       <c r="J22" s="203">
         <f ca="1">'October 2025 - December 2025'!E163</f>
-        <v>2013.8</v>
-      </c>
-    </row>
-    <row r="23" ht="24.75" customHeight="1" spans="1:10">
+        <v>3013.8</v>
+      </c>
+    </row>
+    <row r="23" ht="35" customHeight="1" spans="1:10">
       <c r="A23" s="17" t="s">
         <v>29</v>
       </c>
@@ -37216,10 +37213,10 @@
       </c>
       <c r="J23" s="203">
         <f ca="1">'October 2025 - December 2025'!E190</f>
-        <v>1072.6</v>
-      </c>
-    </row>
-    <row r="24" ht="52.5" customHeight="1" spans="1:10">
+        <v>3555.6</v>
+      </c>
+    </row>
+    <row r="24" ht="35" customHeight="1" spans="1:10">
       <c r="A24" s="19" t="s">
         <v>51</v>
       </c>
@@ -37241,10 +37238,10 @@
       </c>
       <c r="J24" s="203">
         <f ca="1">'January 2026 - March 2026'!E136</f>
-        <v>1905.4</v>
-      </c>
-    </row>
-    <row r="25" ht="30" customHeight="1" spans="1:10">
+        <v>4388.4</v>
+      </c>
+    </row>
+    <row r="25" ht="35" customHeight="1" spans="1:10">
       <c r="A25" s="19"/>
       <c r="B25" s="21"/>
       <c r="C25" s="22"/>
@@ -37260,10 +37257,10 @@
       </c>
       <c r="J25" s="203">
         <f ca="1">'January 2026 - March 2026'!E163</f>
-        <v>2287.2</v>
-      </c>
-    </row>
-    <row r="26" ht="30" customHeight="1" spans="1:10">
+        <v>4770.2</v>
+      </c>
+    </row>
+    <row r="26" ht="35" customHeight="1" spans="1:10">
       <c r="A26" s="19"/>
       <c r="B26" s="21"/>
       <c r="C26" s="22"/>
@@ -37279,10 +37276,10 @@
       </c>
       <c r="J26" s="203">
         <f ca="1">'January 2026 - March 2026'!E190</f>
-        <v>3120</v>
-      </c>
-    </row>
-    <row r="27" ht="30" customHeight="1" spans="1:10">
+        <v>5603</v>
+      </c>
+    </row>
+    <row r="27" ht="35" customHeight="1" spans="1:10">
       <c r="A27" s="19"/>
       <c r="B27" s="21"/>
       <c r="C27" s="22"/>
@@ -37298,10 +37295,10 @@
       </c>
       <c r="J27" s="203">
         <f ca="1">'April 2026 - June 2026'!E136</f>
-        <v>3661.8</v>
-      </c>
-    </row>
-    <row r="28" ht="30" customHeight="1" spans="1:10">
+        <v>6144.8</v>
+      </c>
+    </row>
+    <row r="28" ht="35" customHeight="1" spans="1:10">
       <c r="A28" s="19"/>
       <c r="B28" s="21"/>
       <c r="C28" s="22"/>
@@ -37317,10 +37314,10 @@
       </c>
       <c r="J28" s="203">
         <f ca="1">'April 2026 - June 2026'!E163</f>
-        <v>4334.6</v>
-      </c>
-    </row>
-    <row r="29" ht="30" customHeight="1" spans="1:10">
+        <v>6817.6</v>
+      </c>
+    </row>
+    <row r="29" ht="35" customHeight="1" spans="1:10">
       <c r="A29" s="19"/>
       <c r="B29" s="21"/>
       <c r="C29" s="22"/>
@@ -37336,10 +37333,10 @@
       </c>
       <c r="J29" s="199">
         <f ca="1">'April 2026 - June 2026'!E190</f>
-        <v>4876.4</v>
-      </c>
-    </row>
-    <row r="30" ht="30" customHeight="1" spans="1:10">
+        <v>7359.4</v>
+      </c>
+    </row>
+    <row r="30" ht="35" customHeight="1" spans="1:10">
       <c r="A30" s="171"/>
       <c r="B30" s="172"/>
       <c r="C30" s="173"/>
@@ -37358,40 +37355,40 @@
       </c>
       <c r="J30" s="206">
         <f ca="1">'July 2026 - September 2026'!E136</f>
-        <v>5709.2</v>
-      </c>
-    </row>
-    <row r="31" ht="30" customHeight="1" spans="9:10">
+        <v>8192.2</v>
+      </c>
+    </row>
+    <row r="31" ht="35" customHeight="1" spans="9:10">
       <c r="I31" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,28),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*28)+28,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,29)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*29+28),"dd mmmm yyyy"))</f>
         <v>20 August 2026 - 19 September 2026</v>
       </c>
       <c r="J31" s="203">
         <f ca="1">'July 2026 - September 2026'!E163</f>
-        <v>6091</v>
-      </c>
-    </row>
-    <row r="32" ht="27.75" customHeight="1" spans="9:10">
+        <v>8574</v>
+      </c>
+    </row>
+    <row r="32" ht="35" customHeight="1" spans="9:10">
       <c r="I32" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,29),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*29)+29,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,30)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*30+29),"dd mmmm yyyy"))</f>
         <v>20 September 2026 - 19 October 2026</v>
       </c>
       <c r="J32" s="203">
         <f ca="1">'July 2026 - September 2026'!E190</f>
-        <v>6923.8</v>
-      </c>
-    </row>
-    <row r="33" ht="30" customHeight="1" spans="9:10">
+        <v>9406.8</v>
+      </c>
+    </row>
+    <row r="33" ht="35" customHeight="1" spans="9:10">
       <c r="I33" s="204" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,30),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*30)+30,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,31)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*31+30),"dd mmmm yyyy"))</f>
         <v>20 October 2026 - 19 November 2026</v>
       </c>
       <c r="J33" s="203">
         <f ca="1">'October 2026 - December 2026'!E136</f>
-        <v>7465.6</v>
-      </c>
-    </row>
-    <row r="34" ht="30" customHeight="1" spans="1:10">
+        <v>9948.6</v>
+      </c>
+    </row>
+    <row r="34" ht="35" customHeight="1" spans="1:10">
       <c r="A34" s="15" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,1),"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)+1,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,2)-1,"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)*2+1,"dd mmmm yyyy"))&amp;" (Revenue / Deferred Debts Or Expenses)"</f>
         <v>20 May 2024 - 19 June 2024 (Revenue / Deferred Debts Or Expenses)</v>
@@ -37408,10 +37405,10 @@
       </c>
       <c r="J34" s="203">
         <f ca="1">'October 2026 - December 2026'!E163</f>
-        <v>8138.4</v>
-      </c>
-    </row>
-    <row r="35" ht="24.75" customHeight="1" spans="1:10">
+        <v>10621.4</v>
+      </c>
+    </row>
+    <row r="35" ht="35" customHeight="1" spans="1:10">
       <c r="A35" s="17" t="s">
         <v>29</v>
       </c>
@@ -37433,10 +37430,10 @@
       </c>
       <c r="J35" s="203">
         <f ca="1">'October 2026 - December 2026'!E190</f>
-        <v>8680.2</v>
-      </c>
-    </row>
-    <row r="36" ht="54.75" customHeight="1" spans="1:10">
+        <v>11163.2</v>
+      </c>
+    </row>
+    <row r="36" ht="35" customHeight="1" spans="1:10">
       <c r="A36" s="19" t="s">
         <v>55</v>
       </c>
@@ -37458,10 +37455,10 @@
       </c>
       <c r="J36" s="203">
         <f ca="1">'January 2027 - March 2027'!E136</f>
-        <v>9513</v>
-      </c>
-    </row>
-    <row r="37" ht="24.75" customHeight="1" spans="1:10">
+        <v>11996</v>
+      </c>
+    </row>
+    <row r="37" ht="35" customHeight="1" spans="1:10">
       <c r="A37" s="19" t="s">
         <v>56</v>
       </c>
@@ -37483,10 +37480,10 @@
       </c>
       <c r="J37" s="203">
         <f ca="1">'January 2027 - March 2027'!E163</f>
-        <v>9894.8</v>
-      </c>
-    </row>
-    <row r="38" ht="20.25" customHeight="1" spans="1:10">
+        <v>12377.8</v>
+      </c>
+    </row>
+    <row r="38" ht="35" customHeight="1" spans="1:10">
       <c r="A38" s="19" t="s">
         <v>58</v>
       </c>
@@ -37508,10 +37505,10 @@
       </c>
       <c r="J38" s="203">
         <f ca="1">'January 2027 - March 2027'!E190</f>
-        <v>10727.6</v>
-      </c>
-    </row>
-    <row r="39" ht="24.75" customHeight="1" spans="1:10">
+        <v>13210.6</v>
+      </c>
+    </row>
+    <row r="39" ht="35" customHeight="1" spans="1:10">
       <c r="A39" s="19"/>
       <c r="B39" s="21"/>
       <c r="C39" s="22"/>
@@ -37527,10 +37524,10 @@
       </c>
       <c r="J39" s="203">
         <f ca="1">'April 2027 - June 2027'!E136</f>
-        <v>11269.4</v>
-      </c>
-    </row>
-    <row r="40" ht="24.75" customHeight="1" spans="1:10">
+        <v>13752.4</v>
+      </c>
+    </row>
+    <row r="40" ht="35" customHeight="1" spans="1:10">
       <c r="A40" s="19"/>
       <c r="B40" s="21"/>
       <c r="C40" s="22"/>
@@ -37546,10 +37543,10 @@
       </c>
       <c r="J40" s="203">
         <f ca="1">'April 2027 - June 2027'!E163</f>
-        <v>11942.2</v>
-      </c>
-    </row>
-    <row r="41" ht="24.75" customHeight="1" spans="1:10">
+        <v>14425.2</v>
+      </c>
+    </row>
+    <row r="41" ht="35" customHeight="1" spans="1:10">
       <c r="A41" s="19"/>
       <c r="B41" s="21"/>
       <c r="C41" s="22"/>
@@ -37565,10 +37562,10 @@
       </c>
       <c r="J41" s="203">
         <f ca="1">'April 2027 - June 2027'!E190</f>
-        <v>12484</v>
-      </c>
-    </row>
-    <row r="42" ht="24.75" customHeight="1" spans="1:10">
+        <v>14967</v>
+      </c>
+    </row>
+    <row r="42" ht="35" customHeight="1" spans="1:10">
       <c r="A42" s="171"/>
       <c r="B42" s="172"/>
       <c r="C42" s="173"/>
@@ -37587,40 +37584,40 @@
       </c>
       <c r="J42" s="203">
         <f ca="1">Forecast_14!E136</f>
-        <v>12484</v>
-      </c>
-    </row>
-    <row r="43" ht="24.75" customHeight="1" spans="9:10">
+        <v>14967</v>
+      </c>
+    </row>
+    <row r="43" ht="35" customHeight="1" spans="9:10">
       <c r="I43" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,40),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*40)+40,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,41)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*41+40),"dd mmmm yyyy"))</f>
         <v>20 August 2027 - 19 September 2027</v>
       </c>
       <c r="J43" s="203">
         <f ca="1">Forecast_14!E163</f>
-        <v>12484</v>
-      </c>
-    </row>
-    <row r="44" ht="24.75" customHeight="1" spans="9:10">
+        <v>14967</v>
+      </c>
+    </row>
+    <row r="44" ht="35" customHeight="1" spans="9:10">
       <c r="I44" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,41),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*41)+41,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,42)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42+41),"dd mmmm yyyy"))</f>
         <v>20 September 2027 - 19 October 2027</v>
       </c>
       <c r="J44" s="203">
         <f ca="1">Forecast_14!E190</f>
-        <v>12484</v>
-      </c>
-    </row>
-    <row r="45" ht="24.75" customHeight="1" spans="9:10">
+        <v>14967</v>
+      </c>
+    </row>
+    <row r="45" ht="35" customHeight="1" spans="9:10">
       <c r="I45" s="200" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,42),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*42)+42,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,43)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*43+42),"dd mmmm yyyy"))</f>
         <v>20 October 2027 - 19 November 2027</v>
       </c>
       <c r="J45" s="203">
         <f ca="1">Forecast_15!E136</f>
-        <v>12484</v>
-      </c>
-    </row>
-    <row r="46" ht="24.75" customHeight="1" spans="1:10">
+        <v>14967</v>
+      </c>
+    </row>
+    <row r="46" ht="35" customHeight="1" spans="1:10">
       <c r="A46" s="15" t="str">
         <f>IF(Main!B2,TEXT(EDATE(Main!B3,2),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*2)+2,"dd mmmm yyyy"))&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,3)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*3+2),"dd mmmm yyyy"))&amp;" (Revenue / Deferred Debts Or Expenses)"</f>
         <v>20 June 2024 - 19 July 2024 (Revenue / Deferred Debts Or Expenses)</v>
@@ -37637,10 +37634,10 @@
       </c>
       <c r="J46" s="203">
         <f ca="1">Forecast_15!E163</f>
-        <v>12484</v>
-      </c>
-    </row>
-    <row r="47" ht="24.75" customHeight="1" spans="1:10">
+        <v>14967</v>
+      </c>
+    </row>
+    <row r="47" ht="35" customHeight="1" spans="1:10">
       <c r="A47" s="17" t="s">
         <v>29</v>
       </c>
@@ -37662,10 +37659,10 @@
       </c>
       <c r="J47" s="203">
         <f ca="1">Forecast_15!E190</f>
-        <v>12484</v>
-      </c>
-    </row>
-    <row r="48" ht="24.75" customHeight="1" spans="1:10">
+        <v>14967</v>
+      </c>
+    </row>
+    <row r="48" ht="35" customHeight="1" spans="1:10">
       <c r="A48" s="95" t="s">
         <v>61</v>
       </c>
@@ -37687,10 +37684,10 @@
       </c>
       <c r="J48" s="203">
         <f ca="1">Forecast_16!E136</f>
-        <v>12484</v>
-      </c>
-    </row>
-    <row r="49" ht="24.75" customHeight="1" spans="1:10">
+        <v>14967</v>
+      </c>
+    </row>
+    <row r="49" ht="35" customHeight="1" spans="1:10">
       <c r="A49" s="95" t="s">
         <v>64</v>
       </c>
@@ -37712,10 +37709,10 @@
       </c>
       <c r="J49" s="203">
         <f ca="1">Forecast_16!E163</f>
-        <v>12484</v>
-      </c>
-    </row>
-    <row r="50" ht="24.75" customHeight="1" spans="1:10">
+        <v>14967</v>
+      </c>
+    </row>
+    <row r="50" ht="35" customHeight="1" spans="1:10">
       <c r="A50" s="95" t="s">
         <v>65</v>
       </c>
@@ -37737,10 +37734,10 @@
       </c>
       <c r="J50" s="199">
         <f ca="1">Forecast_16!E190</f>
-        <v>12484</v>
-      </c>
-    </row>
-    <row r="51" ht="41" customHeight="1" spans="1:7">
+        <v>14967</v>
+      </c>
+    </row>
+    <row r="51" ht="35" customHeight="1" spans="1:7">
       <c r="A51" s="176" t="s">
         <v>68</v>
       </c>
@@ -37755,7 +37752,7 @@
       </c>
       <c r="G51" s="42"/>
     </row>
-    <row r="52" ht="24.75" customHeight="1" spans="1:7">
+    <row r="52" ht="35" customHeight="1" spans="1:7">
       <c r="A52" s="178" t="s">
         <v>70</v>
       </c>
@@ -37772,7 +37769,7 @@
       </c>
       <c r="G52" s="42"/>
     </row>
-    <row r="53" ht="24.75" customHeight="1" spans="1:7">
+    <row r="53" ht="35" customHeight="1" spans="1:7">
       <c r="A53" s="19"/>
       <c r="B53" s="21"/>
       <c r="C53" s="22"/>
@@ -37783,7 +37780,7 @@
       </c>
       <c r="G53" s="42"/>
     </row>
-    <row r="54" ht="24.75" customHeight="1" spans="1:7">
+    <row r="54" ht="35" customHeight="1" spans="1:7">
       <c r="A54" s="171"/>
       <c r="B54" s="172"/>
       <c r="C54" s="173"/>
@@ -37797,8 +37794,10 @@
       </c>
       <c r="G54" s="46"/>
     </row>
-    <row r="55" ht="24.75" customHeight="1"/>
-    <row r="58" ht="20.4" spans="1:3">
+    <row r="55" ht="35" customHeight="1"/>
+    <row r="56" ht="35" customHeight="1"/>
+    <row r="57" ht="35" customHeight="1"/>
+    <row r="58" ht="35" customHeight="1" spans="1:3">
       <c r="A58" s="179" t="str">
         <f>"Fixed Expense For the Year "&amp;TEXT(Main!B3,"mmmm yyyy")&amp;" - "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,3)-1,"mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*3+2),"mmmm yyyy"))</f>
         <v>Fixed Expense For the Year April 2024 - July 2024</v>
@@ -37806,7 +37805,7 @@
       <c r="B58" s="180"/>
       <c r="C58" s="181"/>
     </row>
-    <row r="59" ht="21" spans="1:3">
+    <row r="59" ht="35" customHeight="1" spans="1:3">
       <c r="A59" s="182" t="s">
         <v>48</v>
       </c>
@@ -37817,14 +37816,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" ht="35" customHeight="1" spans="1:3">
       <c r="A60" s="184" t="s">
         <v>73</v>
       </c>
       <c r="B60" s="185"/>
       <c r="C60" s="186"/>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" ht="35" customHeight="1" spans="1:3">
       <c r="A61" s="50" t="s">
         <v>74</v>
       </c>
@@ -37833,7 +37832,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" ht="35" customHeight="1" spans="1:3">
       <c r="A62" s="50" t="s">
         <v>75</v>
       </c>
@@ -37842,7 +37841,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="63" ht="21" customHeight="1" spans="1:3">
+    <row r="63" ht="35" customHeight="1" spans="1:3">
       <c r="A63" s="188" t="s">
         <v>76</v>
       </c>
@@ -37851,7 +37850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" ht="35" customHeight="1" spans="1:3">
       <c r="A64" s="50" t="s">
         <v>59</v>
       </c>
@@ -37860,7 +37859,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" ht="35" customHeight="1" spans="1:3">
       <c r="A65" s="50" t="s">
         <v>77</v>
       </c>
@@ -37869,28 +37868,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" ht="35" customHeight="1" spans="1:3">
       <c r="A66" s="50"/>
       <c r="B66" s="187"/>
       <c r="C66" s="211">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" ht="35" customHeight="1" spans="1:3">
       <c r="A67" s="50"/>
       <c r="B67" s="187"/>
       <c r="C67" s="211">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" ht="35" customHeight="1" spans="1:3">
       <c r="A68" s="50"/>
       <c r="B68" s="187"/>
       <c r="C68" s="211">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" ht="35" customHeight="1" spans="1:3">
       <c r="A69" s="38"/>
       <c r="B69" s="39" t="s">
         <v>78</v>
@@ -37900,14 +37899,14 @@
         <v>443</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" ht="35" customHeight="1" spans="1:3">
       <c r="A70" s="184" t="s">
         <v>79</v>
       </c>
       <c r="B70" s="185"/>
       <c r="C70" s="186"/>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" ht="35" customHeight="1" spans="1:3">
       <c r="A71" s="50" t="s">
         <v>80</v>
       </c>
@@ -37916,7 +37915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" ht="35" customHeight="1" spans="1:3">
       <c r="A72" s="50" t="s">
         <v>81</v>
       </c>
@@ -37925,7 +37924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" ht="35" customHeight="1" spans="1:3">
       <c r="A73" s="50" t="s">
         <v>82</v>
       </c>
@@ -37934,7 +37933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" ht="35" customHeight="1" spans="1:3">
       <c r="A74" s="50" t="s">
         <v>83</v>
       </c>
@@ -37943,42 +37942,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" ht="35" customHeight="1" spans="1:3">
       <c r="A75" s="50"/>
       <c r="B75" s="187"/>
       <c r="C75" s="211">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" ht="35" customHeight="1" spans="1:3">
       <c r="A76" s="50"/>
       <c r="B76" s="187"/>
       <c r="C76" s="211">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" ht="35" customHeight="1" spans="1:3">
       <c r="A77" s="50"/>
       <c r="B77" s="187"/>
       <c r="C77" s="211">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" ht="35" customHeight="1" spans="1:3">
       <c r="A78" s="50"/>
       <c r="B78" s="187"/>
       <c r="C78" s="211">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" ht="35" customHeight="1" spans="1:3">
       <c r="A79" s="50"/>
       <c r="B79" s="187"/>
       <c r="C79" s="211">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" ht="35" customHeight="1" spans="1:3">
       <c r="A80" s="212"/>
       <c r="B80" s="213" t="s">
         <v>78</v>
@@ -37988,14 +37987,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" ht="35" customHeight="1" spans="1:3">
       <c r="A81" s="184" t="s">
         <v>84</v>
       </c>
       <c r="B81" s="185"/>
       <c r="C81" s="186"/>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" ht="35" customHeight="1" spans="1:3">
       <c r="A82" s="50" t="s">
         <v>85</v>
       </c>
@@ -38006,7 +38005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" ht="35" customHeight="1" spans="1:3">
       <c r="A83" s="214" t="s">
         <v>87</v>
       </c>
@@ -38017,42 +38016,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" ht="35" customHeight="1" spans="1:3">
       <c r="A84" s="51"/>
       <c r="B84" s="187"/>
       <c r="C84" s="36">
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" ht="35" customHeight="1" spans="1:3">
       <c r="A85" s="50"/>
       <c r="B85" s="187"/>
       <c r="C85" s="36">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" ht="35" customHeight="1" spans="1:3">
       <c r="A86" s="50"/>
       <c r="B86" s="187"/>
       <c r="C86" s="36">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" ht="35" customHeight="1" spans="1:3">
       <c r="A87" s="50"/>
       <c r="B87" s="187"/>
       <c r="C87" s="36">
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" ht="35" customHeight="1" spans="1:3">
       <c r="A88" s="50"/>
       <c r="B88" s="187"/>
       <c r="C88" s="36">
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" ht="35" customHeight="1" spans="1:3">
       <c r="A89" s="212"/>
       <c r="B89" s="213" t="s">
         <v>78</v>
@@ -38062,14 +38061,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" ht="35" customHeight="1" spans="1:3">
       <c r="A90" s="184" t="s">
         <v>89</v>
       </c>
       <c r="B90" s="185"/>
       <c r="C90" s="186"/>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" ht="35" customHeight="1" spans="1:3">
       <c r="A91" s="215" t="s">
         <v>90</v>
       </c>
@@ -38078,56 +38077,56 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" ht="35" customHeight="1" spans="1:3">
       <c r="A92" s="51"/>
       <c r="B92" s="187"/>
       <c r="C92" s="211">
         <v>0</v>
       </c>
     </row>
-    <row r="93" ht="20.25" customHeight="1" spans="1:3">
+    <row r="93" ht="35" customHeight="1" spans="1:3">
       <c r="A93" s="51"/>
       <c r="B93" s="187"/>
       <c r="C93" s="211">
         <v>0</v>
       </c>
     </row>
-    <row r="94" ht="15.75" customHeight="1" spans="1:3">
+    <row r="94" ht="35" customHeight="1" spans="1:3">
       <c r="A94" s="50"/>
       <c r="B94" s="187"/>
       <c r="C94" s="211">
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" ht="35" customHeight="1" spans="1:3">
       <c r="A95" s="50"/>
       <c r="B95" s="187"/>
       <c r="C95" s="211">
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" ht="35" customHeight="1" spans="1:3">
       <c r="A96" s="50"/>
       <c r="B96" s="187"/>
       <c r="C96" s="211">
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" ht="35" customHeight="1" spans="1:3">
       <c r="A97" s="50"/>
       <c r="B97" s="187"/>
       <c r="C97" s="211">
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" ht="35" customHeight="1" spans="1:3">
       <c r="A98" s="50"/>
       <c r="B98" s="187"/>
       <c r="C98" s="211">
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" ht="35" customHeight="1" spans="1:3">
       <c r="A99" s="49"/>
       <c r="B99" s="39" t="s">
         <v>78</v>
@@ -38137,14 +38136,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" ht="35" customHeight="1" spans="1:3">
       <c r="A100" s="184" t="s">
         <v>91</v>
       </c>
       <c r="B100" s="185"/>
       <c r="C100" s="186"/>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" ht="35" customHeight="1" spans="1:3">
       <c r="A101" s="50" t="s">
         <v>92</v>
       </c>
@@ -38155,7 +38154,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" ht="35" customHeight="1" spans="1:3">
       <c r="A102" s="51" t="s">
         <v>94</v>
       </c>
@@ -38166,7 +38165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" ht="34" spans="1:3">
+    <row r="103" ht="35" customHeight="1" spans="1:3">
       <c r="A103" s="50" t="s">
         <v>96</v>
       </c>
@@ -38177,7 +38176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" ht="35" customHeight="1" spans="1:3">
       <c r="A104" s="50" t="s">
         <v>98</v>
       </c>
@@ -38188,35 +38187,35 @@
         <v>760</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" ht="35" customHeight="1" spans="1:3">
       <c r="A105" s="50"/>
       <c r="B105" s="187"/>
       <c r="C105" s="211">
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" ht="35" customHeight="1" spans="1:3">
       <c r="A106" s="50"/>
       <c r="B106" s="187"/>
       <c r="C106" s="211">
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" ht="35" customHeight="1" spans="1:3">
       <c r="A107" s="50"/>
       <c r="B107" s="187"/>
       <c r="C107" s="211">
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" ht="35" customHeight="1" spans="1:3">
       <c r="A108" s="50"/>
       <c r="B108" s="187"/>
       <c r="C108" s="211">
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" ht="35" customHeight="1" spans="1:3">
       <c r="A109" s="51"/>
       <c r="B109" s="39" t="s">
         <v>78</v>
@@ -38226,7 +38225,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" ht="35" customHeight="1" spans="1:3">
       <c r="A110" s="49"/>
       <c r="B110" s="39" t="s">
         <v>100</v>
@@ -38236,14 +38235,14 @@
         <v>1503</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" ht="35" customHeight="1" spans="1:3">
       <c r="A111" s="184" t="s">
         <v>101</v>
       </c>
       <c r="B111" s="185"/>
       <c r="C111" s="186"/>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" ht="35" customHeight="1" spans="1:8">
       <c r="A112" s="218" t="s">
         <v>102</v>
       </c>
@@ -38257,7 +38256,7 @@
       <c r="G112" s="14"/>
       <c r="H112" s="14"/>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" ht="35" customHeight="1" spans="1:8">
       <c r="A113" s="218" t="s">
         <v>103</v>
       </c>
@@ -38272,7 +38271,7 @@
       <c r="G113" s="14"/>
       <c r="H113" s="14"/>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" ht="35" customHeight="1" spans="1:8">
       <c r="A114" s="218" t="s">
         <v>104</v>
       </c>
@@ -38287,7 +38286,7 @@
       <c r="G114" s="14"/>
       <c r="H114" s="14"/>
     </row>
-    <row r="115" ht="34" spans="1:8">
+    <row r="115" ht="35" customHeight="1" spans="1:8">
       <c r="A115" s="223" t="s">
         <v>105</v>
       </c>
@@ -38301,7 +38300,7 @@
       <c r="G115" s="14"/>
       <c r="H115" s="14"/>
     </row>
-    <row r="116" ht="34" spans="1:8">
+    <row r="116" ht="35" customHeight="1" spans="1:8">
       <c r="A116" s="223" t="s">
         <v>106</v>
       </c>
@@ -38315,7 +38314,7 @@
       <c r="G116" s="14"/>
       <c r="H116" s="14"/>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" ht="35" customHeight="1" spans="1:8">
       <c r="A117" s="50" t="s">
         <v>107</v>
       </c>
@@ -38329,7 +38328,7 @@
       <c r="G117" s="14"/>
       <c r="H117" s="14"/>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" ht="35" customHeight="1" spans="1:8">
       <c r="A118" s="50"/>
       <c r="B118" s="187"/>
       <c r="C118" s="36">
@@ -38341,7 +38340,7 @@
       <c r="G118" s="14"/>
       <c r="H118" s="14"/>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" ht="35" customHeight="1" spans="1:8">
       <c r="A119" s="50"/>
       <c r="B119" s="187"/>
       <c r="C119" s="36">
@@ -38353,7 +38352,7 @@
       <c r="G119" s="14"/>
       <c r="H119" s="14"/>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" ht="35" customHeight="1" spans="1:8">
       <c r="A120" s="50"/>
       <c r="B120" s="187"/>
       <c r="C120" s="36">
@@ -38365,7 +38364,7 @@
       <c r="G120" s="14"/>
       <c r="H120" s="14"/>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" ht="35" customHeight="1" spans="1:8">
       <c r="A121" s="50"/>
       <c r="B121" s="187"/>
       <c r="C121" s="36">
@@ -38377,7 +38376,7 @@
       <c r="G121" s="14"/>
       <c r="H121" s="14"/>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" ht="35" customHeight="1" spans="1:3">
       <c r="A122" s="212"/>
       <c r="B122" s="213" t="s">
         <v>108</v>
@@ -38387,7 +38386,7 @@
         <v>24333</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" ht="35" customHeight="1" spans="1:3">
       <c r="A123" s="212"/>
       <c r="B123" s="213" t="s">
         <v>109</v>
@@ -38397,14 +38396,15 @@
         <v>25836</v>
       </c>
     </row>
-    <row r="124" spans="5:5">
+    <row r="124" ht="35" customHeight="1" spans="5:5">
       <c r="E124" s="224"/>
     </row>
-    <row r="125" spans="5:5">
+    <row r="125" ht="35" customHeight="1" spans="5:5">
       <c r="E125" s="224"/>
     </row>
-    <row r="127" ht="45" customHeight="1"/>
-    <row r="128" ht="45" customHeight="1" spans="1:5">
+    <row r="126" ht="35" customHeight="1"/>
+    <row r="127" ht="35" customHeight="1"/>
+    <row r="128" ht="35" customHeight="1" spans="1:5">
       <c r="A128" s="52" t="str">
         <f>"Debts Or Credits For the Comming "&amp;TEXT(Main!B3,"mmmm dd yyyy")&amp;" to "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,1)-1,"mmmm dd yyyy"),TEXT(Main!B3+Main!B5-Main!B3,"dd mmmm yyyy"))</f>
         <v>Debts Or Credits For the Comming April 20 2024 to May 19 2024</v>
@@ -38414,7 +38414,7 @@
       <c r="D128" s="53"/>
       <c r="E128" s="54"/>
     </row>
-    <row r="129" ht="45" customHeight="1" spans="1:5">
+    <row r="129" ht="35" customHeight="1" spans="1:5">
       <c r="A129" s="52" t="s">
         <v>110</v>
       </c>
@@ -38427,7 +38427,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="130" ht="24.75" customHeight="1" spans="1:5">
+    <row r="130" ht="35" customHeight="1" spans="1:5">
       <c r="A130" s="58" t="s">
         <v>91</v>
       </c>
@@ -38438,7 +38438,7 @@
       <c r="D130" s="61"/>
       <c r="E130" s="71"/>
     </row>
-    <row r="131" ht="24.75" customHeight="1" spans="1:8">
+    <row r="131" ht="35" customHeight="1" spans="1:8">
       <c r="A131" s="62"/>
       <c r="B131" s="63"/>
       <c r="C131" s="64"/>
@@ -38450,7 +38450,7 @@
       <c r="G131" s="14"/>
       <c r="H131" s="14"/>
     </row>
-    <row r="132" ht="24.75" customHeight="1" spans="1:8">
+    <row r="132" ht="35" customHeight="1" spans="1:8">
       <c r="A132" s="62"/>
       <c r="B132" s="63"/>
       <c r="C132" s="64"/>
@@ -38462,7 +38462,7 @@
       <c r="G132" s="14"/>
       <c r="H132" s="14"/>
     </row>
-    <row r="133" ht="24.75" customHeight="1" spans="1:8">
+    <row r="133" ht="35" customHeight="1" spans="1:8">
       <c r="A133" s="62"/>
       <c r="B133" s="63"/>
       <c r="C133" s="64"/>
@@ -38474,7 +38474,7 @@
       <c r="G133" s="14"/>
       <c r="H133" s="14"/>
     </row>
-    <row r="134" ht="24.75" customHeight="1" spans="1:8">
+    <row r="134" ht="35" customHeight="1" spans="1:8">
       <c r="A134" s="62"/>
       <c r="B134" s="63"/>
       <c r="C134" s="64"/>
@@ -38486,7 +38486,7 @@
       <c r="G134" s="14"/>
       <c r="H134" s="14"/>
     </row>
-    <row r="135" ht="24.75" customHeight="1" spans="1:8">
+    <row r="135" ht="35" customHeight="1" spans="1:8">
       <c r="A135" s="62"/>
       <c r="B135" s="63"/>
       <c r="C135" s="64"/>
@@ -38498,7 +38498,7 @@
       <c r="G135" s="14"/>
       <c r="H135" s="14"/>
     </row>
-    <row r="136" ht="24.75" customHeight="1" spans="1:8">
+    <row r="136" ht="35" customHeight="1" spans="1:8">
       <c r="A136" s="62"/>
       <c r="B136" s="63"/>
       <c r="C136" s="64"/>
@@ -38510,7 +38510,7 @@
       <c r="G136" s="14"/>
       <c r="H136" s="14"/>
     </row>
-    <row r="137" ht="24.75" customHeight="1" spans="1:8">
+    <row r="137" ht="35" customHeight="1" spans="1:8">
       <c r="A137" s="62"/>
       <c r="B137" s="63"/>
       <c r="C137" s="64"/>
@@ -38522,7 +38522,7 @@
       <c r="G137" s="14"/>
       <c r="H137" s="14"/>
     </row>
-    <row r="138" ht="24.75" customHeight="1" spans="1:8">
+    <row r="138" ht="35" customHeight="1" spans="1:8">
       <c r="A138" s="62"/>
       <c r="B138" s="63"/>
       <c r="C138" s="64"/>
@@ -38534,7 +38534,7 @@
       <c r="G138" s="14"/>
       <c r="H138" s="14"/>
     </row>
-    <row r="139" ht="24.75" customHeight="1" spans="1:8">
+    <row r="139" ht="35" customHeight="1" spans="1:8">
       <c r="A139" s="62"/>
       <c r="B139" s="63"/>
       <c r="C139" s="64"/>
@@ -38546,7 +38546,7 @@
       <c r="G139" s="14"/>
       <c r="H139" s="14"/>
     </row>
-    <row r="140" ht="24.75" customHeight="1" spans="1:8">
+    <row r="140" ht="35" customHeight="1" spans="1:8">
       <c r="A140" s="62"/>
       <c r="B140" s="63"/>
       <c r="C140" s="64"/>
@@ -38558,7 +38558,7 @@
       <c r="G140" s="14"/>
       <c r="H140" s="14"/>
     </row>
-    <row r="141" ht="24.75" customHeight="1" spans="1:5">
+    <row r="141" ht="35" customHeight="1" spans="1:5">
       <c r="A141" s="62"/>
       <c r="B141" s="63"/>
       <c r="C141" s="66" t="s">
@@ -38567,7 +38567,7 @@
       <c r="D141" s="61"/>
       <c r="E141" s="71"/>
     </row>
-    <row r="142" ht="45" customHeight="1" spans="1:5">
+    <row r="142" ht="35" customHeight="1" spans="1:5">
       <c r="A142" s="62"/>
       <c r="B142" s="63"/>
       <c r="C142" s="72"/>
@@ -38576,7 +38576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" ht="24.75" customHeight="1" spans="1:5">
+    <row r="143" ht="35" customHeight="1" spans="1:5">
       <c r="A143" s="62"/>
       <c r="B143" s="63"/>
       <c r="C143" s="64"/>
@@ -38585,7 +38585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" ht="24.75" customHeight="1" spans="1:5">
+    <row r="144" ht="35" customHeight="1" spans="1:5">
       <c r="A144" s="62"/>
       <c r="B144" s="63"/>
       <c r="C144" s="64"/>
@@ -38594,7 +38594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" ht="24" customHeight="1" spans="1:5">
+    <row r="145" ht="35" customHeight="1" spans="1:5">
       <c r="A145" s="62"/>
       <c r="B145" s="63"/>
       <c r="C145" s="64"/>
@@ -38603,7 +38603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" ht="24.75" customHeight="1" spans="1:5">
+    <row r="146" ht="35" customHeight="1" spans="1:5">
       <c r="A146" s="62"/>
       <c r="B146" s="63"/>
       <c r="C146" s="64"/>
@@ -38612,7 +38612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" ht="24.75" customHeight="1" spans="1:5">
+    <row r="147" ht="35" customHeight="1" spans="1:5">
       <c r="A147" s="74"/>
       <c r="B147" s="75"/>
       <c r="C147" s="64"/>
@@ -38621,7 +38621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" ht="24.75" customHeight="1" spans="1:5">
+    <row r="148" ht="35" customHeight="1" spans="1:5">
       <c r="A148" s="55" t="s">
         <v>113</v>
       </c>
@@ -38633,7 +38633,7 @@
         <v>1503</v>
       </c>
     </row>
-    <row r="149" ht="45" customHeight="1" spans="1:5">
+    <row r="149" ht="35" customHeight="1" spans="1:5">
       <c r="A149" s="79"/>
       <c r="B149" s="80"/>
       <c r="C149" s="81" t="s">
@@ -38644,8 +38644,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" ht="21.75" customHeight="1"/>
-    <row r="154" ht="24.75" customHeight="1" spans="1:5">
+    <row r="150" ht="35" customHeight="1"/>
+    <row r="151" ht="35" customHeight="1"/>
+    <row r="152" ht="35" customHeight="1"/>
+    <row r="153" ht="35" customHeight="1"/>
+    <row r="154" ht="35" customHeight="1" spans="1:5">
       <c r="A154" s="52" t="str">
         <f>"Debts Or Credits For the Comming "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,1),"mmmm dd yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)+1,"mmmm dd yyyy"))&amp;" to "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,2)-1,"dd mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)*2+1,"dd mmmm yyyy"))</f>
         <v>Debts Or Credits For the Comming May 20 2024 to 19 June 2024</v>
@@ -38655,7 +38658,7 @@
       <c r="D154" s="53"/>
       <c r="E154" s="54"/>
     </row>
-    <row r="155" ht="24.75" customHeight="1" spans="1:5">
+    <row r="155" ht="35" customHeight="1" spans="1:5">
       <c r="A155" s="52" t="s">
         <v>110</v>
       </c>
@@ -38668,7 +38671,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="156" ht="24.75" customHeight="1" spans="1:5">
+    <row r="156" ht="35" customHeight="1" spans="1:5">
       <c r="A156" s="55" t="str">
         <f>"Balance Brought Forward From "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,1)-1,"mmmm yyyy"),TEXT(Main!B3+Main!B5-Main!B3,"mmmm yyyy"))</f>
         <v>Balance Brought Forward From May 2024</v>
@@ -38681,7 +38684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" ht="24.75" customHeight="1" spans="1:5">
+    <row r="157" ht="35" customHeight="1" spans="1:5">
       <c r="A157" s="58" t="s">
         <v>91</v>
       </c>
@@ -38692,7 +38695,7 @@
       <c r="D157" s="85"/>
       <c r="E157" s="89"/>
     </row>
-    <row r="158" ht="24.75" customHeight="1" spans="1:8">
+    <row r="158" ht="35" customHeight="1" spans="1:8">
       <c r="A158" s="62"/>
       <c r="B158" s="63"/>
       <c r="C158" s="64" t="s">
@@ -38706,7 +38709,7 @@
       <c r="G158" s="14"/>
       <c r="H158" s="14"/>
     </row>
-    <row r="159" ht="24.75" customHeight="1" spans="1:8">
+    <row r="159" ht="35" customHeight="1" spans="1:8">
       <c r="A159" s="62"/>
       <c r="B159" s="63"/>
       <c r="C159" s="72" t="s">
@@ -38720,7 +38723,7 @@
       <c r="G159" s="14"/>
       <c r="H159" s="14"/>
     </row>
-    <row r="160" ht="24.75" customHeight="1" spans="1:8">
+    <row r="160" ht="35" customHeight="1" spans="1:8">
       <c r="A160" s="62"/>
       <c r="B160" s="63"/>
       <c r="C160" s="64"/>
@@ -38732,7 +38735,7 @@
       <c r="G160" s="14"/>
       <c r="H160" s="14"/>
     </row>
-    <row r="161" ht="24.75" customHeight="1" spans="1:8">
+    <row r="161" ht="35" customHeight="1" spans="1:8">
       <c r="A161" s="62"/>
       <c r="B161" s="63"/>
       <c r="C161" s="64"/>
@@ -38744,7 +38747,7 @@
       <c r="G161" s="14"/>
       <c r="H161" s="14"/>
     </row>
-    <row r="162" ht="24.75" customHeight="1" spans="1:8">
+    <row r="162" ht="35" customHeight="1" spans="1:8">
       <c r="A162" s="62"/>
       <c r="B162" s="63"/>
       <c r="C162" s="64"/>
@@ -38756,7 +38759,7 @@
       <c r="G162" s="14"/>
       <c r="H162" s="14"/>
     </row>
-    <row r="163" ht="24.75" customHeight="1" spans="1:8">
+    <row r="163" ht="35" customHeight="1" spans="1:8">
       <c r="A163" s="62"/>
       <c r="B163" s="63"/>
       <c r="C163" s="64"/>
@@ -38768,7 +38771,7 @@
       <c r="G163" s="14"/>
       <c r="H163" s="14"/>
     </row>
-    <row r="164" ht="22.5" customHeight="1" spans="1:8">
+    <row r="164" ht="35" customHeight="1" spans="1:8">
       <c r="A164" s="62"/>
       <c r="B164" s="63"/>
       <c r="C164" s="64"/>
@@ -38780,7 +38783,7 @@
       <c r="G164" s="14"/>
       <c r="H164" s="14"/>
     </row>
-    <row r="165" ht="24.75" customHeight="1" spans="1:8">
+    <row r="165" ht="35" customHeight="1" spans="1:8">
       <c r="A165" s="62"/>
       <c r="B165" s="63"/>
       <c r="C165" s="64"/>
@@ -38792,7 +38795,7 @@
       <c r="G165" s="14"/>
       <c r="H165" s="14"/>
     </row>
-    <row r="166" ht="24.75" customHeight="1" spans="1:8">
+    <row r="166" ht="35" customHeight="1" spans="1:8">
       <c r="A166" s="62"/>
       <c r="B166" s="63"/>
       <c r="C166" s="64"/>
@@ -38804,7 +38807,7 @@
       <c r="G166" s="14"/>
       <c r="H166" s="14"/>
     </row>
-    <row r="167" ht="24.75" customHeight="1" spans="1:8">
+    <row r="167" ht="35" customHeight="1" spans="1:8">
       <c r="A167" s="62"/>
       <c r="B167" s="63"/>
       <c r="C167" s="64"/>
@@ -38816,7 +38819,7 @@
       <c r="G167" s="14"/>
       <c r="H167" s="14"/>
     </row>
-    <row r="168" ht="24.75" customHeight="1" spans="1:5">
+    <row r="168" ht="35" customHeight="1" spans="1:5">
       <c r="A168" s="62"/>
       <c r="B168" s="63"/>
       <c r="C168" s="66" t="s">
@@ -38825,7 +38828,7 @@
       <c r="D168" s="61"/>
       <c r="E168" s="71"/>
     </row>
-    <row r="169" ht="24.75" customHeight="1" spans="1:5">
+    <row r="169" ht="35" customHeight="1" spans="1:5">
       <c r="A169" s="62"/>
       <c r="B169" s="63"/>
       <c r="C169" s="109" t="s">
@@ -38836,7 +38839,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="170" ht="24.75" customHeight="1" spans="1:5">
+    <row r="170" ht="35" customHeight="1" spans="1:5">
       <c r="A170" s="62"/>
       <c r="B170" s="63"/>
       <c r="C170" s="109" t="s">
@@ -38847,7 +38850,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="171" ht="24.75" customHeight="1" spans="1:5">
+    <row r="171" ht="35" customHeight="1" spans="1:5">
       <c r="A171" s="62"/>
       <c r="B171" s="63"/>
       <c r="C171" s="109" t="s">
@@ -38858,7 +38861,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="172" ht="40" customHeight="1" spans="1:5">
+    <row r="172" ht="35" customHeight="1" spans="1:5">
       <c r="A172" s="62"/>
       <c r="B172" s="63"/>
       <c r="C172" s="100" t="s">
@@ -38869,7 +38872,7 @@
         <v>775.68</v>
       </c>
     </row>
-    <row r="173" ht="24.75" customHeight="1" spans="1:5">
+    <row r="173" ht="35" customHeight="1" spans="1:5">
       <c r="A173" s="62"/>
       <c r="B173" s="63"/>
       <c r="C173" s="64"/>
@@ -38878,7 +38881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" ht="24.75" customHeight="1" spans="1:5">
+    <row r="174" ht="35" customHeight="1" spans="1:5">
       <c r="A174" s="74"/>
       <c r="B174" s="75"/>
       <c r="C174" s="64"/>
@@ -38887,7 +38890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" ht="24.75" customHeight="1" spans="1:5">
+    <row r="175" ht="35" customHeight="1" spans="1:5">
       <c r="A175" s="55" t="s">
         <v>113</v>
       </c>
@@ -38899,7 +38902,7 @@
         <v>1503</v>
       </c>
     </row>
-    <row r="176" ht="24.75" customHeight="1" spans="1:5">
+    <row r="176" ht="35" customHeight="1" spans="1:5">
       <c r="A176" s="79"/>
       <c r="B176" s="80"/>
       <c r="C176" s="81" t="s">
@@ -38911,8 +38914,11 @@
         <v>-416.68</v>
       </c>
     </row>
-    <row r="180" ht="24.75" customHeight="1"/>
-    <row r="181" ht="24.75" customHeight="1" spans="1:5">
+    <row r="177" ht="35" customHeight="1"/>
+    <row r="178" ht="35" customHeight="1"/>
+    <row r="179" ht="35" customHeight="1"/>
+    <row r="180" ht="35" customHeight="1"/>
+    <row r="181" ht="35" customHeight="1" spans="1:5">
       <c r="A181" s="52" t="str">
         <f>"Debts Or Credits For the Comming "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,2),"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*2)+2,"dd mmmm yyyy"))&amp;" to "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,3)-1,"dd mmmm yyyy"),TEXT(Main!B3+((Main!B5-Main!B3)*3+2),"dd mmmm yyyy"))</f>
         <v>Debts Or Credits For the Comming 20 June 2024 to 19 July 2024</v>
@@ -38922,7 +38928,7 @@
       <c r="D181" s="53"/>
       <c r="E181" s="54"/>
     </row>
-    <row r="182" ht="24.75" customHeight="1" spans="1:5">
+    <row r="182" ht="35" customHeight="1" spans="1:5">
       <c r="A182" s="52" t="s">
         <v>110</v>
       </c>
@@ -38935,7 +38941,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="183" ht="24.75" customHeight="1" spans="1:5">
+    <row r="183" ht="35" customHeight="1" spans="1:5">
       <c r="A183" s="55" t="str">
         <f>"Balance Brought Forward From "&amp;IF(Main!B2,TEXT(EDATE(Main!B3,2)-1,"mmmm yyyy"),TEXT(Main!B3+(Main!B5-Main!B3)*2+1,"mmmm yyyy"))</f>
         <v>Balance Brought Forward From June 2024</v>
@@ -38948,7 +38954,7 @@
         <v>-416.68</v>
       </c>
     </row>
-    <row r="184" ht="24.75" customHeight="1" spans="1:5">
+    <row r="184" ht="35" customHeight="1" spans="1:5">
       <c r="A184" s="58" t="s">
         <v>91</v>
       </c>
@@ -38959,7 +38965,7 @@
       <c r="D184" s="85"/>
       <c r="E184" s="89"/>
     </row>
-    <row r="185" ht="24.75" customHeight="1" spans="1:8">
+    <row r="185" ht="35" customHeight="1" spans="1:8">
       <c r="A185" s="62"/>
       <c r="B185" s="63"/>
       <c r="C185" s="109" t="s">
@@ -38973,7 +38979,7 @@
       <c r="G185" s="14"/>
       <c r="H185" s="14"/>
     </row>
-    <row r="186" ht="24.75" customHeight="1" spans="1:8">
+    <row r="186" ht="35" customHeight="1" spans="1:8">
       <c r="A186" s="62"/>
       <c r="B186" s="63"/>
       <c r="C186" s="64" t="s">
@@ -38987,7 +38993,7 @@
       <c r="G186" s="14"/>
       <c r="H186" s="14"/>
     </row>
-    <row r="187" ht="24.75" customHeight="1" spans="1:8">
+    <row r="187" ht="35" customHeight="1" spans="1:8">
       <c r="A187" s="62"/>
       <c r="B187" s="63"/>
       <c r="C187" s="64"/>
@@ -38999,7 +39005,7 @@
       <c r="G187" s="14"/>
       <c r="H187" s="14"/>
     </row>
-    <row r="188" ht="24.75" customHeight="1" spans="1:8">
+    <row r="188" ht="35" customHeight="1" spans="1:8">
       <c r="A188" s="62"/>
       <c r="B188" s="63"/>
       <c r="C188" s="64"/>
@@ -39011,7 +39017,7 @@
       <c r="G188" s="14"/>
       <c r="H188" s="14"/>
     </row>
-    <row r="189" ht="24.75" customHeight="1" spans="1:8">
+    <row r="189" ht="35" customHeight="1" spans="1:8">
       <c r="A189" s="62"/>
       <c r="B189" s="63"/>
       <c r="C189" s="64"/>
@@ -39023,7 +39029,7 @@
       <c r="G189" s="14"/>
       <c r="H189" s="14"/>
     </row>
-    <row r="190" ht="24.75" customHeight="1" spans="1:8">
+    <row r="190" ht="35" customHeight="1" spans="1:8">
       <c r="A190" s="62"/>
       <c r="B190" s="63"/>
       <c r="C190" s="64"/>
@@ -39035,7 +39041,7 @@
       <c r="G190" s="14"/>
       <c r="H190" s="14"/>
     </row>
-    <row r="191" ht="24.75" customHeight="1" spans="1:8">
+    <row r="191" ht="35" customHeight="1" spans="1:8">
       <c r="A191" s="62"/>
       <c r="B191" s="63"/>
       <c r="C191" s="64"/>
@@ -39047,7 +39053,7 @@
       <c r="G191" s="14"/>
       <c r="H191" s="14"/>
     </row>
-    <row r="192" ht="24.75" customHeight="1" spans="1:8">
+    <row r="192" ht="35" customHeight="1" spans="1:8">
       <c r="A192" s="62"/>
       <c r="B192" s="63"/>
       <c r="C192" s="64"/>
@@ -39059,7 +39065,7 @@
       <c r="G192" s="14"/>
       <c r="H192" s="14"/>
     </row>
-    <row r="193" ht="24.75" customHeight="1" spans="1:8">
+    <row r="193" ht="35" customHeight="1" spans="1:8">
       <c r="A193" s="62"/>
       <c r="B193" s="63"/>
       <c r="C193" s="64"/>
@@ -39071,7 +39077,7 @@
       <c r="G193" s="14"/>
       <c r="H193" s="14"/>
     </row>
-    <row r="194" ht="24.75" customHeight="1" spans="1:8">
+    <row r="194" ht="35" customHeight="1" spans="1:8">
       <c r="A194" s="62"/>
       <c r="B194" s="63"/>
       <c r="C194" s="64"/>
@@ -39083,7 +39089,7 @@
       <c r="G194" s="14"/>
       <c r="H194" s="14"/>
     </row>
-    <row r="195" ht="24.75" customHeight="1" spans="1:5">
+    <row r="195" ht="35" customHeight="1" spans="1:5">
       <c r="A195" s="62"/>
       <c r="B195" s="63"/>
       <c r="C195" s="66" t="s">
@@ -39092,7 +39098,7 @@
       <c r="D195" s="61"/>
       <c r="E195" s="71"/>
     </row>
-    <row r="196" ht="24.75" customHeight="1" spans="1:5">
+    <row r="196" ht="35" customHeight="1" spans="1:5">
       <c r="A196" s="62"/>
       <c r="B196" s="63"/>
       <c r="C196" s="109" t="s">
@@ -39103,7 +39109,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="197" ht="24.75" customHeight="1" spans="1:5">
+    <row r="197" ht="35" customHeight="1" spans="1:5">
       <c r="A197" s="62"/>
       <c r="B197" s="63"/>
       <c r="C197" s="100" t="s">
@@ -39114,7 +39120,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="198" ht="24.75" customHeight="1" spans="1:5">
+    <row r="198" ht="35" customHeight="1" spans="1:5">
       <c r="A198" s="62"/>
       <c r="B198" s="63"/>
       <c r="C198" s="109" t="s">
@@ -39125,7 +39131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" ht="214" customHeight="1" spans="1:5">
+    <row r="199" ht="35" customHeight="1" spans="1:5">
       <c r="A199" s="62"/>
       <c r="B199" s="63"/>
       <c r="C199" s="72" t="s">
@@ -39136,7 +39142,7 @@
         <v>2556</v>
       </c>
     </row>
-    <row r="200" ht="24.75" customHeight="1" spans="1:5">
+    <row r="200" ht="35" customHeight="1" spans="1:5">
       <c r="A200" s="62"/>
       <c r="B200" s="63"/>
       <c r="C200" s="64" t="s">
@@ -39147,7 +39153,7 @@
         <v>966.7</v>
       </c>
     </row>
-    <row r="201" ht="24.75" customHeight="1" spans="1:5">
+    <row r="201" ht="35" customHeight="1" spans="1:5">
       <c r="A201" s="74"/>
       <c r="B201" s="75"/>
       <c r="C201" s="64"/>
@@ -39156,7 +39162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" ht="24.75" customHeight="1" spans="1:5">
+    <row r="202" ht="35" customHeight="1" spans="1:5">
       <c r="A202" s="55" t="s">
         <v>113</v>
       </c>
@@ -39168,7 +39174,7 @@
         <v>1503</v>
       </c>
     </row>
-    <row r="203" ht="24.75" customHeight="1" spans="1:5">
+    <row r="203" ht="35" customHeight="1" spans="1:5">
       <c r="A203" s="79"/>
       <c r="B203" s="80"/>
       <c r="C203" s="81" t="s">
@@ -39180,7 +39186,7 @@
         <v>3260.12</v>
       </c>
     </row>
-    <row r="204" ht="24.75" customHeight="1"/>
+    <row r="204" ht="35" customHeight="1"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="170">
@@ -39649,7 +39655,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
+    <sheetView topLeftCell="A107" workbookViewId="0">
       <selection activeCell="F124" sqref="F124"/>
     </sheetView>
   </sheetViews>
@@ -43106,7 +43112,7 @@
   <sheetPr/>
   <dimension ref="A1:I192"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" workbookViewId="0">
+    <sheetView topLeftCell="A182" workbookViewId="0">
       <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
@@ -46655,7 +46661,7 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A174" workbookViewId="0">
+    <sheetView topLeftCell="A157" workbookViewId="0">
       <selection activeCell="F184" sqref="F184"/>
     </sheetView>
   </sheetViews>
@@ -50168,8 +50174,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="C130" sqref="C130:D130"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="E120" sqref="E120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -50220,7 +50226,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>3661.8</v>
+        <v>2161.8</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -50236,7 +50242,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>4052.2</v>
+        <v>2552.2</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -50252,7 +50258,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-6983</v>
+        <v>-5483</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -51785,7 +51791,7 @@
       </c>
       <c r="C98" s="36" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B18")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-5900</v>
+        <v>-4400</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -51981,7 +51987,7 @@
       </c>
       <c r="C108" s="36">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-6983</v>
+        <v>-5483</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -51997,7 +52003,7 @@
       </c>
       <c r="C109" s="36">
         <f ca="1">C108-C96</f>
-        <v>-7330</v>
+        <v>-5830</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -52273,7 +52279,7 @@
       <c r="H129" s="14"/>
       <c r="I129" s="47"/>
     </row>
-    <row r="130" ht="197" customHeight="1" spans="1:9">
+    <row r="130" ht="143" customHeight="1" spans="1:9">
       <c r="A130" s="62"/>
       <c r="B130" s="63"/>
       <c r="C130" s="113" t="s">
@@ -52483,11 +52489,11 @@
       <c r="A145" s="62"/>
       <c r="B145" s="63"/>
       <c r="C145" s="109" t="s">
-        <v>115</v>
+        <v>152</v>
       </c>
       <c r="D145" s="109"/>
       <c r="E145" s="36">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="F145" s="14"/>
       <c r="G145" s="14"/>
@@ -52639,7 +52645,7 @@
       <c r="H156" s="14"/>
       <c r="I156" s="47"/>
     </row>
-    <row r="157" ht="185" customHeight="1" spans="1:9">
+    <row r="157" ht="156" customHeight="1" spans="1:9">
       <c r="A157" s="62"/>
       <c r="B157" s="63"/>
       <c r="C157" s="100" t="s">
@@ -52731,7 +52737,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>2935</v>
+        <v>1935</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -52823,7 +52829,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>2935</v>
+        <v>1935</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -52849,11 +52855,11 @@
       <c r="A172" s="62"/>
       <c r="B172" s="63"/>
       <c r="C172" s="109" t="s">
-        <v>115</v>
+        <v>240</v>
       </c>
       <c r="D172" s="109"/>
       <c r="E172" s="36">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="F172" s="14"/>
       <c r="G172" s="14"/>
@@ -53005,7 +53011,7 @@
       <c r="H183" s="14"/>
       <c r="I183" s="47"/>
     </row>
-    <row r="184" ht="184" customHeight="1" spans="1:9">
+    <row r="184" ht="160" customHeight="1" spans="1:9">
       <c r="A184" s="62"/>
       <c r="B184" s="63"/>
       <c r="C184" s="100" t="s">
@@ -53097,7 +53103,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>3661.8</v>
+        <v>2161.8</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -53613,8 +53619,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="F132" sqref="F132"/>
+    <sheetView topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="F157" sqref="F157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -53663,7 +53669,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>3004.2</v>
+        <v>1504.2</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -53679,7 +53685,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>3394.6</v>
+        <v>1894.6</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -53695,7 +53701,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>-3983</v>
+        <v>-2483</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -55220,7 +55226,7 @@
       </c>
       <c r="C98" s="108" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>-2900</v>
+        <v>-1400</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -55416,7 +55422,7 @@
       </c>
       <c r="C108" s="108">
         <f ca="1">SUM(C98:C107)</f>
-        <v>-3983</v>
+        <v>-2483</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -55432,7 +55438,7 @@
       </c>
       <c r="C109" s="108">
         <f ca="1">C108-C96</f>
-        <v>-4330</v>
+        <v>-2830</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -55526,7 +55532,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B21")&amp;"'!E190")</f>
-        <v>3661.8</v>
+        <v>2161.8</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -55693,7 +55699,7 @@
       <c r="H128" s="14"/>
       <c r="I128" s="47"/>
     </row>
-    <row r="129" ht="131" customHeight="1" spans="1:9">
+    <row r="129" ht="104" customHeight="1" spans="1:9">
       <c r="A129" s="62"/>
       <c r="B129" s="63"/>
       <c r="C129" s="100" t="s">
@@ -55708,7 +55714,7 @@
       <c r="H129" s="14"/>
       <c r="I129" s="47"/>
     </row>
-    <row r="130" ht="208" customHeight="1" spans="1:9">
+    <row r="130" ht="149" customHeight="1" spans="1:9">
       <c r="A130" s="62"/>
       <c r="B130" s="63"/>
       <c r="C130" s="100" t="s">
@@ -55800,7 +55806,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>3494.6</v>
+        <v>1994.6</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -55892,7 +55898,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>3494.6</v>
+        <v>1994.6</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -56074,7 +56080,7 @@
       <c r="H156" s="14"/>
       <c r="I156" s="47"/>
     </row>
-    <row r="157" ht="180" customHeight="1" spans="1:9">
+    <row r="157" ht="150" customHeight="1" spans="1:9">
       <c r="A157" s="62"/>
       <c r="B157" s="63"/>
       <c r="C157" s="100" t="s">
@@ -56166,7 +56172,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>3171.4</v>
+        <v>1671.4</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -56258,7 +56264,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>3171.4</v>
+        <v>1671.4</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -56440,7 +56446,7 @@
       <c r="H183" s="14"/>
       <c r="I183" s="47"/>
     </row>
-    <row r="184" ht="194" customHeight="1" spans="1:9">
+    <row r="184" ht="163" customHeight="1" spans="1:9">
       <c r="A184" s="62"/>
       <c r="B184" s="63"/>
       <c r="C184" s="100" t="s">
@@ -56532,7 +56538,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>3004.2</v>
+        <v>1504.2</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>
@@ -57042,8 +57048,8 @@
   <sheetPr/>
   <dimension ref="A1:I193"/>
   <sheetViews>
-    <sheetView topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="F134" sqref="F134"/>
+    <sheetView topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="C118" sqref="C118:D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6"/>
@@ -57092,7 +57098,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">E190</f>
-        <v>1072.6</v>
+        <v>3555.6</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -57108,7 +57114,7 @@
       <c r="B4" s="9"/>
       <c r="C4" s="10">
         <f ca="1">SUM(C2:G3)</f>
-        <v>1463</v>
+        <v>3946</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -57124,7 +57130,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="12">
         <f ca="1">C108</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -58649,7 +58655,7 @@
       </c>
       <c r="C98" s="108" cm="1">
         <f ca="1" t="array" ref="C98">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!C98")+SUM(E118+E145+E172)</f>
-        <v>0</v>
+        <v>-1400</v>
       </c>
       <c r="D98" s="14"/>
       <c r="E98" s="94"/>
@@ -58749,7 +58755,7 @@
       </c>
       <c r="C103" s="108" cm="1">
         <f ca="1" t="array" ref="C103">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!C103")+SUM(E123+E150+E177)</f>
-        <v>0</v>
+        <v>-1083</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
@@ -58845,7 +58851,7 @@
       </c>
       <c r="C108" s="108">
         <f ca="1">SUM(C98:C107)</f>
-        <v>0</v>
+        <v>-2483</v>
       </c>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
@@ -58861,7 +58867,7 @@
       </c>
       <c r="C109" s="108">
         <f ca="1">C108-C96</f>
-        <v>-347</v>
+        <v>-2830</v>
       </c>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
@@ -58955,7 +58961,7 @@
       <c r="D116" s="57"/>
       <c r="E116" s="70" cm="1">
         <f ca="1" t="array" ref="E116">INDIRECT("'"&amp;INDIRECT("Main!B24")&amp;"'!E190")</f>
-        <v>3004.2</v>
+        <v>1504.2</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -58980,12 +58986,10 @@
     <row r="118" ht="24.75" customHeight="1" spans="1:9">
       <c r="A118" s="62"/>
       <c r="B118" s="63"/>
-      <c r="C118" s="64" t="s">
-        <v>152</v>
-      </c>
+      <c r="C118" s="64"/>
       <c r="D118" s="65"/>
       <c r="E118" s="36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F118" s="14"/>
       <c r="G118" s="14"/>
@@ -59229,7 +59233,7 @@
       <c r="D136" s="81"/>
       <c r="E136" s="87">
         <f ca="1">(F16+E116)-(SUM(E118:E127)+SUM(E129:E135))</f>
-        <v>2731</v>
+        <v>2231</v>
       </c>
       <c r="F136" s="14"/>
       <c r="G136" s="14"/>
@@ -59321,7 +59325,7 @@
       <c r="D143" s="57"/>
       <c r="E143" s="87">
         <f ca="1">E136</f>
-        <v>2731</v>
+        <v>2231</v>
       </c>
       <c r="F143" s="14"/>
       <c r="G143" s="14"/>
@@ -59346,12 +59350,10 @@
     <row r="145" ht="24.75" customHeight="1" spans="1:9">
       <c r="A145" s="62"/>
       <c r="B145" s="63"/>
-      <c r="C145" s="64" t="s">
-        <v>152</v>
-      </c>
+      <c r="C145" s="64"/>
       <c r="D145" s="65"/>
       <c r="E145" s="36">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F145" s="14"/>
       <c r="G145" s="14"/>
@@ -59413,12 +59415,10 @@
     <row r="150" ht="24.75" customHeight="1" spans="1:9">
       <c r="A150" s="62"/>
       <c r="B150" s="63"/>
-      <c r="C150" s="64" t="s">
-        <v>267</v>
-      </c>
+      <c r="C150" s="64"/>
       <c r="D150" s="65"/>
       <c r="E150" s="36">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="F150" s="14"/>
       <c r="G150" s="14"/>
@@ -59494,7 +59494,7 @@
       <c r="A156" s="62"/>
       <c r="B156" s="63"/>
       <c r="C156" s="100" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D156" s="100"/>
       <c r="E156" s="102">
@@ -59597,7 +59597,7 @@
       <c r="D163" s="81"/>
       <c r="E163" s="90">
         <f ca="1">(F28+E143)-(SUM(E145:E154)+SUM(E156:E162))</f>
-        <v>2013.8</v>
+        <v>3013.8</v>
       </c>
       <c r="F163" s="14"/>
       <c r="G163" s="14"/>
@@ -59689,7 +59689,7 @@
       <c r="D170" s="57"/>
       <c r="E170" s="90">
         <f ca="1">E163</f>
-        <v>2013.8</v>
+        <v>3013.8</v>
       </c>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>
@@ -59714,12 +59714,10 @@
     <row r="172" ht="24.75" customHeight="1" spans="1:9">
       <c r="A172" s="62"/>
       <c r="B172" s="63"/>
-      <c r="C172" s="64" t="s">
-        <v>269</v>
-      </c>
+      <c r="C172" s="64"/>
       <c r="D172" s="65"/>
       <c r="E172" s="36">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="F172" s="14"/>
       <c r="G172" s="14"/>
@@ -59781,12 +59779,10 @@
     <row r="177" ht="24.75" customHeight="1" spans="1:9">
       <c r="A177" s="62"/>
       <c r="B177" s="63"/>
-      <c r="C177" s="64" t="s">
-        <v>270</v>
-      </c>
+      <c r="C177" s="64"/>
       <c r="D177" s="65"/>
       <c r="E177" s="36">
-        <v>583</v>
+        <v>0</v>
       </c>
       <c r="F177" s="14"/>
       <c r="G177" s="14"/>
@@ -59858,11 +59854,11 @@
       <c r="H182" s="14"/>
       <c r="I182" s="47"/>
     </row>
-    <row r="183" ht="88" customHeight="1" spans="1:9">
+    <row r="183" ht="66" customHeight="1" spans="1:9">
       <c r="A183" s="62"/>
       <c r="B183" s="63"/>
       <c r="C183" s="100" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D183" s="100"/>
       <c r="E183" s="98">
@@ -59873,7 +59869,7 @@
       <c r="H183" s="14"/>
       <c r="I183" s="47"/>
     </row>
-    <row r="184" ht="118" customHeight="1" spans="1:9">
+    <row r="184" ht="33" customHeight="1" spans="1:9">
       <c r="A184" s="62"/>
       <c r="B184" s="63"/>
       <c r="C184" s="100" t="s">
@@ -59965,7 +59961,7 @@
       <c r="D190" s="81"/>
       <c r="E190" s="90">
         <f ca="1">(F40+E170)-(SUM(E172:E181)+SUM(E183:E189))</f>
-        <v>1072.6</v>
+        <v>3555.6</v>
       </c>
       <c r="F190" s="14"/>
       <c r="G190" s="14"/>

</xml_diff>